<commit_message>
finish refactoring of charts into the pages module and the config modules
</commit_message>
<xml_diff>
--- a/docs/session_variables.xlsx
+++ b/docs/session_variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robhay/git_repo/share_screener/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6667071-6BF0-DE42-B272-59D28EA6ACB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8907D4-EFF6-024D-A5EB-1A4C2B368E96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="25600" windowHeight="14300" xr2:uid="{EB3C945B-FE01-FA47-AE59-A0DC3CDF521B}"/>
   </bookViews>
@@ -3587,7 +3587,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="CK1" sqref="CK1:CU1048576"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
fix issue with user settings not being added to the page.template properly
</commit_message>
<xml_diff>
--- a/docs/session_variables.xlsx
+++ b/docs/session_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robhay/git_repo/share_screener/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FB1273-FFD1-5341-B04F-9B40A0E5C995}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752C6711-90D1-BE4F-BD05-366E79C23321}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25620" yWindow="12040" windowWidth="25600" windowHeight="15500" xr2:uid="{EB3C945B-FE01-FA47-AE59-A0DC3CDF521B}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14300" xr2:uid="{EB3C945B-FE01-FA47-AE59-A0DC3CDF521B}"/>
   </bookViews>
   <sheets>
     <sheet name="Application Structure" sheetId="6" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="518">
   <si>
     <t>chart_colours</t>
   </si>
@@ -1840,6 +1840,48 @@
   </si>
   <si>
     <t>Login to Use the Application</t>
+  </si>
+  <si>
+    <t>user_list</t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>Rob,
+Fliss</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="7" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>login_name</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>ticker_search</t>
+  </si>
+  <si>
+    <t>search_results</t>
   </si>
 </sst>
 </file>
@@ -2417,7 +2459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="299">
+  <cellXfs count="313">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2865,6 +2907,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2877,153 +2925,147 @@
     <xf numFmtId="0" fontId="38" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3296,6 +3338,48 @@
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3612,13 +3696,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB030FA-EA0F-904E-89A7-6D6B5810B515}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:FO47"/>
+  <dimension ref="A1:FR47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AQ7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="BH4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="BC18" sqref="BC18"/>
+      <selection pane="bottomRight" activeCell="BN3" sqref="BN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3668,38 +3752,40 @@
     <col min="50" max="51" width="10.33203125" customWidth="1"/>
     <col min="52" max="52" width="11" customWidth="1"/>
     <col min="53" max="53" width="7.6640625" customWidth="1"/>
-    <col min="54" max="54" width="12.6640625" customWidth="1"/>
-    <col min="55" max="57" width="7.6640625" customWidth="1"/>
-    <col min="58" max="58" width="10.5" customWidth="1"/>
-    <col min="59" max="59" width="9.83203125" customWidth="1"/>
-    <col min="60" max="60" width="4.83203125" customWidth="1"/>
-    <col min="61" max="61" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="63" width="10.5" customWidth="1"/>
-    <col min="64" max="64" width="9.6640625" customWidth="1"/>
-    <col min="65" max="65" width="5.33203125" customWidth="1"/>
-    <col min="66" max="66" width="13.1640625" customWidth="1"/>
-    <col min="67" max="67" width="7.5" customWidth="1"/>
-    <col min="68" max="68" width="8.83203125" customWidth="1"/>
-    <col min="69" max="70" width="12" customWidth="1"/>
-    <col min="71" max="71" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="72" max="73" width="10.1640625" customWidth="1"/>
-    <col min="74" max="74" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="11.5" customWidth="1"/>
-    <col min="77" max="79" width="9.33203125" customWidth="1"/>
-    <col min="80" max="80" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="10.33203125" customWidth="1"/>
-    <col min="82" max="82" width="7.83203125" customWidth="1"/>
-    <col min="83" max="83" width="13.83203125" customWidth="1"/>
-    <col min="84" max="84" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="6.6640625" customWidth="1"/>
-    <col min="87" max="90" width="5.1640625" customWidth="1"/>
-    <col min="91" max="91" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="12.6640625" customWidth="1"/>
+    <col min="56" max="58" width="7.6640625" customWidth="1"/>
+    <col min="59" max="59" width="10.5" customWidth="1"/>
+    <col min="60" max="60" width="9.83203125" customWidth="1"/>
+    <col min="61" max="61" width="16.1640625" customWidth="1"/>
+    <col min="62" max="62" width="4.83203125" customWidth="1"/>
+    <col min="63" max="63" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="64" max="65" width="10.5" customWidth="1"/>
+    <col min="66" max="66" width="9.6640625" customWidth="1"/>
+    <col min="67" max="67" width="5.33203125" customWidth="1"/>
+    <col min="68" max="68" width="13.1640625" customWidth="1"/>
+    <col min="69" max="69" width="7.5" customWidth="1"/>
+    <col min="70" max="70" width="8.83203125" customWidth="1"/>
+    <col min="71" max="72" width="12" customWidth="1"/>
+    <col min="73" max="73" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="74" max="75" width="10.1640625" customWidth="1"/>
+    <col min="76" max="76" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="6.6640625" customWidth="1"/>
+    <col min="78" max="78" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.5" customWidth="1"/>
+    <col min="80" max="82" width="9.33203125" customWidth="1"/>
+    <col min="83" max="83" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="10.33203125" customWidth="1"/>
+    <col min="85" max="85" width="7.83203125" customWidth="1"/>
+    <col min="86" max="86" width="13.83203125" customWidth="1"/>
+    <col min="87" max="87" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="6.6640625" customWidth="1"/>
+    <col min="90" max="93" width="5.1640625" customWidth="1"/>
+    <col min="94" max="94" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="4.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:171" ht="44">
+    <row r="1" spans="1:174" ht="44">
       <c r="A1" s="150" t="s">
         <v>481</v>
       </c>
@@ -3707,17 +3793,17 @@
         <v>505</v>
       </c>
     </row>
-    <row r="2" spans="1:171">
+    <row r="2" spans="1:174">
       <c r="A2" s="137" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="3" spans="1:171">
+    <row r="3" spans="1:174">
       <c r="A3" s="126" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="4" spans="1:171">
+    <row r="4" spans="1:174">
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -3769,12 +3855,12 @@
       <c r="AY4" s="6"/>
       <c r="AZ4" s="6"/>
     </row>
-    <row r="5" spans="1:171" s="60" customFormat="1" ht="37" customHeight="1">
+    <row r="5" spans="1:174" s="60" customFormat="1" ht="37" customHeight="1">
       <c r="A5" s="109" t="s">
         <v>343</v>
       </c>
       <c r="B5" s="108"/>
-      <c r="C5" s="158" t="s">
+      <c r="C5" s="160" t="s">
         <v>289</v>
       </c>
       <c r="D5" s="212" t="s">
@@ -3831,26 +3917,26 @@
       <c r="AY5" s="213"/>
       <c r="AZ5" s="213"/>
       <c r="BA5" s="214"/>
-      <c r="BB5" s="212" t="s">
+      <c r="BB5" s="299" t="s">
         <v>509</v>
       </c>
-      <c r="BC5" s="213"/>
-      <c r="BD5" s="213"/>
-      <c r="BE5" s="214"/>
-      <c r="BF5" s="212" t="s">
+      <c r="BC5" s="300"/>
+      <c r="BD5" s="300"/>
+      <c r="BE5" s="300"/>
+      <c r="BF5" s="301"/>
+      <c r="BG5" s="212" t="s">
         <v>310</v>
       </c>
-      <c r="BG5" s="213"/>
       <c r="BH5" s="213"/>
       <c r="BI5" s="213"/>
       <c r="BJ5" s="213"/>
       <c r="BK5" s="213"/>
-      <c r="BL5" s="214"/>
-      <c r="BM5" s="215" t="s">
+      <c r="BL5" s="213"/>
+      <c r="BM5" s="213"/>
+      <c r="BN5" s="214"/>
+      <c r="BO5" s="215" t="s">
         <v>257</v>
       </c>
-      <c r="BN5" s="215"/>
-      <c r="BO5" s="215"/>
       <c r="BP5" s="215"/>
       <c r="BQ5" s="215"/>
       <c r="BR5" s="215"/>
@@ -3863,12 +3949,12 @@
       <c r="BY5" s="215"/>
       <c r="BZ5" s="215"/>
       <c r="CA5" s="215"/>
-      <c r="CB5" s="216" t="s">
+      <c r="CB5" s="215"/>
+      <c r="CC5" s="215"/>
+      <c r="CD5" s="215"/>
+      <c r="CE5" s="216" t="s">
         <v>468</v>
       </c>
-      <c r="CC5" s="216"/>
-      <c r="CD5" s="216"/>
-      <c r="CE5" s="216"/>
       <c r="CF5" s="216"/>
       <c r="CG5" s="216"/>
       <c r="CH5" s="216"/>
@@ -3878,8 +3964,11 @@
       <c r="CL5" s="216"/>
       <c r="CM5" s="216"/>
       <c r="CN5" s="216"/>
-    </row>
-    <row r="6" spans="1:171" s="60" customFormat="1" ht="26" customHeight="1">
+      <c r="CO5" s="216"/>
+      <c r="CP5" s="216"/>
+      <c r="CQ5" s="216"/>
+    </row>
+    <row r="6" spans="1:174" s="60" customFormat="1" ht="26" customHeight="1">
       <c r="A6" s="204" t="s">
         <v>344</v>
       </c>
@@ -3951,83 +4040,90 @@
       <c r="AY6" s="184"/>
       <c r="AZ6" s="184"/>
       <c r="BA6" s="184"/>
-      <c r="BB6" s="185" t="s">
-        <v>509</v>
-      </c>
-      <c r="BC6" s="185" t="s">
-        <v>137</v>
-      </c>
-      <c r="BD6" s="185"/>
-      <c r="BE6" s="185"/>
-      <c r="BF6" s="185" t="s">
+      <c r="BB6" s="302" t="s">
+        <v>514</v>
+      </c>
+      <c r="BC6" s="303" t="s">
+        <v>511</v>
+      </c>
+      <c r="BD6" s="302" t="s">
+        <v>513</v>
+      </c>
+      <c r="BE6" s="304"/>
+      <c r="BF6" s="305"/>
+      <c r="BG6" s="185" t="s">
         <v>290</v>
       </c>
-      <c r="BG6" s="185" t="s">
+      <c r="BH6" s="185" t="s">
         <v>387</v>
       </c>
-      <c r="BH6" s="184" t="s">
+      <c r="BI6" s="185" t="s">
+        <v>516</v>
+      </c>
+      <c r="BJ6" s="184" t="s">
         <v>259</v>
       </c>
-      <c r="BI6" s="184"/>
-      <c r="BJ6" s="184"/>
       <c r="BK6" s="184"/>
       <c r="BL6" s="184"/>
-      <c r="BM6" s="163" t="s">
+      <c r="BM6" s="184"/>
+      <c r="BN6" s="184"/>
+      <c r="BO6" s="163" t="s">
         <v>353</v>
       </c>
-      <c r="BN6" s="163" t="s">
+      <c r="BP6" s="163" t="s">
         <v>354</v>
       </c>
-      <c r="BO6" s="163" t="s">
+      <c r="BQ6" s="163" t="s">
         <v>297</v>
       </c>
-      <c r="BP6" s="163" t="s">
+      <c r="BR6" s="163" t="s">
         <v>391</v>
       </c>
-      <c r="BQ6" s="178" t="s">
+      <c r="BS6" s="178" t="s">
         <v>266</v>
       </c>
-      <c r="BR6" s="180"/>
-      <c r="BS6" s="165" t="s">
+      <c r="BT6" s="180"/>
+      <c r="BU6" s="165" t="s">
         <v>480</v>
       </c>
-      <c r="BT6" s="169"/>
-      <c r="BU6" s="169"/>
       <c r="BV6" s="169"/>
       <c r="BW6" s="169"/>
       <c r="BX6" s="169"/>
       <c r="BY6" s="169"/>
       <c r="BZ6" s="169"/>
-      <c r="CA6" s="166"/>
-      <c r="CB6" s="163" t="s">
+      <c r="CA6" s="169"/>
+      <c r="CB6" s="169"/>
+      <c r="CC6" s="169"/>
+      <c r="CD6" s="166"/>
+      <c r="CE6" s="163" t="s">
         <v>137</v>
       </c>
-      <c r="CC6" s="163" t="s">
+      <c r="CF6" s="163" t="s">
         <v>283</v>
       </c>
-      <c r="CD6" s="165" t="s">
+      <c r="CG6" s="165" t="s">
         <v>306</v>
       </c>
-      <c r="CE6" s="166"/>
-      <c r="CF6" s="163" t="s">
+      <c r="CH6" s="166"/>
+      <c r="CI6" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="CG6" s="163" t="s">
+      <c r="CJ6" s="163" t="s">
         <v>386</v>
       </c>
-      <c r="CH6" s="165" t="s">
+      <c r="CK6" s="165" t="s">
         <v>305</v>
       </c>
-      <c r="CI6" s="169"/>
-      <c r="CJ6" s="169"/>
-      <c r="CK6" s="169"/>
-      <c r="CL6" s="166"/>
-      <c r="CM6" s="171" t="s">
+      <c r="CL6" s="169"/>
+      <c r="CM6" s="169"/>
+      <c r="CN6" s="169"/>
+      <c r="CO6" s="166"/>
+      <c r="CP6" s="171" t="s">
         <v>307</v>
       </c>
-      <c r="CN6" s="172"/>
-    </row>
-    <row r="7" spans="1:171" s="59" customFormat="1" ht="104" customHeight="1">
+      <c r="CQ6" s="172"/>
+    </row>
+    <row r="7" spans="1:174" s="59" customFormat="1" ht="104" customHeight="1">
       <c r="A7" s="204"/>
       <c r="B7" s="101"/>
       <c r="C7" s="177"/>
@@ -4085,47 +4181,50 @@
       <c r="AY7" s="184"/>
       <c r="AZ7" s="184"/>
       <c r="BA7" s="184"/>
-      <c r="BB7" s="185"/>
-      <c r="BC7" s="185"/>
-      <c r="BD7" s="185"/>
-      <c r="BE7" s="185"/>
-      <c r="BF7" s="185"/>
+      <c r="BB7" s="302"/>
+      <c r="BC7" s="306"/>
+      <c r="BD7" s="302"/>
+      <c r="BE7" s="307"/>
+      <c r="BF7" s="308"/>
       <c r="BG7" s="185"/>
-      <c r="BH7" s="184"/>
-      <c r="BI7" s="184"/>
+      <c r="BH7" s="185"/>
+      <c r="BI7" s="185"/>
       <c r="BJ7" s="184"/>
       <c r="BK7" s="184"/>
       <c r="BL7" s="184"/>
-      <c r="BM7" s="164"/>
-      <c r="BN7" s="164"/>
+      <c r="BM7" s="184"/>
+      <c r="BN7" s="184"/>
       <c r="BO7" s="164"/>
       <c r="BP7" s="164"/>
-      <c r="BQ7" s="181"/>
-      <c r="BR7" s="183"/>
-      <c r="BS7" s="167"/>
-      <c r="BT7" s="170"/>
-      <c r="BU7" s="170"/>
+      <c r="BQ7" s="164"/>
+      <c r="BR7" s="164"/>
+      <c r="BS7" s="181"/>
+      <c r="BT7" s="183"/>
+      <c r="BU7" s="167"/>
       <c r="BV7" s="170"/>
       <c r="BW7" s="170"/>
       <c r="BX7" s="170"/>
       <c r="BY7" s="170"/>
       <c r="BZ7" s="170"/>
-      <c r="CA7" s="168"/>
-      <c r="CB7" s="164"/>
-      <c r="CC7" s="164"/>
-      <c r="CD7" s="167"/>
-      <c r="CE7" s="168"/>
+      <c r="CA7" s="170"/>
+      <c r="CB7" s="170"/>
+      <c r="CC7" s="170"/>
+      <c r="CD7" s="168"/>
+      <c r="CE7" s="164"/>
       <c r="CF7" s="164"/>
-      <c r="CG7" s="164"/>
-      <c r="CH7" s="167"/>
-      <c r="CI7" s="170"/>
-      <c r="CJ7" s="170"/>
-      <c r="CK7" s="170"/>
-      <c r="CL7" s="168"/>
-      <c r="CM7" s="173"/>
-      <c r="CN7" s="174"/>
-    </row>
-    <row r="8" spans="1:171" ht="23" customHeight="1">
+      <c r="CG7" s="167"/>
+      <c r="CH7" s="168"/>
+      <c r="CI7" s="164"/>
+      <c r="CJ7" s="164"/>
+      <c r="CK7" s="167"/>
+      <c r="CL7" s="170"/>
+      <c r="CM7" s="170"/>
+      <c r="CN7" s="170"/>
+      <c r="CO7" s="168"/>
+      <c r="CP7" s="173"/>
+      <c r="CQ7" s="174"/>
+    </row>
+    <row r="8" spans="1:174" ht="23" customHeight="1">
       <c r="A8" s="231" t="s">
         <v>373</v>
       </c>
@@ -4241,87 +4340,96 @@
       <c r="BA8" s="206" t="s">
         <v>273</v>
       </c>
-      <c r="BB8" s="159"/>
-      <c r="BC8" s="159"/>
-      <c r="BD8" s="159"/>
-      <c r="BE8" s="159"/>
-      <c r="BF8" s="161" t="s">
-        <v>269</v>
-      </c>
+      <c r="BB8" s="309" t="s">
+        <v>515</v>
+      </c>
+      <c r="BC8" s="309" t="s">
+        <v>515</v>
+      </c>
+      <c r="BD8" s="302"/>
+      <c r="BE8" s="309"/>
+      <c r="BF8" s="309"/>
       <c r="BG8" s="161" t="s">
         <v>269</v>
       </c>
-      <c r="BH8" s="206" t="s">
+      <c r="BH8" s="161" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI8" s="311"/>
+      <c r="BJ8" s="206" t="s">
         <v>270</v>
       </c>
-      <c r="BI8" s="206" t="s">
+      <c r="BK8" s="206" t="s">
         <v>268</v>
       </c>
-      <c r="BJ8" s="206" t="s">
+      <c r="BL8" s="206" t="s">
         <v>314</v>
       </c>
-      <c r="BK8" s="206" t="s">
+      <c r="BM8" s="206" t="s">
         <v>313</v>
       </c>
-      <c r="BL8" s="206" t="s">
+      <c r="BN8" s="206" t="s">
         <v>312</v>
       </c>
-      <c r="BM8" s="195"/>
-      <c r="BN8" s="195"/>
       <c r="BO8" s="195"/>
       <c r="BP8" s="195"/>
-      <c r="BQ8" s="206" t="s">
+      <c r="BQ8" s="195"/>
+      <c r="BR8" s="195"/>
+      <c r="BS8" s="206" t="s">
         <v>356</v>
       </c>
-      <c r="BR8" s="206" t="s">
+      <c r="BT8" s="206" t="s">
         <v>1</v>
       </c>
-      <c r="BS8" s="188" t="s">
+      <c r="BU8" s="188" t="s">
         <v>388</v>
       </c>
-      <c r="BT8" s="189"/>
-      <c r="BU8" s="189"/>
-      <c r="BV8" s="190"/>
-      <c r="BW8" s="206" t="s">
+      <c r="BV8" s="189"/>
+      <c r="BW8" s="189"/>
+      <c r="BX8" s="190"/>
+      <c r="BY8" s="206" t="s">
+        <v>517</v>
+      </c>
+      <c r="BZ8" s="206" t="s">
         <v>422</v>
       </c>
-      <c r="BX8" s="206" t="s">
+      <c r="CA8" s="206" t="s">
         <v>506</v>
       </c>
-      <c r="BY8" s="188" t="s">
+      <c r="CB8" s="188" t="s">
         <v>502</v>
       </c>
-      <c r="BZ8" s="190"/>
-      <c r="CA8" s="206" t="s">
+      <c r="CC8" s="190"/>
+      <c r="CD8" s="206" t="s">
         <v>484</v>
       </c>
-      <c r="CB8" s="195"/>
-      <c r="CC8" s="195"/>
-      <c r="CD8" s="203" t="s">
+      <c r="CE8" s="195"/>
+      <c r="CF8" s="195"/>
+      <c r="CG8" s="203" t="s">
         <v>471</v>
       </c>
-      <c r="CE8" s="203" t="s">
+      <c r="CH8" s="203" t="s">
         <v>472</v>
       </c>
-      <c r="CF8" s="195"/>
-      <c r="CG8" s="195"/>
-      <c r="CH8" s="194" t="s">
+      <c r="CI8" s="195"/>
+      <c r="CJ8" s="195"/>
+      <c r="CK8" s="194" t="s">
         <v>384</v>
       </c>
-      <c r="CI8" s="194" t="s">
+      <c r="CL8" s="194" t="s">
         <v>385</v>
       </c>
-      <c r="CJ8" s="194"/>
-      <c r="CK8" s="194"/>
-      <c r="CL8" s="194"/>
-      <c r="CM8" s="203" t="s">
+      <c r="CM8" s="194"/>
+      <c r="CN8" s="194"/>
+      <c r="CO8" s="194"/>
+      <c r="CP8" s="203" t="s">
         <v>308</v>
       </c>
-      <c r="CN8" s="203" t="s">
+      <c r="CQ8" s="203" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="9" spans="1:171" ht="47" customHeight="1">
+    <row r="9" spans="1:174" ht="47" customHeight="1">
       <c r="A9" s="232"/>
       <c r="B9" s="101"/>
       <c r="C9" s="177"/>
@@ -4379,51 +4487,54 @@
       <c r="AY9" s="207"/>
       <c r="AZ9" s="207"/>
       <c r="BA9" s="207"/>
-      <c r="BB9" s="160"/>
-      <c r="BC9" s="160"/>
-      <c r="BD9" s="160"/>
-      <c r="BE9" s="160"/>
-      <c r="BF9" s="162" t="s">
+      <c r="BB9" s="310"/>
+      <c r="BC9" s="310"/>
+      <c r="BD9" s="302"/>
+      <c r="BE9" s="310"/>
+      <c r="BF9" s="310"/>
+      <c r="BG9" s="162" t="s">
         <v>456</v>
       </c>
-      <c r="BG9" s="162" t="s">
+      <c r="BH9" s="162" t="s">
         <v>457</v>
       </c>
-      <c r="BH9" s="207"/>
-      <c r="BI9" s="207"/>
+      <c r="BI9" s="312"/>
       <c r="BJ9" s="207"/>
       <c r="BK9" s="207"/>
       <c r="BL9" s="207"/>
-      <c r="BM9" s="196"/>
-      <c r="BN9" s="196"/>
+      <c r="BM9" s="207"/>
+      <c r="BN9" s="207"/>
       <c r="BO9" s="196"/>
       <c r="BP9" s="196"/>
-      <c r="BQ9" s="207"/>
-      <c r="BR9" s="207"/>
-      <c r="BS9" s="191"/>
-      <c r="BT9" s="192"/>
-      <c r="BU9" s="192"/>
-      <c r="BV9" s="193"/>
-      <c r="BW9" s="207"/>
-      <c r="BX9" s="207"/>
-      <c r="BY9" s="191"/>
-      <c r="BZ9" s="193"/>
+      <c r="BQ9" s="196"/>
+      <c r="BR9" s="196"/>
+      <c r="BS9" s="207"/>
+      <c r="BT9" s="207"/>
+      <c r="BU9" s="191"/>
+      <c r="BV9" s="192"/>
+      <c r="BW9" s="192"/>
+      <c r="BX9" s="193"/>
+      <c r="BY9" s="207"/>
+      <c r="BZ9" s="207"/>
       <c r="CA9" s="207"/>
-      <c r="CB9" s="196"/>
-      <c r="CC9" s="196"/>
-      <c r="CD9" s="203"/>
-      <c r="CE9" s="203"/>
+      <c r="CB9" s="191"/>
+      <c r="CC9" s="193"/>
+      <c r="CD9" s="207"/>
+      <c r="CE9" s="196"/>
       <c r="CF9" s="196"/>
-      <c r="CG9" s="196"/>
-      <c r="CH9" s="194"/>
-      <c r="CI9" s="194"/>
-      <c r="CJ9" s="194"/>
+      <c r="CG9" s="203"/>
+      <c r="CH9" s="203"/>
+      <c r="CI9" s="196"/>
+      <c r="CJ9" s="196"/>
       <c r="CK9" s="194"/>
       <c r="CL9" s="194"/>
-      <c r="CM9" s="203"/>
-      <c r="CN9" s="203"/>
-    </row>
-    <row r="10" spans="1:171" ht="32" customHeight="1">
+      <c r="CM9" s="194"/>
+      <c r="CN9" s="194"/>
+      <c r="CO9" s="194"/>
+      <c r="CP9" s="203"/>
+      <c r="CQ9" s="203"/>
+    </row>
+    <row r="10" spans="1:174" ht="32" customHeight="1">
       <c r="A10" s="204" t="s">
         <v>374</v>
       </c>
@@ -4482,78 +4593,81 @@
       <c r="AV10" s="201"/>
       <c r="AW10" s="201"/>
       <c r="AX10" s="201"/>
-      <c r="AY10" s="155"/>
+      <c r="AY10" s="157"/>
       <c r="AZ10" s="201"/>
       <c r="BA10" s="201"/>
-      <c r="BB10" s="155"/>
-      <c r="BC10" s="155"/>
-      <c r="BD10" s="155"/>
-      <c r="BE10" s="155"/>
-      <c r="BF10" s="201"/>
+      <c r="BB10" s="157"/>
+      <c r="BC10" s="157"/>
+      <c r="BD10" s="157"/>
+      <c r="BE10" s="157"/>
+      <c r="BF10" s="157"/>
       <c r="BG10" s="201"/>
       <c r="BH10" s="201"/>
-      <c r="BI10" s="201"/>
-      <c r="BJ10" s="143" t="s">
+      <c r="BI10" s="157"/>
+      <c r="BJ10" s="201"/>
+      <c r="BK10" s="201"/>
+      <c r="BL10" s="143" t="s">
         <v>269</v>
       </c>
-      <c r="BK10" s="201"/>
-      <c r="BL10" s="69"/>
-      <c r="BM10" s="196"/>
-      <c r="BN10" s="196"/>
+      <c r="BM10" s="201"/>
+      <c r="BN10" s="69"/>
       <c r="BO10" s="196"/>
       <c r="BP10" s="196"/>
-      <c r="BQ10" s="146" t="s">
+      <c r="BQ10" s="196"/>
+      <c r="BR10" s="196"/>
+      <c r="BS10" s="146" t="s">
         <v>467</v>
       </c>
-      <c r="BR10" s="146" t="s">
+      <c r="BT10" s="146" t="s">
         <v>466</v>
       </c>
-      <c r="BS10" s="194" t="s">
+      <c r="BU10" s="194" t="s">
         <v>301</v>
       </c>
-      <c r="BT10" s="194" t="s">
+      <c r="BV10" s="194" t="s">
         <v>268</v>
       </c>
-      <c r="BU10" s="194" t="s">
+      <c r="BW10" s="194" t="s">
         <v>261</v>
       </c>
-      <c r="BV10" s="194" t="s">
+      <c r="BX10" s="194" t="s">
         <v>269</v>
       </c>
-      <c r="BW10" s="195"/>
-      <c r="BX10" s="143" t="s">
+      <c r="BY10" s="155"/>
+      <c r="BZ10" s="195"/>
+      <c r="CA10" s="143" t="s">
         <v>269</v>
       </c>
-      <c r="BY10" s="228" t="s">
+      <c r="CB10" s="228" t="s">
         <v>269</v>
       </c>
-      <c r="BZ10" s="228"/>
-      <c r="CA10" s="153" t="s">
+      <c r="CC10" s="228"/>
+      <c r="CD10" s="153" t="s">
         <v>269</v>
       </c>
-      <c r="CB10" s="196"/>
-      <c r="CC10" s="196"/>
-      <c r="CD10" s="186"/>
-      <c r="CE10" s="186"/>
+      <c r="CE10" s="196"/>
       <c r="CF10" s="196"/>
-      <c r="CG10" s="196"/>
+      <c r="CG10" s="186"/>
       <c r="CH10" s="186"/>
-      <c r="CI10" s="203">
+      <c r="CI10" s="196"/>
+      <c r="CJ10" s="196"/>
+      <c r="CK10" s="186"/>
+      <c r="CL10" s="203">
         <v>1</v>
       </c>
-      <c r="CJ10" s="203">
+      <c r="CM10" s="203">
         <v>2</v>
       </c>
-      <c r="CK10" s="203">
+      <c r="CN10" s="203">
         <v>3</v>
       </c>
-      <c r="CL10" s="203">
+      <c r="CO10" s="203">
         <v>4</v>
       </c>
-      <c r="CM10" s="186"/>
-      <c r="CN10" s="186"/>
-    </row>
-    <row r="11" spans="1:171" ht="34">
+      <c r="CP10" s="186"/>
+      <c r="CQ10" s="186"/>
+    </row>
+    <row r="11" spans="1:174" ht="34">
       <c r="A11" s="204"/>
       <c r="B11" s="127"/>
       <c r="C11" s="177"/>
@@ -4622,62 +4736,65 @@
       <c r="AV11" s="202"/>
       <c r="AW11" s="202"/>
       <c r="AX11" s="202"/>
-      <c r="AY11" s="156"/>
+      <c r="AY11" s="158"/>
       <c r="AZ11" s="202"/>
       <c r="BA11" s="202"/>
-      <c r="BB11" s="156"/>
-      <c r="BC11" s="156"/>
-      <c r="BD11" s="156"/>
-      <c r="BE11" s="156"/>
-      <c r="BF11" s="202"/>
+      <c r="BB11" s="158"/>
+      <c r="BC11" s="158"/>
+      <c r="BD11" s="158"/>
+      <c r="BE11" s="158"/>
+      <c r="BF11" s="158"/>
       <c r="BG11" s="202"/>
       <c r="BH11" s="202"/>
-      <c r="BI11" s="202"/>
-      <c r="BJ11" s="96" t="s">
+      <c r="BI11" s="158"/>
+      <c r="BJ11" s="202"/>
+      <c r="BK11" s="202"/>
+      <c r="BL11" s="96" t="s">
         <v>459</v>
       </c>
-      <c r="BK11" s="202"/>
-      <c r="BL11" s="69"/>
-      <c r="BM11" s="196"/>
-      <c r="BN11" s="196"/>
+      <c r="BM11" s="202"/>
+      <c r="BN11" s="69"/>
       <c r="BO11" s="196"/>
       <c r="BP11" s="196"/>
-      <c r="BQ11" s="54" t="s">
+      <c r="BQ11" s="196"/>
+      <c r="BR11" s="196"/>
+      <c r="BS11" s="54" t="s">
         <v>465</v>
       </c>
-      <c r="BR11" s="54" t="s">
+      <c r="BT11" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="BS11" s="194"/>
-      <c r="BT11" s="194"/>
       <c r="BU11" s="194"/>
       <c r="BV11" s="194"/>
-      <c r="BW11" s="196"/>
-      <c r="BX11" s="96" t="s">
+      <c r="BW11" s="194"/>
+      <c r="BX11" s="194"/>
+      <c r="BY11" s="155"/>
+      <c r="BZ11" s="196"/>
+      <c r="CA11" s="96" t="s">
         <v>459</v>
       </c>
-      <c r="BY11" s="229" t="s">
+      <c r="CB11" s="229" t="s">
         <v>456</v>
       </c>
-      <c r="BZ11" s="229"/>
-      <c r="CA11" s="154" t="s">
+      <c r="CC11" s="229"/>
+      <c r="CD11" s="154" t="s">
         <v>456</v>
       </c>
-      <c r="CB11" s="196"/>
-      <c r="CC11" s="196"/>
-      <c r="CD11" s="187"/>
-      <c r="CE11" s="187"/>
+      <c r="CE11" s="196"/>
       <c r="CF11" s="196"/>
-      <c r="CG11" s="196"/>
+      <c r="CG11" s="187"/>
       <c r="CH11" s="187"/>
-      <c r="CI11" s="203"/>
-      <c r="CJ11" s="203"/>
-      <c r="CK11" s="203"/>
+      <c r="CI11" s="196"/>
+      <c r="CJ11" s="196"/>
+      <c r="CK11" s="187"/>
       <c r="CL11" s="203"/>
-      <c r="CM11" s="187"/>
-      <c r="CN11" s="187"/>
-    </row>
-    <row r="12" spans="1:171" ht="37" customHeight="1">
+      <c r="CM11" s="203"/>
+      <c r="CN11" s="203"/>
+      <c r="CO11" s="203"/>
+      <c r="CP11" s="187"/>
+      <c r="CQ11" s="187"/>
+    </row>
+    <row r="12" spans="1:174" ht="37" customHeight="1">
       <c r="A12" s="231" t="s">
         <v>404</v>
       </c>
@@ -4756,52 +4873,55 @@
       <c r="AV12" s="202"/>
       <c r="AW12" s="202"/>
       <c r="AX12" s="202"/>
-      <c r="AY12" s="156"/>
+      <c r="AY12" s="158"/>
       <c r="AZ12" s="202"/>
       <c r="BA12" s="202"/>
-      <c r="BB12" s="156"/>
-      <c r="BC12" s="156"/>
-      <c r="BD12" s="156"/>
-      <c r="BE12" s="156"/>
-      <c r="BF12" s="202"/>
+      <c r="BB12" s="158"/>
+      <c r="BC12" s="158"/>
+      <c r="BD12" s="158"/>
+      <c r="BE12" s="158"/>
+      <c r="BF12" s="158"/>
       <c r="BG12" s="202"/>
       <c r="BH12" s="202"/>
-      <c r="BI12" s="202"/>
-      <c r="BJ12" s="197"/>
+      <c r="BI12" s="158"/>
+      <c r="BJ12" s="202"/>
       <c r="BK12" s="202"/>
-      <c r="BL12" s="69"/>
-      <c r="BM12" s="196"/>
-      <c r="BN12" s="196"/>
+      <c r="BL12" s="197"/>
+      <c r="BM12" s="202"/>
+      <c r="BN12" s="69"/>
       <c r="BO12" s="196"/>
       <c r="BP12" s="196"/>
-      <c r="BQ12" s="197"/>
-      <c r="BR12" s="197"/>
+      <c r="BQ12" s="196"/>
+      <c r="BR12" s="196"/>
       <c r="BS12" s="197"/>
       <c r="BT12" s="197"/>
-      <c r="BU12" s="149"/>
+      <c r="BU12" s="197"/>
       <c r="BV12" s="197"/>
-      <c r="BW12" s="196"/>
-      <c r="BX12" s="134"/>
-      <c r="BY12" s="230" t="s">
+      <c r="BW12" s="149"/>
+      <c r="BX12" s="197"/>
+      <c r="BY12" s="155"/>
+      <c r="BZ12" s="196"/>
+      <c r="CA12" s="134"/>
+      <c r="CB12" s="230" t="s">
         <v>485</v>
       </c>
-      <c r="BZ12" s="230"/>
-      <c r="CA12" s="197"/>
-      <c r="CB12" s="196"/>
-      <c r="CC12" s="196"/>
-      <c r="CD12" s="187"/>
-      <c r="CE12" s="187"/>
+      <c r="CC12" s="230"/>
+      <c r="CD12" s="197"/>
+      <c r="CE12" s="196"/>
       <c r="CF12" s="196"/>
-      <c r="CG12" s="196"/>
+      <c r="CG12" s="187"/>
       <c r="CH12" s="187"/>
-      <c r="CI12" s="197"/>
-      <c r="CJ12" s="197"/>
-      <c r="CK12" s="197"/>
+      <c r="CI12" s="196"/>
+      <c r="CJ12" s="196"/>
+      <c r="CK12" s="187"/>
       <c r="CL12" s="197"/>
-      <c r="CM12" s="187"/>
-      <c r="CN12" s="187"/>
-    </row>
-    <row r="13" spans="1:171" ht="47" customHeight="1">
+      <c r="CM12" s="197"/>
+      <c r="CN12" s="197"/>
+      <c r="CO12" s="197"/>
+      <c r="CP12" s="187"/>
+      <c r="CQ12" s="187"/>
+    </row>
+    <row r="13" spans="1:174" ht="47" customHeight="1">
       <c r="A13" s="232"/>
       <c r="B13" s="101"/>
       <c r="C13" s="177"/>
@@ -4852,54 +4972,57 @@
       <c r="AV13" s="202"/>
       <c r="AW13" s="202"/>
       <c r="AX13" s="202"/>
-      <c r="AY13" s="156"/>
+      <c r="AY13" s="158"/>
       <c r="AZ13" s="202"/>
       <c r="BA13" s="202"/>
-      <c r="BB13" s="156"/>
-      <c r="BC13" s="156"/>
-      <c r="BD13" s="156"/>
-      <c r="BE13" s="156"/>
-      <c r="BF13" s="202"/>
+      <c r="BB13" s="158"/>
+      <c r="BC13" s="158"/>
+      <c r="BD13" s="158"/>
+      <c r="BE13" s="158"/>
+      <c r="BF13" s="158"/>
       <c r="BG13" s="202"/>
       <c r="BH13" s="202"/>
-      <c r="BI13" s="202"/>
-      <c r="BJ13" s="198"/>
+      <c r="BI13" s="158"/>
+      <c r="BJ13" s="202"/>
       <c r="BK13" s="202"/>
-      <c r="BL13" s="69"/>
-      <c r="BM13" s="196"/>
-      <c r="BN13" s="196"/>
+      <c r="BL13" s="198"/>
+      <c r="BM13" s="202"/>
+      <c r="BN13" s="69"/>
       <c r="BO13" s="196"/>
       <c r="BP13" s="196"/>
-      <c r="BQ13" s="198"/>
-      <c r="BR13" s="198"/>
+      <c r="BQ13" s="196"/>
+      <c r="BR13" s="196"/>
       <c r="BS13" s="198"/>
       <c r="BT13" s="198"/>
-      <c r="BU13" s="148"/>
+      <c r="BU13" s="198"/>
       <c r="BV13" s="198"/>
-      <c r="BW13" s="196"/>
-      <c r="BX13" s="134"/>
-      <c r="BY13" s="96" t="s">
+      <c r="BW13" s="148"/>
+      <c r="BX13" s="198"/>
+      <c r="BY13" s="155"/>
+      <c r="BZ13" s="196"/>
+      <c r="CA13" s="134"/>
+      <c r="CB13" s="96" t="s">
         <v>478</v>
       </c>
-      <c r="BZ13" s="96" t="s">
+      <c r="CC13" s="96" t="s">
         <v>483</v>
       </c>
-      <c r="CA13" s="198"/>
-      <c r="CB13" s="196"/>
-      <c r="CC13" s="196"/>
-      <c r="CD13" s="187"/>
-      <c r="CE13" s="187"/>
+      <c r="CD13" s="198"/>
+      <c r="CE13" s="196"/>
       <c r="CF13" s="196"/>
-      <c r="CG13" s="196"/>
+      <c r="CG13" s="187"/>
       <c r="CH13" s="187"/>
-      <c r="CI13" s="198"/>
-      <c r="CJ13" s="198"/>
-      <c r="CK13" s="198"/>
+      <c r="CI13" s="196"/>
+      <c r="CJ13" s="196"/>
+      <c r="CK13" s="187"/>
       <c r="CL13" s="198"/>
-      <c r="CM13" s="187"/>
-      <c r="CN13" s="187"/>
-    </row>
-    <row r="14" spans="1:171" ht="51" customHeight="1">
+      <c r="CM13" s="198"/>
+      <c r="CN13" s="198"/>
+      <c r="CO13" s="198"/>
+      <c r="CP13" s="187"/>
+      <c r="CQ13" s="187"/>
+    </row>
+    <row r="14" spans="1:174" ht="51" customHeight="1">
       <c r="A14" s="204" t="s">
         <v>477</v>
       </c>
@@ -4952,50 +5075,53 @@
       <c r="AV14" s="202"/>
       <c r="AW14" s="202"/>
       <c r="AX14" s="202"/>
-      <c r="AY14" s="156"/>
+      <c r="AY14" s="158"/>
       <c r="AZ14" s="202"/>
       <c r="BA14" s="202"/>
-      <c r="BB14" s="156"/>
-      <c r="BC14" s="156"/>
-      <c r="BD14" s="156"/>
-      <c r="BE14" s="156"/>
-      <c r="BF14" s="202"/>
+      <c r="BB14" s="158"/>
+      <c r="BC14" s="158"/>
+      <c r="BD14" s="158"/>
+      <c r="BE14" s="158"/>
+      <c r="BF14" s="158"/>
       <c r="BG14" s="202"/>
       <c r="BH14" s="202"/>
-      <c r="BI14" s="202"/>
-      <c r="BJ14" s="198"/>
+      <c r="BI14" s="158"/>
+      <c r="BJ14" s="202"/>
       <c r="BK14" s="202"/>
-      <c r="BL14" s="175"/>
-      <c r="BM14" s="196"/>
-      <c r="BN14" s="196"/>
+      <c r="BL14" s="198"/>
+      <c r="BM14" s="202"/>
+      <c r="BN14" s="175"/>
       <c r="BO14" s="196"/>
       <c r="BP14" s="196"/>
-      <c r="BQ14" s="198"/>
-      <c r="BR14" s="198"/>
+      <c r="BQ14" s="196"/>
+      <c r="BR14" s="196"/>
       <c r="BS14" s="198"/>
       <c r="BT14" s="198"/>
-      <c r="BU14" s="148"/>
+      <c r="BU14" s="198"/>
       <c r="BV14" s="198"/>
-      <c r="BW14" s="196"/>
-      <c r="BX14" s="134"/>
-      <c r="BY14" s="134"/>
-      <c r="BZ14" s="134"/>
-      <c r="CA14" s="198"/>
-      <c r="CB14" s="196"/>
-      <c r="CC14" s="196"/>
-      <c r="CD14" s="187"/>
-      <c r="CE14" s="187"/>
+      <c r="BW14" s="148"/>
+      <c r="BX14" s="198"/>
+      <c r="BY14" s="155"/>
+      <c r="BZ14" s="196"/>
+      <c r="CA14" s="134"/>
+      <c r="CB14" s="134"/>
+      <c r="CC14" s="134"/>
+      <c r="CD14" s="198"/>
+      <c r="CE14" s="196"/>
       <c r="CF14" s="196"/>
-      <c r="CG14" s="196"/>
+      <c r="CG14" s="187"/>
       <c r="CH14" s="187"/>
-      <c r="CI14" s="198"/>
-      <c r="CJ14" s="198"/>
-      <c r="CK14" s="198"/>
+      <c r="CI14" s="196"/>
+      <c r="CJ14" s="196"/>
+      <c r="CK14" s="187"/>
       <c r="CL14" s="198"/>
-      <c r="CM14" s="187"/>
-      <c r="CN14" s="187"/>
-    </row>
-    <row r="15" spans="1:171" ht="47" customHeight="1">
+      <c r="CM14" s="198"/>
+      <c r="CN14" s="198"/>
+      <c r="CO14" s="198"/>
+      <c r="CP14" s="187"/>
+      <c r="CQ14" s="187"/>
+    </row>
+    <row r="15" spans="1:174" ht="47" customHeight="1">
       <c r="A15" s="204"/>
       <c r="B15" s="101"/>
       <c r="C15" s="177"/>
@@ -5046,50 +5172,53 @@
       <c r="AV15" s="202"/>
       <c r="AW15" s="202"/>
       <c r="AX15" s="202"/>
-      <c r="AY15" s="156"/>
+      <c r="AY15" s="158"/>
       <c r="AZ15" s="202"/>
       <c r="BA15" s="202"/>
-      <c r="BB15" s="156"/>
-      <c r="BC15" s="156"/>
-      <c r="BD15" s="156"/>
-      <c r="BE15" s="156"/>
-      <c r="BF15" s="202"/>
+      <c r="BB15" s="158"/>
+      <c r="BC15" s="158"/>
+      <c r="BD15" s="158"/>
+      <c r="BE15" s="158"/>
+      <c r="BF15" s="158"/>
       <c r="BG15" s="202"/>
       <c r="BH15" s="202"/>
-      <c r="BI15" s="202"/>
-      <c r="BJ15" s="198"/>
+      <c r="BI15" s="158"/>
+      <c r="BJ15" s="202"/>
       <c r="BK15" s="202"/>
-      <c r="BL15" s="175"/>
-      <c r="BM15" s="196"/>
-      <c r="BN15" s="196"/>
+      <c r="BL15" s="198"/>
+      <c r="BM15" s="202"/>
+      <c r="BN15" s="175"/>
       <c r="BO15" s="196"/>
       <c r="BP15" s="196"/>
-      <c r="BQ15" s="198"/>
-      <c r="BR15" s="198"/>
+      <c r="BQ15" s="196"/>
+      <c r="BR15" s="196"/>
       <c r="BS15" s="198"/>
       <c r="BT15" s="198"/>
-      <c r="BU15" s="148"/>
+      <c r="BU15" s="198"/>
       <c r="BV15" s="198"/>
-      <c r="BW15" s="196"/>
-      <c r="BX15" s="134"/>
-      <c r="BY15" s="134"/>
-      <c r="BZ15" s="134"/>
-      <c r="CA15" s="198"/>
-      <c r="CB15" s="196"/>
-      <c r="CC15" s="196"/>
-      <c r="CD15" s="187"/>
-      <c r="CE15" s="187"/>
+      <c r="BW15" s="148"/>
+      <c r="BX15" s="198"/>
+      <c r="BY15" s="155"/>
+      <c r="BZ15" s="196"/>
+      <c r="CA15" s="134"/>
+      <c r="CB15" s="134"/>
+      <c r="CC15" s="134"/>
+      <c r="CD15" s="198"/>
+      <c r="CE15" s="196"/>
       <c r="CF15" s="196"/>
-      <c r="CG15" s="196"/>
+      <c r="CG15" s="187"/>
       <c r="CH15" s="187"/>
-      <c r="CI15" s="198"/>
-      <c r="CJ15" s="198"/>
-      <c r="CK15" s="198"/>
+      <c r="CI15" s="196"/>
+      <c r="CJ15" s="196"/>
+      <c r="CK15" s="187"/>
       <c r="CL15" s="198"/>
-      <c r="CM15" s="187"/>
-      <c r="CN15" s="187"/>
-    </row>
-    <row r="16" spans="1:171" ht="24">
+      <c r="CM15" s="198"/>
+      <c r="CN15" s="198"/>
+      <c r="CO15" s="198"/>
+      <c r="CP15" s="187"/>
+      <c r="CQ15" s="187"/>
+    </row>
+    <row r="16" spans="1:174" ht="24">
       <c r="A16" s="127"/>
       <c r="B16" s="127"/>
       <c r="C16" s="127"/>
@@ -5261,8 +5390,11 @@
       <c r="FM16" s="127"/>
       <c r="FN16" s="127"/>
       <c r="FO16" s="127"/>
-    </row>
-    <row r="17" spans="1:92" ht="25">
+      <c r="FP16" s="127"/>
+      <c r="FQ16" s="127"/>
+      <c r="FR16" s="127"/>
+    </row>
+    <row r="17" spans="1:95" ht="25">
       <c r="A17" s="131" t="s">
         <v>433</v>
       </c>
@@ -5423,117 +5555,126 @@
         <v>454</v>
       </c>
       <c r="BC17" s="133" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD17" s="133" t="s">
         <v>97</v>
       </c>
-      <c r="BD17" s="133"/>
       <c r="BE17" s="133"/>
-      <c r="BF17" s="133" t="s">
-        <v>454</v>
-      </c>
+      <c r="BF17" s="133"/>
       <c r="BG17" s="133" t="s">
         <v>454</v>
       </c>
       <c r="BH17" s="133" t="s">
+        <v>454</v>
+      </c>
+      <c r="BI17" s="133" t="s">
+        <v>475</v>
+      </c>
+      <c r="BJ17" s="133" t="s">
         <v>90</v>
-      </c>
-      <c r="BI17" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="BJ17" s="133" t="s">
-        <v>454</v>
       </c>
       <c r="BK17" s="133" t="s">
         <v>91</v>
       </c>
-      <c r="BL17" s="144" t="s">
+      <c r="BL17" s="133" t="s">
+        <v>454</v>
+      </c>
+      <c r="BM17" s="133" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN17" s="144" t="s">
         <v>458</v>
       </c>
-      <c r="BM17" s="133" t="s">
+      <c r="BO17" s="133" t="s">
         <v>90</v>
       </c>
-      <c r="BN17" s="133" t="s">
+      <c r="BP17" s="133" t="s">
         <v>97</v>
       </c>
-      <c r="BO17" s="133" t="s">
+      <c r="BQ17" s="133" t="s">
         <v>462</v>
       </c>
-      <c r="BP17" s="133" t="s">
+      <c r="BR17" s="133" t="s">
         <v>91</v>
       </c>
-      <c r="BQ17" s="133" t="s">
+      <c r="BS17" s="133" t="s">
         <v>122</v>
       </c>
-      <c r="BR17" s="133" t="s">
+      <c r="BT17" s="133" t="s">
         <v>122</v>
       </c>
-      <c r="BS17" s="133" t="s">
+      <c r="BU17" s="133" t="s">
         <v>479</v>
       </c>
-      <c r="BT17" s="133" t="s">
+      <c r="BV17" s="133" t="s">
         <v>469</v>
-      </c>
-      <c r="BU17" s="133" t="s">
-        <v>469</v>
-      </c>
-      <c r="BV17" s="133" t="s">
-        <v>479</v>
       </c>
       <c r="BW17" s="133" t="s">
         <v>469</v>
       </c>
       <c r="BX17" s="133" t="s">
+        <v>479</v>
+      </c>
+      <c r="BY17" s="133" t="s">
+        <v>475</v>
+      </c>
+      <c r="BZ17" s="133" t="s">
+        <v>469</v>
+      </c>
+      <c r="CA17" s="133" t="s">
         <v>122</v>
       </c>
-      <c r="BY17" s="133" t="s">
+      <c r="CB17" s="133" t="s">
         <v>122</v>
       </c>
-      <c r="BZ17" s="133" t="s">
+      <c r="CC17" s="133" t="s">
         <v>122</v>
       </c>
-      <c r="CA17" s="133" t="s">
+      <c r="CD17" s="133" t="s">
         <v>454</v>
       </c>
-      <c r="CB17" s="133" t="s">
+      <c r="CE17" s="133" t="s">
         <v>97</v>
       </c>
-      <c r="CC17" s="133" t="s">
+      <c r="CF17" s="133" t="s">
         <v>469</v>
       </c>
-      <c r="CD17" s="133" t="s">
+      <c r="CG17" s="133" t="s">
         <v>475</v>
       </c>
-      <c r="CE17" s="133" t="s">
+      <c r="CH17" s="133" t="s">
         <v>469</v>
       </c>
-      <c r="CF17" s="133" t="s">
+      <c r="CI17" s="133" t="s">
         <v>475</v>
       </c>
-      <c r="CG17" s="133" t="s">
+      <c r="CJ17" s="133" t="s">
         <v>122</v>
       </c>
-      <c r="CH17" s="133" t="s">
+      <c r="CK17" s="133" t="s">
         <v>122</v>
-      </c>
-      <c r="CI17" s="133" t="s">
-        <v>476</v>
-      </c>
-      <c r="CJ17" s="133" t="s">
-        <v>476</v>
-      </c>
-      <c r="CK17" s="133" t="s">
-        <v>476</v>
       </c>
       <c r="CL17" s="133" t="s">
         <v>476</v>
       </c>
       <c r="CM17" s="133" t="s">
-        <v>90</v>
+        <v>476</v>
       </c>
       <c r="CN17" s="133" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="18" spans="1:92" ht="60">
+      <c r="CO17" s="133" t="s">
+        <v>476</v>
+      </c>
+      <c r="CP17" s="133" t="s">
+        <v>90</v>
+      </c>
+      <c r="CQ17" s="133" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="18" spans="1:95" ht="60">
       <c r="A18" s="131" t="s">
         <v>434</v>
       </c>
@@ -5633,124 +5774,129 @@
       <c r="AV18" s="11"/>
       <c r="AW18" s="11"/>
       <c r="AX18" s="11"/>
-      <c r="AY18" s="157" t="s">
+      <c r="AY18" s="159" t="s">
         <v>114</v>
       </c>
       <c r="AZ18" s="11"/>
       <c r="BA18" s="11"/>
       <c r="BB18" s="11"/>
-      <c r="BC18" s="298" t="s">
+      <c r="BC18" s="11"/>
+      <c r="BD18" s="298" t="s">
         <v>510</v>
       </c>
-      <c r="BD18" s="11"/>
       <c r="BE18" s="11"/>
-      <c r="BF18" s="141" t="s">
-        <v>474</v>
-      </c>
+      <c r="BF18" s="11"/>
       <c r="BG18" s="141" t="s">
         <v>474</v>
       </c>
-      <c r="BH18" s="116">
+      <c r="BH18" s="141" t="s">
+        <v>474</v>
+      </c>
+      <c r="BI18" s="141"/>
+      <c r="BJ18" s="116">
         <v>7</v>
       </c>
-      <c r="BI18" s="141" t="s">
+      <c r="BK18" s="141" t="s">
         <v>482</v>
-      </c>
-      <c r="BJ18" s="141" t="s">
-        <v>474</v>
-      </c>
-      <c r="BK18" s="141" t="s">
-        <v>473</v>
       </c>
       <c r="BL18" s="141" t="s">
         <v>474</v>
       </c>
-      <c r="BM18" s="116">
+      <c r="BM18" s="141" t="s">
+        <v>473</v>
+      </c>
+      <c r="BN18" s="141" t="s">
+        <v>474</v>
+      </c>
+      <c r="BO18" s="116">
         <v>100</v>
       </c>
-      <c r="BN18" s="136" t="s">
+      <c r="BP18" s="136" t="s">
         <v>107</v>
       </c>
-      <c r="BO18" s="116" t="s">
+      <c r="BQ18" s="116" t="s">
         <v>99</v>
       </c>
-      <c r="BP18" s="138" t="s">
+      <c r="BR18" s="138" t="s">
         <v>464</v>
       </c>
-      <c r="BQ18" s="116" t="s">
+      <c r="BS18" s="116" t="s">
         <v>411</v>
       </c>
-      <c r="BR18" s="116" t="s">
+      <c r="BT18" s="116" t="s">
         <v>411</v>
       </c>
-      <c r="BS18" s="147" t="s">
+      <c r="BU18" s="147" t="s">
         <v>108</v>
       </c>
-      <c r="BT18" s="141" t="s">
+      <c r="BV18" s="141" t="s">
         <v>473</v>
-      </c>
-      <c r="BU18" s="141" t="s">
-        <v>473</v>
-      </c>
-      <c r="BV18" s="147" t="s">
-        <v>109</v>
       </c>
       <c r="BW18" s="141" t="s">
         <v>473</v>
       </c>
-      <c r="BX18" s="141" t="s">
-        <v>474</v>
+      <c r="BX18" s="147" t="s">
+        <v>109</v>
       </c>
       <c r="BY18" s="141" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="BZ18" s="141" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="CA18" s="141" t="s">
         <v>474</v>
       </c>
-      <c r="CB18" s="147" t="s">
-        <v>129</v>
-      </c>
-      <c r="CC18" s="138" t="s">
-        <v>470</v>
+      <c r="CB18" s="141" t="s">
+        <v>474</v>
+      </c>
+      <c r="CC18" s="141" t="s">
+        <v>474</v>
       </c>
       <c r="CD18" s="141" t="s">
         <v>474</v>
       </c>
-      <c r="CE18" s="141" t="s">
+      <c r="CE18" s="147" t="s">
+        <v>129</v>
+      </c>
+      <c r="CF18" s="138" t="s">
+        <v>470</v>
+      </c>
+      <c r="CG18" s="141" t="s">
+        <v>474</v>
+      </c>
+      <c r="CH18" s="141" t="s">
         <v>473</v>
       </c>
-      <c r="CF18" s="141" t="s">
+      <c r="CI18" s="141" t="s">
         <v>474</v>
       </c>
-      <c r="CG18" s="116" t="b">
+      <c r="CJ18" s="116" t="b">
         <v>1</v>
       </c>
-      <c r="CH18" s="116" t="b">
+      <c r="CK18" s="116" t="b">
         <v>1</v>
-      </c>
-      <c r="CI18" s="141" t="s">
-        <v>461</v>
-      </c>
-      <c r="CJ18" s="141" t="s">
-        <v>461</v>
-      </c>
-      <c r="CK18" s="141" t="s">
-        <v>461</v>
       </c>
       <c r="CL18" s="141" t="s">
         <v>461</v>
       </c>
-      <c r="CM18" s="116">
-        <v>0</v>
+      <c r="CM18" s="141" t="s">
+        <v>461</v>
       </c>
       <c r="CN18" s="141" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="19" spans="1:92" ht="34">
+      <c r="CO18" s="141" t="s">
+        <v>461</v>
+      </c>
+      <c r="CP18" s="116">
+        <v>0</v>
+      </c>
+      <c r="CQ18" s="141" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="19" spans="1:95" ht="34">
       <c r="A19" s="131" t="s">
         <v>219</v>
       </c>
@@ -5844,22 +5990,24 @@
       <c r="BB19" s="116" t="s">
         <v>455</v>
       </c>
-      <c r="BC19" s="11"/>
+      <c r="BC19" s="138" t="s">
+        <v>512</v>
+      </c>
       <c r="BD19" s="11"/>
       <c r="BE19" s="11"/>
-      <c r="BF19" s="116" t="s">
-        <v>455</v>
-      </c>
+      <c r="BF19" s="11"/>
       <c r="BG19" s="116" t="s">
         <v>455</v>
       </c>
-      <c r="BH19" s="11"/>
-      <c r="BI19" s="11"/>
-      <c r="BJ19" s="116" t="s">
+      <c r="BH19" s="116" t="s">
         <v>455</v>
       </c>
+      <c r="BI19" s="116"/>
+      <c r="BJ19" s="11"/>
       <c r="BK19" s="11"/>
-      <c r="BL19" s="11"/>
+      <c r="BL19" s="116" t="s">
+        <v>455</v>
+      </c>
       <c r="BM19" s="11"/>
       <c r="BN19" s="11"/>
       <c r="BO19" s="11"/>
@@ -5870,24 +6018,24 @@
       <c r="BT19" s="11"/>
       <c r="BU19" s="11"/>
       <c r="BV19" s="11"/>
-      <c r="BW19" s="116" t="s">
+      <c r="BW19" s="11"/>
+      <c r="BX19" s="11"/>
+      <c r="BY19" s="11"/>
+      <c r="BZ19" s="116" t="s">
         <v>421</v>
       </c>
-      <c r="BX19" s="116" t="s">
+      <c r="CA19" s="116" t="s">
         <v>411</v>
       </c>
-      <c r="BY19" s="116" t="s">
+      <c r="CB19" s="116" t="s">
         <v>411</v>
       </c>
-      <c r="BZ19" s="116" t="s">
+      <c r="CC19" s="116" t="s">
         <v>411</v>
       </c>
-      <c r="CA19" s="68" t="s">
+      <c r="CD19" s="68" t="s">
         <v>412</v>
       </c>
-      <c r="CB19" s="11"/>
-      <c r="CC19" s="11"/>
-      <c r="CD19" s="11"/>
       <c r="CE19" s="11"/>
       <c r="CF19" s="11"/>
       <c r="CG19" s="11"/>
@@ -5898,15 +6046,16 @@
       <c r="CL19" s="11"/>
       <c r="CM19" s="11"/>
       <c r="CN19" s="11"/>
-    </row>
-    <row r="20" spans="1:92" ht="24">
+      <c r="CO19" s="11"/>
+      <c r="CP19" s="11"/>
+      <c r="CQ19" s="11"/>
+    </row>
+    <row r="20" spans="1:95" ht="24">
       <c r="A20" s="132"/>
       <c r="C20" s="130"/>
       <c r="G20" s="130"/>
       <c r="AF20" s="58"/>
       <c r="AG20" s="58"/>
-      <c r="BQ20" s="130"/>
-      <c r="BR20" s="130"/>
       <c r="BS20" s="130"/>
       <c r="BT20" s="130"/>
       <c r="BU20" s="130"/>
@@ -5916,8 +6065,11 @@
       <c r="BY20" s="130"/>
       <c r="BZ20" s="130"/>
       <c r="CA20" s="130"/>
-    </row>
-    <row r="21" spans="1:92" ht="36" customHeight="1">
+      <c r="CB20" s="130"/>
+      <c r="CC20" s="130"/>
+      <c r="CD20" s="130"/>
+    </row>
+    <row r="21" spans="1:95" ht="36" customHeight="1">
       <c r="C21" t="s">
         <v>355</v>
       </c>
@@ -5936,14 +6088,14 @@
       <c r="AT21" s="142" t="s">
         <v>453</v>
       </c>
-      <c r="BL21" s="145" t="s">
+      <c r="BN21" s="145" t="s">
         <v>460</v>
       </c>
-      <c r="BO21" s="145" t="s">
+      <c r="BQ21" s="145" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="22" spans="1:92">
+    <row r="22" spans="1:95">
       <c r="C22" t="s">
         <v>220</v>
       </c>
@@ -5958,7 +6110,7 @@
       <c r="AJ22" s="57"/>
       <c r="AK22" s="57"/>
     </row>
-    <row r="23" spans="1:92">
+    <row r="23" spans="1:95">
       <c r="AE23" s="58"/>
       <c r="AF23" s="58"/>
       <c r="AG23" s="58"/>
@@ -5967,91 +6119,92 @@
       <c r="AJ23" s="58"/>
       <c r="AK23" s="58"/>
     </row>
-    <row r="24" spans="1:92" ht="44" customHeight="1">
-      <c r="BQ24" t="s">
+    <row r="24" spans="1:95" ht="44" customHeight="1">
+      <c r="BS24" t="s">
         <v>413</v>
       </c>
-      <c r="BS24" s="218" t="s">
+      <c r="BU24" s="218" t="s">
         <v>424</v>
       </c>
-      <c r="BT24" s="218"/>
-      <c r="BU24" s="218"/>
       <c r="BV24" s="218"/>
-    </row>
-    <row r="25" spans="1:92">
-      <c r="BR25" t="s">
+      <c r="BW24" s="218"/>
+      <c r="BX24" s="218"/>
+      <c r="BY24" s="156"/>
+    </row>
+    <row r="25" spans="1:95">
+      <c r="BT25" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="28" spans="1:92">
+    <row r="28" spans="1:95">
       <c r="O28" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="32" spans="1:92">
+    <row r="32" spans="1:95">
       <c r="E32" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="33" spans="5:70">
+    <row r="33" spans="5:72">
       <c r="E33" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="34" spans="5:70">
+    <row r="34" spans="5:72">
       <c r="E34" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="35" spans="5:70">
+    <row r="35" spans="5:72">
       <c r="E35" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="37" spans="5:70">
-      <c r="BR37">
+    <row r="37" spans="5:72">
+      <c r="BT37">
         <v>5.6109999999999998</v>
       </c>
     </row>
-    <row r="38" spans="5:70">
-      <c r="BR38">
-        <f>BR37*11</f>
+    <row r="38" spans="5:72">
+      <c r="BT38">
+        <f>BT37*11</f>
         <v>61.720999999999997</v>
       </c>
     </row>
-    <row r="44" spans="5:70">
-      <c r="BR44">
+    <row r="44" spans="5:72">
+      <c r="BT44">
         <v>169</v>
       </c>
     </row>
-    <row r="45" spans="5:70">
-      <c r="BR45">
+    <row r="45" spans="5:72">
+      <c r="BT45">
         <v>181</v>
       </c>
     </row>
-    <row r="46" spans="5:70">
-      <c r="BR46">
-        <f>BR45-BR44</f>
+    <row r="46" spans="5:72">
+      <c r="BT46">
+        <f>BT45-BT44</f>
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="5:70">
-      <c r="BR47">
-        <f>BR46/BR44</f>
+    <row r="47" spans="5:72">
+      <c r="BT47">
+        <f>BT46/BT44</f>
         <v>7.1005917159763315E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="202">
+  <mergeCells count="204">
     <mergeCell ref="A6:A7"/>
+    <mergeCell ref="CD8:CD9"/>
+    <mergeCell ref="CD12:CD15"/>
     <mergeCell ref="CA8:CA9"/>
-    <mergeCell ref="CA12:CA15"/>
-    <mergeCell ref="BX8:BX9"/>
     <mergeCell ref="N6:AL6"/>
-    <mergeCell ref="BY8:BZ9"/>
-    <mergeCell ref="BY10:BZ10"/>
-    <mergeCell ref="BY11:BZ11"/>
-    <mergeCell ref="BY12:BZ12"/>
+    <mergeCell ref="CB8:CC9"/>
+    <mergeCell ref="CB10:CC10"/>
+    <mergeCell ref="CB11:CC11"/>
+    <mergeCell ref="CB12:CC12"/>
     <mergeCell ref="AX8:AX9"/>
     <mergeCell ref="AZ10:AZ15"/>
     <mergeCell ref="BA10:BA15"/>
@@ -6064,9 +6217,9 @@
     <mergeCell ref="N8:N9"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="AY8:AY9"/>
-    <mergeCell ref="BC6:BC7"/>
+    <mergeCell ref="BD6:BD7"/>
     <mergeCell ref="BB6:BB7"/>
-    <mergeCell ref="BS24:BV24"/>
+    <mergeCell ref="BU24:BX24"/>
     <mergeCell ref="AA10:AL10"/>
     <mergeCell ref="AR8:AR9"/>
     <mergeCell ref="AW8:AW9"/>
@@ -6092,22 +6245,22 @@
     <mergeCell ref="AQ8:AQ9"/>
     <mergeCell ref="D5:AR5"/>
     <mergeCell ref="AS5:BA5"/>
-    <mergeCell ref="BF5:BL5"/>
-    <mergeCell ref="BM5:CA5"/>
-    <mergeCell ref="CB5:CN5"/>
+    <mergeCell ref="BG5:BN5"/>
+    <mergeCell ref="BO5:CD5"/>
+    <mergeCell ref="CE5:CQ5"/>
     <mergeCell ref="N7:V7"/>
     <mergeCell ref="W7:AL7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:M7"/>
-    <mergeCell ref="BO6:BO7"/>
-    <mergeCell ref="BP6:BP7"/>
-    <mergeCell ref="BQ6:BR7"/>
-    <mergeCell ref="BS6:CA7"/>
-    <mergeCell ref="BB5:BE5"/>
-    <mergeCell ref="BD6:BD7"/>
-    <mergeCell ref="BE6:BE7"/>
+    <mergeCell ref="BQ6:BQ7"/>
+    <mergeCell ref="BR6:BR7"/>
+    <mergeCell ref="BS6:BT7"/>
+    <mergeCell ref="BU6:CD7"/>
+    <mergeCell ref="BB5:BF5"/>
+    <mergeCell ref="BC6:BC7"/>
+    <mergeCell ref="BI6:BI7"/>
     <mergeCell ref="L8:L9"/>
     <mergeCell ref="K8:K9"/>
     <mergeCell ref="J8:J9"/>
@@ -6123,17 +6276,17 @@
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="P10:V10"/>
     <mergeCell ref="P8:V8"/>
-    <mergeCell ref="BQ12:BQ15"/>
-    <mergeCell ref="BR12:BR15"/>
+    <mergeCell ref="BS12:BS15"/>
+    <mergeCell ref="BT12:BT15"/>
+    <mergeCell ref="BN8:BN9"/>
+    <mergeCell ref="BM8:BM9"/>
     <mergeCell ref="BL8:BL9"/>
     <mergeCell ref="BK8:BK9"/>
     <mergeCell ref="BJ8:BJ9"/>
-    <mergeCell ref="BI8:BI9"/>
-    <mergeCell ref="BH8:BH9"/>
-    <mergeCell ref="BF10:BF15"/>
     <mergeCell ref="BG10:BG15"/>
     <mergeCell ref="BH10:BH15"/>
-    <mergeCell ref="BI10:BI15"/>
+    <mergeCell ref="BJ10:BJ15"/>
+    <mergeCell ref="BK10:BK15"/>
     <mergeCell ref="V12:V13"/>
     <mergeCell ref="AA12:AA15"/>
     <mergeCell ref="AB12:AB15"/>
@@ -6144,8 +6297,8 @@
     <mergeCell ref="AJ12:AJ13"/>
     <mergeCell ref="AI12:AI13"/>
     <mergeCell ref="AH12:AH13"/>
-    <mergeCell ref="CD8:CD9"/>
-    <mergeCell ref="CE8:CE9"/>
+    <mergeCell ref="CG8:CG9"/>
+    <mergeCell ref="CH8:CH9"/>
     <mergeCell ref="W10:W15"/>
     <mergeCell ref="X10:X15"/>
     <mergeCell ref="Y10:Y15"/>
@@ -6157,14 +6310,16 @@
     <mergeCell ref="AQ10:AQ15"/>
     <mergeCell ref="AR10:AR15"/>
     <mergeCell ref="AS10:AS15"/>
-    <mergeCell ref="BW8:BW9"/>
-    <mergeCell ref="BR8:BR9"/>
-    <mergeCell ref="BQ8:BQ9"/>
+    <mergeCell ref="BZ8:BZ9"/>
+    <mergeCell ref="BT8:BT9"/>
+    <mergeCell ref="BS8:BS9"/>
+    <mergeCell ref="BQ8:BQ15"/>
+    <mergeCell ref="BR8:BR15"/>
+    <mergeCell ref="AX10:AX15"/>
     <mergeCell ref="BO8:BO15"/>
-    <mergeCell ref="BP8:BP15"/>
-    <mergeCell ref="AX10:AX15"/>
-    <mergeCell ref="BM8:BM15"/>
-    <mergeCell ref="CN8:CN9"/>
+    <mergeCell ref="BD8:BD9"/>
+    <mergeCell ref="BY8:BY9"/>
+    <mergeCell ref="CQ8:CQ9"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="D8:D15"/>
     <mergeCell ref="E8:E15"/>
@@ -6176,26 +6331,26 @@
     <mergeCell ref="K10:K15"/>
     <mergeCell ref="L10:L15"/>
     <mergeCell ref="M10:M15"/>
-    <mergeCell ref="CB8:CB15"/>
-    <mergeCell ref="CC8:CC15"/>
+    <mergeCell ref="CE8:CE15"/>
     <mergeCell ref="CF8:CF15"/>
-    <mergeCell ref="CG8:CG15"/>
-    <mergeCell ref="CM8:CM9"/>
-    <mergeCell ref="CH8:CH9"/>
-    <mergeCell ref="CI8:CL9"/>
-    <mergeCell ref="CI10:CI11"/>
-    <mergeCell ref="CJ10:CJ11"/>
-    <mergeCell ref="CK10:CK11"/>
+    <mergeCell ref="CI8:CI15"/>
+    <mergeCell ref="CJ8:CJ15"/>
+    <mergeCell ref="CP8:CP9"/>
+    <mergeCell ref="CK8:CK9"/>
+    <mergeCell ref="CL8:CO9"/>
+    <mergeCell ref="CL10:CL11"/>
+    <mergeCell ref="CM10:CM11"/>
+    <mergeCell ref="CN10:CN11"/>
     <mergeCell ref="AD12:AD15"/>
     <mergeCell ref="AG12:AG13"/>
-    <mergeCell ref="BN8:BN15"/>
-    <mergeCell ref="BJ12:BJ15"/>
+    <mergeCell ref="BP8:BP15"/>
+    <mergeCell ref="BL12:BL15"/>
     <mergeCell ref="R14:R15"/>
     <mergeCell ref="S14:S15"/>
     <mergeCell ref="T14:T15"/>
     <mergeCell ref="U14:U15"/>
     <mergeCell ref="V14:V15"/>
-    <mergeCell ref="BK10:BK15"/>
+    <mergeCell ref="BM10:BM15"/>
     <mergeCell ref="AE14:AE15"/>
     <mergeCell ref="AF14:AF15"/>
     <mergeCell ref="AG14:AG15"/>
@@ -6209,42 +6364,42 @@
     <mergeCell ref="AV10:AV15"/>
     <mergeCell ref="AW10:AW15"/>
     <mergeCell ref="AF12:AF13"/>
-    <mergeCell ref="BW10:BW15"/>
-    <mergeCell ref="CJ12:CJ15"/>
-    <mergeCell ref="CK12:CK15"/>
+    <mergeCell ref="BZ10:BZ15"/>
+    <mergeCell ref="CM12:CM15"/>
+    <mergeCell ref="CN12:CN15"/>
+    <mergeCell ref="CO12:CO15"/>
+    <mergeCell ref="CG10:CG15"/>
+    <mergeCell ref="CH10:CH15"/>
+    <mergeCell ref="CK10:CK15"/>
+    <mergeCell ref="BU12:BU15"/>
+    <mergeCell ref="BV12:BV15"/>
+    <mergeCell ref="BX12:BX15"/>
     <mergeCell ref="CL12:CL15"/>
-    <mergeCell ref="CD10:CD15"/>
-    <mergeCell ref="CE10:CE15"/>
-    <mergeCell ref="CH10:CH15"/>
-    <mergeCell ref="BS12:BS15"/>
-    <mergeCell ref="BT12:BT15"/>
-    <mergeCell ref="BV12:BV15"/>
-    <mergeCell ref="CI12:CI15"/>
-    <mergeCell ref="CL10:CL11"/>
-    <mergeCell ref="CB6:CB7"/>
-    <mergeCell ref="CC6:CC7"/>
-    <mergeCell ref="CD6:CE7"/>
+    <mergeCell ref="CO10:CO11"/>
+    <mergeCell ref="CE6:CE7"/>
     <mergeCell ref="CF6:CF7"/>
-    <mergeCell ref="CG6:CG7"/>
-    <mergeCell ref="CH6:CL7"/>
-    <mergeCell ref="CM6:CN7"/>
-    <mergeCell ref="BL14:BL15"/>
+    <mergeCell ref="CG6:CH7"/>
+    <mergeCell ref="CI6:CI7"/>
+    <mergeCell ref="CJ6:CJ7"/>
+    <mergeCell ref="CK6:CO7"/>
+    <mergeCell ref="CP6:CQ7"/>
+    <mergeCell ref="BN14:BN15"/>
     <mergeCell ref="C6:C15"/>
     <mergeCell ref="AM6:AR7"/>
     <mergeCell ref="AS6:AW7"/>
     <mergeCell ref="AX6:BA7"/>
-    <mergeCell ref="BF6:BF7"/>
     <mergeCell ref="BG6:BG7"/>
-    <mergeCell ref="BH6:BL7"/>
-    <mergeCell ref="BM6:BM7"/>
-    <mergeCell ref="BN6:BN7"/>
-    <mergeCell ref="CM10:CM15"/>
-    <mergeCell ref="CN10:CN15"/>
-    <mergeCell ref="BS8:BV9"/>
+    <mergeCell ref="BH6:BH7"/>
+    <mergeCell ref="BJ6:BN7"/>
+    <mergeCell ref="BO6:BO7"/>
+    <mergeCell ref="BP6:BP7"/>
+    <mergeCell ref="CP10:CP15"/>
+    <mergeCell ref="CQ10:CQ15"/>
+    <mergeCell ref="BU8:BX9"/>
+    <mergeCell ref="BX10:BX11"/>
     <mergeCell ref="BV10:BV11"/>
-    <mergeCell ref="BT10:BT11"/>
-    <mergeCell ref="BS10:BS11"/>
     <mergeCell ref="BU10:BU11"/>
+    <mergeCell ref="BW10:BW11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remove the variable refresh dropdowns - function will be called as needed
</commit_message>
<xml_diff>
--- a/docs/session_variables.xlsx
+++ b/docs/session_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robhay/git_repo/share_screener/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474BCC5C-6A2C-3448-829D-2F57C4DAD29A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D4FD93-B9C1-3143-B76E-C9F9AD5AFE95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="25600" windowHeight="14500" activeTab="1" xr2:uid="{EB3C945B-FE01-FA47-AE59-A0DC3CDF521B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14500" xr2:uid="{EB3C945B-FE01-FA47-AE59-A0DC3CDF521B}"/>
   </bookViews>
   <sheets>
     <sheet name="Application Structure (2)" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="612">
   <si>
     <t>chart_colours</t>
   </si>
@@ -2280,6 +2280,12 @@
   </si>
   <si>
     <t>shoul be widgets</t>
+  </si>
+  <si>
+    <t>This will include the dataframes and the column status and the dataframe status</t>
+  </si>
+  <si>
+    <t>might be able to remove this one</t>
   </si>
 </sst>
 </file>
@@ -3004,7 +3010,7 @@
     <xf numFmtId="43" fontId="43" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="43" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="425">
+  <cellXfs count="432">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4019,6 +4025,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4031,12 +4040,18 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="58" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4106,24 +4121,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4183,6 +4180,36 @@
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4388,358 +4415,6 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>Ticker Index</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Rectangle 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAED6741-B8D6-4E4F-99DB-8B863BDB231A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8267700" y="355600"/>
-          <a:ext cx="4279900" cy="1054100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="7030A0"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Apps</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>(single, screener, intraday)</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Rectangle 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52136218-B114-8145-9504-DA3E8E555742}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8293100" y="3302000"/>
-          <a:ext cx="4254500" cy="520700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="7030A0"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Ticker</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> List</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>(list of selected Tickers for app)</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectangle 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3672E898-7CEE-3145-8372-CCB797AC1D28}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8280400" y="1460500"/>
-          <a:ext cx="2273300" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent2">
-            <a:lumMod val="40000"/>
-            <a:lumOff val="60000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Config</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Rectangle 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94E58870-0488-6243-AA2D-30280F4CE05F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8293100" y="2184400"/>
-          <a:ext cx="4254500" cy="1028700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="7030A0"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Ticker Selectors</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Rectangle 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93ADA72F-C282-8B45-A9B1-377309A11040}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10604500" y="1460500"/>
-          <a:ext cx="1917700" cy="584200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent2"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Search Results</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5349,15 +5024,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5372,8 +5047,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14465300" y="2781300"/>
-          <a:ext cx="3378200" cy="520700"/>
+          <a:off x="14490700" y="3022600"/>
+          <a:ext cx="2768600" cy="520700"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -5423,7 +5098,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:colOff>635000</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -5441,7 +5116,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15989300" y="812800"/>
-          <a:ext cx="977900" cy="520700"/>
+          <a:ext cx="1155700" cy="520700"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -5491,9 +5166,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5509,7 +5184,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14452600" y="800100"/>
-          <a:ext cx="1231900" cy="1130300"/>
+          <a:ext cx="1422400" cy="1206500"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -5635,16 +5310,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5659,7 +5334,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17119600" y="1422400"/>
+          <a:off x="15621000" y="2197100"/>
           <a:ext cx="660400" cy="571500"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -5704,15 +5379,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5730,8 +5405,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="15186025" y="1812925"/>
-          <a:ext cx="850900" cy="1085850"/>
+          <a:off x="15011400" y="2159000"/>
+          <a:ext cx="1016000" cy="711200"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -5762,15 +5437,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5785,8 +5460,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16002000" y="1587500"/>
-          <a:ext cx="977900" cy="533400"/>
+          <a:off x="15989300" y="1460500"/>
+          <a:ext cx="1168400" cy="533400"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -5830,15 +5505,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>806450</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5856,8 +5531,122 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="15992475" y="2282825"/>
-          <a:ext cx="660400" cy="336550"/>
+          <a:off x="15709900" y="2159000"/>
+          <a:ext cx="1028700" cy="698500"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Elbow Connector 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{114A1E03-F3E2-AE4D-9165-03430541E8F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="26" idx="2"/>
+          <a:endCxn id="33" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="16506825" y="1393825"/>
+          <a:ext cx="127000" cy="6350"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="Elbow Connector 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A00101B8-BD77-AF47-AB51-7F020F0EE8FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="27" idx="2"/>
+          <a:endCxn id="29" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="15462250" y="1708150"/>
+          <a:ext cx="190500" cy="787400"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -5888,94 +5677,38 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>793750</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>806450</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="37" name="Elbow Connector 36">
+        <xdr:cNvPr id="63" name="Elbow Connector 62">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{114A1E03-F3E2-AE4D-9165-03430541E8F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D2AAB6E-906A-FE4F-BEDE-7FC971739F25}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="26" idx="2"/>
-          <a:endCxn id="33" idx="0"/>
+          <a:stCxn id="33" idx="2"/>
+          <a:endCxn id="29" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="16357600" y="1454150"/>
-          <a:ext cx="254000" cy="12700"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="45" name="Elbow Connector 44">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A00101B8-BD77-AF47-AB51-7F020F0EE8FC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="27" idx="2"/>
-          <a:endCxn id="29" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="16227425" y="771525"/>
-          <a:ext cx="63500" cy="2381250"/>
+        <a:xfrm rot="5400000">
+          <a:off x="16160750" y="1784350"/>
+          <a:ext cx="203200" cy="622300"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 460000"/>
+            <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -6001,58 +5734,375 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="63" name="Elbow Connector 62">
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="109" name="Rounded Rectangle 108">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D2AAB6E-906A-FE4F-BEDE-7FC971739F25}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{079DC555-4BB1-894A-9B9E-877366A6D344}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="33" idx="3"/>
-          <a:endCxn id="29" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="16979900" y="1708150"/>
-          <a:ext cx="139700" cy="146050"/>
+        <a:xfrm>
+          <a:off x="17754600" y="254000"/>
+          <a:ext cx="2705100" cy="647700"/>
         </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
+        <a:prstGeom prst="roundRect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
         </a:lnRef>
-        <a:fillRef idx="0">
+        <a:fillRef idx="1">
           <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
-    </xdr:cxnSp>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Apps</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(single, screener, intraday)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="110" name="Rounded Rectangle 109">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37FFC2D1-A46C-2943-ABF6-963534CA788D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17703800" y="1028700"/>
+          <a:ext cx="1587500" cy="558800"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Config</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="111" name="Rounded Rectangle 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4426E487-C44B-0044-AF70-2D9E7E617A4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19392900" y="1028700"/>
+          <a:ext cx="1574800" cy="584200"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Search</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Results</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="112" name="Rounded Rectangle 111">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF66E79A-CFA0-4D48-A325-7EC954927411}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17678400" y="1765300"/>
+          <a:ext cx="3340100" cy="1041400"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Selectors</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>( for Ticker(s) )</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="113" name="Rounded Rectangle 112">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C0B758D-6FFB-114C-BEF5-70DA154EAB70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17703800" y="2933700"/>
+          <a:ext cx="3378200" cy="1041400"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Ticker List</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>( list of selected tickers for each App)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6357,17 +6407,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4BE9BCD-FFB7-0845-95F9-377ADF3DB526}">
   <dimension ref="A1:T112"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C75" sqref="C75:D79"/>
+      <selection pane="bottomRight" activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
   <cols>
     <col min="1" max="1" width="4.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="20.5" style="374" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="376" customWidth="1"/>
     <col min="3" max="3" width="9" style="70" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" style="70" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.1640625" style="70" customWidth="1"/>
@@ -6399,22 +6449,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="59" customHeight="1">
-      <c r="A1" s="421" t="s">
+      <c r="A1" s="418" t="s">
         <v>480</v>
       </c>
-      <c r="B1" s="422"/>
-      <c r="C1" s="422"/>
-      <c r="D1" s="422"/>
-      <c r="E1" s="422"/>
-      <c r="F1" s="422"/>
-      <c r="G1" s="422"/>
-      <c r="H1" s="422"/>
-      <c r="J1" s="419" t="s">
+      <c r="B1" s="419"/>
+      <c r="C1" s="419"/>
+      <c r="D1" s="419"/>
+      <c r="E1" s="419"/>
+      <c r="F1" s="419"/>
+      <c r="G1" s="419"/>
+      <c r="H1" s="419"/>
+      <c r="J1" s="416" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="J2" s="420" t="s">
+      <c r="J2" s="417" t="s">
         <v>503</v>
       </c>
     </row>
@@ -6449,39 +6499,39 @@
       </c>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="370"/>
-      <c r="B4" s="375"/>
-      <c r="C4" s="378"/>
-      <c r="D4" s="378"/>
-      <c r="E4" s="378"/>
-      <c r="F4" s="378"/>
-      <c r="G4" s="378"/>
-      <c r="H4" s="378"/>
-      <c r="I4" s="378"/>
-      <c r="J4" s="378"/>
+      <c r="A4" s="371"/>
+      <c r="B4" s="377"/>
+      <c r="C4" s="381"/>
+      <c r="D4" s="381"/>
+      <c r="E4" s="381"/>
+      <c r="F4" s="381"/>
+      <c r="G4" s="381"/>
+      <c r="H4" s="381"/>
+      <c r="I4" s="381"/>
+      <c r="J4" s="381"/>
       <c r="K4" s="6"/>
-      <c r="L4" s="370"/>
-      <c r="M4" s="370"/>
-      <c r="N4" s="370"/>
-      <c r="O4" s="370"/>
-      <c r="P4" s="370"/>
-      <c r="Q4" s="370"/>
-      <c r="R4" s="370"/>
-      <c r="S4" s="370"/>
-      <c r="T4" s="370"/>
+      <c r="L4" s="371"/>
+      <c r="M4" s="371"/>
+      <c r="N4" s="371"/>
+      <c r="O4" s="371"/>
+      <c r="P4" s="371"/>
+      <c r="Q4" s="371"/>
+      <c r="R4" s="371"/>
+      <c r="S4" s="371"/>
+      <c r="T4" s="371"/>
     </row>
     <row r="5" spans="1:20" ht="31" customHeight="1">
-      <c r="B5" s="393" t="s">
+      <c r="B5" s="396" t="s">
         <v>289</v>
       </c>
-      <c r="C5" s="379"/>
-      <c r="D5" s="379"/>
-      <c r="E5" s="379"/>
-      <c r="F5" s="379"/>
-      <c r="G5" s="379"/>
-      <c r="H5" s="379"/>
-      <c r="I5" s="379"/>
-      <c r="J5" s="379"/>
+      <c r="C5" s="382"/>
+      <c r="D5" s="382"/>
+      <c r="E5" s="382"/>
+      <c r="F5" s="382"/>
+      <c r="G5" s="382"/>
+      <c r="H5" s="382"/>
+      <c r="I5" s="382"/>
+      <c r="J5" s="382"/>
       <c r="K5" s="6"/>
       <c r="L5" s="133" t="s">
         <v>96</v>
@@ -6492,40 +6542,40 @@
       <c r="N5" s="11"/>
     </row>
     <row r="6" spans="1:20" ht="31" customHeight="1">
-      <c r="B6" s="376" t="s">
+      <c r="B6" s="429" t="s">
         <v>263</v>
       </c>
-      <c r="C6" s="391" t="s">
+      <c r="C6" s="370" t="s">
         <v>286</v>
       </c>
-      <c r="D6" s="391"/>
-      <c r="E6" s="380"/>
-      <c r="F6" s="380"/>
-      <c r="G6" s="380"/>
-      <c r="H6" s="380"/>
-      <c r="I6" s="380"/>
-      <c r="J6" s="380"/>
+      <c r="D6" s="370"/>
+      <c r="E6" s="383"/>
+      <c r="F6" s="383"/>
+      <c r="G6" s="383"/>
+      <c r="H6" s="383"/>
+      <c r="I6" s="383"/>
+      <c r="J6" s="383"/>
       <c r="K6" s="6"/>
       <c r="L6" s="133" t="s">
         <v>434</v>
       </c>
-      <c r="M6" s="373" t="s">
+      <c r="M6" s="374" t="s">
         <v>100</v>
       </c>
       <c r="N6" s="11"/>
     </row>
     <row r="7" spans="1:20" ht="31" customHeight="1">
-      <c r="B7" s="376"/>
-      <c r="C7" s="391" t="s">
+      <c r="B7" s="430"/>
+      <c r="C7" s="370" t="s">
         <v>285</v>
       </c>
-      <c r="D7" s="391"/>
-      <c r="E7" s="380"/>
-      <c r="F7" s="380"/>
-      <c r="G7" s="380"/>
-      <c r="H7" s="380"/>
-      <c r="I7" s="380"/>
-      <c r="J7" s="380"/>
+      <c r="D7" s="370"/>
+      <c r="E7" s="383"/>
+      <c r="F7" s="383"/>
+      <c r="G7" s="383"/>
+      <c r="H7" s="383"/>
+      <c r="I7" s="383"/>
+      <c r="J7" s="383"/>
       <c r="K7" s="6"/>
       <c r="L7" s="133" t="s">
         <v>98</v>
@@ -6536,17 +6586,17 @@
       <c r="N7" s="11"/>
     </row>
     <row r="8" spans="1:20" ht="31" customHeight="1">
-      <c r="B8" s="376"/>
-      <c r="C8" s="391" t="s">
+      <c r="B8" s="430"/>
+      <c r="C8" s="370" t="s">
         <v>288</v>
       </c>
-      <c r="D8" s="391"/>
-      <c r="E8" s="380"/>
-      <c r="F8" s="380"/>
-      <c r="G8" s="380"/>
-      <c r="H8" s="380"/>
-      <c r="I8" s="380"/>
-      <c r="J8" s="380"/>
+      <c r="D8" s="370"/>
+      <c r="E8" s="383"/>
+      <c r="F8" s="383"/>
+      <c r="G8" s="383"/>
+      <c r="H8" s="383"/>
+      <c r="I8" s="383"/>
+      <c r="J8" s="383"/>
       <c r="K8" s="6"/>
       <c r="L8" s="133" t="s">
         <v>434</v>
@@ -6557,19 +6607,19 @@
       <c r="N8" s="11"/>
     </row>
     <row r="9" spans="1:20" ht="31" customHeight="1">
-      <c r="B9" s="376"/>
-      <c r="C9" s="372" t="s">
+      <c r="B9" s="430"/>
+      <c r="C9" s="375" t="s">
         <v>262</v>
       </c>
-      <c r="D9" s="372"/>
-      <c r="E9" s="382" t="s">
+      <c r="D9" s="375"/>
+      <c r="E9" s="385" t="s">
         <v>375</v>
       </c>
-      <c r="F9" s="382"/>
-      <c r="G9" s="380"/>
-      <c r="H9" s="380"/>
-      <c r="I9" s="380"/>
-      <c r="J9" s="380"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="383"/>
+      <c r="H9" s="383"/>
+      <c r="I9" s="383"/>
+      <c r="J9" s="383"/>
       <c r="K9" s="6"/>
       <c r="L9" s="133" t="s">
         <v>96</v>
@@ -6578,19 +6628,22 @@
         <v>0</v>
       </c>
       <c r="N9" s="11"/>
+      <c r="O9" s="4" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="10" spans="1:20" ht="31" customHeight="1">
-      <c r="B10" s="376"/>
-      <c r="C10" s="372"/>
-      <c r="D10" s="372"/>
-      <c r="E10" s="382" t="s">
+      <c r="B10" s="430"/>
+      <c r="C10" s="375"/>
+      <c r="D10" s="375"/>
+      <c r="E10" s="385" t="s">
         <v>267</v>
       </c>
-      <c r="F10" s="382"/>
-      <c r="G10" s="380"/>
-      <c r="H10" s="380"/>
-      <c r="I10" s="380"/>
-      <c r="J10" s="380"/>
+      <c r="F10" s="385"/>
+      <c r="G10" s="383"/>
+      <c r="H10" s="383"/>
+      <c r="I10" s="383"/>
+      <c r="J10" s="383"/>
       <c r="K10" s="6"/>
       <c r="L10" s="133" t="s">
         <v>91</v>
@@ -6601,17 +6654,17 @@
       <c r="N10" s="11"/>
     </row>
     <row r="11" spans="1:20" ht="31" customHeight="1">
-      <c r="B11" s="376"/>
-      <c r="C11" s="372"/>
-      <c r="D11" s="372"/>
-      <c r="E11" s="382" t="s">
+      <c r="B11" s="430"/>
+      <c r="C11" s="375"/>
+      <c r="D11" s="375"/>
+      <c r="E11" s="385" t="s">
         <v>268</v>
       </c>
-      <c r="F11" s="382"/>
-      <c r="G11" s="380"/>
-      <c r="H11" s="380"/>
-      <c r="I11" s="380"/>
-      <c r="J11" s="380"/>
+      <c r="F11" s="385"/>
+      <c r="G11" s="383"/>
+      <c r="H11" s="383"/>
+      <c r="I11" s="383"/>
+      <c r="J11" s="383"/>
       <c r="K11" s="6"/>
       <c r="L11" s="133" t="s">
         <v>91</v>
@@ -6622,17 +6675,17 @@
       <c r="N11" s="11"/>
     </row>
     <row r="12" spans="1:20" ht="31" customHeight="1">
-      <c r="B12" s="376"/>
-      <c r="C12" s="372"/>
-      <c r="D12" s="372"/>
-      <c r="E12" s="382" t="s">
+      <c r="B12" s="430"/>
+      <c r="C12" s="375"/>
+      <c r="D12" s="375"/>
+      <c r="E12" s="385" t="s">
         <v>261</v>
       </c>
-      <c r="F12" s="382"/>
-      <c r="G12" s="380"/>
-      <c r="H12" s="380"/>
-      <c r="I12" s="380"/>
-      <c r="J12" s="380"/>
+      <c r="F12" s="385"/>
+      <c r="G12" s="383"/>
+      <c r="H12" s="383"/>
+      <c r="I12" s="383"/>
+      <c r="J12" s="383"/>
       <c r="K12" s="6"/>
       <c r="L12" s="133" t="s">
         <v>91</v>
@@ -6643,17 +6696,17 @@
       <c r="N12" s="11"/>
     </row>
     <row r="13" spans="1:20" ht="31" customHeight="1">
-      <c r="B13" s="376"/>
-      <c r="C13" s="372"/>
-      <c r="D13" s="372"/>
-      <c r="E13" s="382" t="s">
+      <c r="B13" s="430"/>
+      <c r="C13" s="375"/>
+      <c r="D13" s="375"/>
+      <c r="E13" s="385" t="s">
         <v>269</v>
       </c>
-      <c r="F13" s="382"/>
-      <c r="G13" s="380"/>
-      <c r="H13" s="380"/>
-      <c r="I13" s="380"/>
-      <c r="J13" s="380"/>
+      <c r="F13" s="385"/>
+      <c r="G13" s="383"/>
+      <c r="H13" s="383"/>
+      <c r="I13" s="383"/>
+      <c r="J13" s="383"/>
       <c r="K13" s="6"/>
       <c r="L13" s="133" t="s">
         <v>91</v>
@@ -6664,17 +6717,17 @@
       <c r="N13" s="11"/>
     </row>
     <row r="14" spans="1:20" ht="31" customHeight="1">
-      <c r="B14" s="376"/>
-      <c r="C14" s="372"/>
-      <c r="D14" s="372"/>
-      <c r="E14" s="382" t="s">
+      <c r="B14" s="430"/>
+      <c r="C14" s="375"/>
+      <c r="D14" s="375"/>
+      <c r="E14" s="385" t="s">
         <v>284</v>
       </c>
-      <c r="F14" s="382"/>
-      <c r="G14" s="380"/>
-      <c r="H14" s="380"/>
-      <c r="I14" s="380"/>
-      <c r="J14" s="380"/>
+      <c r="F14" s="385"/>
+      <c r="G14" s="383"/>
+      <c r="H14" s="383"/>
+      <c r="I14" s="383"/>
+      <c r="J14" s="383"/>
       <c r="K14" s="6"/>
       <c r="L14" s="133" t="s">
         <v>91</v>
@@ -6685,17 +6738,17 @@
       <c r="N14" s="11"/>
     </row>
     <row r="15" spans="1:20" ht="31" customHeight="1">
-      <c r="B15" s="376"/>
-      <c r="C15" s="372"/>
-      <c r="D15" s="372"/>
-      <c r="E15" s="382" t="s">
+      <c r="B15" s="431"/>
+      <c r="C15" s="375"/>
+      <c r="D15" s="375"/>
+      <c r="E15" s="385" t="s">
         <v>283</v>
       </c>
-      <c r="F15" s="382"/>
-      <c r="G15" s="380"/>
-      <c r="H15" s="380"/>
-      <c r="I15" s="380"/>
-      <c r="J15" s="380"/>
+      <c r="F15" s="385"/>
+      <c r="G15" s="383"/>
+      <c r="H15" s="383"/>
+      <c r="I15" s="383"/>
+      <c r="J15" s="383"/>
       <c r="K15" s="6"/>
       <c r="L15" s="133" t="s">
         <v>91</v>
@@ -6706,216 +6759,188 @@
       <c r="N15" s="11"/>
     </row>
     <row r="16" spans="1:20" ht="31" customHeight="1">
-      <c r="B16" s="376"/>
-      <c r="C16" s="365" t="s">
-        <v>502</v>
-      </c>
-      <c r="D16" s="391" t="s">
-        <v>429</v>
-      </c>
-      <c r="E16" s="382" t="s">
-        <v>431</v>
-      </c>
-      <c r="F16" s="382"/>
-      <c r="G16" s="380"/>
-      <c r="H16" s="380"/>
-      <c r="I16" s="380"/>
-      <c r="J16" s="380"/>
+      <c r="B16" s="378" t="s">
+        <v>258</v>
+      </c>
+      <c r="C16" s="375" t="s">
+        <v>275</v>
+      </c>
+      <c r="D16" s="375"/>
+      <c r="E16" s="385" t="s">
+        <v>258</v>
+      </c>
+      <c r="F16" s="385"/>
+      <c r="G16" s="383"/>
+      <c r="H16" s="383"/>
+      <c r="I16" s="383"/>
+      <c r="J16" s="383"/>
       <c r="K16" s="6"/>
       <c r="L16" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="M16" s="138" t="s">
-        <v>438</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="M16" s="11"/>
       <c r="N16" s="11"/>
     </row>
     <row r="17" spans="2:14" ht="31" customHeight="1">
-      <c r="B17" s="376"/>
-      <c r="C17" s="365"/>
-      <c r="D17" s="391"/>
-      <c r="E17" s="382" t="s">
-        <v>395</v>
-      </c>
-      <c r="F17" s="382"/>
-      <c r="G17" s="380"/>
-      <c r="H17" s="380"/>
-      <c r="I17" s="380"/>
-      <c r="J17" s="380"/>
-      <c r="K17" s="6"/>
+      <c r="B17" s="378"/>
+      <c r="C17" s="375"/>
+      <c r="D17" s="375"/>
+      <c r="E17" s="385" t="s">
+        <v>274</v>
+      </c>
+      <c r="F17" s="385"/>
+      <c r="G17" s="383"/>
+      <c r="H17" s="383"/>
+      <c r="I17" s="383"/>
+      <c r="J17" s="383"/>
       <c r="L17" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="M17" s="138" t="s">
-        <v>592</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="M17" s="11"/>
       <c r="N17" s="11"/>
     </row>
     <row r="18" spans="2:14" ht="31" customHeight="1">
-      <c r="B18" s="376"/>
-      <c r="C18" s="365"/>
-      <c r="D18" s="391"/>
-      <c r="E18" s="365" t="s">
-        <v>499</v>
-      </c>
-      <c r="F18" s="398" t="s">
-        <v>445</v>
-      </c>
-      <c r="G18" s="365" t="s">
-        <v>263</v>
-      </c>
-      <c r="H18" s="381" t="s">
-        <v>136</v>
-      </c>
-      <c r="I18" s="364"/>
-      <c r="J18" s="364"/>
-      <c r="K18" s="6"/>
+      <c r="B18" s="378"/>
+      <c r="C18" s="375"/>
+      <c r="D18" s="375"/>
+      <c r="E18" s="385" t="s">
+        <v>277</v>
+      </c>
+      <c r="F18" s="385"/>
+      <c r="G18" s="383"/>
+      <c r="H18" s="383"/>
+      <c r="I18" s="383"/>
+      <c r="J18" s="383"/>
       <c r="L18" s="133" t="s">
-        <v>96</v>
-      </c>
-      <c r="M18" s="116" t="s">
-        <v>411</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="M18" s="11"/>
       <c r="N18" s="11"/>
     </row>
     <row r="19" spans="2:14" ht="31" customHeight="1">
-      <c r="B19" s="376"/>
-      <c r="C19" s="365"/>
-      <c r="D19" s="391"/>
-      <c r="E19" s="365"/>
-      <c r="F19" s="398"/>
-      <c r="G19" s="365"/>
-      <c r="H19" s="381" t="s">
-        <v>137</v>
-      </c>
-      <c r="I19" s="364"/>
-      <c r="J19" s="364"/>
-      <c r="K19" s="6"/>
+      <c r="B19" s="378"/>
+      <c r="C19" s="375"/>
+      <c r="D19" s="375"/>
+      <c r="E19" s="385" t="s">
+        <v>261</v>
+      </c>
+      <c r="F19" s="385"/>
+      <c r="G19" s="383"/>
+      <c r="H19" s="383"/>
+      <c r="I19" s="383"/>
+      <c r="J19" s="383"/>
       <c r="L19" s="133" t="s">
-        <v>434</v>
+        <v>113</v>
       </c>
       <c r="M19" s="11"/>
-      <c r="N19" s="175" t="s">
-        <v>436</v>
-      </c>
+      <c r="N19" s="11"/>
     </row>
     <row r="20" spans="2:14" ht="31" customHeight="1">
-      <c r="B20" s="376"/>
-      <c r="C20" s="365"/>
-      <c r="D20" s="391"/>
-      <c r="E20" s="365"/>
-      <c r="F20" s="398"/>
-      <c r="G20" s="365"/>
-      <c r="H20" s="382" t="s">
-        <v>426</v>
-      </c>
-      <c r="I20" s="413" t="s">
-        <v>141</v>
-      </c>
-      <c r="J20" s="414"/>
-      <c r="K20" s="6"/>
+      <c r="B20" s="378"/>
+      <c r="C20" s="375"/>
+      <c r="D20" s="375"/>
+      <c r="E20" s="385" t="s">
+        <v>273</v>
+      </c>
+      <c r="F20" s="385"/>
+      <c r="G20" s="383"/>
+      <c r="H20" s="383"/>
+      <c r="I20" s="383"/>
+      <c r="J20" s="383"/>
       <c r="L20" s="133" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="M20" s="11"/>
-      <c r="N20" s="141" t="s">
-        <v>244</v>
-      </c>
+      <c r="N20" s="11"/>
     </row>
     <row r="21" spans="2:14" ht="31" customHeight="1">
-      <c r="B21" s="376"/>
-      <c r="C21" s="365"/>
-      <c r="D21" s="391"/>
-      <c r="E21" s="365"/>
-      <c r="F21" s="398"/>
-      <c r="G21" s="365"/>
-      <c r="H21" s="382"/>
-      <c r="I21" s="411" t="s">
-        <v>146</v>
-      </c>
-      <c r="J21" s="412"/>
-      <c r="K21" s="6"/>
+      <c r="B21" s="378"/>
+      <c r="C21" s="375" t="s">
+        <v>276</v>
+      </c>
+      <c r="D21" s="375"/>
+      <c r="E21" s="385" t="s">
+        <v>508</v>
+      </c>
+      <c r="F21" s="385"/>
+      <c r="G21" s="383"/>
+      <c r="H21" s="383"/>
+      <c r="I21" s="383"/>
+      <c r="J21" s="383"/>
       <c r="L21" s="133" t="s">
-        <v>434</v>
+        <v>97</v>
       </c>
       <c r="M21" s="11"/>
-      <c r="N21" s="175" t="s">
-        <v>245</v>
-      </c>
+      <c r="N21" s="11"/>
     </row>
     <row r="22" spans="2:14" ht="31" customHeight="1">
-      <c r="B22" s="376"/>
-      <c r="C22" s="365"/>
-      <c r="D22" s="391"/>
-      <c r="E22" s="365"/>
-      <c r="F22" s="398"/>
-      <c r="G22" s="365"/>
-      <c r="H22" s="382"/>
-      <c r="I22" s="411" t="s">
-        <v>408</v>
-      </c>
-      <c r="J22" s="412"/>
-      <c r="K22" s="6"/>
+      <c r="B22" s="378"/>
+      <c r="C22" s="375"/>
+      <c r="D22" s="375"/>
+      <c r="E22" s="385" t="s">
+        <v>272</v>
+      </c>
+      <c r="F22" s="385"/>
+      <c r="G22" s="383"/>
+      <c r="H22" s="383"/>
+      <c r="I22" s="383"/>
+      <c r="J22" s="383"/>
       <c r="L22" s="133" t="s">
-        <v>434</v>
-      </c>
-      <c r="M22" s="11"/>
-      <c r="N22" s="175" t="s">
-        <v>246</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="M22" s="175" t="s">
+        <v>114</v>
+      </c>
+      <c r="N22" s="11"/>
     </row>
     <row r="23" spans="2:14" ht="31" customHeight="1">
-      <c r="B23" s="376"/>
-      <c r="C23" s="365"/>
-      <c r="D23" s="391"/>
-      <c r="E23" s="365"/>
-      <c r="F23" s="398"/>
-      <c r="G23" s="365"/>
-      <c r="H23" s="382"/>
-      <c r="I23" s="411" t="s">
-        <v>409</v>
-      </c>
-      <c r="J23" s="412"/>
-      <c r="K23" s="6"/>
+      <c r="B23" s="378"/>
+      <c r="C23" s="375"/>
+      <c r="D23" s="375"/>
+      <c r="E23" s="385" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="385"/>
+      <c r="G23" s="383"/>
+      <c r="H23" s="383"/>
+      <c r="I23" s="383"/>
+      <c r="J23" s="383"/>
       <c r="L23" s="133" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="M23" s="11"/>
-      <c r="N23" s="68">
-        <v>4</v>
-      </c>
+      <c r="N23" s="11"/>
     </row>
     <row r="24" spans="2:14" ht="31" customHeight="1">
-      <c r="B24" s="376"/>
-      <c r="C24" s="365"/>
-      <c r="D24" s="391"/>
-      <c r="E24" s="365"/>
-      <c r="F24" s="398"/>
-      <c r="G24" s="365"/>
-      <c r="H24" s="382"/>
-      <c r="I24" s="411" t="s">
-        <v>410</v>
-      </c>
-      <c r="J24" s="412"/>
-      <c r="K24" s="6"/>
+      <c r="B24" s="378"/>
+      <c r="C24" s="375"/>
+      <c r="D24" s="375"/>
+      <c r="E24" s="385" t="s">
+        <v>273</v>
+      </c>
+      <c r="F24" s="385"/>
+      <c r="G24" s="383"/>
+      <c r="H24" s="383"/>
+      <c r="I24" s="383"/>
+      <c r="J24" s="383"/>
       <c r="L24" s="133" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="M24" s="11"/>
-      <c r="N24" s="68">
-        <v>10</v>
-      </c>
+      <c r="N24" s="11"/>
     </row>
     <row r="25" spans="2:14" ht="31" customHeight="1">
-      <c r="B25" s="376"/>
-      <c r="C25" s="365"/>
-      <c r="D25" s="391" t="s">
-        <v>430</v>
-      </c>
-      <c r="E25" s="382" t="s">
-        <v>379</v>
-      </c>
-      <c r="F25" s="382"/>
+      <c r="B25" s="428"/>
+      <c r="C25" s="365" t="s">
+        <v>502</v>
+      </c>
+      <c r="D25" s="394" t="s">
+        <v>429</v>
+      </c>
+      <c r="E25" s="385" t="s">
+        <v>431</v>
+      </c>
+      <c r="F25" s="385"/>
       <c r="G25" s="383"/>
       <c r="H25" s="383"/>
       <c r="I25" s="383"/>
@@ -6924,649 +6949,677 @@
       <c r="L25" s="133" t="s">
         <v>91</v>
       </c>
-      <c r="M25" s="177"/>
-      <c r="N25" s="138" t="s">
-        <v>440</v>
-      </c>
+      <c r="M25" s="138" t="s">
+        <v>438</v>
+      </c>
+      <c r="N25" s="11"/>
     </row>
     <row r="26" spans="2:14" ht="31" customHeight="1">
-      <c r="B26" s="376"/>
+      <c r="B26" s="428"/>
       <c r="C26" s="365"/>
-      <c r="D26" s="391"/>
-      <c r="E26" s="382" t="s">
-        <v>279</v>
-      </c>
-      <c r="F26" s="382"/>
+      <c r="D26" s="394"/>
+      <c r="E26" s="385" t="s">
+        <v>395</v>
+      </c>
+      <c r="F26" s="385"/>
       <c r="G26" s="383"/>
       <c r="H26" s="383"/>
       <c r="I26" s="383"/>
       <c r="J26" s="383"/>
       <c r="K26" s="6"/>
       <c r="L26" s="133" t="s">
-        <v>90</v>
-      </c>
-      <c r="M26" s="116">
-        <v>500</v>
+        <v>91</v>
+      </c>
+      <c r="M26" s="138" t="s">
+        <v>592</v>
       </c>
       <c r="N26" s="11"/>
     </row>
     <row r="27" spans="2:14" ht="31" customHeight="1">
-      <c r="B27" s="376"/>
+      <c r="B27" s="428"/>
       <c r="C27" s="365"/>
-      <c r="D27" s="391"/>
-      <c r="E27" s="382" t="s">
-        <v>507</v>
-      </c>
-      <c r="F27" s="382"/>
-      <c r="G27" s="383"/>
-      <c r="H27" s="383"/>
-      <c r="I27" s="383"/>
-      <c r="J27" s="383"/>
+      <c r="D27" s="394"/>
+      <c r="E27" s="365" t="s">
+        <v>499</v>
+      </c>
+      <c r="F27" s="401" t="s">
+        <v>445</v>
+      </c>
+      <c r="G27" s="365" t="s">
+        <v>263</v>
+      </c>
+      <c r="H27" s="384" t="s">
+        <v>136</v>
+      </c>
+      <c r="I27" s="364"/>
+      <c r="J27" s="364"/>
       <c r="K27" s="6"/>
       <c r="L27" s="133" t="s">
-        <v>90</v>
-      </c>
-      <c r="M27" s="116">
-        <v>500</v>
+        <v>96</v>
+      </c>
+      <c r="M27" s="116" t="s">
+        <v>411</v>
       </c>
       <c r="N27" s="11"/>
     </row>
     <row r="28" spans="2:14" ht="31" customHeight="1">
-      <c r="B28" s="376"/>
+      <c r="B28" s="428"/>
       <c r="C28" s="365"/>
-      <c r="D28" s="391"/>
-      <c r="E28" s="382" t="s">
-        <v>399</v>
-      </c>
-      <c r="F28" s="382"/>
-      <c r="G28" s="383"/>
-      <c r="H28" s="383"/>
-      <c r="I28" s="383"/>
-      <c r="J28" s="383"/>
+      <c r="D28" s="394"/>
+      <c r="E28" s="365"/>
+      <c r="F28" s="401"/>
+      <c r="G28" s="365"/>
+      <c r="H28" s="384" t="s">
+        <v>137</v>
+      </c>
+      <c r="I28" s="364"/>
+      <c r="J28" s="364"/>
       <c r="K28" s="6"/>
       <c r="L28" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="M28" s="138" t="s">
-        <v>593</v>
-      </c>
-      <c r="N28" s="11"/>
+        <v>434</v>
+      </c>
+      <c r="M28" s="11"/>
+      <c r="N28" s="175" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="29" spans="2:14" ht="31" customHeight="1">
-      <c r="B29" s="376"/>
+      <c r="B29" s="428"/>
       <c r="C29" s="365"/>
-      <c r="D29" s="391"/>
-      <c r="E29" s="365" t="s">
-        <v>500</v>
-      </c>
-      <c r="F29" s="398" t="s">
-        <v>444</v>
-      </c>
-      <c r="G29" s="365" t="s">
-        <v>263</v>
-      </c>
-      <c r="H29" s="384" t="s">
-        <v>136</v>
-      </c>
-      <c r="I29" s="364"/>
-      <c r="J29" s="364"/>
+      <c r="D29" s="394"/>
+      <c r="E29" s="365"/>
+      <c r="F29" s="401"/>
+      <c r="G29" s="365"/>
+      <c r="H29" s="385" t="s">
+        <v>426</v>
+      </c>
+      <c r="I29" s="410" t="s">
+        <v>141</v>
+      </c>
+      <c r="J29" s="411"/>
       <c r="K29" s="6"/>
       <c r="L29" s="133" t="s">
-        <v>122</v>
-      </c>
-      <c r="M29" s="116" t="s">
-        <v>411</v>
-      </c>
-      <c r="N29" s="11"/>
+        <v>141</v>
+      </c>
+      <c r="M29" s="11"/>
+      <c r="N29" s="141" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="30" spans="2:14" ht="31" customHeight="1">
-      <c r="B30" s="376"/>
+      <c r="B30" s="428"/>
       <c r="C30" s="365"/>
-      <c r="D30" s="391"/>
+      <c r="D30" s="394"/>
       <c r="E30" s="365"/>
-      <c r="F30" s="398"/>
+      <c r="F30" s="401"/>
       <c r="G30" s="365"/>
-      <c r="H30" s="384" t="s">
-        <v>137</v>
-      </c>
-      <c r="I30" s="364"/>
-      <c r="J30" s="364"/>
+      <c r="H30" s="385"/>
+      <c r="I30" s="408" t="s">
+        <v>146</v>
+      </c>
+      <c r="J30" s="409"/>
       <c r="K30" s="6"/>
       <c r="L30" s="133" t="s">
         <v>434</v>
       </c>
       <c r="M30" s="11"/>
       <c r="N30" s="175" t="s">
-        <v>150</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="2:14" ht="31" customHeight="1">
-      <c r="B31" s="376"/>
+      <c r="B31" s="428"/>
       <c r="C31" s="365"/>
-      <c r="D31" s="391"/>
+      <c r="D31" s="394"/>
       <c r="E31" s="365"/>
-      <c r="F31" s="398"/>
+      <c r="F31" s="401"/>
       <c r="G31" s="365"/>
-      <c r="H31" s="384" t="s">
-        <v>282</v>
-      </c>
-      <c r="I31" s="364"/>
-      <c r="J31" s="364"/>
+      <c r="H31" s="385"/>
+      <c r="I31" s="408" t="s">
+        <v>408</v>
+      </c>
+      <c r="J31" s="409"/>
       <c r="K31" s="6"/>
       <c r="L31" s="133" t="s">
-        <v>122</v>
+        <v>434</v>
       </c>
       <c r="M31" s="11"/>
-      <c r="N31" s="116" t="b">
-        <v>0</v>
+      <c r="N31" s="175" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="2:14" ht="31" customHeight="1">
-      <c r="B32" s="376"/>
+      <c r="B32" s="428"/>
       <c r="C32" s="365"/>
-      <c r="D32" s="391"/>
+      <c r="D32" s="394"/>
       <c r="E32" s="365"/>
-      <c r="F32" s="398"/>
+      <c r="F32" s="401"/>
       <c r="G32" s="365"/>
-      <c r="H32" s="384" t="s">
-        <v>281</v>
-      </c>
-      <c r="I32" s="364"/>
-      <c r="J32" s="364"/>
+      <c r="H32" s="385"/>
+      <c r="I32" s="408" t="s">
+        <v>409</v>
+      </c>
+      <c r="J32" s="409"/>
       <c r="K32" s="6"/>
       <c r="L32" s="133" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="M32" s="11"/>
-      <c r="N32" s="116" t="b">
-        <v>0</v>
+      <c r="N32" s="68">
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="2:14" ht="31" customHeight="1">
-      <c r="B33" s="376"/>
+      <c r="B33" s="428"/>
       <c r="C33" s="365"/>
-      <c r="D33" s="391"/>
+      <c r="D33" s="394"/>
       <c r="E33" s="365"/>
-      <c r="F33" s="398"/>
+      <c r="F33" s="401"/>
       <c r="G33" s="365"/>
-      <c r="H33" s="385" t="s">
-        <v>426</v>
-      </c>
-      <c r="I33" s="385" t="s">
-        <v>141</v>
-      </c>
-      <c r="J33" s="385"/>
+      <c r="H33" s="385"/>
+      <c r="I33" s="408" t="s">
+        <v>410</v>
+      </c>
+      <c r="J33" s="409"/>
       <c r="K33" s="6"/>
       <c r="L33" s="133" t="s">
-        <v>141</v>
+        <v>90</v>
       </c>
       <c r="M33" s="11"/>
-      <c r="N33" s="141" t="s">
-        <v>159</v>
+      <c r="N33" s="68">
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="2:14" ht="31" customHeight="1">
-      <c r="B34" s="376"/>
+      <c r="B34" s="428"/>
       <c r="C34" s="365"/>
-      <c r="D34" s="391"/>
-      <c r="E34" s="365"/>
-      <c r="F34" s="398"/>
-      <c r="G34" s="365"/>
-      <c r="H34" s="385"/>
-      <c r="I34" s="385" t="s">
-        <v>146</v>
-      </c>
-      <c r="J34" s="385"/>
+      <c r="D34" s="394" t="s">
+        <v>430</v>
+      </c>
+      <c r="E34" s="385" t="s">
+        <v>379</v>
+      </c>
+      <c r="F34" s="385"/>
+      <c r="G34" s="386"/>
+      <c r="H34" s="386"/>
+      <c r="I34" s="386"/>
+      <c r="J34" s="386"/>
       <c r="K34" s="6"/>
       <c r="L34" s="133" t="s">
-        <v>434</v>
-      </c>
-      <c r="M34" s="11"/>
-      <c r="N34" s="175" t="s">
-        <v>160</v>
+        <v>91</v>
+      </c>
+      <c r="M34" s="177"/>
+      <c r="N34" s="138" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="35" spans="2:14" ht="31" customHeight="1">
-      <c r="B35" s="376"/>
+      <c r="B35" s="428"/>
       <c r="C35" s="365"/>
-      <c r="D35" s="391"/>
-      <c r="E35" s="365"/>
-      <c r="F35" s="398"/>
-      <c r="G35" s="365"/>
-      <c r="H35" s="385"/>
-      <c r="I35" s="385" t="s">
-        <v>400</v>
-      </c>
-      <c r="J35" s="385"/>
+      <c r="D35" s="394"/>
+      <c r="E35" s="385" t="s">
+        <v>279</v>
+      </c>
+      <c r="F35" s="385"/>
+      <c r="G35" s="386"/>
+      <c r="H35" s="386"/>
+      <c r="I35" s="386"/>
+      <c r="J35" s="386"/>
       <c r="K35" s="6"/>
       <c r="L35" s="133" t="s">
         <v>90</v>
       </c>
-      <c r="M35" s="11"/>
-      <c r="N35" s="116">
-        <v>26</v>
-      </c>
+      <c r="M35" s="116">
+        <v>500</v>
+      </c>
+      <c r="N35" s="11"/>
     </row>
     <row r="36" spans="2:14" ht="31" customHeight="1">
-      <c r="B36" s="376"/>
+      <c r="B36" s="428"/>
       <c r="C36" s="365"/>
-      <c r="D36" s="391"/>
-      <c r="E36" s="365"/>
-      <c r="F36" s="398"/>
-      <c r="G36" s="365"/>
-      <c r="H36" s="385"/>
-      <c r="I36" s="385" t="s">
-        <v>401</v>
-      </c>
-      <c r="J36" s="385"/>
+      <c r="D36" s="394"/>
+      <c r="E36" s="385" t="s">
+        <v>507</v>
+      </c>
+      <c r="F36" s="385"/>
+      <c r="G36" s="386"/>
+      <c r="H36" s="386"/>
+      <c r="I36" s="386"/>
+      <c r="J36" s="386"/>
       <c r="K36" s="6"/>
       <c r="L36" s="133" t="s">
         <v>90</v>
       </c>
-      <c r="M36" s="11"/>
-      <c r="N36" s="116">
-        <v>12</v>
-      </c>
+      <c r="M36" s="116">
+        <v>500</v>
+      </c>
+      <c r="N36" s="11"/>
     </row>
     <row r="37" spans="2:14" ht="31" customHeight="1">
-      <c r="B37" s="376"/>
+      <c r="B37" s="428"/>
       <c r="C37" s="365"/>
-      <c r="D37" s="391"/>
-      <c r="E37" s="365"/>
-      <c r="F37" s="398"/>
-      <c r="G37" s="365"/>
-      <c r="H37" s="385" t="s">
-        <v>140</v>
-      </c>
-      <c r="I37" s="385" t="s">
-        <v>141</v>
-      </c>
-      <c r="J37" s="385"/>
+      <c r="D37" s="394"/>
+      <c r="E37" s="385" t="s">
+        <v>399</v>
+      </c>
+      <c r="F37" s="385"/>
+      <c r="G37" s="386"/>
+      <c r="H37" s="386"/>
+      <c r="I37" s="386"/>
+      <c r="J37" s="386"/>
       <c r="K37" s="6"/>
       <c r="L37" s="133" t="s">
-        <v>141</v>
-      </c>
-      <c r="M37" s="11"/>
-      <c r="N37" s="141" t="s">
-        <v>158</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="M37" s="138" t="s">
+        <v>593</v>
+      </c>
+      <c r="N37" s="11"/>
     </row>
     <row r="38" spans="2:14" ht="31" customHeight="1">
-      <c r="B38" s="376"/>
+      <c r="B38" s="428"/>
       <c r="C38" s="365"/>
-      <c r="D38" s="391"/>
-      <c r="E38" s="365"/>
-      <c r="F38" s="398"/>
-      <c r="G38" s="365"/>
-      <c r="H38" s="385"/>
-      <c r="I38" s="385" t="s">
-        <v>142</v>
-      </c>
-      <c r="J38" s="385"/>
+      <c r="D38" s="394"/>
+      <c r="E38" s="365" t="s">
+        <v>500</v>
+      </c>
+      <c r="F38" s="401" t="s">
+        <v>444</v>
+      </c>
+      <c r="G38" s="365" t="s">
+        <v>263</v>
+      </c>
+      <c r="H38" s="387" t="s">
+        <v>136</v>
+      </c>
+      <c r="I38" s="364"/>
+      <c r="J38" s="364"/>
       <c r="K38" s="6"/>
       <c r="L38" s="133" t="s">
-        <v>434</v>
-      </c>
-      <c r="M38" s="11"/>
-      <c r="N38" s="175" t="s">
-        <v>150</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="M38" s="116" t="s">
+        <v>411</v>
+      </c>
+      <c r="N38" s="11"/>
     </row>
     <row r="39" spans="2:14" ht="31" customHeight="1">
-      <c r="B39" s="376"/>
+      <c r="B39" s="428"/>
       <c r="C39" s="365"/>
-      <c r="D39" s="391"/>
+      <c r="D39" s="394"/>
       <c r="E39" s="365"/>
-      <c r="F39" s="398"/>
+      <c r="F39" s="401"/>
       <c r="G39" s="365"/>
-      <c r="H39" s="385"/>
-      <c r="I39" s="385" t="s">
-        <v>143</v>
-      </c>
-      <c r="J39" s="385"/>
+      <c r="H39" s="387" t="s">
+        <v>137</v>
+      </c>
+      <c r="I39" s="364"/>
+      <c r="J39" s="364"/>
       <c r="K39" s="6"/>
       <c r="L39" s="133" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="M39" s="11"/>
-      <c r="N39" s="140" t="s">
-        <v>441</v>
+      <c r="N39" s="175" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="2:14" ht="31" customHeight="1">
-      <c r="B40" s="376"/>
+      <c r="B40" s="428"/>
       <c r="C40" s="365"/>
-      <c r="D40" s="391"/>
+      <c r="D40" s="394"/>
       <c r="E40" s="365"/>
-      <c r="F40" s="398"/>
+      <c r="F40" s="401"/>
       <c r="G40" s="365"/>
-      <c r="H40" s="385"/>
-      <c r="I40" s="385" t="s">
-        <v>144</v>
-      </c>
-      <c r="J40" s="385"/>
+      <c r="H40" s="387" t="s">
+        <v>282</v>
+      </c>
+      <c r="I40" s="364"/>
+      <c r="J40" s="364"/>
       <c r="K40" s="6"/>
       <c r="L40" s="133" t="s">
-        <v>434</v>
+        <v>122</v>
       </c>
       <c r="M40" s="11"/>
-      <c r="N40" s="175" t="s">
-        <v>157</v>
+      <c r="N40" s="116" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:14" ht="31" customHeight="1">
-      <c r="B41" s="376"/>
-      <c r="C41" s="372" t="s">
-        <v>28</v>
-      </c>
-      <c r="D41" s="397" t="s">
-        <v>446</v>
-      </c>
-      <c r="E41" s="386"/>
-      <c r="F41" s="386"/>
-      <c r="G41" s="386"/>
-      <c r="H41" s="386"/>
-      <c r="I41" s="386"/>
-      <c r="J41" s="386"/>
+      <c r="B41" s="428"/>
+      <c r="C41" s="365"/>
+      <c r="D41" s="394"/>
+      <c r="E41" s="365"/>
+      <c r="F41" s="401"/>
+      <c r="G41" s="365"/>
+      <c r="H41" s="387" t="s">
+        <v>281</v>
+      </c>
+      <c r="I41" s="364"/>
+      <c r="J41" s="364"/>
       <c r="K41" s="6"/>
       <c r="L41" s="133" t="s">
-        <v>434</v>
-      </c>
-      <c r="M41" s="141" t="s">
-        <v>460</v>
-      </c>
-      <c r="N41" s="11"/>
+        <v>122</v>
+      </c>
+      <c r="M41" s="11"/>
+      <c r="N41" s="116" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="2:14" ht="31" customHeight="1">
-      <c r="B42" s="376"/>
-      <c r="C42" s="372"/>
-      <c r="D42" s="397" t="s">
-        <v>447</v>
-      </c>
-      <c r="E42" s="386"/>
-      <c r="F42" s="386"/>
-      <c r="G42" s="386"/>
-      <c r="H42" s="386"/>
-      <c r="I42" s="386"/>
-      <c r="J42" s="386"/>
+      <c r="B42" s="428"/>
+      <c r="C42" s="365"/>
+      <c r="D42" s="394"/>
+      <c r="E42" s="365"/>
+      <c r="F42" s="401"/>
+      <c r="G42" s="365"/>
+      <c r="H42" s="388" t="s">
+        <v>426</v>
+      </c>
+      <c r="I42" s="388" t="s">
+        <v>141</v>
+      </c>
+      <c r="J42" s="388"/>
       <c r="K42" s="6"/>
       <c r="L42" s="133" t="s">
-        <v>434</v>
-      </c>
-      <c r="M42" s="141" t="s">
-        <v>460</v>
-      </c>
-      <c r="N42" s="11"/>
+        <v>141</v>
+      </c>
+      <c r="M42" s="11"/>
+      <c r="N42" s="141" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="43" spans="2:14" ht="31" customHeight="1">
-      <c r="B43" s="376"/>
-      <c r="C43" s="372"/>
-      <c r="D43" s="397" t="s">
-        <v>448</v>
-      </c>
-      <c r="E43" s="386"/>
-      <c r="F43" s="386"/>
-      <c r="G43" s="386"/>
-      <c r="H43" s="386"/>
-      <c r="I43" s="386"/>
-      <c r="J43" s="386"/>
+      <c r="B43" s="428"/>
+      <c r="C43" s="365"/>
+      <c r="D43" s="394"/>
+      <c r="E43" s="365"/>
+      <c r="F43" s="401"/>
+      <c r="G43" s="365"/>
+      <c r="H43" s="388"/>
+      <c r="I43" s="388" t="s">
+        <v>146</v>
+      </c>
+      <c r="J43" s="388"/>
       <c r="K43" s="6"/>
       <c r="L43" s="133" t="s">
         <v>434</v>
       </c>
-      <c r="M43" s="141" t="s">
-        <v>460</v>
-      </c>
-      <c r="N43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="175" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="44" spans="2:14" ht="31" customHeight="1">
-      <c r="B44" s="376"/>
-      <c r="C44" s="372"/>
-      <c r="D44" s="397" t="s">
-        <v>449</v>
-      </c>
-      <c r="E44" s="386"/>
-      <c r="F44" s="386"/>
-      <c r="G44" s="386"/>
-      <c r="H44" s="386"/>
-      <c r="I44" s="386"/>
-      <c r="J44" s="386"/>
+      <c r="B44" s="428"/>
+      <c r="C44" s="365"/>
+      <c r="D44" s="394"/>
+      <c r="E44" s="365"/>
+      <c r="F44" s="401"/>
+      <c r="G44" s="365"/>
+      <c r="H44" s="388"/>
+      <c r="I44" s="388" t="s">
+        <v>400</v>
+      </c>
+      <c r="J44" s="388"/>
       <c r="K44" s="6"/>
       <c r="L44" s="133" t="s">
         <v>90</v>
       </c>
-      <c r="M44" s="116">
-        <v>0</v>
-      </c>
-      <c r="N44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="116">
+        <v>26</v>
+      </c>
     </row>
     <row r="45" spans="2:14" ht="31" customHeight="1">
-      <c r="B45" s="376"/>
-      <c r="C45" s="372"/>
-      <c r="D45" s="397" t="s">
-        <v>450</v>
-      </c>
-      <c r="E45" s="386"/>
-      <c r="F45" s="386"/>
-      <c r="G45" s="386"/>
-      <c r="H45" s="386"/>
-      <c r="I45" s="386"/>
-      <c r="J45" s="386"/>
+      <c r="B45" s="428"/>
+      <c r="C45" s="365"/>
+      <c r="D45" s="394"/>
+      <c r="E45" s="365"/>
+      <c r="F45" s="401"/>
+      <c r="G45" s="365"/>
+      <c r="H45" s="388"/>
+      <c r="I45" s="388" t="s">
+        <v>401</v>
+      </c>
+      <c r="J45" s="388"/>
       <c r="K45" s="6"/>
       <c r="L45" s="133" t="s">
         <v>90</v>
       </c>
-      <c r="M45" s="116">
-        <v>0</v>
-      </c>
-      <c r="N45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="116">
+        <v>12</v>
+      </c>
     </row>
     <row r="46" spans="2:14" ht="31" customHeight="1">
-      <c r="B46" s="376"/>
-      <c r="C46" s="372"/>
-      <c r="D46" s="397" t="s">
-        <v>451</v>
-      </c>
-      <c r="E46" s="386"/>
-      <c r="F46" s="386"/>
-      <c r="G46" s="386"/>
-      <c r="H46" s="386"/>
-      <c r="I46" s="386"/>
-      <c r="J46" s="386"/>
+      <c r="B46" s="428"/>
+      <c r="C46" s="365"/>
+      <c r="D46" s="394"/>
+      <c r="E46" s="365"/>
+      <c r="F46" s="401"/>
+      <c r="G46" s="365"/>
+      <c r="H46" s="388" t="s">
+        <v>140</v>
+      </c>
+      <c r="I46" s="388" t="s">
+        <v>141</v>
+      </c>
+      <c r="J46" s="388"/>
       <c r="K46" s="6"/>
       <c r="L46" s="133" t="s">
-        <v>90</v>
-      </c>
-      <c r="M46" s="116">
-        <v>0</v>
-      </c>
-      <c r="N46" s="11"/>
+        <v>141</v>
+      </c>
+      <c r="M46" s="11"/>
+      <c r="N46" s="141" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="47" spans="2:14" ht="31" customHeight="1">
-      <c r="B47" s="376" t="s">
-        <v>258</v>
-      </c>
-      <c r="C47" s="372" t="s">
-        <v>275</v>
-      </c>
-      <c r="D47" s="372"/>
-      <c r="E47" s="382" t="s">
-        <v>258</v>
-      </c>
-      <c r="F47" s="382"/>
-      <c r="G47" s="380"/>
-      <c r="H47" s="380"/>
-      <c r="I47" s="380"/>
-      <c r="J47" s="380"/>
+      <c r="B47" s="428"/>
+      <c r="C47" s="365"/>
+      <c r="D47" s="394"/>
+      <c r="E47" s="365"/>
+      <c r="F47" s="401"/>
+      <c r="G47" s="365"/>
+      <c r="H47" s="388"/>
+      <c r="I47" s="388" t="s">
+        <v>142</v>
+      </c>
+      <c r="J47" s="388"/>
       <c r="K47" s="6"/>
       <c r="L47" s="133" t="s">
-        <v>113</v>
+        <v>434</v>
       </c>
       <c r="M47" s="11"/>
-      <c r="N47" s="11"/>
+      <c r="N47" s="175" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="48" spans="2:14" ht="31" customHeight="1">
-      <c r="B48" s="376"/>
-      <c r="C48" s="372"/>
-      <c r="D48" s="372"/>
-      <c r="E48" s="382" t="s">
-        <v>274</v>
-      </c>
-      <c r="F48" s="382"/>
-      <c r="G48" s="380"/>
-      <c r="H48" s="380"/>
-      <c r="I48" s="380"/>
-      <c r="J48" s="380"/>
+      <c r="B48" s="428"/>
+      <c r="C48" s="365"/>
+      <c r="D48" s="394"/>
+      <c r="E48" s="365"/>
+      <c r="F48" s="401"/>
+      <c r="G48" s="365"/>
+      <c r="H48" s="388"/>
+      <c r="I48" s="388" t="s">
+        <v>143</v>
+      </c>
+      <c r="J48" s="388"/>
+      <c r="K48" s="6"/>
       <c r="L48" s="133" t="s">
-        <v>113</v>
+        <v>442</v>
       </c>
       <c r="M48" s="11"/>
-      <c r="N48" s="11"/>
+      <c r="N48" s="140" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="49" spans="2:15" ht="31" customHeight="1">
-      <c r="B49" s="376"/>
-      <c r="C49" s="372"/>
-      <c r="D49" s="372"/>
-      <c r="E49" s="382" t="s">
-        <v>277</v>
-      </c>
-      <c r="F49" s="382"/>
-      <c r="G49" s="380"/>
-      <c r="H49" s="380"/>
-      <c r="I49" s="380"/>
-      <c r="J49" s="380"/>
+      <c r="B49" s="428"/>
+      <c r="C49" s="365"/>
+      <c r="D49" s="394"/>
+      <c r="E49" s="365"/>
+      <c r="F49" s="401"/>
+      <c r="G49" s="365"/>
+      <c r="H49" s="388"/>
+      <c r="I49" s="388" t="s">
+        <v>144</v>
+      </c>
+      <c r="J49" s="388"/>
+      <c r="K49" s="6"/>
       <c r="L49" s="133" t="s">
-        <v>113</v>
+        <v>434</v>
       </c>
       <c r="M49" s="11"/>
-      <c r="N49" s="11"/>
+      <c r="N49" s="175" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="50" spans="2:15" ht="31" customHeight="1">
-      <c r="B50" s="376"/>
-      <c r="C50" s="372"/>
-      <c r="D50" s="372"/>
-      <c r="E50" s="382" t="s">
-        <v>261</v>
-      </c>
-      <c r="F50" s="382"/>
-      <c r="G50" s="380"/>
-      <c r="H50" s="380"/>
-      <c r="I50" s="380"/>
-      <c r="J50" s="380"/>
+      <c r="B50" s="428"/>
+      <c r="C50" s="373" t="s">
+        <v>28</v>
+      </c>
+      <c r="D50" s="400" t="s">
+        <v>446</v>
+      </c>
+      <c r="E50" s="389"/>
+      <c r="F50" s="389"/>
+      <c r="G50" s="389"/>
+      <c r="H50" s="389"/>
+      <c r="I50" s="389"/>
+      <c r="J50" s="389"/>
+      <c r="K50" s="6"/>
       <c r="L50" s="133" t="s">
-        <v>113</v>
-      </c>
-      <c r="M50" s="11"/>
+        <v>434</v>
+      </c>
+      <c r="M50" s="141" t="s">
+        <v>460</v>
+      </c>
       <c r="N50" s="11"/>
     </row>
     <row r="51" spans="2:15" ht="31" customHeight="1">
-      <c r="B51" s="376"/>
-      <c r="C51" s="372"/>
-      <c r="D51" s="372"/>
-      <c r="E51" s="382" t="s">
-        <v>273</v>
-      </c>
-      <c r="F51" s="382"/>
-      <c r="G51" s="380"/>
-      <c r="H51" s="380"/>
-      <c r="I51" s="380"/>
-      <c r="J51" s="380"/>
+      <c r="B51" s="428"/>
+      <c r="C51" s="373"/>
+      <c r="D51" s="400" t="s">
+        <v>447</v>
+      </c>
+      <c r="E51" s="389"/>
+      <c r="F51" s="389"/>
+      <c r="G51" s="389"/>
+      <c r="H51" s="389"/>
+      <c r="I51" s="389"/>
+      <c r="J51" s="389"/>
+      <c r="K51" s="6"/>
       <c r="L51" s="133" t="s">
-        <v>113</v>
-      </c>
-      <c r="M51" s="11"/>
+        <v>434</v>
+      </c>
+      <c r="M51" s="141" t="s">
+        <v>460</v>
+      </c>
       <c r="N51" s="11"/>
     </row>
     <row r="52" spans="2:15" ht="31" customHeight="1">
-      <c r="B52" s="376"/>
-      <c r="C52" s="372" t="s">
-        <v>276</v>
-      </c>
-      <c r="D52" s="372"/>
-      <c r="E52" s="382" t="s">
+      <c r="B52" s="428"/>
+      <c r="C52" s="373"/>
+      <c r="D52" s="400" t="s">
+        <v>448</v>
+      </c>
+      <c r="E52" s="389"/>
+      <c r="F52" s="389"/>
+      <c r="G52" s="389"/>
+      <c r="H52" s="389"/>
+      <c r="I52" s="389"/>
+      <c r="J52" s="389"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="133" t="s">
+        <v>434</v>
+      </c>
+      <c r="M52" s="141" t="s">
+        <v>460</v>
+      </c>
+      <c r="N52" s="11"/>
+    </row>
+    <row r="53" spans="2:15" ht="31" customHeight="1">
+      <c r="B53" s="428"/>
+      <c r="C53" s="373"/>
+      <c r="D53" s="400" t="s">
+        <v>449</v>
+      </c>
+      <c r="E53" s="389"/>
+      <c r="F53" s="389"/>
+      <c r="G53" s="389"/>
+      <c r="H53" s="389"/>
+      <c r="I53" s="389"/>
+      <c r="J53" s="389"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="133" t="s">
+        <v>90</v>
+      </c>
+      <c r="M53" s="116">
+        <v>0</v>
+      </c>
+      <c r="N53" s="11"/>
+    </row>
+    <row r="54" spans="2:15" ht="31" customHeight="1">
+      <c r="B54" s="428"/>
+      <c r="C54" s="373"/>
+      <c r="D54" s="400" t="s">
+        <v>450</v>
+      </c>
+      <c r="E54" s="389"/>
+      <c r="F54" s="389"/>
+      <c r="G54" s="389"/>
+      <c r="H54" s="389"/>
+      <c r="I54" s="389"/>
+      <c r="J54" s="389"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="133" t="s">
+        <v>90</v>
+      </c>
+      <c r="M54" s="116">
+        <v>0</v>
+      </c>
+      <c r="N54" s="11"/>
+    </row>
+    <row r="55" spans="2:15" ht="31" customHeight="1">
+      <c r="B55" s="428"/>
+      <c r="C55" s="373"/>
+      <c r="D55" s="400" t="s">
+        <v>451</v>
+      </c>
+      <c r="E55" s="389"/>
+      <c r="F55" s="389"/>
+      <c r="G55" s="389"/>
+      <c r="H55" s="389"/>
+      <c r="I55" s="389"/>
+      <c r="J55" s="389"/>
+      <c r="K55" s="6"/>
+      <c r="L55" s="133" t="s">
+        <v>90</v>
+      </c>
+      <c r="M55" s="116">
+        <v>0</v>
+      </c>
+      <c r="N55" s="11"/>
+    </row>
+    <row r="56" spans="2:15" ht="31" customHeight="1">
+      <c r="B56" s="379" t="s">
         <v>508</v>
       </c>
-      <c r="F52" s="382"/>
-      <c r="G52" s="380"/>
-      <c r="H52" s="380"/>
-      <c r="I52" s="380"/>
-      <c r="J52" s="380"/>
-      <c r="L52" s="133" t="s">
-        <v>97</v>
-      </c>
-      <c r="M52" s="11"/>
-      <c r="N52" s="11"/>
-    </row>
-    <row r="53" spans="2:15" ht="31" customHeight="1">
-      <c r="B53" s="376"/>
-      <c r="C53" s="372"/>
-      <c r="D53" s="372"/>
-      <c r="E53" s="382" t="s">
-        <v>272</v>
-      </c>
-      <c r="F53" s="382"/>
-      <c r="G53" s="380"/>
-      <c r="H53" s="380"/>
-      <c r="I53" s="380"/>
-      <c r="J53" s="380"/>
-      <c r="L53" s="133" t="s">
-        <v>97</v>
-      </c>
-      <c r="M53" s="175" t="s">
-        <v>114</v>
-      </c>
-      <c r="N53" s="11"/>
-    </row>
-    <row r="54" spans="2:15" ht="31" customHeight="1">
-      <c r="B54" s="376"/>
-      <c r="C54" s="372"/>
-      <c r="D54" s="372"/>
-      <c r="E54" s="382" t="s">
-        <v>44</v>
-      </c>
-      <c r="F54" s="382"/>
-      <c r="G54" s="380"/>
-      <c r="H54" s="380"/>
-      <c r="I54" s="380"/>
-      <c r="J54" s="380"/>
-      <c r="L54" s="133" t="s">
-        <v>97</v>
-      </c>
-      <c r="M54" s="11"/>
-      <c r="N54" s="11"/>
-    </row>
-    <row r="55" spans="2:15" ht="31" customHeight="1">
-      <c r="B55" s="376"/>
-      <c r="C55" s="372"/>
-      <c r="D55" s="372"/>
-      <c r="E55" s="382" t="s">
-        <v>273</v>
-      </c>
-      <c r="F55" s="382"/>
-      <c r="G55" s="380"/>
-      <c r="H55" s="380"/>
-      <c r="I55" s="380"/>
-      <c r="J55" s="380"/>
-      <c r="L55" s="133" t="s">
-        <v>97</v>
-      </c>
-      <c r="M55" s="11"/>
-      <c r="N55" s="11"/>
-    </row>
-    <row r="56" spans="2:15" ht="31" customHeight="1">
-      <c r="B56" s="376" t="s">
-        <v>508</v>
-      </c>
-      <c r="C56" s="372" t="s">
+      <c r="C56" s="373" t="s">
         <v>513</v>
       </c>
-      <c r="D56" s="372"/>
-      <c r="E56" s="380"/>
-      <c r="F56" s="380"/>
-      <c r="G56" s="380"/>
-      <c r="H56" s="380"/>
-      <c r="I56" s="380"/>
-      <c r="J56" s="380"/>
+      <c r="D56" s="373"/>
+      <c r="E56" s="383"/>
+      <c r="F56" s="383"/>
+      <c r="G56" s="383"/>
+      <c r="H56" s="383"/>
+      <c r="I56" s="383"/>
+      <c r="J56" s="383"/>
       <c r="L56" s="133" t="s">
         <v>453</v>
       </c>
@@ -7576,17 +7629,17 @@
       </c>
     </row>
     <row r="57" spans="2:15" ht="31" customHeight="1">
-      <c r="B57" s="376"/>
-      <c r="C57" s="372" t="s">
+      <c r="B57" s="379"/>
+      <c r="C57" s="373" t="s">
         <v>510</v>
       </c>
-      <c r="D57" s="372"/>
-      <c r="E57" s="380"/>
-      <c r="F57" s="380"/>
-      <c r="G57" s="380"/>
-      <c r="H57" s="380"/>
-      <c r="I57" s="380"/>
-      <c r="J57" s="380"/>
+      <c r="D57" s="373"/>
+      <c r="E57" s="383"/>
+      <c r="F57" s="383"/>
+      <c r="G57" s="383"/>
+      <c r="H57" s="383"/>
+      <c r="I57" s="383"/>
+      <c r="J57" s="383"/>
       <c r="L57" s="133" t="s">
         <v>91</v>
       </c>
@@ -7596,17 +7649,17 @@
       </c>
     </row>
     <row r="58" spans="2:15" ht="31" customHeight="1">
-      <c r="B58" s="376"/>
-      <c r="C58" s="372" t="s">
+      <c r="B58" s="379"/>
+      <c r="C58" s="373" t="s">
         <v>512</v>
       </c>
-      <c r="D58" s="372"/>
-      <c r="E58" s="380"/>
-      <c r="F58" s="380"/>
-      <c r="G58" s="380"/>
-      <c r="H58" s="380"/>
-      <c r="I58" s="380"/>
-      <c r="J58" s="380"/>
+      <c r="D58" s="373"/>
+      <c r="E58" s="383"/>
+      <c r="F58" s="383"/>
+      <c r="G58" s="383"/>
+      <c r="H58" s="383"/>
+      <c r="I58" s="383"/>
+      <c r="J58" s="383"/>
       <c r="L58" s="133" t="s">
         <v>97</v>
       </c>
@@ -7616,15 +7669,15 @@
       <c r="N58" s="11"/>
     </row>
     <row r="59" spans="2:15" ht="31" customHeight="1">
-      <c r="B59" s="376"/>
-      <c r="C59" s="387"/>
-      <c r="D59" s="387"/>
-      <c r="E59" s="387"/>
-      <c r="F59" s="387"/>
-      <c r="G59" s="387"/>
-      <c r="H59" s="387"/>
-      <c r="I59" s="387"/>
-      <c r="J59" s="387"/>
+      <c r="B59" s="379"/>
+      <c r="C59" s="390"/>
+      <c r="D59" s="390"/>
+      <c r="E59" s="390"/>
+      <c r="F59" s="390"/>
+      <c r="G59" s="390"/>
+      <c r="H59" s="390"/>
+      <c r="I59" s="390"/>
+      <c r="J59" s="390"/>
       <c r="K59" s="361"/>
       <c r="L59" s="366"/>
       <c r="M59" s="366"/>
@@ -7632,15 +7685,15 @@
       <c r="O59" s="361"/>
     </row>
     <row r="60" spans="2:15" ht="31" customHeight="1">
-      <c r="B60" s="376"/>
-      <c r="C60" s="387"/>
-      <c r="D60" s="387"/>
-      <c r="E60" s="387"/>
-      <c r="F60" s="387"/>
-      <c r="G60" s="387"/>
-      <c r="H60" s="387"/>
-      <c r="I60" s="387"/>
-      <c r="J60" s="387"/>
+      <c r="B60" s="379"/>
+      <c r="C60" s="390"/>
+      <c r="D60" s="390"/>
+      <c r="E60" s="390"/>
+      <c r="F60" s="390"/>
+      <c r="G60" s="390"/>
+      <c r="H60" s="390"/>
+      <c r="I60" s="390"/>
+      <c r="J60" s="390"/>
       <c r="K60" s="361"/>
       <c r="L60" s="366"/>
       <c r="M60" s="366"/>
@@ -7648,23 +7701,23 @@
       <c r="O60" s="361"/>
     </row>
     <row r="61" spans="2:15" ht="31" customHeight="1">
-      <c r="B61" s="376" t="s">
+      <c r="B61" s="379" t="s">
         <v>310</v>
       </c>
-      <c r="C61" s="391" t="s">
+      <c r="C61" s="370" t="s">
         <v>290</v>
       </c>
-      <c r="D61" s="391"/>
-      <c r="E61" s="395" t="s">
+      <c r="D61" s="370"/>
+      <c r="E61" s="398" t="s">
         <v>269</v>
       </c>
-      <c r="F61" s="396" t="s">
+      <c r="F61" s="399" t="s">
         <v>455</v>
       </c>
-      <c r="G61" s="380"/>
-      <c r="H61" s="380"/>
-      <c r="I61" s="380"/>
-      <c r="J61" s="380"/>
+      <c r="G61" s="383"/>
+      <c r="H61" s="383"/>
+      <c r="I61" s="383"/>
+      <c r="J61" s="383"/>
       <c r="L61" s="133" t="s">
         <v>453</v>
       </c>
@@ -7676,21 +7729,21 @@
       </c>
     </row>
     <row r="62" spans="2:15" ht="31" customHeight="1">
-      <c r="B62" s="376"/>
-      <c r="C62" s="391" t="s">
+      <c r="B62" s="379"/>
+      <c r="C62" s="370" t="s">
         <v>387</v>
       </c>
-      <c r="D62" s="391"/>
-      <c r="E62" s="395" t="s">
+      <c r="D62" s="370"/>
+      <c r="E62" s="398" t="s">
         <v>269</v>
       </c>
-      <c r="F62" s="396" t="s">
+      <c r="F62" s="399" t="s">
         <v>456</v>
       </c>
-      <c r="G62" s="380"/>
-      <c r="H62" s="380"/>
-      <c r="I62" s="380"/>
-      <c r="J62" s="380"/>
+      <c r="G62" s="383"/>
+      <c r="H62" s="383"/>
+      <c r="I62" s="383"/>
+      <c r="J62" s="383"/>
       <c r="L62" s="133" t="s">
         <v>453</v>
       </c>
@@ -7700,23 +7753,26 @@
       <c r="N62" s="116" t="s">
         <v>454</v>
       </c>
+      <c r="O62" s="9" t="s">
+        <v>610</v>
+      </c>
     </row>
     <row r="63" spans="2:15" ht="31" customHeight="1">
-      <c r="B63" s="376"/>
-      <c r="C63" s="399" t="s">
+      <c r="B63" s="379"/>
+      <c r="C63" s="422" t="s">
         <v>261</v>
       </c>
-      <c r="D63" s="400"/>
-      <c r="E63" s="405" t="s">
+      <c r="D63" s="423"/>
+      <c r="E63" s="402" t="s">
         <v>269</v>
       </c>
-      <c r="F63" s="408" t="s">
+      <c r="F63" s="405" t="s">
         <v>455</v>
       </c>
-      <c r="G63" s="382" t="s">
+      <c r="G63" s="385" t="s">
         <v>403</v>
       </c>
-      <c r="H63" s="382"/>
+      <c r="H63" s="385"/>
       <c r="I63" s="364"/>
       <c r="J63" s="364"/>
       <c r="L63" s="133" t="s">
@@ -7728,15 +7784,15 @@
       <c r="N63" s="11"/>
     </row>
     <row r="64" spans="2:15" ht="31" customHeight="1">
-      <c r="B64" s="376"/>
-      <c r="C64" s="401"/>
-      <c r="D64" s="402"/>
-      <c r="E64" s="406"/>
-      <c r="F64" s="409"/>
-      <c r="G64" s="415" t="s">
+      <c r="B64" s="379"/>
+      <c r="C64" s="424"/>
+      <c r="D64" s="425"/>
+      <c r="E64" s="403"/>
+      <c r="F64" s="406"/>
+      <c r="G64" s="412" t="s">
         <v>601</v>
       </c>
-      <c r="H64" s="416"/>
+      <c r="H64" s="413"/>
       <c r="I64" s="364"/>
       <c r="J64" s="364"/>
       <c r="L64" s="133" t="s">
@@ -7750,13 +7806,13 @@
       </c>
     </row>
     <row r="65" spans="2:15" ht="31" customHeight="1">
-      <c r="B65" s="376"/>
-      <c r="C65" s="401"/>
-      <c r="D65" s="402"/>
-      <c r="E65" s="406"/>
-      <c r="F65" s="409"/>
-      <c r="G65" s="423"/>
-      <c r="H65" s="424"/>
+      <c r="B65" s="379"/>
+      <c r="C65" s="424"/>
+      <c r="D65" s="425"/>
+      <c r="E65" s="403"/>
+      <c r="F65" s="406"/>
+      <c r="G65" s="420"/>
+      <c r="H65" s="421"/>
       <c r="I65" s="364"/>
       <c r="J65" s="364"/>
       <c r="L65" s="133" t="s">
@@ -7770,13 +7826,13 @@
       </c>
     </row>
     <row r="66" spans="2:15" ht="31" customHeight="1">
-      <c r="B66" s="376"/>
-      <c r="C66" s="401"/>
-      <c r="D66" s="402"/>
-      <c r="E66" s="406"/>
-      <c r="F66" s="409"/>
-      <c r="G66" s="417"/>
-      <c r="H66" s="418"/>
+      <c r="B66" s="379"/>
+      <c r="C66" s="424"/>
+      <c r="D66" s="425"/>
+      <c r="E66" s="403"/>
+      <c r="F66" s="406"/>
+      <c r="G66" s="414"/>
+      <c r="H66" s="415"/>
       <c r="I66" s="364"/>
       <c r="J66" s="364"/>
       <c r="L66" s="133" t="s">
@@ -7790,15 +7846,15 @@
       </c>
     </row>
     <row r="67" spans="2:15" ht="31" customHeight="1">
-      <c r="B67" s="376"/>
-      <c r="C67" s="401"/>
-      <c r="D67" s="402"/>
-      <c r="E67" s="406"/>
-      <c r="F67" s="409"/>
-      <c r="G67" s="413" t="s">
+      <c r="B67" s="379"/>
+      <c r="C67" s="424"/>
+      <c r="D67" s="425"/>
+      <c r="E67" s="403"/>
+      <c r="F67" s="406"/>
+      <c r="G67" s="410" t="s">
         <v>505</v>
       </c>
-      <c r="H67" s="414"/>
+      <c r="H67" s="411"/>
       <c r="I67" s="364"/>
       <c r="J67" s="364"/>
       <c r="L67" s="133" t="s">
@@ -7813,19 +7869,19 @@
       </c>
     </row>
     <row r="68" spans="2:15" ht="31" customHeight="1">
-      <c r="B68" s="376"/>
-      <c r="C68" s="401"/>
-      <c r="D68" s="402"/>
-      <c r="E68" s="406"/>
-      <c r="F68" s="409"/>
-      <c r="G68" s="415" t="s">
+      <c r="B68" s="379"/>
+      <c r="C68" s="424"/>
+      <c r="D68" s="425"/>
+      <c r="E68" s="403"/>
+      <c r="F68" s="406"/>
+      <c r="G68" s="412" t="s">
         <v>501</v>
       </c>
-      <c r="H68" s="416"/>
+      <c r="H68" s="413"/>
       <c r="I68" s="368" t="s">
         <v>484</v>
       </c>
-      <c r="J68" s="388" t="s">
+      <c r="J68" s="391" t="s">
         <v>477</v>
       </c>
       <c r="L68" s="133" t="s">
@@ -7840,15 +7896,15 @@
       </c>
     </row>
     <row r="69" spans="2:15" ht="31" customHeight="1">
-      <c r="B69" s="376"/>
-      <c r="C69" s="401"/>
-      <c r="D69" s="402"/>
-      <c r="E69" s="407"/>
-      <c r="F69" s="410"/>
-      <c r="G69" s="417"/>
-      <c r="H69" s="418"/>
+      <c r="B69" s="379"/>
+      <c r="C69" s="424"/>
+      <c r="D69" s="425"/>
+      <c r="E69" s="404"/>
+      <c r="F69" s="407"/>
+      <c r="G69" s="414"/>
+      <c r="H69" s="415"/>
       <c r="I69" s="369"/>
-      <c r="J69" s="388" t="s">
+      <c r="J69" s="391" t="s">
         <v>482</v>
       </c>
       <c r="L69" s="133" t="s">
@@ -7860,19 +7916,19 @@
       <c r="N69" s="11"/>
     </row>
     <row r="70" spans="2:15" ht="31" customHeight="1">
-      <c r="B70" s="376"/>
-      <c r="C70" s="401"/>
-      <c r="D70" s="402"/>
-      <c r="E70" s="405" t="s">
+      <c r="B70" s="379"/>
+      <c r="C70" s="424"/>
+      <c r="D70" s="425"/>
+      <c r="E70" s="402" t="s">
         <v>269</v>
       </c>
-      <c r="F70" s="408" t="s">
+      <c r="F70" s="405" t="s">
         <v>598</v>
       </c>
-      <c r="G70" s="382" t="s">
+      <c r="G70" s="385" t="s">
         <v>591</v>
       </c>
-      <c r="H70" s="382"/>
+      <c r="H70" s="385"/>
       <c r="I70" s="364"/>
       <c r="J70" s="364"/>
       <c r="L70" s="133" t="s">
@@ -7884,15 +7940,15 @@
       <c r="N70" s="11"/>
     </row>
     <row r="71" spans="2:15" ht="31" customHeight="1">
-      <c r="B71" s="376"/>
-      <c r="C71" s="401"/>
-      <c r="D71" s="402"/>
-      <c r="E71" s="406"/>
-      <c r="F71" s="409"/>
-      <c r="G71" s="413" t="s">
+      <c r="B71" s="379"/>
+      <c r="C71" s="424"/>
+      <c r="D71" s="425"/>
+      <c r="E71" s="403"/>
+      <c r="F71" s="406"/>
+      <c r="G71" s="410" t="s">
         <v>505</v>
       </c>
-      <c r="H71" s="414"/>
+      <c r="H71" s="411"/>
       <c r="I71" s="364"/>
       <c r="J71" s="364"/>
       <c r="L71" s="133" t="s">
@@ -7904,19 +7960,19 @@
       <c r="N71" s="11"/>
     </row>
     <row r="72" spans="2:15" ht="31" customHeight="1">
-      <c r="B72" s="376"/>
-      <c r="C72" s="401"/>
-      <c r="D72" s="402"/>
-      <c r="E72" s="406"/>
-      <c r="F72" s="409"/>
-      <c r="G72" s="415" t="s">
+      <c r="B72" s="379"/>
+      <c r="C72" s="424"/>
+      <c r="D72" s="425"/>
+      <c r="E72" s="403"/>
+      <c r="F72" s="406"/>
+      <c r="G72" s="412" t="s">
         <v>501</v>
       </c>
-      <c r="H72" s="416"/>
+      <c r="H72" s="413"/>
       <c r="I72" s="368" t="s">
         <v>484</v>
       </c>
-      <c r="J72" s="388" t="s">
+      <c r="J72" s="391" t="s">
         <v>477</v>
       </c>
       <c r="L72" s="133" t="s">
@@ -7928,15 +7984,15 @@
       <c r="N72" s="11"/>
     </row>
     <row r="73" spans="2:15" ht="31" customHeight="1">
-      <c r="B73" s="376"/>
-      <c r="C73" s="403"/>
-      <c r="D73" s="404"/>
-      <c r="E73" s="407"/>
-      <c r="F73" s="410"/>
-      <c r="G73" s="417"/>
-      <c r="H73" s="418"/>
+      <c r="B73" s="379"/>
+      <c r="C73" s="426"/>
+      <c r="D73" s="427"/>
+      <c r="E73" s="404"/>
+      <c r="F73" s="407"/>
+      <c r="G73" s="414"/>
+      <c r="H73" s="415"/>
       <c r="I73" s="369"/>
-      <c r="J73" s="388" t="s">
+      <c r="J73" s="391" t="s">
         <v>482</v>
       </c>
       <c r="L73" s="133" t="s">
@@ -7948,17 +8004,17 @@
       <c r="N73" s="11"/>
     </row>
     <row r="74" spans="2:15" ht="31" customHeight="1">
-      <c r="B74" s="376"/>
-      <c r="C74" s="391" t="s">
+      <c r="B74" s="379"/>
+      <c r="C74" s="370" t="s">
         <v>515</v>
       </c>
-      <c r="D74" s="391"/>
-      <c r="E74" s="380"/>
-      <c r="F74" s="380"/>
-      <c r="G74" s="380"/>
-      <c r="H74" s="380"/>
-      <c r="I74" s="380"/>
-      <c r="J74" s="380"/>
+      <c r="D74" s="370"/>
+      <c r="E74" s="383"/>
+      <c r="F74" s="383"/>
+      <c r="G74" s="383"/>
+      <c r="H74" s="383"/>
+      <c r="I74" s="383"/>
+      <c r="J74" s="383"/>
       <c r="L74" s="133" t="s">
         <v>474</v>
       </c>
@@ -7966,19 +8022,19 @@
       <c r="N74" s="11"/>
     </row>
     <row r="75" spans="2:15" ht="31" customHeight="1">
-      <c r="B75" s="376"/>
-      <c r="C75" s="372" t="s">
+      <c r="B75" s="379"/>
+      <c r="C75" s="375" t="s">
         <v>259</v>
       </c>
-      <c r="D75" s="372"/>
-      <c r="E75" s="382" t="s">
+      <c r="D75" s="375"/>
+      <c r="E75" s="385" t="s">
         <v>270</v>
       </c>
-      <c r="F75" s="382"/>
-      <c r="G75" s="380"/>
-      <c r="H75" s="380"/>
-      <c r="I75" s="380"/>
-      <c r="J75" s="380"/>
+      <c r="F75" s="385"/>
+      <c r="G75" s="383"/>
+      <c r="H75" s="383"/>
+      <c r="I75" s="383"/>
+      <c r="J75" s="383"/>
       <c r="L75" s="133" t="s">
         <v>90</v>
       </c>
@@ -7988,17 +8044,17 @@
       <c r="N75" s="11"/>
     </row>
     <row r="76" spans="2:15" ht="31" customHeight="1">
-      <c r="B76" s="376"/>
-      <c r="C76" s="372"/>
-      <c r="D76" s="372"/>
-      <c r="E76" s="382" t="s">
+      <c r="B76" s="379"/>
+      <c r="C76" s="375"/>
+      <c r="D76" s="375"/>
+      <c r="E76" s="385" t="s">
         <v>268</v>
       </c>
-      <c r="F76" s="382"/>
-      <c r="G76" s="380"/>
-      <c r="H76" s="380"/>
-      <c r="I76" s="380"/>
-      <c r="J76" s="380"/>
+      <c r="F76" s="385"/>
+      <c r="G76" s="383"/>
+      <c r="H76" s="383"/>
+      <c r="I76" s="383"/>
+      <c r="J76" s="383"/>
       <c r="L76" s="133" t="s">
         <v>91</v>
       </c>
@@ -8008,17 +8064,17 @@
       <c r="N76" s="11"/>
     </row>
     <row r="77" spans="2:15" ht="31" customHeight="1">
-      <c r="B77" s="376"/>
-      <c r="C77" s="372"/>
-      <c r="D77" s="372"/>
-      <c r="E77" s="382" t="s">
+      <c r="B77" s="379"/>
+      <c r="C77" s="375"/>
+      <c r="D77" s="375"/>
+      <c r="E77" s="385" t="s">
         <v>314</v>
       </c>
-      <c r="F77" s="382"/>
+      <c r="F77" s="385"/>
       <c r="G77" s="172" t="s">
         <v>269</v>
       </c>
-      <c r="H77" s="388" t="s">
+      <c r="H77" s="391" t="s">
         <v>458</v>
       </c>
       <c r="I77" s="364"/>
@@ -8034,17 +8090,17 @@
       </c>
     </row>
     <row r="78" spans="2:15" ht="31" customHeight="1">
-      <c r="B78" s="376"/>
-      <c r="C78" s="372"/>
-      <c r="D78" s="372"/>
-      <c r="E78" s="382" t="s">
+      <c r="B78" s="379"/>
+      <c r="C78" s="375"/>
+      <c r="D78" s="375"/>
+      <c r="E78" s="385" t="s">
         <v>313</v>
       </c>
-      <c r="F78" s="382"/>
-      <c r="G78" s="380"/>
-      <c r="H78" s="380"/>
-      <c r="I78" s="380"/>
-      <c r="J78" s="380"/>
+      <c r="F78" s="385"/>
+      <c r="G78" s="383"/>
+      <c r="H78" s="383"/>
+      <c r="I78" s="383"/>
+      <c r="J78" s="383"/>
       <c r="L78" s="133" t="s">
         <v>91</v>
       </c>
@@ -8054,17 +8110,17 @@
       <c r="N78" s="11"/>
     </row>
     <row r="79" spans="2:15" ht="31" customHeight="1">
-      <c r="B79" s="376"/>
-      <c r="C79" s="372"/>
-      <c r="D79" s="372"/>
-      <c r="E79" s="382" t="s">
+      <c r="B79" s="379"/>
+      <c r="C79" s="375"/>
+      <c r="D79" s="375"/>
+      <c r="E79" s="385" t="s">
         <v>312</v>
       </c>
-      <c r="F79" s="382"/>
-      <c r="G79" s="380"/>
-      <c r="H79" s="380"/>
-      <c r="I79" s="380"/>
-      <c r="J79" s="380"/>
+      <c r="F79" s="385"/>
+      <c r="G79" s="383"/>
+      <c r="H79" s="383"/>
+      <c r="I79" s="383"/>
+      <c r="J79" s="383"/>
       <c r="L79" s="144" t="s">
         <v>457</v>
       </c>
@@ -8072,24 +8128,24 @@
         <v>473</v>
       </c>
       <c r="N79" s="11"/>
-      <c r="O79" s="371" t="s">
+      <c r="O79" s="372" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="80" spans="2:15" ht="31" customHeight="1">
-      <c r="B80" s="376" t="s">
+      <c r="B80" s="379" t="s">
         <v>257</v>
       </c>
-      <c r="C80" s="391" t="s">
+      <c r="C80" s="394" t="s">
         <v>353</v>
       </c>
-      <c r="D80" s="391"/>
-      <c r="E80" s="380"/>
-      <c r="F80" s="380"/>
-      <c r="G80" s="380"/>
-      <c r="H80" s="380"/>
-      <c r="I80" s="380"/>
-      <c r="J80" s="380"/>
+      <c r="D80" s="394"/>
+      <c r="E80" s="383"/>
+      <c r="F80" s="383"/>
+      <c r="G80" s="383"/>
+      <c r="H80" s="383"/>
+      <c r="I80" s="383"/>
+      <c r="J80" s="383"/>
       <c r="L80" s="133" t="s">
         <v>90</v>
       </c>
@@ -8099,17 +8155,17 @@
       <c r="N80" s="11"/>
     </row>
     <row r="81" spans="2:14" ht="31" customHeight="1">
-      <c r="B81" s="376"/>
-      <c r="C81" s="391" t="s">
+      <c r="B81" s="379"/>
+      <c r="C81" s="394" t="s">
         <v>354</v>
       </c>
-      <c r="D81" s="391"/>
-      <c r="E81" s="380"/>
-      <c r="F81" s="380"/>
-      <c r="G81" s="380"/>
-      <c r="H81" s="380"/>
-      <c r="I81" s="380"/>
-      <c r="J81" s="380"/>
+      <c r="D81" s="394"/>
+      <c r="E81" s="383"/>
+      <c r="F81" s="383"/>
+      <c r="G81" s="383"/>
+      <c r="H81" s="383"/>
+      <c r="I81" s="383"/>
+      <c r="J81" s="383"/>
       <c r="L81" s="133" t="s">
         <v>97</v>
       </c>
@@ -8119,17 +8175,17 @@
       <c r="N81" s="11"/>
     </row>
     <row r="82" spans="2:14" ht="31" customHeight="1">
-      <c r="B82" s="376"/>
-      <c r="C82" s="391" t="s">
+      <c r="B82" s="379"/>
+      <c r="C82" s="394" t="s">
         <v>297</v>
       </c>
-      <c r="D82" s="391"/>
-      <c r="E82" s="380"/>
-      <c r="F82" s="380"/>
-      <c r="G82" s="380"/>
-      <c r="H82" s="380"/>
-      <c r="I82" s="380"/>
-      <c r="J82" s="380"/>
+      <c r="D82" s="394"/>
+      <c r="E82" s="383"/>
+      <c r="F82" s="383"/>
+      <c r="G82" s="383"/>
+      <c r="H82" s="383"/>
+      <c r="I82" s="383"/>
+      <c r="J82" s="383"/>
       <c r="L82" s="133" t="s">
         <v>596</v>
       </c>
@@ -8139,17 +8195,17 @@
       <c r="N82" s="11"/>
     </row>
     <row r="83" spans="2:14" ht="31" customHeight="1">
-      <c r="B83" s="376"/>
-      <c r="C83" s="391" t="s">
+      <c r="B83" s="379"/>
+      <c r="C83" s="394" t="s">
         <v>391</v>
       </c>
-      <c r="D83" s="391"/>
-      <c r="E83" s="380"/>
-      <c r="F83" s="380"/>
-      <c r="G83" s="380"/>
-      <c r="H83" s="380"/>
-      <c r="I83" s="380"/>
-      <c r="J83" s="380"/>
+      <c r="D83" s="394"/>
+      <c r="E83" s="383"/>
+      <c r="F83" s="383"/>
+      <c r="G83" s="383"/>
+      <c r="H83" s="383"/>
+      <c r="I83" s="383"/>
+      <c r="J83" s="383"/>
       <c r="L83" s="133" t="s">
         <v>91</v>
       </c>
@@ -8159,15 +8215,15 @@
       <c r="N83" s="11"/>
     </row>
     <row r="84" spans="2:14" ht="31" customHeight="1">
-      <c r="B84" s="376"/>
-      <c r="C84" s="372" t="s">
+      <c r="B84" s="379"/>
+      <c r="C84" s="373" t="s">
         <v>266</v>
       </c>
-      <c r="D84" s="372"/>
-      <c r="E84" s="382" t="s">
+      <c r="D84" s="373"/>
+      <c r="E84" s="385" t="s">
         <v>356</v>
       </c>
-      <c r="F84" s="382"/>
+      <c r="F84" s="385"/>
       <c r="G84" s="173" t="s">
         <v>466</v>
       </c>
@@ -8185,13 +8241,13 @@
       <c r="N84" s="11"/>
     </row>
     <row r="85" spans="2:14" ht="31" customHeight="1">
-      <c r="B85" s="376"/>
-      <c r="C85" s="372"/>
-      <c r="D85" s="372"/>
-      <c r="E85" s="382" t="s">
+      <c r="B85" s="379"/>
+      <c r="C85" s="373"/>
+      <c r="D85" s="373"/>
+      <c r="E85" s="385" t="s">
         <v>1</v>
       </c>
-      <c r="F85" s="382"/>
+      <c r="F85" s="385"/>
       <c r="G85" s="173" t="s">
         <v>465</v>
       </c>
@@ -8209,19 +8265,19 @@
       <c r="N85" s="11"/>
     </row>
     <row r="86" spans="2:14" ht="31" customHeight="1">
-      <c r="B86" s="376"/>
-      <c r="C86" s="391" t="s">
+      <c r="B86" s="379"/>
+      <c r="C86" s="394" t="s">
         <v>479</v>
       </c>
-      <c r="D86" s="391"/>
-      <c r="E86" s="382" t="s">
+      <c r="D86" s="394"/>
+      <c r="E86" s="385" t="s">
         <v>388</v>
       </c>
-      <c r="F86" s="382"/>
-      <c r="G86" s="413" t="s">
+      <c r="F86" s="385"/>
+      <c r="G86" s="410" t="s">
         <v>301</v>
       </c>
-      <c r="H86" s="414"/>
+      <c r="H86" s="411"/>
       <c r="I86" s="88"/>
       <c r="J86" s="88"/>
       <c r="L86" s="133" t="s">
@@ -8233,15 +8289,15 @@
       <c r="N86" s="11"/>
     </row>
     <row r="87" spans="2:14" ht="31" customHeight="1">
-      <c r="B87" s="376"/>
-      <c r="C87" s="391"/>
-      <c r="D87" s="391"/>
-      <c r="E87" s="382"/>
-      <c r="F87" s="382"/>
-      <c r="G87" s="413" t="s">
+      <c r="B87" s="379"/>
+      <c r="C87" s="394"/>
+      <c r="D87" s="394"/>
+      <c r="E87" s="385"/>
+      <c r="F87" s="385"/>
+      <c r="G87" s="410" t="s">
         <v>268</v>
       </c>
-      <c r="H87" s="414"/>
+      <c r="H87" s="411"/>
       <c r="I87" s="88"/>
       <c r="J87" s="88"/>
       <c r="L87" s="133" t="s">
@@ -8253,15 +8309,15 @@
       <c r="N87" s="11"/>
     </row>
     <row r="88" spans="2:14" ht="31" customHeight="1">
-      <c r="B88" s="376"/>
-      <c r="C88" s="391"/>
-      <c r="D88" s="391"/>
-      <c r="E88" s="382"/>
-      <c r="F88" s="382"/>
-      <c r="G88" s="413" t="s">
+      <c r="B88" s="379"/>
+      <c r="C88" s="394"/>
+      <c r="D88" s="394"/>
+      <c r="E88" s="385"/>
+      <c r="F88" s="385"/>
+      <c r="G88" s="410" t="s">
         <v>261</v>
       </c>
-      <c r="H88" s="414"/>
+      <c r="H88" s="411"/>
       <c r="I88" s="88"/>
       <c r="J88" s="88"/>
       <c r="L88" s="133" t="s">
@@ -8273,15 +8329,15 @@
       <c r="N88" s="11"/>
     </row>
     <row r="89" spans="2:14" ht="31" customHeight="1">
-      <c r="B89" s="376"/>
-      <c r="C89" s="391"/>
-      <c r="D89" s="391"/>
-      <c r="E89" s="382"/>
-      <c r="F89" s="382"/>
-      <c r="G89" s="413" t="s">
+      <c r="B89" s="379"/>
+      <c r="C89" s="394"/>
+      <c r="D89" s="394"/>
+      <c r="E89" s="385"/>
+      <c r="F89" s="385"/>
+      <c r="G89" s="410" t="s">
         <v>269</v>
       </c>
-      <c r="H89" s="414"/>
+      <c r="H89" s="411"/>
       <c r="I89" s="88"/>
       <c r="J89" s="88"/>
       <c r="L89" s="133" t="s">
@@ -8293,17 +8349,17 @@
       <c r="N89" s="11"/>
     </row>
     <row r="90" spans="2:14" ht="31" customHeight="1">
-      <c r="B90" s="376"/>
-      <c r="C90" s="391"/>
-      <c r="D90" s="391"/>
-      <c r="E90" s="382" t="s">
+      <c r="B90" s="379"/>
+      <c r="C90" s="394"/>
+      <c r="D90" s="394"/>
+      <c r="E90" s="385" t="s">
         <v>516</v>
       </c>
-      <c r="F90" s="382"/>
-      <c r="G90" s="380"/>
-      <c r="H90" s="380"/>
-      <c r="I90" s="380"/>
-      <c r="J90" s="380"/>
+      <c r="F90" s="385"/>
+      <c r="G90" s="383"/>
+      <c r="H90" s="383"/>
+      <c r="I90" s="383"/>
+      <c r="J90" s="383"/>
       <c r="L90" s="133" t="s">
         <v>474</v>
       </c>
@@ -8313,17 +8369,17 @@
       <c r="N90" s="11"/>
     </row>
     <row r="91" spans="2:14" ht="31" customHeight="1">
-      <c r="B91" s="376"/>
-      <c r="C91" s="391"/>
-      <c r="D91" s="391"/>
-      <c r="E91" s="382" t="s">
+      <c r="B91" s="379"/>
+      <c r="C91" s="394"/>
+      <c r="D91" s="394"/>
+      <c r="E91" s="385" t="s">
         <v>422</v>
       </c>
-      <c r="F91" s="382"/>
-      <c r="G91" s="380"/>
-      <c r="H91" s="380"/>
-      <c r="I91" s="380"/>
-      <c r="J91" s="380"/>
+      <c r="F91" s="385"/>
+      <c r="G91" s="383"/>
+      <c r="H91" s="383"/>
+      <c r="I91" s="383"/>
+      <c r="J91" s="383"/>
       <c r="L91" s="133" t="s">
         <v>468</v>
       </c>
@@ -8335,17 +8391,17 @@
       </c>
     </row>
     <row r="92" spans="2:14" ht="31" customHeight="1">
-      <c r="B92" s="376"/>
-      <c r="C92" s="391"/>
-      <c r="D92" s="391"/>
-      <c r="E92" s="382" t="s">
+      <c r="B92" s="379"/>
+      <c r="C92" s="394"/>
+      <c r="D92" s="394"/>
+      <c r="E92" s="385" t="s">
         <v>505</v>
       </c>
-      <c r="F92" s="382"/>
-      <c r="G92" s="380"/>
-      <c r="H92" s="380"/>
-      <c r="I92" s="380"/>
-      <c r="J92" s="380"/>
+      <c r="F92" s="385"/>
+      <c r="G92" s="383"/>
+      <c r="H92" s="383"/>
+      <c r="I92" s="383"/>
+      <c r="J92" s="383"/>
       <c r="L92" s="133" t="s">
         <v>122</v>
       </c>
@@ -8357,23 +8413,23 @@
       </c>
     </row>
     <row r="93" spans="2:14" ht="31" customHeight="1">
-      <c r="B93" s="376"/>
-      <c r="C93" s="391"/>
-      <c r="D93" s="391"/>
-      <c r="E93" s="382" t="s">
+      <c r="B93" s="379"/>
+      <c r="C93" s="394"/>
+      <c r="D93" s="394"/>
+      <c r="E93" s="385" t="s">
         <v>501</v>
       </c>
-      <c r="F93" s="382"/>
-      <c r="G93" s="389" t="s">
+      <c r="F93" s="385"/>
+      <c r="G93" s="392" t="s">
         <v>269</v>
       </c>
-      <c r="H93" s="390" t="s">
+      <c r="H93" s="393" t="s">
         <v>455</v>
       </c>
       <c r="I93" s="368" t="s">
         <v>484</v>
       </c>
-      <c r="J93" s="388" t="s">
+      <c r="J93" s="391" t="s">
         <v>477</v>
       </c>
       <c r="L93" s="133" t="s">
@@ -8387,15 +8443,15 @@
       </c>
     </row>
     <row r="94" spans="2:14" ht="31" customHeight="1">
-      <c r="B94" s="376"/>
-      <c r="C94" s="391"/>
-      <c r="D94" s="391"/>
-      <c r="E94" s="382"/>
-      <c r="F94" s="382"/>
-      <c r="G94" s="389"/>
-      <c r="H94" s="390"/>
+      <c r="B94" s="379"/>
+      <c r="C94" s="394"/>
+      <c r="D94" s="394"/>
+      <c r="E94" s="385"/>
+      <c r="F94" s="385"/>
+      <c r="G94" s="392"/>
+      <c r="H94" s="393"/>
       <c r="I94" s="369"/>
-      <c r="J94" s="388" t="s">
+      <c r="J94" s="391" t="s">
         <v>482</v>
       </c>
       <c r="L94" s="133" t="s">
@@ -8409,13 +8465,13 @@
       </c>
     </row>
     <row r="95" spans="2:14" ht="31" customHeight="1">
-      <c r="B95" s="376"/>
-      <c r="C95" s="391"/>
-      <c r="D95" s="391"/>
-      <c r="E95" s="415" t="s">
+      <c r="B95" s="379"/>
+      <c r="C95" s="394"/>
+      <c r="D95" s="394"/>
+      <c r="E95" s="412" t="s">
         <v>483</v>
       </c>
-      <c r="F95" s="416"/>
+      <c r="F95" s="413"/>
       <c r="G95" s="367" t="s">
         <v>269</v>
       </c>
@@ -8433,11 +8489,11 @@
       <c r="N95" s="11"/>
     </row>
     <row r="96" spans="2:14" ht="31" customHeight="1">
-      <c r="B96" s="376"/>
-      <c r="C96" s="391"/>
-      <c r="D96" s="391"/>
-      <c r="E96" s="423"/>
-      <c r="F96" s="424"/>
+      <c r="B96" s="379"/>
+      <c r="C96" s="394"/>
+      <c r="D96" s="394"/>
+      <c r="E96" s="420"/>
+      <c r="F96" s="421"/>
       <c r="G96" s="367" t="s">
         <v>269</v>
       </c>
@@ -8455,11 +8511,11 @@
       <c r="N96" s="11"/>
     </row>
     <row r="97" spans="2:14" ht="31" customHeight="1">
-      <c r="B97" s="376"/>
-      <c r="C97" s="391"/>
-      <c r="D97" s="391"/>
-      <c r="E97" s="423"/>
-      <c r="F97" s="424"/>
+      <c r="B97" s="379"/>
+      <c r="C97" s="394"/>
+      <c r="D97" s="394"/>
+      <c r="E97" s="420"/>
+      <c r="F97" s="421"/>
       <c r="G97" s="367" t="s">
         <v>269</v>
       </c>
@@ -8477,19 +8533,19 @@
       <c r="N97" s="11"/>
     </row>
     <row r="98" spans="2:14" ht="31" customHeight="1">
-      <c r="B98" s="394" t="s">
+      <c r="B98" s="397" t="s">
         <v>467</v>
       </c>
-      <c r="C98" s="391" t="s">
+      <c r="C98" s="394" t="s">
         <v>137</v>
       </c>
-      <c r="D98" s="391"/>
-      <c r="E98" s="380"/>
-      <c r="F98" s="380"/>
-      <c r="G98" s="380"/>
-      <c r="H98" s="380"/>
-      <c r="I98" s="380"/>
-      <c r="J98" s="380"/>
+      <c r="D98" s="394"/>
+      <c r="E98" s="383"/>
+      <c r="F98" s="383"/>
+      <c r="G98" s="383"/>
+      <c r="H98" s="383"/>
+      <c r="I98" s="383"/>
+      <c r="J98" s="383"/>
       <c r="L98" s="133" t="s">
         <v>97</v>
       </c>
@@ -8499,17 +8555,17 @@
       <c r="N98" s="11"/>
     </row>
     <row r="99" spans="2:14" ht="31" customHeight="1">
-      <c r="B99" s="394"/>
-      <c r="C99" s="391" t="s">
+      <c r="B99" s="397"/>
+      <c r="C99" s="394" t="s">
         <v>283</v>
       </c>
-      <c r="D99" s="391"/>
-      <c r="E99" s="380"/>
-      <c r="F99" s="380"/>
-      <c r="G99" s="380"/>
-      <c r="H99" s="380"/>
-      <c r="I99" s="380"/>
-      <c r="J99" s="380"/>
+      <c r="D99" s="394"/>
+      <c r="E99" s="383"/>
+      <c r="F99" s="383"/>
+      <c r="G99" s="383"/>
+      <c r="H99" s="383"/>
+      <c r="I99" s="383"/>
+      <c r="J99" s="383"/>
       <c r="L99" s="133" t="s">
         <v>468</v>
       </c>
@@ -8519,19 +8575,19 @@
       <c r="N99" s="11"/>
     </row>
     <row r="100" spans="2:14" ht="31" customHeight="1">
-      <c r="B100" s="394"/>
-      <c r="C100" s="391" t="s">
+      <c r="B100" s="397"/>
+      <c r="C100" s="394" t="s">
         <v>306</v>
       </c>
-      <c r="D100" s="391"/>
-      <c r="E100" s="382" t="s">
+      <c r="D100" s="394"/>
+      <c r="E100" s="385" t="s">
         <v>470</v>
       </c>
-      <c r="F100" s="382"/>
-      <c r="G100" s="380"/>
-      <c r="H100" s="380"/>
-      <c r="I100" s="380"/>
-      <c r="J100" s="380"/>
+      <c r="F100" s="385"/>
+      <c r="G100" s="383"/>
+      <c r="H100" s="383"/>
+      <c r="I100" s="383"/>
+      <c r="J100" s="383"/>
       <c r="L100" s="133" t="s">
         <v>474</v>
       </c>
@@ -8541,17 +8597,17 @@
       <c r="N100" s="11"/>
     </row>
     <row r="101" spans="2:14" ht="31" customHeight="1">
-      <c r="B101" s="394"/>
-      <c r="C101" s="391"/>
-      <c r="D101" s="391"/>
-      <c r="E101" s="382" t="s">
+      <c r="B101" s="397"/>
+      <c r="C101" s="394"/>
+      <c r="D101" s="394"/>
+      <c r="E101" s="385" t="s">
         <v>471</v>
       </c>
-      <c r="F101" s="382"/>
-      <c r="G101" s="380"/>
-      <c r="H101" s="380"/>
-      <c r="I101" s="380"/>
-      <c r="J101" s="380"/>
+      <c r="F101" s="385"/>
+      <c r="G101" s="383"/>
+      <c r="H101" s="383"/>
+      <c r="I101" s="383"/>
+      <c r="J101" s="383"/>
       <c r="L101" s="133" t="s">
         <v>468</v>
       </c>
@@ -8561,17 +8617,17 @@
       <c r="N101" s="11"/>
     </row>
     <row r="102" spans="2:14" ht="31" customHeight="1">
-      <c r="B102" s="394"/>
-      <c r="C102" s="391" t="s">
+      <c r="B102" s="397"/>
+      <c r="C102" s="394" t="s">
         <v>28</v>
       </c>
-      <c r="D102" s="391"/>
-      <c r="E102" s="380"/>
-      <c r="F102" s="380"/>
-      <c r="G102" s="380"/>
-      <c r="H102" s="380"/>
-      <c r="I102" s="380"/>
-      <c r="J102" s="380"/>
+      <c r="D102" s="394"/>
+      <c r="E102" s="383"/>
+      <c r="F102" s="383"/>
+      <c r="G102" s="383"/>
+      <c r="H102" s="383"/>
+      <c r="I102" s="383"/>
+      <c r="J102" s="383"/>
       <c r="L102" s="133" t="s">
         <v>474</v>
       </c>
@@ -8581,17 +8637,17 @@
       <c r="N102" s="11"/>
     </row>
     <row r="103" spans="2:14" ht="31" customHeight="1">
-      <c r="B103" s="394"/>
-      <c r="C103" s="391" t="s">
+      <c r="B103" s="397"/>
+      <c r="C103" s="394" t="s">
         <v>386</v>
       </c>
-      <c r="D103" s="391"/>
-      <c r="E103" s="380"/>
-      <c r="F103" s="380"/>
-      <c r="G103" s="380"/>
-      <c r="H103" s="380"/>
-      <c r="I103" s="380"/>
-      <c r="J103" s="380"/>
+      <c r="D103" s="394"/>
+      <c r="E103" s="383"/>
+      <c r="F103" s="383"/>
+      <c r="G103" s="383"/>
+      <c r="H103" s="383"/>
+      <c r="I103" s="383"/>
+      <c r="J103" s="383"/>
       <c r="L103" s="133" t="s">
         <v>122</v>
       </c>
@@ -8601,19 +8657,19 @@
       <c r="N103" s="11"/>
     </row>
     <row r="104" spans="2:14" ht="31" customHeight="1">
-      <c r="B104" s="394"/>
-      <c r="C104" s="391" t="s">
+      <c r="B104" s="397"/>
+      <c r="C104" s="394" t="s">
         <v>305</v>
       </c>
-      <c r="D104" s="391"/>
-      <c r="E104" s="382" t="s">
+      <c r="D104" s="394"/>
+      <c r="E104" s="385" t="s">
         <v>384</v>
       </c>
-      <c r="F104" s="382"/>
-      <c r="G104" s="380"/>
-      <c r="H104" s="380"/>
-      <c r="I104" s="380"/>
-      <c r="J104" s="380"/>
+      <c r="F104" s="385"/>
+      <c r="G104" s="383"/>
+      <c r="H104" s="383"/>
+      <c r="I104" s="383"/>
+      <c r="J104" s="383"/>
       <c r="L104" s="133" t="s">
         <v>122</v>
       </c>
@@ -8623,13 +8679,13 @@
       <c r="N104" s="11"/>
     </row>
     <row r="105" spans="2:14" ht="31" customHeight="1">
-      <c r="B105" s="394"/>
-      <c r="C105" s="391"/>
-      <c r="D105" s="391"/>
-      <c r="E105" s="382" t="s">
+      <c r="B105" s="397"/>
+      <c r="C105" s="394"/>
+      <c r="D105" s="394"/>
+      <c r="E105" s="385" t="s">
         <v>385</v>
       </c>
-      <c r="F105" s="382"/>
+      <c r="F105" s="385"/>
       <c r="G105" s="249">
         <v>1</v>
       </c>
@@ -8645,11 +8701,11 @@
       <c r="N105" s="11"/>
     </row>
     <row r="106" spans="2:14" ht="31" customHeight="1">
-      <c r="B106" s="394"/>
-      <c r="C106" s="391"/>
-      <c r="D106" s="391"/>
-      <c r="E106" s="382"/>
-      <c r="F106" s="382"/>
+      <c r="B106" s="397"/>
+      <c r="C106" s="394"/>
+      <c r="D106" s="394"/>
+      <c r="E106" s="385"/>
+      <c r="F106" s="385"/>
       <c r="G106" s="249">
         <v>2</v>
       </c>
@@ -8665,11 +8721,11 @@
       <c r="N106" s="11"/>
     </row>
     <row r="107" spans="2:14" ht="31" customHeight="1">
-      <c r="B107" s="394"/>
-      <c r="C107" s="391"/>
-      <c r="D107" s="391"/>
-      <c r="E107" s="382"/>
-      <c r="F107" s="382"/>
+      <c r="B107" s="397"/>
+      <c r="C107" s="394"/>
+      <c r="D107" s="394"/>
+      <c r="E107" s="385"/>
+      <c r="F107" s="385"/>
       <c r="G107" s="249">
         <v>3</v>
       </c>
@@ -8685,11 +8741,11 @@
       <c r="N107" s="11"/>
     </row>
     <row r="108" spans="2:14" ht="31" customHeight="1">
-      <c r="B108" s="394"/>
-      <c r="C108" s="391"/>
-      <c r="D108" s="391"/>
-      <c r="E108" s="382"/>
-      <c r="F108" s="382"/>
+      <c r="B108" s="397"/>
+      <c r="C108" s="394"/>
+      <c r="D108" s="394"/>
+      <c r="E108" s="385"/>
+      <c r="F108" s="385"/>
       <c r="G108" s="249">
         <v>4</v>
       </c>
@@ -8705,19 +8761,19 @@
       <c r="N108" s="11"/>
     </row>
     <row r="109" spans="2:14" ht="31" customHeight="1">
-      <c r="B109" s="394"/>
-      <c r="C109" s="391" t="s">
+      <c r="B109" s="397"/>
+      <c r="C109" s="394" t="s">
         <v>307</v>
       </c>
-      <c r="D109" s="391"/>
-      <c r="E109" s="382" t="s">
+      <c r="D109" s="394"/>
+      <c r="E109" s="385" t="s">
         <v>308</v>
       </c>
-      <c r="F109" s="382"/>
-      <c r="G109" s="380"/>
-      <c r="H109" s="380"/>
-      <c r="I109" s="380"/>
-      <c r="J109" s="380"/>
+      <c r="F109" s="385"/>
+      <c r="G109" s="383"/>
+      <c r="H109" s="383"/>
+      <c r="I109" s="383"/>
+      <c r="J109" s="383"/>
       <c r="L109" s="133" t="s">
         <v>90</v>
       </c>
@@ -8727,17 +8783,17 @@
       <c r="N109" s="11"/>
     </row>
     <row r="110" spans="2:14" ht="31" customHeight="1">
-      <c r="B110" s="394"/>
-      <c r="C110" s="391"/>
-      <c r="D110" s="391"/>
-      <c r="E110" s="382" t="s">
+      <c r="B110" s="397"/>
+      <c r="C110" s="394"/>
+      <c r="D110" s="394"/>
+      <c r="E110" s="385" t="s">
         <v>309</v>
       </c>
-      <c r="F110" s="382"/>
-      <c r="G110" s="380"/>
-      <c r="H110" s="380"/>
-      <c r="I110" s="380"/>
-      <c r="J110" s="380"/>
+      <c r="F110" s="385"/>
+      <c r="G110" s="383"/>
+      <c r="H110" s="383"/>
+      <c r="I110" s="383"/>
+      <c r="J110" s="383"/>
       <c r="L110" s="133" t="s">
         <v>475</v>
       </c>
@@ -8747,15 +8803,16 @@
       <c r="N110" s="11"/>
     </row>
     <row r="111" spans="2:14" ht="26">
-      <c r="B111" s="377"/>
-      <c r="C111" s="392"/>
+      <c r="B111" s="380"/>
+      <c r="C111" s="395"/>
     </row>
     <row r="112" spans="2:14" ht="26">
-      <c r="B112" s="377"/>
-      <c r="C112" s="392"/>
+      <c r="B112" s="380"/>
+      <c r="C112" s="395"/>
     </row>
   </sheetData>
   <mergeCells count="210">
+    <mergeCell ref="B6:B15"/>
     <mergeCell ref="I96:J96"/>
     <mergeCell ref="I97:J97"/>
     <mergeCell ref="G64:H66"/>
@@ -8765,8 +8822,8 @@
     <mergeCell ref="G86:H86"/>
     <mergeCell ref="G87:H87"/>
     <mergeCell ref="G88:H88"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I27:J27"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E70:E73"/>
     <mergeCell ref="F70:F73"/>
@@ -8775,25 +8832,25 @@
     <mergeCell ref="G71:H71"/>
     <mergeCell ref="I71:J71"/>
     <mergeCell ref="G72:H73"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I68:I69"/>
-    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="I42:J42"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I68:I69"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I39:J39"/>
     <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="I46:J46"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="I93:I94"/>
     <mergeCell ref="I105:J105"/>
@@ -8879,69 +8936,69 @@
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C61:D61"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E51:J51"/>
+    <mergeCell ref="E50:J50"/>
     <mergeCell ref="C58:D58"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="C56:D56"/>
     <mergeCell ref="E56:J56"/>
     <mergeCell ref="E57:J57"/>
     <mergeCell ref="E58:J58"/>
-    <mergeCell ref="G53:J53"/>
-    <mergeCell ref="G54:J54"/>
-    <mergeCell ref="G55:J55"/>
-    <mergeCell ref="E43:J43"/>
-    <mergeCell ref="E44:J44"/>
-    <mergeCell ref="E45:J45"/>
-    <mergeCell ref="E46:J46"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="G47:J47"/>
-    <mergeCell ref="G48:J48"/>
-    <mergeCell ref="G49:J49"/>
-    <mergeCell ref="G50:J50"/>
-    <mergeCell ref="G51:J51"/>
-    <mergeCell ref="G52:J52"/>
-    <mergeCell ref="C41:C46"/>
-    <mergeCell ref="C47:D51"/>
-    <mergeCell ref="C52:D55"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="G29:G40"/>
-    <mergeCell ref="H33:H36"/>
-    <mergeCell ref="H37:H40"/>
-    <mergeCell ref="E29:E40"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="F29:F40"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="E52:J52"/>
+    <mergeCell ref="E53:J53"/>
+    <mergeCell ref="E54:J54"/>
+    <mergeCell ref="E55:J55"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="C50:C55"/>
+    <mergeCell ref="C16:D20"/>
+    <mergeCell ref="C21:D24"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="G38:G49"/>
+    <mergeCell ref="H42:H45"/>
+    <mergeCell ref="H46:H49"/>
+    <mergeCell ref="E38:E49"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="F38:F49"/>
     <mergeCell ref="G11:J11"/>
     <mergeCell ref="G12:J12"/>
     <mergeCell ref="G13:J13"/>
     <mergeCell ref="G14:J14"/>
     <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G25:J25"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G18:G24"/>
-    <mergeCell ref="H20:H24"/>
+    <mergeCell ref="G27:G33"/>
+    <mergeCell ref="H29:H33"/>
     <mergeCell ref="E6:J6"/>
     <mergeCell ref="E7:J7"/>
     <mergeCell ref="E8:J8"/>
     <mergeCell ref="G9:J9"/>
     <mergeCell ref="G10:J10"/>
-    <mergeCell ref="D25:D40"/>
+    <mergeCell ref="D34:D49"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="E9:F9"/>
@@ -8949,23 +9006,22 @@
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E25:F25"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C9:D15"/>
-    <mergeCell ref="C16:C40"/>
-    <mergeCell ref="D16:D24"/>
+    <mergeCell ref="C25:C49"/>
+    <mergeCell ref="D25:D33"/>
     <mergeCell ref="B80:B97"/>
-    <mergeCell ref="B6:B46"/>
     <mergeCell ref="B98:B110"/>
     <mergeCell ref="B56:B60"/>
     <mergeCell ref="B61:B79"/>
-    <mergeCell ref="B47:B55"/>
-    <mergeCell ref="F18:F24"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:E24"/>
-    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="B16:B24"/>
+    <mergeCell ref="F27:F33"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:E33"/>
+    <mergeCell ref="G26:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10082,8 +10138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{657F1319-18D0-224C-96EE-875DBB0E113F}">
   <dimension ref="K25:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
more removal of the page name
</commit_message>
<xml_diff>
--- a/docs/session_variables.xlsx
+++ b/docs/session_variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robhay/git_repo/share_screener/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D4FD93-B9C1-3143-B76E-C9F9AD5AFE95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFE77E8-6B2D-8D47-A1C5-DB4EAA8C37B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14500" xr2:uid="{EB3C945B-FE01-FA47-AE59-A0DC3CDF521B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2015" uniqueCount="613">
   <si>
     <t>chart_colours</t>
   </si>
@@ -2285,7 +2285,10 @@
     <t>This will include the dataframes and the column status and the dataframe status</t>
   </si>
   <si>
-    <t>might be able to remove this one</t>
+    <t>progress</t>
+  </si>
+  <si>
+    <t>apps</t>
   </si>
 </sst>
 </file>
@@ -3010,7 +3013,7 @@
     <xf numFmtId="43" fontId="43" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="43" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="432">
+  <cellXfs count="438">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4055,6 +4058,9 @@
     <xf numFmtId="0" fontId="58" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="59" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4106,18 +4112,12 @@
     <xf numFmtId="0" fontId="58" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4199,9 +4199,6 @@
     <xf numFmtId="0" fontId="60" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="58" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4210,6 +4207,30 @@
     </xf>
     <xf numFmtId="0" fontId="58" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6405,13 +6426,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4BE9BCD-FFB7-0845-95F9-377ADF3DB526}">
-  <dimension ref="A1:T112"/>
+  <dimension ref="A1:T111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="O9" sqref="O9"/>
+      <selection pane="bottomRight" activeCell="D30" sqref="D30:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -6449,22 +6470,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="59" customHeight="1">
-      <c r="A1" s="418" t="s">
+      <c r="A1" s="417" t="s">
         <v>480</v>
       </c>
-      <c r="B1" s="419"/>
-      <c r="C1" s="419"/>
-      <c r="D1" s="419"/>
-      <c r="E1" s="419"/>
-      <c r="F1" s="419"/>
-      <c r="G1" s="419"/>
-      <c r="H1" s="419"/>
-      <c r="J1" s="416" t="s">
+      <c r="B1" s="418"/>
+      <c r="C1" s="418"/>
+      <c r="D1" s="418"/>
+      <c r="E1" s="418"/>
+      <c r="F1" s="418"/>
+      <c r="G1" s="418"/>
+      <c r="H1" s="418"/>
+      <c r="J1" s="415" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="J2" s="417" t="s">
+      <c r="J2" s="416" t="s">
         <v>503</v>
       </c>
     </row>
@@ -6501,14 +6522,14 @@
     <row r="4" spans="1:20">
       <c r="A4" s="371"/>
       <c r="B4" s="377"/>
-      <c r="C4" s="381"/>
-      <c r="D4" s="381"/>
-      <c r="E4" s="381"/>
-      <c r="F4" s="381"/>
-      <c r="G4" s="381"/>
-      <c r="H4" s="381"/>
-      <c r="I4" s="381"/>
-      <c r="J4" s="381"/>
+      <c r="C4" s="382"/>
+      <c r="D4" s="382"/>
+      <c r="E4" s="382"/>
+      <c r="F4" s="382"/>
+      <c r="G4" s="382"/>
+      <c r="H4" s="382"/>
+      <c r="I4" s="382"/>
+      <c r="J4" s="382"/>
       <c r="K4" s="6"/>
       <c r="L4" s="371"/>
       <c r="M4" s="371"/>
@@ -6521,17 +6542,17 @@
       <c r="T4" s="371"/>
     </row>
     <row r="5" spans="1:20" ht="31" customHeight="1">
-      <c r="B5" s="396" t="s">
+      <c r="B5" s="397" t="s">
         <v>289</v>
       </c>
-      <c r="C5" s="382"/>
-      <c r="D5" s="382"/>
-      <c r="E5" s="382"/>
-      <c r="F5" s="382"/>
-      <c r="G5" s="382"/>
-      <c r="H5" s="382"/>
-      <c r="I5" s="382"/>
-      <c r="J5" s="382"/>
+      <c r="C5" s="383"/>
+      <c r="D5" s="383"/>
+      <c r="E5" s="383"/>
+      <c r="F5" s="383"/>
+      <c r="G5" s="383"/>
+      <c r="H5" s="383"/>
+      <c r="I5" s="383"/>
+      <c r="J5" s="383"/>
       <c r="K5" s="6"/>
       <c r="L5" s="133" t="s">
         <v>96</v>
@@ -6542,19 +6563,19 @@
       <c r="N5" s="11"/>
     </row>
     <row r="6" spans="1:20" ht="31" customHeight="1">
-      <c r="B6" s="429" t="s">
+      <c r="B6" s="427" t="s">
         <v>263</v>
       </c>
       <c r="C6" s="370" t="s">
         <v>286</v>
       </c>
       <c r="D6" s="370"/>
-      <c r="E6" s="383"/>
-      <c r="F6" s="383"/>
-      <c r="G6" s="383"/>
-      <c r="H6" s="383"/>
-      <c r="I6" s="383"/>
-      <c r="J6" s="383"/>
+      <c r="E6" s="384"/>
+      <c r="F6" s="384"/>
+      <c r="G6" s="384"/>
+      <c r="H6" s="384"/>
+      <c r="I6" s="384"/>
+      <c r="J6" s="384"/>
       <c r="K6" s="6"/>
       <c r="L6" s="133" t="s">
         <v>434</v>
@@ -6565,17 +6586,17 @@
       <c r="N6" s="11"/>
     </row>
     <row r="7" spans="1:20" ht="31" customHeight="1">
-      <c r="B7" s="430"/>
+      <c r="B7" s="428"/>
       <c r="C7" s="370" t="s">
         <v>285</v>
       </c>
       <c r="D7" s="370"/>
-      <c r="E7" s="383"/>
-      <c r="F7" s="383"/>
-      <c r="G7" s="383"/>
-      <c r="H7" s="383"/>
-      <c r="I7" s="383"/>
-      <c r="J7" s="383"/>
+      <c r="E7" s="384"/>
+      <c r="F7" s="384"/>
+      <c r="G7" s="384"/>
+      <c r="H7" s="384"/>
+      <c r="I7" s="384"/>
+      <c r="J7" s="384"/>
       <c r="K7" s="6"/>
       <c r="L7" s="133" t="s">
         <v>98</v>
@@ -6586,17 +6607,17 @@
       <c r="N7" s="11"/>
     </row>
     <row r="8" spans="1:20" ht="31" customHeight="1">
-      <c r="B8" s="430"/>
+      <c r="B8" s="428"/>
       <c r="C8" s="370" t="s">
         <v>288</v>
       </c>
       <c r="D8" s="370"/>
-      <c r="E8" s="383"/>
-      <c r="F8" s="383"/>
-      <c r="G8" s="383"/>
-      <c r="H8" s="383"/>
-      <c r="I8" s="383"/>
-      <c r="J8" s="383"/>
+      <c r="E8" s="384"/>
+      <c r="F8" s="384"/>
+      <c r="G8" s="384"/>
+      <c r="H8" s="384"/>
+      <c r="I8" s="384"/>
+      <c r="J8" s="384"/>
       <c r="K8" s="6"/>
       <c r="L8" s="133" t="s">
         <v>434</v>
@@ -6607,43 +6628,40 @@
       <c r="N8" s="11"/>
     </row>
     <row r="9" spans="1:20" ht="31" customHeight="1">
-      <c r="B9" s="430"/>
-      <c r="C9" s="375" t="s">
+      <c r="B9" s="428"/>
+      <c r="C9" s="430" t="s">
         <v>262</v>
       </c>
-      <c r="D9" s="375"/>
-      <c r="E9" s="385" t="s">
-        <v>375</v>
-      </c>
-      <c r="F9" s="385"/>
-      <c r="G9" s="383"/>
-      <c r="H9" s="383"/>
-      <c r="I9" s="383"/>
-      <c r="J9" s="383"/>
+      <c r="D9" s="431"/>
+      <c r="E9" s="386" t="s">
+        <v>267</v>
+      </c>
+      <c r="F9" s="386"/>
+      <c r="G9" s="384"/>
+      <c r="H9" s="384"/>
+      <c r="I9" s="384"/>
+      <c r="J9" s="384"/>
       <c r="K9" s="6"/>
       <c r="L9" s="133" t="s">
-        <v>96</v>
-      </c>
-      <c r="M9" s="116" t="b">
-        <v>0</v>
+        <v>91</v>
+      </c>
+      <c r="M9" s="141" t="s">
+        <v>472</v>
       </c>
       <c r="N9" s="11"/>
-      <c r="O9" s="4" t="s">
-        <v>611</v>
-      </c>
     </row>
     <row r="10" spans="1:20" ht="31" customHeight="1">
-      <c r="B10" s="430"/>
-      <c r="C10" s="375"/>
-      <c r="D10" s="375"/>
-      <c r="E10" s="385" t="s">
-        <v>267</v>
-      </c>
-      <c r="F10" s="385"/>
-      <c r="G10" s="383"/>
-      <c r="H10" s="383"/>
-      <c r="I10" s="383"/>
-      <c r="J10" s="383"/>
+      <c r="B10" s="428"/>
+      <c r="C10" s="432"/>
+      <c r="D10" s="433"/>
+      <c r="E10" s="386" t="s">
+        <v>268</v>
+      </c>
+      <c r="F10" s="386"/>
+      <c r="G10" s="384"/>
+      <c r="H10" s="384"/>
+      <c r="I10" s="384"/>
+      <c r="J10" s="384"/>
       <c r="K10" s="6"/>
       <c r="L10" s="133" t="s">
         <v>91</v>
@@ -6654,17 +6672,17 @@
       <c r="N10" s="11"/>
     </row>
     <row r="11" spans="1:20" ht="31" customHeight="1">
-      <c r="B11" s="430"/>
-      <c r="C11" s="375"/>
-      <c r="D11" s="375"/>
-      <c r="E11" s="385" t="s">
-        <v>268</v>
-      </c>
-      <c r="F11" s="385"/>
-      <c r="G11" s="383"/>
-      <c r="H11" s="383"/>
-      <c r="I11" s="383"/>
-      <c r="J11" s="383"/>
+      <c r="B11" s="428"/>
+      <c r="C11" s="432"/>
+      <c r="D11" s="433"/>
+      <c r="E11" s="386" t="s">
+        <v>261</v>
+      </c>
+      <c r="F11" s="386"/>
+      <c r="G11" s="384"/>
+      <c r="H11" s="384"/>
+      <c r="I11" s="384"/>
+      <c r="J11" s="384"/>
       <c r="K11" s="6"/>
       <c r="L11" s="133" t="s">
         <v>91</v>
@@ -6675,17 +6693,17 @@
       <c r="N11" s="11"/>
     </row>
     <row r="12" spans="1:20" ht="31" customHeight="1">
-      <c r="B12" s="430"/>
-      <c r="C12" s="375"/>
-      <c r="D12" s="375"/>
-      <c r="E12" s="385" t="s">
-        <v>261</v>
-      </c>
-      <c r="F12" s="385"/>
-      <c r="G12" s="383"/>
-      <c r="H12" s="383"/>
-      <c r="I12" s="383"/>
-      <c r="J12" s="383"/>
+      <c r="B12" s="428"/>
+      <c r="C12" s="432"/>
+      <c r="D12" s="433"/>
+      <c r="E12" s="386" t="s">
+        <v>269</v>
+      </c>
+      <c r="F12" s="386"/>
+      <c r="G12" s="384"/>
+      <c r="H12" s="384"/>
+      <c r="I12" s="384"/>
+      <c r="J12" s="384"/>
       <c r="K12" s="6"/>
       <c r="L12" s="133" t="s">
         <v>91</v>
@@ -6696,38 +6714,38 @@
       <c r="N12" s="11"/>
     </row>
     <row r="13" spans="1:20" ht="31" customHeight="1">
-      <c r="B13" s="430"/>
-      <c r="C13" s="375"/>
-      <c r="D13" s="375"/>
-      <c r="E13" s="385" t="s">
-        <v>269</v>
-      </c>
-      <c r="F13" s="385"/>
-      <c r="G13" s="383"/>
-      <c r="H13" s="383"/>
-      <c r="I13" s="383"/>
-      <c r="J13" s="383"/>
+      <c r="B13" s="428"/>
+      <c r="C13" s="432"/>
+      <c r="D13" s="433"/>
+      <c r="E13" s="386" t="s">
+        <v>284</v>
+      </c>
+      <c r="F13" s="386"/>
+      <c r="G13" s="384"/>
+      <c r="H13" s="384"/>
+      <c r="I13" s="384"/>
+      <c r="J13" s="384"/>
       <c r="K13" s="6"/>
       <c r="L13" s="133" t="s">
         <v>91</v>
       </c>
-      <c r="M13" s="141" t="s">
-        <v>472</v>
+      <c r="M13" s="138" t="s">
+        <v>437</v>
       </c>
       <c r="N13" s="11"/>
     </row>
     <row r="14" spans="1:20" ht="31" customHeight="1">
-      <c r="B14" s="430"/>
-      <c r="C14" s="375"/>
-      <c r="D14" s="375"/>
-      <c r="E14" s="385" t="s">
-        <v>284</v>
-      </c>
-      <c r="F14" s="385"/>
-      <c r="G14" s="383"/>
-      <c r="H14" s="383"/>
-      <c r="I14" s="383"/>
-      <c r="J14" s="383"/>
+      <c r="B14" s="429"/>
+      <c r="C14" s="434"/>
+      <c r="D14" s="435"/>
+      <c r="E14" s="386" t="s">
+        <v>283</v>
+      </c>
+      <c r="F14" s="386"/>
+      <c r="G14" s="384"/>
+      <c r="H14" s="384"/>
+      <c r="I14" s="384"/>
+      <c r="J14" s="384"/>
       <c r="K14" s="6"/>
       <c r="L14" s="133" t="s">
         <v>91</v>
@@ -6738,43 +6756,40 @@
       <c r="N14" s="11"/>
     </row>
     <row r="15" spans="1:20" ht="31" customHeight="1">
-      <c r="B15" s="431"/>
-      <c r="C15" s="375"/>
+      <c r="B15" s="378" t="s">
+        <v>258</v>
+      </c>
+      <c r="C15" s="375" t="s">
+        <v>275</v>
+      </c>
       <c r="D15" s="375"/>
-      <c r="E15" s="385" t="s">
-        <v>283</v>
-      </c>
-      <c r="F15" s="385"/>
-      <c r="G15" s="383"/>
-      <c r="H15" s="383"/>
-      <c r="I15" s="383"/>
-      <c r="J15" s="383"/>
+      <c r="E15" s="386" t="s">
+        <v>258</v>
+      </c>
+      <c r="F15" s="386"/>
+      <c r="G15" s="384"/>
+      <c r="H15" s="384"/>
+      <c r="I15" s="384"/>
+      <c r="J15" s="384"/>
       <c r="K15" s="6"/>
       <c r="L15" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="M15" s="138" t="s">
-        <v>437</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="M15" s="11"/>
       <c r="N15" s="11"/>
     </row>
     <row r="16" spans="1:20" ht="31" customHeight="1">
-      <c r="B16" s="378" t="s">
-        <v>258</v>
-      </c>
-      <c r="C16" s="375" t="s">
-        <v>275</v>
-      </c>
+      <c r="B16" s="378"/>
+      <c r="C16" s="375"/>
       <c r="D16" s="375"/>
-      <c r="E16" s="385" t="s">
-        <v>258</v>
-      </c>
-      <c r="F16" s="385"/>
-      <c r="G16" s="383"/>
-      <c r="H16" s="383"/>
-      <c r="I16" s="383"/>
-      <c r="J16" s="383"/>
-      <c r="K16" s="6"/>
+      <c r="E16" s="386" t="s">
+        <v>274</v>
+      </c>
+      <c r="F16" s="386"/>
+      <c r="G16" s="384"/>
+      <c r="H16" s="384"/>
+      <c r="I16" s="384"/>
+      <c r="J16" s="384"/>
       <c r="L16" s="133" t="s">
         <v>113</v>
       </c>
@@ -6785,14 +6800,14 @@
       <c r="B17" s="378"/>
       <c r="C17" s="375"/>
       <c r="D17" s="375"/>
-      <c r="E17" s="385" t="s">
-        <v>274</v>
-      </c>
-      <c r="F17" s="385"/>
-      <c r="G17" s="383"/>
-      <c r="H17" s="383"/>
-      <c r="I17" s="383"/>
-      <c r="J17" s="383"/>
+      <c r="E17" s="386" t="s">
+        <v>277</v>
+      </c>
+      <c r="F17" s="386"/>
+      <c r="G17" s="384"/>
+      <c r="H17" s="384"/>
+      <c r="I17" s="384"/>
+      <c r="J17" s="384"/>
       <c r="L17" s="133" t="s">
         <v>113</v>
       </c>
@@ -6803,14 +6818,14 @@
       <c r="B18" s="378"/>
       <c r="C18" s="375"/>
       <c r="D18" s="375"/>
-      <c r="E18" s="385" t="s">
-        <v>277</v>
-      </c>
-      <c r="F18" s="385"/>
-      <c r="G18" s="383"/>
-      <c r="H18" s="383"/>
-      <c r="I18" s="383"/>
-      <c r="J18" s="383"/>
+      <c r="E18" s="386" t="s">
+        <v>261</v>
+      </c>
+      <c r="F18" s="386"/>
+      <c r="G18" s="384"/>
+      <c r="H18" s="384"/>
+      <c r="I18" s="384"/>
+      <c r="J18" s="384"/>
       <c r="L18" s="133" t="s">
         <v>113</v>
       </c>
@@ -6821,14 +6836,14 @@
       <c r="B19" s="378"/>
       <c r="C19" s="375"/>
       <c r="D19" s="375"/>
-      <c r="E19" s="385" t="s">
-        <v>261</v>
-      </c>
-      <c r="F19" s="385"/>
-      <c r="G19" s="383"/>
-      <c r="H19" s="383"/>
-      <c r="I19" s="383"/>
-      <c r="J19" s="383"/>
+      <c r="E19" s="386" t="s">
+        <v>273</v>
+      </c>
+      <c r="F19" s="386"/>
+      <c r="G19" s="384"/>
+      <c r="H19" s="384"/>
+      <c r="I19" s="384"/>
+      <c r="J19" s="384"/>
       <c r="L19" s="133" t="s">
         <v>113</v>
       </c>
@@ -6837,74 +6852,74 @@
     </row>
     <row r="20" spans="2:14" ht="31" customHeight="1">
       <c r="B20" s="378"/>
-      <c r="C20" s="375"/>
+      <c r="C20" s="375" t="s">
+        <v>276</v>
+      </c>
       <c r="D20" s="375"/>
-      <c r="E20" s="385" t="s">
-        <v>273</v>
-      </c>
-      <c r="F20" s="385"/>
-      <c r="G20" s="383"/>
-      <c r="H20" s="383"/>
-      <c r="I20" s="383"/>
-      <c r="J20" s="383"/>
+      <c r="E20" s="386" t="s">
+        <v>508</v>
+      </c>
+      <c r="F20" s="386"/>
+      <c r="G20" s="384"/>
+      <c r="H20" s="384"/>
+      <c r="I20" s="384"/>
+      <c r="J20" s="384"/>
       <c r="L20" s="133" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="M20" s="11"/>
       <c r="N20" s="11"/>
     </row>
     <row r="21" spans="2:14" ht="31" customHeight="1">
       <c r="B21" s="378"/>
-      <c r="C21" s="375" t="s">
-        <v>276</v>
-      </c>
+      <c r="C21" s="375"/>
       <c r="D21" s="375"/>
-      <c r="E21" s="385" t="s">
-        <v>508</v>
-      </c>
-      <c r="F21" s="385"/>
-      <c r="G21" s="383"/>
-      <c r="H21" s="383"/>
-      <c r="I21" s="383"/>
-      <c r="J21" s="383"/>
+      <c r="E21" s="386" t="s">
+        <v>272</v>
+      </c>
+      <c r="F21" s="386"/>
+      <c r="G21" s="384"/>
+      <c r="H21" s="384"/>
+      <c r="I21" s="384"/>
+      <c r="J21" s="384"/>
       <c r="L21" s="133" t="s">
         <v>97</v>
       </c>
-      <c r="M21" s="11"/>
+      <c r="M21" s="175" t="s">
+        <v>114</v>
+      </c>
       <c r="N21" s="11"/>
     </row>
     <row r="22" spans="2:14" ht="31" customHeight="1">
       <c r="B22" s="378"/>
       <c r="C22" s="375"/>
       <c r="D22" s="375"/>
-      <c r="E22" s="385" t="s">
-        <v>272</v>
-      </c>
-      <c r="F22" s="385"/>
-      <c r="G22" s="383"/>
-      <c r="H22" s="383"/>
-      <c r="I22" s="383"/>
-      <c r="J22" s="383"/>
+      <c r="E22" s="386" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="386"/>
+      <c r="G22" s="384"/>
+      <c r="H22" s="384"/>
+      <c r="I22" s="384"/>
+      <c r="J22" s="384"/>
       <c r="L22" s="133" t="s">
         <v>97</v>
       </c>
-      <c r="M22" s="175" t="s">
-        <v>114</v>
-      </c>
+      <c r="M22" s="11"/>
       <c r="N22" s="11"/>
     </row>
     <row r="23" spans="2:14" ht="31" customHeight="1">
       <c r="B23" s="378"/>
       <c r="C23" s="375"/>
       <c r="D23" s="375"/>
-      <c r="E23" s="385" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="385"/>
-      <c r="G23" s="383"/>
-      <c r="H23" s="383"/>
-      <c r="I23" s="383"/>
-      <c r="J23" s="383"/>
+      <c r="E23" s="386" t="s">
+        <v>273</v>
+      </c>
+      <c r="F23" s="386"/>
+      <c r="G23" s="384"/>
+      <c r="H23" s="384"/>
+      <c r="I23" s="384"/>
+      <c r="J23" s="384"/>
       <c r="L23" s="133" t="s">
         <v>97</v>
       </c>
@@ -6912,772 +6927,774 @@
       <c r="N23" s="11"/>
     </row>
     <row r="24" spans="2:14" ht="31" customHeight="1">
-      <c r="B24" s="378"/>
-      <c r="C24" s="375"/>
-      <c r="D24" s="375"/>
-      <c r="E24" s="385" t="s">
-        <v>273</v>
-      </c>
-      <c r="F24" s="385"/>
-      <c r="G24" s="383"/>
-      <c r="H24" s="383"/>
-      <c r="I24" s="383"/>
-      <c r="J24" s="383"/>
+      <c r="B24" s="375" t="s">
+        <v>611</v>
+      </c>
+      <c r="C24" s="436" t="s">
+        <v>446</v>
+      </c>
+      <c r="D24" s="437"/>
+      <c r="E24" s="390"/>
+      <c r="F24" s="390"/>
+      <c r="G24" s="390"/>
+      <c r="H24" s="390"/>
+      <c r="I24" s="390"/>
+      <c r="J24" s="390"/>
+      <c r="K24" s="6"/>
       <c r="L24" s="133" t="s">
-        <v>97</v>
-      </c>
-      <c r="M24" s="11"/>
+        <v>434</v>
+      </c>
+      <c r="M24" s="141" t="s">
+        <v>460</v>
+      </c>
       <c r="N24" s="11"/>
     </row>
     <row r="25" spans="2:14" ht="31" customHeight="1">
-      <c r="B25" s="428"/>
-      <c r="C25" s="365" t="s">
-        <v>502</v>
-      </c>
-      <c r="D25" s="394" t="s">
-        <v>429</v>
-      </c>
-      <c r="E25" s="385" t="s">
-        <v>431</v>
-      </c>
-      <c r="F25" s="385"/>
-      <c r="G25" s="383"/>
-      <c r="H25" s="383"/>
-      <c r="I25" s="383"/>
-      <c r="J25" s="383"/>
+      <c r="B25" s="375"/>
+      <c r="C25" s="436" t="s">
+        <v>447</v>
+      </c>
+      <c r="D25" s="437"/>
+      <c r="E25" s="390"/>
+      <c r="F25" s="390"/>
+      <c r="G25" s="390"/>
+      <c r="H25" s="390"/>
+      <c r="I25" s="390"/>
+      <c r="J25" s="390"/>
       <c r="K25" s="6"/>
       <c r="L25" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="M25" s="138" t="s">
-        <v>438</v>
+        <v>434</v>
+      </c>
+      <c r="M25" s="141" t="s">
+        <v>460</v>
       </c>
       <c r="N25" s="11"/>
     </row>
     <row r="26" spans="2:14" ht="31" customHeight="1">
-      <c r="B26" s="428"/>
-      <c r="C26" s="365"/>
-      <c r="D26" s="394"/>
-      <c r="E26" s="385" t="s">
-        <v>395</v>
-      </c>
-      <c r="F26" s="385"/>
-      <c r="G26" s="383"/>
-      <c r="H26" s="383"/>
-      <c r="I26" s="383"/>
-      <c r="J26" s="383"/>
+      <c r="B26" s="375"/>
+      <c r="C26" s="436" t="s">
+        <v>448</v>
+      </c>
+      <c r="D26" s="437"/>
+      <c r="E26" s="390"/>
+      <c r="F26" s="390"/>
+      <c r="G26" s="390"/>
+      <c r="H26" s="390"/>
+      <c r="I26" s="390"/>
+      <c r="J26" s="390"/>
       <c r="K26" s="6"/>
       <c r="L26" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="M26" s="138" t="s">
-        <v>592</v>
+        <v>434</v>
+      </c>
+      <c r="M26" s="141" t="s">
+        <v>460</v>
       </c>
       <c r="N26" s="11"/>
     </row>
     <row r="27" spans="2:14" ht="31" customHeight="1">
-      <c r="B27" s="428"/>
-      <c r="C27" s="365"/>
-      <c r="D27" s="394"/>
-      <c r="E27" s="365" t="s">
-        <v>499</v>
-      </c>
-      <c r="F27" s="401" t="s">
-        <v>445</v>
-      </c>
-      <c r="G27" s="365" t="s">
-        <v>263</v>
-      </c>
-      <c r="H27" s="384" t="s">
-        <v>136</v>
-      </c>
-      <c r="I27" s="364"/>
-      <c r="J27" s="364"/>
+      <c r="B27" s="375"/>
+      <c r="C27" s="436" t="s">
+        <v>449</v>
+      </c>
+      <c r="D27" s="437"/>
+      <c r="E27" s="390"/>
+      <c r="F27" s="390"/>
+      <c r="G27" s="390"/>
+      <c r="H27" s="390"/>
+      <c r="I27" s="390"/>
+      <c r="J27" s="390"/>
       <c r="K27" s="6"/>
       <c r="L27" s="133" t="s">
-        <v>96</v>
-      </c>
-      <c r="M27" s="116" t="s">
-        <v>411</v>
+        <v>90</v>
+      </c>
+      <c r="M27" s="116">
+        <v>0</v>
       </c>
       <c r="N27" s="11"/>
     </row>
     <row r="28" spans="2:14" ht="31" customHeight="1">
-      <c r="B28" s="428"/>
-      <c r="C28" s="365"/>
-      <c r="D28" s="394"/>
-      <c r="E28" s="365"/>
-      <c r="F28" s="401"/>
-      <c r="G28" s="365"/>
-      <c r="H28" s="384" t="s">
-        <v>137</v>
-      </c>
-      <c r="I28" s="364"/>
-      <c r="J28" s="364"/>
+      <c r="B28" s="375"/>
+      <c r="C28" s="436" t="s">
+        <v>450</v>
+      </c>
+      <c r="D28" s="437"/>
+      <c r="E28" s="390"/>
+      <c r="F28" s="390"/>
+      <c r="G28" s="390"/>
+      <c r="H28" s="390"/>
+      <c r="I28" s="390"/>
+      <c r="J28" s="390"/>
       <c r="K28" s="6"/>
       <c r="L28" s="133" t="s">
-        <v>434</v>
-      </c>
-      <c r="M28" s="11"/>
-      <c r="N28" s="175" t="s">
-        <v>436</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="M28" s="116">
+        <v>0</v>
+      </c>
+      <c r="N28" s="11"/>
     </row>
     <row r="29" spans="2:14" ht="31" customHeight="1">
-      <c r="B29" s="428"/>
-      <c r="C29" s="365"/>
-      <c r="D29" s="394"/>
-      <c r="E29" s="365"/>
-      <c r="F29" s="401"/>
-      <c r="G29" s="365"/>
-      <c r="H29" s="385" t="s">
-        <v>426</v>
-      </c>
-      <c r="I29" s="410" t="s">
-        <v>141</v>
-      </c>
-      <c r="J29" s="411"/>
+      <c r="B29" s="375"/>
+      <c r="C29" s="436" t="s">
+        <v>451</v>
+      </c>
+      <c r="D29" s="437"/>
+      <c r="E29" s="390"/>
+      <c r="F29" s="390"/>
+      <c r="G29" s="390"/>
+      <c r="H29" s="390"/>
+      <c r="I29" s="390"/>
+      <c r="J29" s="390"/>
       <c r="K29" s="6"/>
       <c r="L29" s="133" t="s">
-        <v>141</v>
-      </c>
-      <c r="M29" s="11"/>
-      <c r="N29" s="141" t="s">
-        <v>244</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="M29" s="116">
+        <v>0</v>
+      </c>
+      <c r="N29" s="11"/>
     </row>
     <row r="30" spans="2:14" ht="31" customHeight="1">
-      <c r="B30" s="428"/>
-      <c r="C30" s="365"/>
-      <c r="D30" s="394"/>
-      <c r="E30" s="365"/>
-      <c r="F30" s="401"/>
-      <c r="G30" s="365"/>
-      <c r="H30" s="385"/>
-      <c r="I30" s="408" t="s">
-        <v>146</v>
-      </c>
-      <c r="J30" s="409"/>
+      <c r="B30" s="395" t="s">
+        <v>429</v>
+      </c>
+      <c r="C30" s="365" t="s">
+        <v>502</v>
+      </c>
+      <c r="D30" s="395" t="s">
+        <v>429</v>
+      </c>
+      <c r="E30" s="386" t="s">
+        <v>431</v>
+      </c>
+      <c r="F30" s="386"/>
+      <c r="G30" s="384"/>
+      <c r="H30" s="384"/>
+      <c r="I30" s="384"/>
+      <c r="J30" s="384"/>
       <c r="K30" s="6"/>
       <c r="L30" s="133" t="s">
-        <v>434</v>
-      </c>
-      <c r="M30" s="11"/>
-      <c r="N30" s="175" t="s">
-        <v>245</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="M30" s="138" t="s">
+        <v>438</v>
+      </c>
+      <c r="N30" s="11"/>
     </row>
     <row r="31" spans="2:14" ht="31" customHeight="1">
-      <c r="B31" s="428"/>
+      <c r="B31" s="395"/>
       <c r="C31" s="365"/>
-      <c r="D31" s="394"/>
-      <c r="E31" s="365"/>
-      <c r="F31" s="401"/>
-      <c r="G31" s="365"/>
-      <c r="H31" s="385"/>
-      <c r="I31" s="408" t="s">
-        <v>408</v>
-      </c>
-      <c r="J31" s="409"/>
+      <c r="D31" s="395"/>
+      <c r="E31" s="386" t="s">
+        <v>395</v>
+      </c>
+      <c r="F31" s="386"/>
+      <c r="G31" s="384"/>
+      <c r="H31" s="384"/>
+      <c r="I31" s="384"/>
+      <c r="J31" s="384"/>
       <c r="K31" s="6"/>
       <c r="L31" s="133" t="s">
-        <v>434</v>
-      </c>
-      <c r="M31" s="11"/>
-      <c r="N31" s="175" t="s">
-        <v>246</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="M31" s="138" t="s">
+        <v>592</v>
+      </c>
+      <c r="N31" s="11"/>
     </row>
     <row r="32" spans="2:14" ht="31" customHeight="1">
-      <c r="B32" s="428"/>
+      <c r="B32" s="395"/>
       <c r="C32" s="365"/>
-      <c r="D32" s="394"/>
-      <c r="E32" s="365"/>
-      <c r="F32" s="401"/>
-      <c r="G32" s="365"/>
-      <c r="H32" s="385"/>
-      <c r="I32" s="408" t="s">
-        <v>409</v>
-      </c>
-      <c r="J32" s="409"/>
+      <c r="D32" s="395"/>
+      <c r="E32" s="365" t="s">
+        <v>499</v>
+      </c>
+      <c r="F32" s="400" t="s">
+        <v>445</v>
+      </c>
+      <c r="G32" s="365" t="s">
+        <v>263</v>
+      </c>
+      <c r="H32" s="385" t="s">
+        <v>136</v>
+      </c>
+      <c r="I32" s="364"/>
+      <c r="J32" s="364"/>
       <c r="K32" s="6"/>
       <c r="L32" s="133" t="s">
-        <v>90</v>
-      </c>
-      <c r="M32" s="11"/>
-      <c r="N32" s="68">
-        <v>4</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="M32" s="116" t="s">
+        <v>411</v>
+      </c>
+      <c r="N32" s="11"/>
     </row>
     <row r="33" spans="2:14" ht="31" customHeight="1">
-      <c r="B33" s="428"/>
+      <c r="B33" s="395"/>
       <c r="C33" s="365"/>
-      <c r="D33" s="394"/>
+      <c r="D33" s="395"/>
       <c r="E33" s="365"/>
-      <c r="F33" s="401"/>
+      <c r="F33" s="400"/>
       <c r="G33" s="365"/>
-      <c r="H33" s="385"/>
-      <c r="I33" s="408" t="s">
-        <v>410</v>
-      </c>
-      <c r="J33" s="409"/>
+      <c r="H33" s="385" t="s">
+        <v>137</v>
+      </c>
+      <c r="I33" s="364"/>
+      <c r="J33" s="364"/>
       <c r="K33" s="6"/>
       <c r="L33" s="133" t="s">
-        <v>90</v>
+        <v>434</v>
       </c>
       <c r="M33" s="11"/>
-      <c r="N33" s="68">
-        <v>10</v>
+      <c r="N33" s="175" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="34" spans="2:14" ht="31" customHeight="1">
-      <c r="B34" s="428"/>
+      <c r="B34" s="395"/>
       <c r="C34" s="365"/>
-      <c r="D34" s="394" t="s">
-        <v>430</v>
-      </c>
-      <c r="E34" s="385" t="s">
-        <v>379</v>
-      </c>
-      <c r="F34" s="385"/>
-      <c r="G34" s="386"/>
-      <c r="H34" s="386"/>
-      <c r="I34" s="386"/>
-      <c r="J34" s="386"/>
+      <c r="D34" s="395"/>
+      <c r="E34" s="365"/>
+      <c r="F34" s="400"/>
+      <c r="G34" s="365"/>
+      <c r="H34" s="386" t="s">
+        <v>426</v>
+      </c>
+      <c r="I34" s="409" t="s">
+        <v>141</v>
+      </c>
+      <c r="J34" s="410"/>
       <c r="K34" s="6"/>
       <c r="L34" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="M34" s="177"/>
-      <c r="N34" s="138" t="s">
-        <v>440</v>
+        <v>141</v>
+      </c>
+      <c r="M34" s="11"/>
+      <c r="N34" s="141" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="2:14" ht="31" customHeight="1">
-      <c r="B35" s="428"/>
+      <c r="B35" s="395"/>
       <c r="C35" s="365"/>
-      <c r="D35" s="394"/>
-      <c r="E35" s="385" t="s">
-        <v>279</v>
-      </c>
-      <c r="F35" s="385"/>
-      <c r="G35" s="386"/>
+      <c r="D35" s="395"/>
+      <c r="E35" s="365"/>
+      <c r="F35" s="400"/>
+      <c r="G35" s="365"/>
       <c r="H35" s="386"/>
-      <c r="I35" s="386"/>
-      <c r="J35" s="386"/>
+      <c r="I35" s="407" t="s">
+        <v>146</v>
+      </c>
+      <c r="J35" s="408"/>
       <c r="K35" s="6"/>
       <c r="L35" s="133" t="s">
-        <v>90</v>
-      </c>
-      <c r="M35" s="116">
-        <v>500</v>
-      </c>
-      <c r="N35" s="11"/>
+        <v>434</v>
+      </c>
+      <c r="M35" s="11"/>
+      <c r="N35" s="175" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="36" spans="2:14" ht="31" customHeight="1">
-      <c r="B36" s="428"/>
+      <c r="B36" s="395"/>
       <c r="C36" s="365"/>
-      <c r="D36" s="394"/>
-      <c r="E36" s="385" t="s">
-        <v>507</v>
-      </c>
-      <c r="F36" s="385"/>
-      <c r="G36" s="386"/>
+      <c r="D36" s="395"/>
+      <c r="E36" s="365"/>
+      <c r="F36" s="400"/>
+      <c r="G36" s="365"/>
       <c r="H36" s="386"/>
-      <c r="I36" s="386"/>
-      <c r="J36" s="386"/>
+      <c r="I36" s="407" t="s">
+        <v>408</v>
+      </c>
+      <c r="J36" s="408"/>
       <c r="K36" s="6"/>
       <c r="L36" s="133" t="s">
-        <v>90</v>
-      </c>
-      <c r="M36" s="116">
-        <v>500</v>
-      </c>
-      <c r="N36" s="11"/>
+        <v>434</v>
+      </c>
+      <c r="M36" s="11"/>
+      <c r="N36" s="175" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="37" spans="2:14" ht="31" customHeight="1">
-      <c r="B37" s="428"/>
+      <c r="B37" s="395"/>
       <c r="C37" s="365"/>
-      <c r="D37" s="394"/>
-      <c r="E37" s="385" t="s">
-        <v>399</v>
-      </c>
-      <c r="F37" s="385"/>
-      <c r="G37" s="386"/>
+      <c r="D37" s="395"/>
+      <c r="E37" s="365"/>
+      <c r="F37" s="400"/>
+      <c r="G37" s="365"/>
       <c r="H37" s="386"/>
-      <c r="I37" s="386"/>
-      <c r="J37" s="386"/>
+      <c r="I37" s="407" t="s">
+        <v>409</v>
+      </c>
+      <c r="J37" s="408"/>
       <c r="K37" s="6"/>
       <c r="L37" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="M37" s="138" t="s">
-        <v>593</v>
-      </c>
-      <c r="N37" s="11"/>
+        <v>90</v>
+      </c>
+      <c r="M37" s="11"/>
+      <c r="N37" s="68">
+        <v>4</v>
+      </c>
     </row>
     <row r="38" spans="2:14" ht="31" customHeight="1">
-      <c r="B38" s="428"/>
+      <c r="B38" s="395"/>
       <c r="C38" s="365"/>
-      <c r="D38" s="394"/>
-      <c r="E38" s="365" t="s">
-        <v>500</v>
-      </c>
-      <c r="F38" s="401" t="s">
-        <v>444</v>
-      </c>
-      <c r="G38" s="365" t="s">
-        <v>263</v>
-      </c>
-      <c r="H38" s="387" t="s">
-        <v>136</v>
-      </c>
-      <c r="I38" s="364"/>
-      <c r="J38" s="364"/>
+      <c r="D38" s="395"/>
+      <c r="E38" s="365"/>
+      <c r="F38" s="400"/>
+      <c r="G38" s="365"/>
+      <c r="H38" s="386"/>
+      <c r="I38" s="407" t="s">
+        <v>410</v>
+      </c>
+      <c r="J38" s="408"/>
       <c r="K38" s="6"/>
       <c r="L38" s="133" t="s">
-        <v>122</v>
-      </c>
-      <c r="M38" s="116" t="s">
-        <v>411</v>
-      </c>
-      <c r="N38" s="11"/>
+        <v>90</v>
+      </c>
+      <c r="M38" s="11"/>
+      <c r="N38" s="68">
+        <v>10</v>
+      </c>
     </row>
     <row r="39" spans="2:14" ht="31" customHeight="1">
-      <c r="B39" s="428"/>
+      <c r="B39" s="395" t="s">
+        <v>430</v>
+      </c>
       <c r="C39" s="365"/>
-      <c r="D39" s="394"/>
-      <c r="E39" s="365"/>
-      <c r="F39" s="401"/>
-      <c r="G39" s="365"/>
-      <c r="H39" s="387" t="s">
-        <v>137</v>
-      </c>
-      <c r="I39" s="364"/>
-      <c r="J39" s="364"/>
+      <c r="D39" s="395" t="s">
+        <v>430</v>
+      </c>
+      <c r="E39" s="386" t="s">
+        <v>379</v>
+      </c>
+      <c r="F39" s="386"/>
+      <c r="G39" s="387"/>
+      <c r="H39" s="387"/>
+      <c r="I39" s="387"/>
+      <c r="J39" s="387"/>
       <c r="K39" s="6"/>
       <c r="L39" s="133" t="s">
-        <v>434</v>
-      </c>
-      <c r="M39" s="11"/>
-      <c r="N39" s="175" t="s">
-        <v>150</v>
+        <v>91</v>
+      </c>
+      <c r="M39" s="177"/>
+      <c r="N39" s="138" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="40" spans="2:14" ht="31" customHeight="1">
-      <c r="B40" s="428"/>
+      <c r="B40" s="395"/>
       <c r="C40" s="365"/>
-      <c r="D40" s="394"/>
-      <c r="E40" s="365"/>
-      <c r="F40" s="401"/>
-      <c r="G40" s="365"/>
-      <c r="H40" s="387" t="s">
-        <v>282</v>
-      </c>
-      <c r="I40" s="364"/>
-      <c r="J40" s="364"/>
+      <c r="D40" s="395"/>
+      <c r="E40" s="386" t="s">
+        <v>279</v>
+      </c>
+      <c r="F40" s="386"/>
+      <c r="G40" s="387"/>
+      <c r="H40" s="387"/>
+      <c r="I40" s="387"/>
+      <c r="J40" s="387"/>
       <c r="K40" s="6"/>
       <c r="L40" s="133" t="s">
-        <v>122</v>
-      </c>
-      <c r="M40" s="11"/>
-      <c r="N40" s="116" t="b">
-        <v>0</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="M40" s="116">
+        <v>500</v>
+      </c>
+      <c r="N40" s="11"/>
     </row>
     <row r="41" spans="2:14" ht="31" customHeight="1">
-      <c r="B41" s="428"/>
+      <c r="B41" s="395"/>
       <c r="C41" s="365"/>
-      <c r="D41" s="394"/>
-      <c r="E41" s="365"/>
-      <c r="F41" s="401"/>
-      <c r="G41" s="365"/>
-      <c r="H41" s="387" t="s">
-        <v>281</v>
-      </c>
-      <c r="I41" s="364"/>
-      <c r="J41" s="364"/>
+      <c r="D41" s="395"/>
+      <c r="E41" s="386" t="s">
+        <v>507</v>
+      </c>
+      <c r="F41" s="386"/>
+      <c r="G41" s="387"/>
+      <c r="H41" s="387"/>
+      <c r="I41" s="387"/>
+      <c r="J41" s="387"/>
       <c r="K41" s="6"/>
       <c r="L41" s="133" t="s">
-        <v>122</v>
-      </c>
-      <c r="M41" s="11"/>
-      <c r="N41" s="116" t="b">
-        <v>0</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="M41" s="116">
+        <v>500</v>
+      </c>
+      <c r="N41" s="11"/>
     </row>
     <row r="42" spans="2:14" ht="31" customHeight="1">
-      <c r="B42" s="428"/>
+      <c r="B42" s="395"/>
       <c r="C42" s="365"/>
-      <c r="D42" s="394"/>
-      <c r="E42" s="365"/>
-      <c r="F42" s="401"/>
-      <c r="G42" s="365"/>
-      <c r="H42" s="388" t="s">
-        <v>426</v>
-      </c>
-      <c r="I42" s="388" t="s">
-        <v>141</v>
-      </c>
-      <c r="J42" s="388"/>
+      <c r="D42" s="395"/>
+      <c r="E42" s="386" t="s">
+        <v>399</v>
+      </c>
+      <c r="F42" s="386"/>
+      <c r="G42" s="387"/>
+      <c r="H42" s="387"/>
+      <c r="I42" s="387"/>
+      <c r="J42" s="387"/>
       <c r="K42" s="6"/>
       <c r="L42" s="133" t="s">
-        <v>141</v>
-      </c>
-      <c r="M42" s="11"/>
-      <c r="N42" s="141" t="s">
-        <v>159</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="M42" s="138" t="s">
+        <v>593</v>
+      </c>
+      <c r="N42" s="11"/>
     </row>
     <row r="43" spans="2:14" ht="31" customHeight="1">
-      <c r="B43" s="428"/>
+      <c r="B43" s="395"/>
       <c r="C43" s="365"/>
-      <c r="D43" s="394"/>
-      <c r="E43" s="365"/>
-      <c r="F43" s="401"/>
-      <c r="G43" s="365"/>
-      <c r="H43" s="388"/>
-      <c r="I43" s="388" t="s">
-        <v>146</v>
-      </c>
-      <c r="J43" s="388"/>
+      <c r="D43" s="395"/>
+      <c r="E43" s="365" t="s">
+        <v>500</v>
+      </c>
+      <c r="F43" s="400" t="s">
+        <v>444</v>
+      </c>
+      <c r="G43" s="365" t="s">
+        <v>263</v>
+      </c>
+      <c r="H43" s="388" t="s">
+        <v>136</v>
+      </c>
+      <c r="I43" s="364"/>
+      <c r="J43" s="364"/>
       <c r="K43" s="6"/>
       <c r="L43" s="133" t="s">
-        <v>434</v>
-      </c>
-      <c r="M43" s="11"/>
-      <c r="N43" s="175" t="s">
-        <v>160</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="M43" s="116" t="s">
+        <v>411</v>
+      </c>
+      <c r="N43" s="11"/>
     </row>
     <row r="44" spans="2:14" ht="31" customHeight="1">
-      <c r="B44" s="428"/>
+      <c r="B44" s="395"/>
       <c r="C44" s="365"/>
-      <c r="D44" s="394"/>
+      <c r="D44" s="395"/>
       <c r="E44" s="365"/>
-      <c r="F44" s="401"/>
+      <c r="F44" s="400"/>
       <c r="G44" s="365"/>
-      <c r="H44" s="388"/>
-      <c r="I44" s="388" t="s">
-        <v>400</v>
-      </c>
-      <c r="J44" s="388"/>
+      <c r="H44" s="388" t="s">
+        <v>137</v>
+      </c>
+      <c r="I44" s="364"/>
+      <c r="J44" s="364"/>
       <c r="K44" s="6"/>
       <c r="L44" s="133" t="s">
-        <v>90</v>
+        <v>434</v>
       </c>
       <c r="M44" s="11"/>
-      <c r="N44" s="116">
-        <v>26</v>
+      <c r="N44" s="175" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="2:14" ht="31" customHeight="1">
-      <c r="B45" s="428"/>
+      <c r="B45" s="395"/>
       <c r="C45" s="365"/>
-      <c r="D45" s="394"/>
+      <c r="D45" s="395"/>
       <c r="E45" s="365"/>
-      <c r="F45" s="401"/>
+      <c r="F45" s="400"/>
       <c r="G45" s="365"/>
-      <c r="H45" s="388"/>
-      <c r="I45" s="388" t="s">
-        <v>401</v>
-      </c>
-      <c r="J45" s="388"/>
+      <c r="H45" s="388" t="s">
+        <v>282</v>
+      </c>
+      <c r="I45" s="364"/>
+      <c r="J45" s="364"/>
       <c r="K45" s="6"/>
       <c r="L45" s="133" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="M45" s="11"/>
-      <c r="N45" s="116">
-        <v>12</v>
+      <c r="N45" s="116" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:14" ht="31" customHeight="1">
-      <c r="B46" s="428"/>
+      <c r="B46" s="395"/>
       <c r="C46" s="365"/>
-      <c r="D46" s="394"/>
+      <c r="D46" s="395"/>
       <c r="E46" s="365"/>
-      <c r="F46" s="401"/>
+      <c r="F46" s="400"/>
       <c r="G46" s="365"/>
       <c r="H46" s="388" t="s">
-        <v>140</v>
-      </c>
-      <c r="I46" s="388" t="s">
-        <v>141</v>
-      </c>
-      <c r="J46" s="388"/>
+        <v>281</v>
+      </c>
+      <c r="I46" s="364"/>
+      <c r="J46" s="364"/>
       <c r="K46" s="6"/>
       <c r="L46" s="133" t="s">
+        <v>122</v>
+      </c>
+      <c r="M46" s="11"/>
+      <c r="N46" s="116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" ht="31" customHeight="1">
+      <c r="B47" s="395"/>
+      <c r="C47" s="365"/>
+      <c r="D47" s="395"/>
+      <c r="E47" s="365"/>
+      <c r="F47" s="400"/>
+      <c r="G47" s="365"/>
+      <c r="H47" s="389" t="s">
+        <v>426</v>
+      </c>
+      <c r="I47" s="389" t="s">
         <v>141</v>
       </c>
-      <c r="M46" s="11"/>
-      <c r="N46" s="141" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="47" spans="2:14" ht="31" customHeight="1">
-      <c r="B47" s="428"/>
-      <c r="C47" s="365"/>
-      <c r="D47" s="394"/>
-      <c r="E47" s="365"/>
-      <c r="F47" s="401"/>
-      <c r="G47" s="365"/>
-      <c r="H47" s="388"/>
-      <c r="I47" s="388" t="s">
-        <v>142</v>
-      </c>
-      <c r="J47" s="388"/>
+      <c r="J47" s="389"/>
       <c r="K47" s="6"/>
       <c r="L47" s="133" t="s">
-        <v>434</v>
+        <v>141</v>
       </c>
       <c r="M47" s="11"/>
-      <c r="N47" s="175" t="s">
-        <v>150</v>
+      <c r="N47" s="141" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="2:14" ht="31" customHeight="1">
-      <c r="B48" s="428"/>
+      <c r="B48" s="395"/>
       <c r="C48" s="365"/>
-      <c r="D48" s="394"/>
+      <c r="D48" s="395"/>
       <c r="E48" s="365"/>
-      <c r="F48" s="401"/>
+      <c r="F48" s="400"/>
       <c r="G48" s="365"/>
-      <c r="H48" s="388"/>
-      <c r="I48" s="388" t="s">
-        <v>143</v>
-      </c>
-      <c r="J48" s="388"/>
+      <c r="H48" s="389"/>
+      <c r="I48" s="389" t="s">
+        <v>146</v>
+      </c>
+      <c r="J48" s="389"/>
       <c r="K48" s="6"/>
       <c r="L48" s="133" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="M48" s="11"/>
-      <c r="N48" s="140" t="s">
-        <v>441</v>
+      <c r="N48" s="175" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="2:15" ht="31" customHeight="1">
-      <c r="B49" s="428"/>
+      <c r="B49" s="395"/>
       <c r="C49" s="365"/>
-      <c r="D49" s="394"/>
+      <c r="D49" s="395"/>
       <c r="E49" s="365"/>
-      <c r="F49" s="401"/>
+      <c r="F49" s="400"/>
       <c r="G49" s="365"/>
-      <c r="H49" s="388"/>
-      <c r="I49" s="388" t="s">
-        <v>144</v>
-      </c>
-      <c r="J49" s="388"/>
+      <c r="H49" s="389"/>
+      <c r="I49" s="389" t="s">
+        <v>400</v>
+      </c>
+      <c r="J49" s="389"/>
       <c r="K49" s="6"/>
       <c r="L49" s="133" t="s">
-        <v>434</v>
+        <v>90</v>
       </c>
       <c r="M49" s="11"/>
-      <c r="N49" s="175" t="s">
-        <v>157</v>
+      <c r="N49" s="116">
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="2:15" ht="31" customHeight="1">
-      <c r="B50" s="428"/>
-      <c r="C50" s="373" t="s">
-        <v>28</v>
-      </c>
-      <c r="D50" s="400" t="s">
-        <v>446</v>
-      </c>
-      <c r="E50" s="389"/>
-      <c r="F50" s="389"/>
-      <c r="G50" s="389"/>
+      <c r="B50" s="395"/>
+      <c r="C50" s="365"/>
+      <c r="D50" s="395"/>
+      <c r="E50" s="365"/>
+      <c r="F50" s="400"/>
+      <c r="G50" s="365"/>
       <c r="H50" s="389"/>
-      <c r="I50" s="389"/>
+      <c r="I50" s="389" t="s">
+        <v>401</v>
+      </c>
       <c r="J50" s="389"/>
       <c r="K50" s="6"/>
       <c r="L50" s="133" t="s">
-        <v>434</v>
-      </c>
-      <c r="M50" s="141" t="s">
-        <v>460</v>
-      </c>
-      <c r="N50" s="11"/>
+        <v>90</v>
+      </c>
+      <c r="M50" s="11"/>
+      <c r="N50" s="116">
+        <v>12</v>
+      </c>
     </row>
     <row r="51" spans="2:15" ht="31" customHeight="1">
-      <c r="B51" s="428"/>
-      <c r="C51" s="373"/>
-      <c r="D51" s="400" t="s">
-        <v>447</v>
-      </c>
-      <c r="E51" s="389"/>
-      <c r="F51" s="389"/>
-      <c r="G51" s="389"/>
-      <c r="H51" s="389"/>
-      <c r="I51" s="389"/>
+      <c r="B51" s="395"/>
+      <c r="C51" s="365"/>
+      <c r="D51" s="395"/>
+      <c r="E51" s="365"/>
+      <c r="F51" s="400"/>
+      <c r="G51" s="365"/>
+      <c r="H51" s="389" t="s">
+        <v>140</v>
+      </c>
+      <c r="I51" s="389" t="s">
+        <v>141</v>
+      </c>
       <c r="J51" s="389"/>
       <c r="K51" s="6"/>
       <c r="L51" s="133" t="s">
-        <v>434</v>
-      </c>
-      <c r="M51" s="141" t="s">
-        <v>460</v>
-      </c>
-      <c r="N51" s="11"/>
+        <v>141</v>
+      </c>
+      <c r="M51" s="11"/>
+      <c r="N51" s="141" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="52" spans="2:15" ht="31" customHeight="1">
-      <c r="B52" s="428"/>
-      <c r="C52" s="373"/>
-      <c r="D52" s="400" t="s">
-        <v>448</v>
-      </c>
-      <c r="E52" s="389"/>
-      <c r="F52" s="389"/>
-      <c r="G52" s="389"/>
+      <c r="B52" s="395"/>
+      <c r="C52" s="365"/>
+      <c r="D52" s="395"/>
+      <c r="E52" s="365"/>
+      <c r="F52" s="400"/>
+      <c r="G52" s="365"/>
       <c r="H52" s="389"/>
-      <c r="I52" s="389"/>
+      <c r="I52" s="389" t="s">
+        <v>142</v>
+      </c>
       <c r="J52" s="389"/>
       <c r="K52" s="6"/>
       <c r="L52" s="133" t="s">
         <v>434</v>
       </c>
-      <c r="M52" s="141" t="s">
-        <v>460</v>
-      </c>
-      <c r="N52" s="11"/>
+      <c r="M52" s="11"/>
+      <c r="N52" s="175" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="53" spans="2:15" ht="31" customHeight="1">
-      <c r="B53" s="428"/>
-      <c r="C53" s="373"/>
-      <c r="D53" s="400" t="s">
-        <v>449</v>
-      </c>
-      <c r="E53" s="389"/>
-      <c r="F53" s="389"/>
-      <c r="G53" s="389"/>
+      <c r="B53" s="395"/>
+      <c r="C53" s="365"/>
+      <c r="D53" s="395"/>
+      <c r="E53" s="365"/>
+      <c r="F53" s="400"/>
+      <c r="G53" s="365"/>
       <c r="H53" s="389"/>
-      <c r="I53" s="389"/>
+      <c r="I53" s="389" t="s">
+        <v>143</v>
+      </c>
       <c r="J53" s="389"/>
       <c r="K53" s="6"/>
       <c r="L53" s="133" t="s">
-        <v>90</v>
-      </c>
-      <c r="M53" s="116">
-        <v>0</v>
-      </c>
-      <c r="N53" s="11"/>
+        <v>442</v>
+      </c>
+      <c r="M53" s="11"/>
+      <c r="N53" s="140" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="54" spans="2:15" ht="31" customHeight="1">
-      <c r="B54" s="428"/>
-      <c r="C54" s="373"/>
-      <c r="D54" s="400" t="s">
-        <v>450</v>
-      </c>
-      <c r="E54" s="389"/>
-      <c r="F54" s="389"/>
-      <c r="G54" s="389"/>
+      <c r="B54" s="395"/>
+      <c r="C54" s="365"/>
+      <c r="D54" s="395"/>
+      <c r="E54" s="365"/>
+      <c r="F54" s="400"/>
+      <c r="G54" s="365"/>
       <c r="H54" s="389"/>
-      <c r="I54" s="389"/>
+      <c r="I54" s="389" t="s">
+        <v>144</v>
+      </c>
       <c r="J54" s="389"/>
       <c r="K54" s="6"/>
       <c r="L54" s="133" t="s">
-        <v>90</v>
-      </c>
-      <c r="M54" s="116">
-        <v>0</v>
-      </c>
-      <c r="N54" s="11"/>
+        <v>434</v>
+      </c>
+      <c r="M54" s="11"/>
+      <c r="N54" s="175" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="55" spans="2:15" ht="31" customHeight="1">
-      <c r="B55" s="428"/>
-      <c r="C55" s="373"/>
-      <c r="D55" s="400" t="s">
-        <v>451</v>
-      </c>
-      <c r="E55" s="389"/>
-      <c r="F55" s="389"/>
-      <c r="G55" s="389"/>
-      <c r="H55" s="389"/>
-      <c r="I55" s="389"/>
-      <c r="J55" s="389"/>
-      <c r="K55" s="6"/>
+      <c r="B55" s="378" t="s">
+        <v>508</v>
+      </c>
+      <c r="C55" s="373" t="s">
+        <v>513</v>
+      </c>
+      <c r="D55" s="373"/>
+      <c r="E55" s="384"/>
+      <c r="F55" s="384"/>
+      <c r="G55" s="384"/>
+      <c r="H55" s="384"/>
+      <c r="I55" s="384"/>
+      <c r="J55" s="384"/>
       <c r="L55" s="133" t="s">
-        <v>90</v>
-      </c>
-      <c r="M55" s="116">
-        <v>0</v>
-      </c>
-      <c r="N55" s="11"/>
+        <v>453</v>
+      </c>
+      <c r="M55" s="177"/>
+      <c r="N55" s="116" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="56" spans="2:15" ht="31" customHeight="1">
-      <c r="B56" s="379" t="s">
-        <v>508</v>
-      </c>
+      <c r="B56" s="378"/>
       <c r="C56" s="373" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D56" s="373"/>
-      <c r="E56" s="383"/>
-      <c r="F56" s="383"/>
-      <c r="G56" s="383"/>
-      <c r="H56" s="383"/>
-      <c r="I56" s="383"/>
-      <c r="J56" s="383"/>
+      <c r="E56" s="384"/>
+      <c r="F56" s="384"/>
+      <c r="G56" s="384"/>
+      <c r="H56" s="384"/>
+      <c r="I56" s="384"/>
+      <c r="J56" s="384"/>
       <c r="L56" s="133" t="s">
-        <v>453</v>
-      </c>
-      <c r="M56" s="177"/>
-      <c r="N56" s="116" t="s">
-        <v>454</v>
+        <v>91</v>
+      </c>
+      <c r="M56" s="11"/>
+      <c r="N56" s="138" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="57" spans="2:15" ht="31" customHeight="1">
-      <c r="B57" s="379"/>
+      <c r="B57" s="378"/>
       <c r="C57" s="373" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="D57" s="373"/>
-      <c r="E57" s="383"/>
-      <c r="F57" s="383"/>
-      <c r="G57" s="383"/>
-      <c r="H57" s="383"/>
-      <c r="I57" s="383"/>
-      <c r="J57" s="383"/>
+      <c r="E57" s="384"/>
+      <c r="F57" s="384"/>
+      <c r="G57" s="384"/>
+      <c r="H57" s="384"/>
+      <c r="I57" s="384"/>
+      <c r="J57" s="384"/>
       <c r="L57" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="M57" s="11"/>
-      <c r="N57" s="138" t="s">
-        <v>594</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="M57" s="163" t="s">
+        <v>509</v>
+      </c>
+      <c r="N57" s="11"/>
     </row>
     <row r="58" spans="2:15" ht="31" customHeight="1">
-      <c r="B58" s="379"/>
-      <c r="C58" s="373" t="s">
-        <v>512</v>
-      </c>
-      <c r="D58" s="373"/>
-      <c r="E58" s="383"/>
-      <c r="F58" s="383"/>
-      <c r="G58" s="383"/>
-      <c r="H58" s="383"/>
-      <c r="I58" s="383"/>
-      <c r="J58" s="383"/>
-      <c r="L58" s="133" t="s">
-        <v>97</v>
-      </c>
-      <c r="M58" s="163" t="s">
-        <v>509</v>
-      </c>
-      <c r="N58" s="11"/>
+      <c r="B58" s="378"/>
+      <c r="C58" s="391"/>
+      <c r="D58" s="391"/>
+      <c r="E58" s="391"/>
+      <c r="F58" s="391"/>
+      <c r="G58" s="391"/>
+      <c r="H58" s="391"/>
+      <c r="I58" s="391"/>
+      <c r="J58" s="391"/>
+      <c r="K58" s="361"/>
+      <c r="L58" s="366"/>
+      <c r="M58" s="366"/>
+      <c r="N58" s="366"/>
+      <c r="O58" s="361"/>
     </row>
     <row r="59" spans="2:15" ht="31" customHeight="1">
-      <c r="B59" s="379"/>
-      <c r="C59" s="390"/>
-      <c r="D59" s="390"/>
-      <c r="E59" s="390"/>
-      <c r="F59" s="390"/>
-      <c r="G59" s="390"/>
-      <c r="H59" s="390"/>
-      <c r="I59" s="390"/>
-      <c r="J59" s="390"/>
+      <c r="B59" s="378"/>
+      <c r="C59" s="391"/>
+      <c r="D59" s="391"/>
+      <c r="E59" s="391"/>
+      <c r="F59" s="391"/>
+      <c r="G59" s="391"/>
+      <c r="H59" s="391"/>
+      <c r="I59" s="391"/>
+      <c r="J59" s="391"/>
       <c r="K59" s="361"/>
       <c r="L59" s="366"/>
       <c r="M59" s="366"/>
@@ -7685,39 +7702,49 @@
       <c r="O59" s="361"/>
     </row>
     <row r="60" spans="2:15" ht="31" customHeight="1">
-      <c r="B60" s="379"/>
-      <c r="C60" s="390"/>
-      <c r="D60" s="390"/>
-      <c r="E60" s="390"/>
-      <c r="F60" s="390"/>
-      <c r="G60" s="390"/>
-      <c r="H60" s="390"/>
-      <c r="I60" s="390"/>
-      <c r="J60" s="390"/>
-      <c r="K60" s="361"/>
-      <c r="L60" s="366"/>
-      <c r="M60" s="366"/>
-      <c r="N60" s="366"/>
-      <c r="O60" s="361"/>
+      <c r="B60" s="378" t="s">
+        <v>310</v>
+      </c>
+      <c r="C60" s="370" t="s">
+        <v>290</v>
+      </c>
+      <c r="D60" s="370"/>
+      <c r="E60" s="398" t="s">
+        <v>269</v>
+      </c>
+      <c r="F60" s="399" t="s">
+        <v>455</v>
+      </c>
+      <c r="G60" s="384"/>
+      <c r="H60" s="384"/>
+      <c r="I60" s="384"/>
+      <c r="J60" s="384"/>
+      <c r="L60" s="133" t="s">
+        <v>453</v>
+      </c>
+      <c r="M60" s="141" t="s">
+        <v>473</v>
+      </c>
+      <c r="N60" s="116" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="61" spans="2:15" ht="31" customHeight="1">
-      <c r="B61" s="379" t="s">
-        <v>310</v>
-      </c>
+      <c r="B61" s="378"/>
       <c r="C61" s="370" t="s">
-        <v>290</v>
+        <v>387</v>
       </c>
       <c r="D61" s="370"/>
       <c r="E61" s="398" t="s">
         <v>269</v>
       </c>
       <c r="F61" s="399" t="s">
-        <v>455</v>
-      </c>
-      <c r="G61" s="383"/>
-      <c r="H61" s="383"/>
-      <c r="I61" s="383"/>
-      <c r="J61" s="383"/>
+        <v>456</v>
+      </c>
+      <c r="G61" s="384"/>
+      <c r="H61" s="384"/>
+      <c r="I61" s="384"/>
+      <c r="J61" s="384"/>
       <c r="L61" s="133" t="s">
         <v>453</v>
       </c>
@@ -7727,52 +7754,46 @@
       <c r="N61" s="116" t="s">
         <v>454</v>
       </c>
+      <c r="O61" s="9" t="s">
+        <v>610</v>
+      </c>
     </row>
     <row r="62" spans="2:15" ht="31" customHeight="1">
-      <c r="B62" s="379"/>
-      <c r="C62" s="370" t="s">
-        <v>387</v>
-      </c>
-      <c r="D62" s="370"/>
-      <c r="E62" s="398" t="s">
+      <c r="B62" s="378"/>
+      <c r="C62" s="421" t="s">
+        <v>261</v>
+      </c>
+      <c r="D62" s="422"/>
+      <c r="E62" s="401" t="s">
         <v>269</v>
       </c>
-      <c r="F62" s="399" t="s">
-        <v>456</v>
-      </c>
-      <c r="G62" s="383"/>
-      <c r="H62" s="383"/>
-      <c r="I62" s="383"/>
-      <c r="J62" s="383"/>
+      <c r="F62" s="404" t="s">
+        <v>455</v>
+      </c>
+      <c r="G62" s="386" t="s">
+        <v>403</v>
+      </c>
+      <c r="H62" s="386"/>
+      <c r="I62" s="364"/>
+      <c r="J62" s="364"/>
       <c r="L62" s="133" t="s">
         <v>453</v>
       </c>
       <c r="M62" s="141" t="s">
         <v>473</v>
       </c>
-      <c r="N62" s="116" t="s">
-        <v>454</v>
-      </c>
-      <c r="O62" s="9" t="s">
-        <v>610</v>
-      </c>
+      <c r="N62" s="11"/>
     </row>
     <row r="63" spans="2:15" ht="31" customHeight="1">
-      <c r="B63" s="379"/>
-      <c r="C63" s="422" t="s">
-        <v>261</v>
-      </c>
-      <c r="D63" s="423"/>
-      <c r="E63" s="402" t="s">
-        <v>269</v>
-      </c>
-      <c r="F63" s="405" t="s">
-        <v>455</v>
-      </c>
-      <c r="G63" s="385" t="s">
-        <v>403</v>
-      </c>
-      <c r="H63" s="385"/>
+      <c r="B63" s="378"/>
+      <c r="C63" s="423"/>
+      <c r="D63" s="424"/>
+      <c r="E63" s="402"/>
+      <c r="F63" s="405"/>
+      <c r="G63" s="411" t="s">
+        <v>601</v>
+      </c>
+      <c r="H63" s="412"/>
       <c r="I63" s="364"/>
       <c r="J63" s="364"/>
       <c r="L63" s="133" t="s">
@@ -7781,18 +7802,18 @@
       <c r="M63" s="141" t="s">
         <v>473</v>
       </c>
-      <c r="N63" s="11"/>
+      <c r="N63" s="116" t="s">
+        <v>602</v>
+      </c>
     </row>
     <row r="64" spans="2:15" ht="31" customHeight="1">
-      <c r="B64" s="379"/>
-      <c r="C64" s="424"/>
-      <c r="D64" s="425"/>
-      <c r="E64" s="403"/>
-      <c r="F64" s="406"/>
-      <c r="G64" s="412" t="s">
-        <v>601</v>
-      </c>
-      <c r="H64" s="413"/>
+      <c r="B64" s="378"/>
+      <c r="C64" s="423"/>
+      <c r="D64" s="424"/>
+      <c r="E64" s="402"/>
+      <c r="F64" s="405"/>
+      <c r="G64" s="419"/>
+      <c r="H64" s="420"/>
       <c r="I64" s="364"/>
       <c r="J64" s="364"/>
       <c r="L64" s="133" t="s">
@@ -7802,17 +7823,17 @@
         <v>473</v>
       </c>
       <c r="N64" s="116" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="65" spans="2:15" ht="31" customHeight="1">
-      <c r="B65" s="379"/>
-      <c r="C65" s="424"/>
-      <c r="D65" s="425"/>
-      <c r="E65" s="403"/>
-      <c r="F65" s="406"/>
-      <c r="G65" s="420"/>
-      <c r="H65" s="421"/>
+      <c r="B65" s="378"/>
+      <c r="C65" s="423"/>
+      <c r="D65" s="424"/>
+      <c r="E65" s="402"/>
+      <c r="F65" s="405"/>
+      <c r="G65" s="413"/>
+      <c r="H65" s="414"/>
       <c r="I65" s="364"/>
       <c r="J65" s="364"/>
       <c r="L65" s="133" t="s">
@@ -7822,41 +7843,48 @@
         <v>473</v>
       </c>
       <c r="N65" s="116" t="s">
-        <v>603</v>
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="2:15" ht="31" customHeight="1">
-      <c r="B66" s="379"/>
-      <c r="C66" s="424"/>
-      <c r="D66" s="425"/>
-      <c r="E66" s="403"/>
-      <c r="F66" s="406"/>
-      <c r="G66" s="414"/>
-      <c r="H66" s="415"/>
+      <c r="B66" s="378"/>
+      <c r="C66" s="423"/>
+      <c r="D66" s="424"/>
+      <c r="E66" s="402"/>
+      <c r="F66" s="405"/>
+      <c r="G66" s="409" t="s">
+        <v>505</v>
+      </c>
+      <c r="H66" s="410"/>
       <c r="I66" s="364"/>
       <c r="J66" s="364"/>
       <c r="L66" s="133" t="s">
-        <v>453</v>
-      </c>
-      <c r="M66" s="141" t="s">
-        <v>473</v>
-      </c>
-      <c r="N66" s="116" t="s">
-        <v>265</v>
+        <v>122</v>
+      </c>
+      <c r="M66" s="116" t="s">
+        <v>411</v>
+      </c>
+      <c r="N66" s="11"/>
+      <c r="O66" s="4" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="67" spans="2:15" ht="31" customHeight="1">
-      <c r="B67" s="379"/>
-      <c r="C67" s="424"/>
-      <c r="D67" s="425"/>
-      <c r="E67" s="403"/>
-      <c r="F67" s="406"/>
-      <c r="G67" s="410" t="s">
-        <v>505</v>
-      </c>
-      <c r="H67" s="411"/>
-      <c r="I67" s="364"/>
-      <c r="J67" s="364"/>
+      <c r="B67" s="378"/>
+      <c r="C67" s="423"/>
+      <c r="D67" s="424"/>
+      <c r="E67" s="402"/>
+      <c r="F67" s="405"/>
+      <c r="G67" s="411" t="s">
+        <v>501</v>
+      </c>
+      <c r="H67" s="412"/>
+      <c r="I67" s="368" t="s">
+        <v>484</v>
+      </c>
+      <c r="J67" s="392" t="s">
+        <v>477</v>
+      </c>
       <c r="L67" s="133" t="s">
         <v>122</v>
       </c>
@@ -7865,24 +7893,20 @@
       </c>
       <c r="N67" s="11"/>
       <c r="O67" s="4" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="68" spans="2:15" ht="31" customHeight="1">
-      <c r="B68" s="379"/>
-      <c r="C68" s="424"/>
-      <c r="D68" s="425"/>
+      <c r="B68" s="378"/>
+      <c r="C68" s="423"/>
+      <c r="D68" s="424"/>
       <c r="E68" s="403"/>
       <c r="F68" s="406"/>
-      <c r="G68" s="412" t="s">
-        <v>501</v>
-      </c>
-      <c r="H68" s="413"/>
-      <c r="I68" s="368" t="s">
-        <v>484</v>
-      </c>
-      <c r="J68" s="391" t="s">
-        <v>477</v>
+      <c r="G68" s="413"/>
+      <c r="H68" s="414"/>
+      <c r="I68" s="369"/>
+      <c r="J68" s="392" t="s">
+        <v>482</v>
       </c>
       <c r="L68" s="133" t="s">
         <v>122</v>
@@ -7891,66 +7915,67 @@
         <v>411</v>
       </c>
       <c r="N68" s="11"/>
-      <c r="O68" s="4" t="s">
-        <v>605</v>
-      </c>
     </row>
     <row r="69" spans="2:15" ht="31" customHeight="1">
-      <c r="B69" s="379"/>
-      <c r="C69" s="424"/>
-      <c r="D69" s="425"/>
-      <c r="E69" s="404"/>
-      <c r="F69" s="407"/>
-      <c r="G69" s="414"/>
-      <c r="H69" s="415"/>
-      <c r="I69" s="369"/>
-      <c r="J69" s="391" t="s">
-        <v>482</v>
-      </c>
+      <c r="B69" s="378"/>
+      <c r="C69" s="423"/>
+      <c r="D69" s="424"/>
+      <c r="E69" s="401" t="s">
+        <v>269</v>
+      </c>
+      <c r="F69" s="404" t="s">
+        <v>598</v>
+      </c>
+      <c r="G69" s="386" t="s">
+        <v>591</v>
+      </c>
+      <c r="H69" s="386"/>
+      <c r="I69" s="364"/>
+      <c r="J69" s="364"/>
       <c r="L69" s="133" t="s">
-        <v>122</v>
-      </c>
-      <c r="M69" s="116" t="s">
-        <v>411</v>
+        <v>597</v>
+      </c>
+      <c r="M69" s="141" t="s">
+        <v>473</v>
       </c>
       <c r="N69" s="11"/>
     </row>
     <row r="70" spans="2:15" ht="31" customHeight="1">
-      <c r="B70" s="379"/>
-      <c r="C70" s="424"/>
-      <c r="D70" s="425"/>
-      <c r="E70" s="402" t="s">
-        <v>269</v>
-      </c>
-      <c r="F70" s="405" t="s">
-        <v>598</v>
-      </c>
-      <c r="G70" s="385" t="s">
-        <v>591</v>
-      </c>
-      <c r="H70" s="385"/>
+      <c r="B70" s="378"/>
+      <c r="C70" s="423"/>
+      <c r="D70" s="424"/>
+      <c r="E70" s="402"/>
+      <c r="F70" s="405"/>
+      <c r="G70" s="409" t="s">
+        <v>505</v>
+      </c>
+      <c r="H70" s="410"/>
       <c r="I70" s="364"/>
       <c r="J70" s="364"/>
       <c r="L70" s="133" t="s">
-        <v>597</v>
-      </c>
-      <c r="M70" s="141" t="s">
-        <v>473</v>
+        <v>122</v>
+      </c>
+      <c r="M70" s="116" t="s">
+        <v>411</v>
       </c>
       <c r="N70" s="11"/>
     </row>
     <row r="71" spans="2:15" ht="31" customHeight="1">
-      <c r="B71" s="379"/>
-      <c r="C71" s="424"/>
-      <c r="D71" s="425"/>
-      <c r="E71" s="403"/>
-      <c r="F71" s="406"/>
-      <c r="G71" s="410" t="s">
-        <v>505</v>
-      </c>
-      <c r="H71" s="411"/>
-      <c r="I71" s="364"/>
-      <c r="J71" s="364"/>
+      <c r="B71" s="378"/>
+      <c r="C71" s="423"/>
+      <c r="D71" s="424"/>
+      <c r="E71" s="402"/>
+      <c r="F71" s="405"/>
+      <c r="G71" s="411" t="s">
+        <v>501</v>
+      </c>
+      <c r="H71" s="412"/>
+      <c r="I71" s="368" t="s">
+        <v>484</v>
+      </c>
+      <c r="J71" s="392" t="s">
+        <v>477</v>
+      </c>
       <c r="L71" s="133" t="s">
         <v>122</v>
       </c>
@@ -7960,20 +7985,16 @@
       <c r="N71" s="11"/>
     </row>
     <row r="72" spans="2:15" ht="31" customHeight="1">
-      <c r="B72" s="379"/>
-      <c r="C72" s="424"/>
-      <c r="D72" s="425"/>
+      <c r="B72" s="378"/>
+      <c r="C72" s="425"/>
+      <c r="D72" s="426"/>
       <c r="E72" s="403"/>
       <c r="F72" s="406"/>
-      <c r="G72" s="412" t="s">
-        <v>501</v>
-      </c>
-      <c r="H72" s="413"/>
-      <c r="I72" s="368" t="s">
-        <v>484</v>
-      </c>
-      <c r="J72" s="391" t="s">
-        <v>477</v>
+      <c r="G72" s="413"/>
+      <c r="H72" s="414"/>
+      <c r="I72" s="369"/>
+      <c r="J72" s="392" t="s">
+        <v>482</v>
       </c>
       <c r="L72" s="133" t="s">
         <v>122</v>
@@ -7984,251 +8005,255 @@
       <c r="N72" s="11"/>
     </row>
     <row r="73" spans="2:15" ht="31" customHeight="1">
-      <c r="B73" s="379"/>
-      <c r="C73" s="426"/>
-      <c r="D73" s="427"/>
-      <c r="E73" s="404"/>
-      <c r="F73" s="407"/>
-      <c r="G73" s="414"/>
-      <c r="H73" s="415"/>
-      <c r="I73" s="369"/>
-      <c r="J73" s="391" t="s">
-        <v>482</v>
-      </c>
+      <c r="B73" s="378"/>
+      <c r="C73" s="370" t="s">
+        <v>515</v>
+      </c>
+      <c r="D73" s="370"/>
+      <c r="E73" s="384"/>
+      <c r="F73" s="384"/>
+      <c r="G73" s="384"/>
+      <c r="H73" s="384"/>
+      <c r="I73" s="384"/>
+      <c r="J73" s="384"/>
       <c r="L73" s="133" t="s">
-        <v>122</v>
-      </c>
-      <c r="M73" s="116" t="s">
-        <v>411</v>
-      </c>
+        <v>474</v>
+      </c>
+      <c r="M73" s="141"/>
       <c r="N73" s="11"/>
     </row>
     <row r="74" spans="2:15" ht="31" customHeight="1">
-      <c r="B74" s="379"/>
-      <c r="C74" s="370" t="s">
-        <v>515</v>
-      </c>
-      <c r="D74" s="370"/>
-      <c r="E74" s="383"/>
-      <c r="F74" s="383"/>
-      <c r="G74" s="383"/>
-      <c r="H74" s="383"/>
-      <c r="I74" s="383"/>
-      <c r="J74" s="383"/>
+      <c r="B74" s="378"/>
+      <c r="C74" s="375" t="s">
+        <v>259</v>
+      </c>
+      <c r="D74" s="375"/>
+      <c r="E74" s="386" t="s">
+        <v>270</v>
+      </c>
+      <c r="F74" s="386"/>
+      <c r="G74" s="384"/>
+      <c r="H74" s="384"/>
+      <c r="I74" s="384"/>
+      <c r="J74" s="384"/>
       <c r="L74" s="133" t="s">
-        <v>474</v>
-      </c>
-      <c r="M74" s="141"/>
+        <v>90</v>
+      </c>
+      <c r="M74" s="116">
+        <v>7</v>
+      </c>
       <c r="N74" s="11"/>
     </row>
     <row r="75" spans="2:15" ht="31" customHeight="1">
-      <c r="B75" s="379"/>
-      <c r="C75" s="375" t="s">
-        <v>259</v>
-      </c>
+      <c r="B75" s="378"/>
+      <c r="C75" s="375"/>
       <c r="D75" s="375"/>
-      <c r="E75" s="385" t="s">
-        <v>270</v>
-      </c>
-      <c r="F75" s="385"/>
-      <c r="G75" s="383"/>
-      <c r="H75" s="383"/>
-      <c r="I75" s="383"/>
-      <c r="J75" s="383"/>
+      <c r="E75" s="386" t="s">
+        <v>268</v>
+      </c>
+      <c r="F75" s="386"/>
+      <c r="G75" s="384"/>
+      <c r="H75" s="384"/>
+      <c r="I75" s="384"/>
+      <c r="J75" s="384"/>
       <c r="L75" s="133" t="s">
-        <v>90</v>
-      </c>
-      <c r="M75" s="116">
-        <v>7</v>
+        <v>91</v>
+      </c>
+      <c r="M75" s="141" t="s">
+        <v>481</v>
       </c>
       <c r="N75" s="11"/>
     </row>
     <row r="76" spans="2:15" ht="31" customHeight="1">
-      <c r="B76" s="379"/>
+      <c r="B76" s="378"/>
       <c r="C76" s="375"/>
       <c r="D76" s="375"/>
-      <c r="E76" s="385" t="s">
-        <v>268</v>
-      </c>
-      <c r="F76" s="385"/>
-      <c r="G76" s="383"/>
-      <c r="H76" s="383"/>
-      <c r="I76" s="383"/>
-      <c r="J76" s="383"/>
+      <c r="E76" s="386" t="s">
+        <v>314</v>
+      </c>
+      <c r="F76" s="386"/>
+      <c r="G76" s="172" t="s">
+        <v>269</v>
+      </c>
+      <c r="H76" s="392" t="s">
+        <v>458</v>
+      </c>
+      <c r="I76" s="364"/>
+      <c r="J76" s="364"/>
       <c r="L76" s="133" t="s">
-        <v>91</v>
+        <v>453</v>
       </c>
       <c r="M76" s="141" t="s">
-        <v>481</v>
-      </c>
-      <c r="N76" s="11"/>
+        <v>473</v>
+      </c>
+      <c r="N76" s="116" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="77" spans="2:15" ht="31" customHeight="1">
-      <c r="B77" s="379"/>
+      <c r="B77" s="378"/>
       <c r="C77" s="375"/>
       <c r="D77" s="375"/>
-      <c r="E77" s="385" t="s">
-        <v>314</v>
-      </c>
-      <c r="F77" s="385"/>
-      <c r="G77" s="172" t="s">
-        <v>269</v>
-      </c>
-      <c r="H77" s="391" t="s">
-        <v>458</v>
-      </c>
-      <c r="I77" s="364"/>
-      <c r="J77" s="364"/>
+      <c r="E77" s="386" t="s">
+        <v>313</v>
+      </c>
+      <c r="F77" s="386"/>
+      <c r="G77" s="384"/>
+      <c r="H77" s="384"/>
+      <c r="I77" s="384"/>
+      <c r="J77" s="384"/>
       <c r="L77" s="133" t="s">
-        <v>453</v>
+        <v>91</v>
       </c>
       <c r="M77" s="141" t="s">
-        <v>473</v>
-      </c>
-      <c r="N77" s="116" t="s">
-        <v>454</v>
-      </c>
+        <v>472</v>
+      </c>
+      <c r="N77" s="11"/>
     </row>
     <row r="78" spans="2:15" ht="31" customHeight="1">
-      <c r="B78" s="379"/>
+      <c r="B78" s="378"/>
       <c r="C78" s="375"/>
       <c r="D78" s="375"/>
-      <c r="E78" s="385" t="s">
-        <v>313</v>
-      </c>
-      <c r="F78" s="385"/>
-      <c r="G78" s="383"/>
-      <c r="H78" s="383"/>
-      <c r="I78" s="383"/>
-      <c r="J78" s="383"/>
-      <c r="L78" s="133" t="s">
-        <v>91</v>
+      <c r="E78" s="386" t="s">
+        <v>312</v>
+      </c>
+      <c r="F78" s="386"/>
+      <c r="G78" s="384"/>
+      <c r="H78" s="384"/>
+      <c r="I78" s="384"/>
+      <c r="J78" s="384"/>
+      <c r="L78" s="144" t="s">
+        <v>457</v>
       </c>
       <c r="M78" s="141" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="N78" s="11"/>
+      <c r="O78" s="372" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="79" spans="2:15" ht="31" customHeight="1">
-      <c r="B79" s="379"/>
-      <c r="C79" s="375"/>
-      <c r="D79" s="375"/>
-      <c r="E79" s="385" t="s">
-        <v>312</v>
-      </c>
-      <c r="F79" s="385"/>
-      <c r="G79" s="383"/>
-      <c r="H79" s="383"/>
-      <c r="I79" s="383"/>
-      <c r="J79" s="383"/>
-      <c r="L79" s="144" t="s">
-        <v>457</v>
-      </c>
-      <c r="M79" s="141" t="s">
-        <v>473</v>
+      <c r="B79" s="379" t="s">
+        <v>612</v>
+      </c>
+      <c r="C79" s="395" t="s">
+        <v>353</v>
+      </c>
+      <c r="D79" s="395"/>
+      <c r="E79" s="384"/>
+      <c r="F79" s="384"/>
+      <c r="G79" s="384"/>
+      <c r="H79" s="384"/>
+      <c r="I79" s="384"/>
+      <c r="J79" s="384"/>
+      <c r="L79" s="133" t="s">
+        <v>90</v>
+      </c>
+      <c r="M79" s="116">
+        <v>100</v>
       </c>
       <c r="N79" s="11"/>
-      <c r="O79" s="372" t="s">
-        <v>459</v>
-      </c>
     </row>
     <row r="80" spans="2:15" ht="31" customHeight="1">
-      <c r="B80" s="379" t="s">
-        <v>257</v>
-      </c>
-      <c r="C80" s="394" t="s">
-        <v>353</v>
-      </c>
-      <c r="D80" s="394"/>
-      <c r="E80" s="383"/>
-      <c r="F80" s="383"/>
-      <c r="G80" s="383"/>
-      <c r="H80" s="383"/>
-      <c r="I80" s="383"/>
-      <c r="J80" s="383"/>
+      <c r="B80" s="379"/>
+      <c r="C80" s="395" t="s">
+        <v>354</v>
+      </c>
+      <c r="D80" s="395"/>
+      <c r="E80" s="384"/>
+      <c r="F80" s="384"/>
+      <c r="G80" s="384"/>
+      <c r="H80" s="384"/>
+      <c r="I80" s="384"/>
+      <c r="J80" s="384"/>
       <c r="L80" s="133" t="s">
-        <v>90</v>
-      </c>
-      <c r="M80" s="116">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="M80" s="174" t="s">
+        <v>107</v>
       </c>
       <c r="N80" s="11"/>
     </row>
     <row r="81" spans="2:14" ht="31" customHeight="1">
       <c r="B81" s="379"/>
-      <c r="C81" s="394" t="s">
-        <v>354</v>
-      </c>
-      <c r="D81" s="394"/>
-      <c r="E81" s="383"/>
-      <c r="F81" s="383"/>
-      <c r="G81" s="383"/>
-      <c r="H81" s="383"/>
-      <c r="I81" s="383"/>
-      <c r="J81" s="383"/>
+      <c r="C81" s="395" t="s">
+        <v>297</v>
+      </c>
+      <c r="D81" s="395"/>
+      <c r="E81" s="384"/>
+      <c r="F81" s="384"/>
+      <c r="G81" s="384"/>
+      <c r="H81" s="384"/>
+      <c r="I81" s="384"/>
+      <c r="J81" s="384"/>
       <c r="L81" s="133" t="s">
-        <v>97</v>
-      </c>
-      <c r="M81" s="174" t="s">
-        <v>107</v>
+        <v>596</v>
+      </c>
+      <c r="M81" s="116" t="s">
+        <v>99</v>
       </c>
       <c r="N81" s="11"/>
     </row>
     <row r="82" spans="2:14" ht="31" customHeight="1">
       <c r="B82" s="379"/>
-      <c r="C82" s="394" t="s">
-        <v>297</v>
-      </c>
-      <c r="D82" s="394"/>
-      <c r="E82" s="383"/>
-      <c r="F82" s="383"/>
-      <c r="G82" s="383"/>
-      <c r="H82" s="383"/>
-      <c r="I82" s="383"/>
-      <c r="J82" s="383"/>
+      <c r="C82" s="395" t="s">
+        <v>391</v>
+      </c>
+      <c r="D82" s="395"/>
+      <c r="E82" s="384"/>
+      <c r="F82" s="384"/>
+      <c r="G82" s="384"/>
+      <c r="H82" s="384"/>
+      <c r="I82" s="384"/>
+      <c r="J82" s="384"/>
       <c r="L82" s="133" t="s">
-        <v>596</v>
-      </c>
-      <c r="M82" s="116" t="s">
-        <v>99</v>
+        <v>91</v>
+      </c>
+      <c r="M82" s="138" t="s">
+        <v>595</v>
       </c>
       <c r="N82" s="11"/>
     </row>
     <row r="83" spans="2:14" ht="31" customHeight="1">
       <c r="B83" s="379"/>
-      <c r="C83" s="394" t="s">
-        <v>391</v>
-      </c>
-      <c r="D83" s="394"/>
-      <c r="E83" s="383"/>
-      <c r="F83" s="383"/>
-      <c r="G83" s="383"/>
-      <c r="H83" s="383"/>
-      <c r="I83" s="383"/>
-      <c r="J83" s="383"/>
+      <c r="C83" s="373" t="s">
+        <v>266</v>
+      </c>
+      <c r="D83" s="373"/>
+      <c r="E83" s="386" t="s">
+        <v>356</v>
+      </c>
+      <c r="F83" s="386"/>
+      <c r="G83" s="173" t="s">
+        <v>466</v>
+      </c>
+      <c r="H83" s="29" t="s">
+        <v>464</v>
+      </c>
+      <c r="I83" s="364"/>
+      <c r="J83" s="364"/>
       <c r="L83" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="M83" s="138" t="s">
-        <v>595</v>
+        <v>122</v>
+      </c>
+      <c r="M83" s="116" t="s">
+        <v>411</v>
       </c>
       <c r="N83" s="11"/>
     </row>
     <row r="84" spans="2:14" ht="31" customHeight="1">
       <c r="B84" s="379"/>
-      <c r="C84" s="373" t="s">
-        <v>266</v>
-      </c>
+      <c r="C84" s="373"/>
       <c r="D84" s="373"/>
-      <c r="E84" s="385" t="s">
-        <v>356</v>
-      </c>
-      <c r="F84" s="385"/>
+      <c r="E84" s="386" t="s">
+        <v>1</v>
+      </c>
+      <c r="F84" s="386"/>
       <c r="G84" s="173" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H84" s="29" t="s">
-        <v>464</v>
+        <v>444</v>
       </c>
       <c r="I84" s="364"/>
       <c r="J84" s="364"/>
@@ -8242,62 +8267,58 @@
     </row>
     <row r="85" spans="2:14" ht="31" customHeight="1">
       <c r="B85" s="379"/>
-      <c r="C85" s="373"/>
-      <c r="D85" s="373"/>
-      <c r="E85" s="385" t="s">
-        <v>1</v>
-      </c>
-      <c r="F85" s="385"/>
-      <c r="G85" s="173" t="s">
-        <v>465</v>
-      </c>
-      <c r="H85" s="29" t="s">
-        <v>444</v>
-      </c>
-      <c r="I85" s="364"/>
-      <c r="J85" s="364"/>
+      <c r="C85" s="395" t="s">
+        <v>479</v>
+      </c>
+      <c r="D85" s="395"/>
+      <c r="E85" s="386" t="s">
+        <v>388</v>
+      </c>
+      <c r="F85" s="386"/>
+      <c r="G85" s="409" t="s">
+        <v>301</v>
+      </c>
+      <c r="H85" s="410"/>
+      <c r="I85" s="88"/>
+      <c r="J85" s="88"/>
       <c r="L85" s="133" t="s">
-        <v>122</v>
-      </c>
-      <c r="M85" s="116" t="s">
-        <v>411</v>
+        <v>478</v>
+      </c>
+      <c r="M85" s="147" t="s">
+        <v>108</v>
       </c>
       <c r="N85" s="11"/>
     </row>
     <row r="86" spans="2:14" ht="31" customHeight="1">
       <c r="B86" s="379"/>
-      <c r="C86" s="394" t="s">
-        <v>479</v>
-      </c>
-      <c r="D86" s="394"/>
-      <c r="E86" s="385" t="s">
-        <v>388</v>
-      </c>
-      <c r="F86" s="385"/>
-      <c r="G86" s="410" t="s">
-        <v>301</v>
-      </c>
-      <c r="H86" s="411"/>
+      <c r="C86" s="395"/>
+      <c r="D86" s="395"/>
+      <c r="E86" s="386"/>
+      <c r="F86" s="386"/>
+      <c r="G86" s="409" t="s">
+        <v>268</v>
+      </c>
+      <c r="H86" s="410"/>
       <c r="I86" s="88"/>
       <c r="J86" s="88"/>
       <c r="L86" s="133" t="s">
-        <v>478</v>
-      </c>
-      <c r="M86" s="147" t="s">
-        <v>108</v>
+        <v>468</v>
+      </c>
+      <c r="M86" s="141" t="s">
+        <v>472</v>
       </c>
       <c r="N86" s="11"/>
     </row>
     <row r="87" spans="2:14" ht="31" customHeight="1">
       <c r="B87" s="379"/>
-      <c r="C87" s="394"/>
-      <c r="D87" s="394"/>
-      <c r="E87" s="385"/>
-      <c r="F87" s="385"/>
-      <c r="G87" s="410" t="s">
-        <v>268</v>
-      </c>
-      <c r="H87" s="411"/>
+      <c r="C87" s="395"/>
+      <c r="D87" s="395"/>
+      <c r="E87" s="386"/>
+      <c r="F87" s="386"/>
+      <c r="G87" s="409" t="s">
+        <v>261</v>
+      </c>
+      <c r="H87" s="410"/>
       <c r="I87" s="88"/>
       <c r="J87" s="88"/>
       <c r="L87" s="133" t="s">
@@ -8310,98 +8331,108 @@
     </row>
     <row r="88" spans="2:14" ht="31" customHeight="1">
       <c r="B88" s="379"/>
-      <c r="C88" s="394"/>
-      <c r="D88" s="394"/>
-      <c r="E88" s="385"/>
-      <c r="F88" s="385"/>
-      <c r="G88" s="410" t="s">
-        <v>261</v>
-      </c>
-      <c r="H88" s="411"/>
+      <c r="C88" s="395"/>
+      <c r="D88" s="395"/>
+      <c r="E88" s="386"/>
+      <c r="F88" s="386"/>
+      <c r="G88" s="409" t="s">
+        <v>269</v>
+      </c>
+      <c r="H88" s="410"/>
       <c r="I88" s="88"/>
       <c r="J88" s="88"/>
       <c r="L88" s="133" t="s">
-        <v>468</v>
-      </c>
-      <c r="M88" s="141" t="s">
-        <v>472</v>
+        <v>478</v>
+      </c>
+      <c r="M88" s="147" t="s">
+        <v>109</v>
       </c>
       <c r="N88" s="11"/>
     </row>
     <row r="89" spans="2:14" ht="31" customHeight="1">
       <c r="B89" s="379"/>
-      <c r="C89" s="394"/>
-      <c r="D89" s="394"/>
-      <c r="E89" s="385"/>
-      <c r="F89" s="385"/>
-      <c r="G89" s="410" t="s">
-        <v>269</v>
-      </c>
-      <c r="H89" s="411"/>
-      <c r="I89" s="88"/>
-      <c r="J89" s="88"/>
+      <c r="C89" s="395"/>
+      <c r="D89" s="395"/>
+      <c r="E89" s="386" t="s">
+        <v>516</v>
+      </c>
+      <c r="F89" s="386"/>
+      <c r="G89" s="384"/>
+      <c r="H89" s="384"/>
+      <c r="I89" s="384"/>
+      <c r="J89" s="384"/>
       <c r="L89" s="133" t="s">
-        <v>478</v>
-      </c>
-      <c r="M89" s="147" t="s">
-        <v>109</v>
+        <v>474</v>
+      </c>
+      <c r="M89" s="141" t="s">
+        <v>472</v>
       </c>
       <c r="N89" s="11"/>
     </row>
     <row r="90" spans="2:14" ht="31" customHeight="1">
       <c r="B90" s="379"/>
-      <c r="C90" s="394"/>
-      <c r="D90" s="394"/>
-      <c r="E90" s="385" t="s">
-        <v>516</v>
-      </c>
-      <c r="F90" s="385"/>
-      <c r="G90" s="383"/>
-      <c r="H90" s="383"/>
-      <c r="I90" s="383"/>
-      <c r="J90" s="383"/>
+      <c r="C90" s="395"/>
+      <c r="D90" s="395"/>
+      <c r="E90" s="386" t="s">
+        <v>422</v>
+      </c>
+      <c r="F90" s="386"/>
+      <c r="G90" s="384"/>
+      <c r="H90" s="384"/>
+      <c r="I90" s="384"/>
+      <c r="J90" s="384"/>
       <c r="L90" s="133" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="M90" s="141" t="s">
         <v>472</v>
       </c>
-      <c r="N90" s="11"/>
+      <c r="N90" s="116" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="91" spans="2:14" ht="31" customHeight="1">
       <c r="B91" s="379"/>
-      <c r="C91" s="394"/>
-      <c r="D91" s="394"/>
-      <c r="E91" s="385" t="s">
-        <v>422</v>
-      </c>
-      <c r="F91" s="385"/>
-      <c r="G91" s="383"/>
-      <c r="H91" s="383"/>
-      <c r="I91" s="383"/>
-      <c r="J91" s="383"/>
+      <c r="C91" s="395"/>
+      <c r="D91" s="395"/>
+      <c r="E91" s="386" t="s">
+        <v>505</v>
+      </c>
+      <c r="F91" s="386"/>
+      <c r="G91" s="384"/>
+      <c r="H91" s="384"/>
+      <c r="I91" s="384"/>
+      <c r="J91" s="384"/>
       <c r="L91" s="133" t="s">
-        <v>468</v>
+        <v>122</v>
       </c>
       <c r="M91" s="141" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="N91" s="116" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
     </row>
     <row r="92" spans="2:14" ht="31" customHeight="1">
       <c r="B92" s="379"/>
-      <c r="C92" s="394"/>
-      <c r="D92" s="394"/>
-      <c r="E92" s="385" t="s">
-        <v>505</v>
-      </c>
-      <c r="F92" s="385"/>
-      <c r="G92" s="383"/>
-      <c r="H92" s="383"/>
-      <c r="I92" s="383"/>
-      <c r="J92" s="383"/>
+      <c r="C92" s="395"/>
+      <c r="D92" s="395"/>
+      <c r="E92" s="386" t="s">
+        <v>501</v>
+      </c>
+      <c r="F92" s="386"/>
+      <c r="G92" s="393" t="s">
+        <v>269</v>
+      </c>
+      <c r="H92" s="394" t="s">
+        <v>455</v>
+      </c>
+      <c r="I92" s="368" t="s">
+        <v>484</v>
+      </c>
+      <c r="J92" s="392" t="s">
+        <v>477</v>
+      </c>
       <c r="L92" s="133" t="s">
         <v>122</v>
       </c>
@@ -8414,23 +8445,15 @@
     </row>
     <row r="93" spans="2:14" ht="31" customHeight="1">
       <c r="B93" s="379"/>
-      <c r="C93" s="394"/>
-      <c r="D93" s="394"/>
-      <c r="E93" s="385" t="s">
-        <v>501</v>
-      </c>
-      <c r="F93" s="385"/>
-      <c r="G93" s="392" t="s">
-        <v>269</v>
-      </c>
-      <c r="H93" s="393" t="s">
-        <v>455</v>
-      </c>
-      <c r="I93" s="368" t="s">
-        <v>484</v>
-      </c>
-      <c r="J93" s="391" t="s">
-        <v>477</v>
+      <c r="C93" s="395"/>
+      <c r="D93" s="395"/>
+      <c r="E93" s="386"/>
+      <c r="F93" s="386"/>
+      <c r="G93" s="393"/>
+      <c r="H93" s="394"/>
+      <c r="I93" s="369"/>
+      <c r="J93" s="392" t="s">
+        <v>482</v>
       </c>
       <c r="L93" s="133" t="s">
         <v>122</v>
@@ -8444,39 +8467,39 @@
     </row>
     <row r="94" spans="2:14" ht="31" customHeight="1">
       <c r="B94" s="379"/>
-      <c r="C94" s="394"/>
-      <c r="D94" s="394"/>
-      <c r="E94" s="385"/>
-      <c r="F94" s="385"/>
-      <c r="G94" s="392"/>
-      <c r="H94" s="393"/>
-      <c r="I94" s="369"/>
-      <c r="J94" s="391" t="s">
-        <v>482</v>
-      </c>
+      <c r="C94" s="395"/>
+      <c r="D94" s="395"/>
+      <c r="E94" s="411" t="s">
+        <v>483</v>
+      </c>
+      <c r="F94" s="412"/>
+      <c r="G94" s="367" t="s">
+        <v>269</v>
+      </c>
+      <c r="H94" s="47" t="s">
+        <v>455</v>
+      </c>
+      <c r="I94" s="364"/>
+      <c r="J94" s="364"/>
       <c r="L94" s="133" t="s">
-        <v>122</v>
+        <v>453</v>
       </c>
       <c r="M94" s="141" t="s">
         <v>473</v>
       </c>
-      <c r="N94" s="116" t="s">
-        <v>411</v>
-      </c>
+      <c r="N94" s="11"/>
     </row>
     <row r="95" spans="2:14" ht="31" customHeight="1">
       <c r="B95" s="379"/>
-      <c r="C95" s="394"/>
-      <c r="D95" s="394"/>
-      <c r="E95" s="412" t="s">
-        <v>483</v>
-      </c>
-      <c r="F95" s="413"/>
+      <c r="C95" s="395"/>
+      <c r="D95" s="395"/>
+      <c r="E95" s="419"/>
+      <c r="F95" s="420"/>
       <c r="G95" s="367" t="s">
         <v>269</v>
       </c>
       <c r="H95" s="47" t="s">
-        <v>455</v>
+        <v>599</v>
       </c>
       <c r="I95" s="364"/>
       <c r="J95" s="364"/>
@@ -8490,15 +8513,15 @@
     </row>
     <row r="96" spans="2:14" ht="31" customHeight="1">
       <c r="B96" s="379"/>
-      <c r="C96" s="394"/>
-      <c r="D96" s="394"/>
-      <c r="E96" s="420"/>
-      <c r="F96" s="421"/>
+      <c r="C96" s="395"/>
+      <c r="D96" s="395"/>
+      <c r="E96" s="419"/>
+      <c r="F96" s="420"/>
       <c r="G96" s="367" t="s">
         <v>269</v>
       </c>
       <c r="H96" s="47" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="I96" s="364"/>
       <c r="J96" s="364"/>
@@ -8511,143 +8534,143 @@
       <c r="N96" s="11"/>
     </row>
     <row r="97" spans="2:14" ht="31" customHeight="1">
-      <c r="B97" s="379"/>
-      <c r="C97" s="394"/>
-      <c r="D97" s="394"/>
-      <c r="E97" s="420"/>
-      <c r="F97" s="421"/>
-      <c r="G97" s="367" t="s">
-        <v>269</v>
-      </c>
-      <c r="H97" s="47" t="s">
-        <v>600</v>
-      </c>
-      <c r="I97" s="364"/>
-      <c r="J97" s="364"/>
+      <c r="B97" s="380" t="s">
+        <v>467</v>
+      </c>
+      <c r="C97" s="395" t="s">
+        <v>137</v>
+      </c>
+      <c r="D97" s="395"/>
+      <c r="E97" s="384"/>
+      <c r="F97" s="384"/>
+      <c r="G97" s="384"/>
+      <c r="H97" s="384"/>
+      <c r="I97" s="384"/>
+      <c r="J97" s="384"/>
       <c r="L97" s="133" t="s">
-        <v>453</v>
-      </c>
-      <c r="M97" s="141" t="s">
+        <v>97</v>
+      </c>
+      <c r="M97" s="147" t="s">
+        <v>129</v>
+      </c>
+      <c r="N97" s="11"/>
+    </row>
+    <row r="98" spans="2:14" ht="31" customHeight="1">
+      <c r="B98" s="380"/>
+      <c r="C98" s="395" t="s">
+        <v>283</v>
+      </c>
+      <c r="D98" s="395"/>
+      <c r="E98" s="384"/>
+      <c r="F98" s="384"/>
+      <c r="G98" s="384"/>
+      <c r="H98" s="384"/>
+      <c r="I98" s="384"/>
+      <c r="J98" s="384"/>
+      <c r="L98" s="133" t="s">
+        <v>468</v>
+      </c>
+      <c r="M98" s="138" t="s">
+        <v>469</v>
+      </c>
+      <c r="N98" s="11"/>
+    </row>
+    <row r="99" spans="2:14" ht="31" customHeight="1">
+      <c r="B99" s="380"/>
+      <c r="C99" s="395" t="s">
+        <v>306</v>
+      </c>
+      <c r="D99" s="395"/>
+      <c r="E99" s="386" t="s">
+        <v>470</v>
+      </c>
+      <c r="F99" s="386"/>
+      <c r="G99" s="384"/>
+      <c r="H99" s="384"/>
+      <c r="I99" s="384"/>
+      <c r="J99" s="384"/>
+      <c r="L99" s="133" t="s">
+        <v>474</v>
+      </c>
+      <c r="M99" s="141" t="s">
         <v>473</v>
       </c>
-      <c r="N97" s="11"/>
-    </row>
-    <row r="98" spans="2:14" ht="31" customHeight="1">
-      <c r="B98" s="397" t="s">
-        <v>467</v>
-      </c>
-      <c r="C98" s="394" t="s">
-        <v>137</v>
-      </c>
-      <c r="D98" s="394"/>
-      <c r="E98" s="383"/>
-      <c r="F98" s="383"/>
-      <c r="G98" s="383"/>
-      <c r="H98" s="383"/>
-      <c r="I98" s="383"/>
-      <c r="J98" s="383"/>
-      <c r="L98" s="133" t="s">
-        <v>97</v>
-      </c>
-      <c r="M98" s="147" t="s">
-        <v>129</v>
-      </c>
-      <c r="N98" s="11"/>
-    </row>
-    <row r="99" spans="2:14" ht="31" customHeight="1">
-      <c r="B99" s="397"/>
-      <c r="C99" s="394" t="s">
-        <v>283</v>
-      </c>
-      <c r="D99" s="394"/>
-      <c r="E99" s="383"/>
-      <c r="F99" s="383"/>
-      <c r="G99" s="383"/>
-      <c r="H99" s="383"/>
-      <c r="I99" s="383"/>
-      <c r="J99" s="383"/>
-      <c r="L99" s="133" t="s">
+      <c r="N99" s="11"/>
+    </row>
+    <row r="100" spans="2:14" ht="31" customHeight="1">
+      <c r="B100" s="380"/>
+      <c r="C100" s="395"/>
+      <c r="D100" s="395"/>
+      <c r="E100" s="386" t="s">
+        <v>471</v>
+      </c>
+      <c r="F100" s="386"/>
+      <c r="G100" s="384"/>
+      <c r="H100" s="384"/>
+      <c r="I100" s="384"/>
+      <c r="J100" s="384"/>
+      <c r="L100" s="133" t="s">
         <v>468</v>
       </c>
-      <c r="M99" s="138" t="s">
-        <v>469</v>
-      </c>
-      <c r="N99" s="11"/>
-    </row>
-    <row r="100" spans="2:14" ht="31" customHeight="1">
-      <c r="B100" s="397"/>
-      <c r="C100" s="394" t="s">
-        <v>306</v>
-      </c>
-      <c r="D100" s="394"/>
-      <c r="E100" s="385" t="s">
-        <v>470</v>
-      </c>
-      <c r="F100" s="385"/>
-      <c r="G100" s="383"/>
-      <c r="H100" s="383"/>
-      <c r="I100" s="383"/>
-      <c r="J100" s="383"/>
-      <c r="L100" s="133" t="s">
+      <c r="M100" s="141" t="s">
+        <v>472</v>
+      </c>
+      <c r="N100" s="11"/>
+    </row>
+    <row r="101" spans="2:14" ht="31" customHeight="1">
+      <c r="B101" s="380"/>
+      <c r="C101" s="395" t="s">
+        <v>28</v>
+      </c>
+      <c r="D101" s="395"/>
+      <c r="E101" s="384"/>
+      <c r="F101" s="384"/>
+      <c r="G101" s="384"/>
+      <c r="H101" s="384"/>
+      <c r="I101" s="384"/>
+      <c r="J101" s="384"/>
+      <c r="L101" s="133" t="s">
         <v>474</v>
       </c>
-      <c r="M100" s="141" t="s">
+      <c r="M101" s="141" t="s">
         <v>473</v>
       </c>
-      <c r="N100" s="11"/>
-    </row>
-    <row r="101" spans="2:14" ht="31" customHeight="1">
-      <c r="B101" s="397"/>
-      <c r="C101" s="394"/>
-      <c r="D101" s="394"/>
-      <c r="E101" s="385" t="s">
-        <v>471</v>
-      </c>
-      <c r="F101" s="385"/>
-      <c r="G101" s="383"/>
-      <c r="H101" s="383"/>
-      <c r="I101" s="383"/>
-      <c r="J101" s="383"/>
-      <c r="L101" s="133" t="s">
-        <v>468</v>
-      </c>
-      <c r="M101" s="141" t="s">
-        <v>472</v>
-      </c>
       <c r="N101" s="11"/>
     </row>
     <row r="102" spans="2:14" ht="31" customHeight="1">
-      <c r="B102" s="397"/>
-      <c r="C102" s="394" t="s">
-        <v>28</v>
-      </c>
-      <c r="D102" s="394"/>
-      <c r="E102" s="383"/>
-      <c r="F102" s="383"/>
-      <c r="G102" s="383"/>
-      <c r="H102" s="383"/>
-      <c r="I102" s="383"/>
-      <c r="J102" s="383"/>
+      <c r="B102" s="380"/>
+      <c r="C102" s="395" t="s">
+        <v>386</v>
+      </c>
+      <c r="D102" s="395"/>
+      <c r="E102" s="384"/>
+      <c r="F102" s="384"/>
+      <c r="G102" s="384"/>
+      <c r="H102" s="384"/>
+      <c r="I102" s="384"/>
+      <c r="J102" s="384"/>
       <c r="L102" s="133" t="s">
-        <v>474</v>
-      </c>
-      <c r="M102" s="141" t="s">
-        <v>473</v>
+        <v>122</v>
+      </c>
+      <c r="M102" s="116" t="b">
+        <v>1</v>
       </c>
       <c r="N102" s="11"/>
     </row>
     <row r="103" spans="2:14" ht="31" customHeight="1">
-      <c r="B103" s="397"/>
-      <c r="C103" s="394" t="s">
-        <v>386</v>
-      </c>
-      <c r="D103" s="394"/>
-      <c r="E103" s="383"/>
-      <c r="F103" s="383"/>
-      <c r="G103" s="383"/>
-      <c r="H103" s="383"/>
-      <c r="I103" s="383"/>
-      <c r="J103" s="383"/>
+      <c r="B103" s="380"/>
+      <c r="C103" s="395" t="s">
+        <v>305</v>
+      </c>
+      <c r="D103" s="395"/>
+      <c r="E103" s="386" t="s">
+        <v>384</v>
+      </c>
+      <c r="F103" s="386"/>
+      <c r="G103" s="384"/>
+      <c r="H103" s="384"/>
+      <c r="I103" s="384"/>
+      <c r="J103" s="384"/>
       <c r="L103" s="133" t="s">
         <v>122</v>
       </c>
@@ -8657,37 +8680,35 @@
       <c r="N103" s="11"/>
     </row>
     <row r="104" spans="2:14" ht="31" customHeight="1">
-      <c r="B104" s="397"/>
-      <c r="C104" s="394" t="s">
-        <v>305</v>
-      </c>
-      <c r="D104" s="394"/>
-      <c r="E104" s="385" t="s">
-        <v>384</v>
-      </c>
-      <c r="F104" s="385"/>
-      <c r="G104" s="383"/>
-      <c r="H104" s="383"/>
-      <c r="I104" s="383"/>
-      <c r="J104" s="383"/>
+      <c r="B104" s="380"/>
+      <c r="C104" s="395"/>
+      <c r="D104" s="395"/>
+      <c r="E104" s="386" t="s">
+        <v>385</v>
+      </c>
+      <c r="F104" s="386"/>
+      <c r="G104" s="249">
+        <v>1</v>
+      </c>
+      <c r="H104" s="249"/>
+      <c r="I104" s="364"/>
+      <c r="J104" s="364"/>
       <c r="L104" s="133" t="s">
-        <v>122</v>
-      </c>
-      <c r="M104" s="116" t="b">
-        <v>1</v>
+        <v>475</v>
+      </c>
+      <c r="M104" s="141" t="s">
+        <v>460</v>
       </c>
       <c r="N104" s="11"/>
     </row>
     <row r="105" spans="2:14" ht="31" customHeight="1">
-      <c r="B105" s="397"/>
-      <c r="C105" s="394"/>
-      <c r="D105" s="394"/>
-      <c r="E105" s="385" t="s">
-        <v>385</v>
-      </c>
-      <c r="F105" s="385"/>
+      <c r="B105" s="380"/>
+      <c r="C105" s="395"/>
+      <c r="D105" s="395"/>
+      <c r="E105" s="386"/>
+      <c r="F105" s="386"/>
       <c r="G105" s="249">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H105" s="249"/>
       <c r="I105" s="364"/>
@@ -8701,13 +8722,13 @@
       <c r="N105" s="11"/>
     </row>
     <row r="106" spans="2:14" ht="31" customHeight="1">
-      <c r="B106" s="397"/>
-      <c r="C106" s="394"/>
-      <c r="D106" s="394"/>
-      <c r="E106" s="385"/>
-      <c r="F106" s="385"/>
+      <c r="B106" s="380"/>
+      <c r="C106" s="395"/>
+      <c r="D106" s="395"/>
+      <c r="E106" s="386"/>
+      <c r="F106" s="386"/>
       <c r="G106" s="249">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H106" s="249"/>
       <c r="I106" s="364"/>
@@ -8721,13 +8742,13 @@
       <c r="N106" s="11"/>
     </row>
     <row r="107" spans="2:14" ht="31" customHeight="1">
-      <c r="B107" s="397"/>
-      <c r="C107" s="394"/>
-      <c r="D107" s="394"/>
-      <c r="E107" s="385"/>
-      <c r="F107" s="385"/>
+      <c r="B107" s="380"/>
+      <c r="C107" s="395"/>
+      <c r="D107" s="395"/>
+      <c r="E107" s="386"/>
+      <c r="F107" s="386"/>
       <c r="G107" s="249">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H107" s="249"/>
       <c r="I107" s="364"/>
@@ -8741,287 +8762,273 @@
       <c r="N107" s="11"/>
     </row>
     <row r="108" spans="2:14" ht="31" customHeight="1">
-      <c r="B108" s="397"/>
-      <c r="C108" s="394"/>
-      <c r="D108" s="394"/>
-      <c r="E108" s="385"/>
-      <c r="F108" s="385"/>
-      <c r="G108" s="249">
-        <v>4</v>
-      </c>
-      <c r="H108" s="249"/>
-      <c r="I108" s="364"/>
-      <c r="J108" s="364"/>
+      <c r="B108" s="380"/>
+      <c r="C108" s="395" t="s">
+        <v>307</v>
+      </c>
+      <c r="D108" s="395"/>
+      <c r="E108" s="386" t="s">
+        <v>308</v>
+      </c>
+      <c r="F108" s="386"/>
+      <c r="G108" s="384"/>
+      <c r="H108" s="384"/>
+      <c r="I108" s="384"/>
+      <c r="J108" s="384"/>
       <c r="L108" s="133" t="s">
+        <v>90</v>
+      </c>
+      <c r="M108" s="116">
+        <v>0</v>
+      </c>
+      <c r="N108" s="11"/>
+    </row>
+    <row r="109" spans="2:14" ht="31" customHeight="1">
+      <c r="B109" s="380"/>
+      <c r="C109" s="395"/>
+      <c r="D109" s="395"/>
+      <c r="E109" s="386" t="s">
+        <v>309</v>
+      </c>
+      <c r="F109" s="386"/>
+      <c r="G109" s="384"/>
+      <c r="H109" s="384"/>
+      <c r="I109" s="384"/>
+      <c r="J109" s="384"/>
+      <c r="L109" s="133" t="s">
         <v>475</v>
       </c>
-      <c r="M108" s="141" t="s">
+      <c r="M109" s="141" t="s">
         <v>460</v>
       </c>
-      <c r="N108" s="11"/>
-    </row>
-    <row r="109" spans="2:14" ht="31" customHeight="1">
-      <c r="B109" s="397"/>
-      <c r="C109" s="394" t="s">
-        <v>307</v>
-      </c>
-      <c r="D109" s="394"/>
-      <c r="E109" s="385" t="s">
-        <v>308</v>
-      </c>
-      <c r="F109" s="385"/>
-      <c r="G109" s="383"/>
-      <c r="H109" s="383"/>
-      <c r="I109" s="383"/>
-      <c r="J109" s="383"/>
-      <c r="L109" s="133" t="s">
-        <v>90</v>
-      </c>
-      <c r="M109" s="116">
-        <v>0</v>
-      </c>
       <c r="N109" s="11"/>
     </row>
-    <row r="110" spans="2:14" ht="31" customHeight="1">
-      <c r="B110" s="397"/>
-      <c r="C110" s="394"/>
-      <c r="D110" s="394"/>
-      <c r="E110" s="385" t="s">
-        <v>309</v>
-      </c>
-      <c r="F110" s="385"/>
-      <c r="G110" s="383"/>
-      <c r="H110" s="383"/>
-      <c r="I110" s="383"/>
-      <c r="J110" s="383"/>
-      <c r="L110" s="133" t="s">
-        <v>475</v>
-      </c>
-      <c r="M110" s="141" t="s">
-        <v>460</v>
-      </c>
-      <c r="N110" s="11"/>
+    <row r="110" spans="2:14" ht="26">
+      <c r="B110" s="381"/>
+      <c r="C110" s="396"/>
     </row>
     <row r="111" spans="2:14" ht="26">
-      <c r="B111" s="380"/>
-      <c r="C111" s="395"/>
-    </row>
-    <row r="112" spans="2:14" ht="26">
-      <c r="B112" s="380"/>
-      <c r="C112" s="395"/>
+      <c r="B111" s="381"/>
+      <c r="C111" s="396"/>
     </row>
   </sheetData>
-  <mergeCells count="210">
-    <mergeCell ref="B6:B15"/>
+  <mergeCells count="216">
+    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="B39:B54"/>
+    <mergeCell ref="B6:B14"/>
+    <mergeCell ref="C9:D14"/>
+    <mergeCell ref="B24:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="I95:J95"/>
     <mergeCell ref="I96:J96"/>
-    <mergeCell ref="I97:J97"/>
-    <mergeCell ref="G64:H66"/>
+    <mergeCell ref="G63:H65"/>
+    <mergeCell ref="I63:J63"/>
     <mergeCell ref="I64:J64"/>
     <mergeCell ref="I65:J65"/>
-    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="G85:H85"/>
     <mergeCell ref="G86:H86"/>
     <mergeCell ref="G87:H87"/>
-    <mergeCell ref="G88:H88"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I32:J32"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="E70:E73"/>
-    <mergeCell ref="F70:F73"/>
+    <mergeCell ref="E69:E72"/>
+    <mergeCell ref="F69:F72"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="I69:J69"/>
     <mergeCell ref="G70:H70"/>
     <mergeCell ref="I70:J70"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="G72:H73"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I68:I69"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="G71:H72"/>
+    <mergeCell ref="I50:J50"/>
     <mergeCell ref="I49:J49"/>
     <mergeCell ref="I48:J48"/>
     <mergeCell ref="I47:J47"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I67:I68"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="I45:J45"/>
     <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="I51:J51"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I93:I94"/>
+    <mergeCell ref="I92:I93"/>
+    <mergeCell ref="I104:J104"/>
     <mergeCell ref="I105:J105"/>
     <mergeCell ref="I106:J106"/>
+    <mergeCell ref="I83:J83"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="G103:J103"/>
+    <mergeCell ref="C62:D72"/>
+    <mergeCell ref="E62:E68"/>
+    <mergeCell ref="F62:F68"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="G108:J108"/>
+    <mergeCell ref="G109:J109"/>
+    <mergeCell ref="G100:J100"/>
     <mergeCell ref="I107:J107"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="I85:J85"/>
-    <mergeCell ref="I77:J77"/>
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="G104:J104"/>
-    <mergeCell ref="C63:D73"/>
-    <mergeCell ref="E63:E69"/>
-    <mergeCell ref="F63:F69"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="G109:J109"/>
-    <mergeCell ref="G110:J110"/>
-    <mergeCell ref="G101:J101"/>
-    <mergeCell ref="I108:J108"/>
-    <mergeCell ref="E100:F100"/>
-    <mergeCell ref="G108:H108"/>
+    <mergeCell ref="E99:F99"/>
     <mergeCell ref="G107:H107"/>
     <mergeCell ref="G106:H106"/>
     <mergeCell ref="G105:H105"/>
+    <mergeCell ref="G104:H104"/>
+    <mergeCell ref="E97:J97"/>
     <mergeCell ref="E98:J98"/>
-    <mergeCell ref="E99:J99"/>
+    <mergeCell ref="E101:J101"/>
     <mergeCell ref="E102:J102"/>
-    <mergeCell ref="E103:J103"/>
-    <mergeCell ref="C109:D110"/>
+    <mergeCell ref="C108:D109"/>
+    <mergeCell ref="E108:F108"/>
     <mergeCell ref="E109:F109"/>
-    <mergeCell ref="E110:F110"/>
-    <mergeCell ref="E105:F108"/>
-    <mergeCell ref="E104:F104"/>
-    <mergeCell ref="E101:F101"/>
-    <mergeCell ref="C100:D101"/>
-    <mergeCell ref="C104:D108"/>
+    <mergeCell ref="E104:F107"/>
+    <mergeCell ref="E103:F103"/>
+    <mergeCell ref="E100:F100"/>
+    <mergeCell ref="C99:D100"/>
+    <mergeCell ref="C103:D107"/>
+    <mergeCell ref="C97:D97"/>
     <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C103:D103"/>
     <mergeCell ref="C102:D102"/>
-    <mergeCell ref="G93:G94"/>
-    <mergeCell ref="H93:H94"/>
-    <mergeCell ref="G100:J100"/>
-    <mergeCell ref="I95:J95"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="G92:G93"/>
+    <mergeCell ref="H92:H93"/>
+    <mergeCell ref="G99:J99"/>
+    <mergeCell ref="I94:J94"/>
+    <mergeCell ref="E81:J81"/>
     <mergeCell ref="E82:J82"/>
-    <mergeCell ref="E83:J83"/>
+    <mergeCell ref="E79:J79"/>
     <mergeCell ref="E80:J80"/>
-    <mergeCell ref="E81:J81"/>
-    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="G88:H88"/>
+    <mergeCell ref="G89:J89"/>
     <mergeCell ref="G90:J90"/>
     <mergeCell ref="G91:J91"/>
-    <mergeCell ref="G92:J92"/>
-    <mergeCell ref="C86:D97"/>
-    <mergeCell ref="E86:F89"/>
-    <mergeCell ref="E93:F94"/>
+    <mergeCell ref="C85:D96"/>
+    <mergeCell ref="E85:F88"/>
+    <mergeCell ref="E92:F93"/>
+    <mergeCell ref="E89:F89"/>
     <mergeCell ref="E90:F90"/>
     <mergeCell ref="E91:F91"/>
-    <mergeCell ref="E92:F92"/>
-    <mergeCell ref="E95:F97"/>
+    <mergeCell ref="E94:F96"/>
+    <mergeCell ref="C79:D79"/>
     <mergeCell ref="C80:D80"/>
     <mergeCell ref="C81:D81"/>
     <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D85"/>
-    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="C83:D84"/>
     <mergeCell ref="E84:F84"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="G60:J60"/>
     <mergeCell ref="G61:J61"/>
-    <mergeCell ref="G62:J62"/>
+    <mergeCell ref="G74:J74"/>
     <mergeCell ref="G75:J75"/>
-    <mergeCell ref="G76:J76"/>
+    <mergeCell ref="G77:J77"/>
     <mergeCell ref="G78:J78"/>
-    <mergeCell ref="G79:J79"/>
-    <mergeCell ref="E74:J74"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="I72:I73"/>
+    <mergeCell ref="E73:J73"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="I71:I72"/>
+    <mergeCell ref="E74:F74"/>
     <mergeCell ref="E75:F75"/>
     <mergeCell ref="E76:F76"/>
     <mergeCell ref="E77:F77"/>
     <mergeCell ref="E78:F78"/>
-    <mergeCell ref="E79:F79"/>
-    <mergeCell ref="G68:H69"/>
-    <mergeCell ref="C75:D79"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="G67:H68"/>
+    <mergeCell ref="C74:D78"/>
+    <mergeCell ref="C73:D73"/>
     <mergeCell ref="C61:D61"/>
-    <mergeCell ref="E51:J51"/>
-    <mergeCell ref="E50:J50"/>
-    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E24:J24"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:J55"/>
     <mergeCell ref="E56:J56"/>
     <mergeCell ref="E57:J57"/>
-    <mergeCell ref="E58:J58"/>
+    <mergeCell ref="G21:J21"/>
     <mergeCell ref="G22:J22"/>
     <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="E52:J52"/>
-    <mergeCell ref="E53:J53"/>
-    <mergeCell ref="E54:J54"/>
-    <mergeCell ref="E55:J55"/>
-    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G15:J15"/>
     <mergeCell ref="G16:J16"/>
     <mergeCell ref="G17:J17"/>
     <mergeCell ref="G18:J18"/>
     <mergeCell ref="G19:J19"/>
     <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="C50:C55"/>
-    <mergeCell ref="C16:D20"/>
-    <mergeCell ref="C21:D24"/>
-    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C15:D19"/>
+    <mergeCell ref="C20:D23"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G37:J37"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="G38:G49"/>
-    <mergeCell ref="H42:H45"/>
-    <mergeCell ref="H46:H49"/>
-    <mergeCell ref="E38:E49"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="F38:F49"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="G41:J41"/>
+    <mergeCell ref="G39:J39"/>
+    <mergeCell ref="G40:J40"/>
+    <mergeCell ref="G43:G54"/>
+    <mergeCell ref="H47:H50"/>
+    <mergeCell ref="H51:H54"/>
+    <mergeCell ref="E43:E54"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="F43:F54"/>
+    <mergeCell ref="G10:J10"/>
     <mergeCell ref="G11:J11"/>
     <mergeCell ref="G12:J12"/>
     <mergeCell ref="G13:J13"/>
     <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G30:J30"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G27:G33"/>
-    <mergeCell ref="H29:H33"/>
+    <mergeCell ref="G32:G38"/>
+    <mergeCell ref="H34:H38"/>
     <mergeCell ref="E6:J6"/>
     <mergeCell ref="E7:J7"/>
     <mergeCell ref="E8:J8"/>
     <mergeCell ref="G9:J9"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="D34:D49"/>
+    <mergeCell ref="D39:D54"/>
+    <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C9:D15"/>
-    <mergeCell ref="C25:C49"/>
-    <mergeCell ref="D25:D33"/>
-    <mergeCell ref="B80:B97"/>
-    <mergeCell ref="B98:B110"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B61:B79"/>
-    <mergeCell ref="B16:B24"/>
-    <mergeCell ref="F27:F33"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:E33"/>
-    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="C30:C54"/>
+    <mergeCell ref="D30:D38"/>
+    <mergeCell ref="B79:B96"/>
+    <mergeCell ref="B97:B109"/>
+    <mergeCell ref="B55:B59"/>
+    <mergeCell ref="B60:B78"/>
+    <mergeCell ref="B15:B23"/>
+    <mergeCell ref="F32:F38"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:E38"/>
+    <mergeCell ref="G31:J31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
a lot of refactoring with the users and making the scope more logical and the login and logout fucntions more succinct. Also fixed the down days which needed an int instead of a float
</commit_message>
<xml_diff>
--- a/docs/session_variables.xlsx
+++ b/docs/session_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robhay/git_repo/share_screener/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B883212-BEAC-9746-8CC5-28B6F77B0891}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A1CDAB-16B4-D442-8FC8-D4D11E709CED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68800" yWindow="-15420" windowWidth="68800" windowHeight="28300" xr2:uid="{EB3C945B-FE01-FA47-AE59-A0DC3CDF521B}"/>
+    <workbookView xWindow="-68800" yWindow="-15420" windowWidth="33180" windowHeight="28300" xr2:uid="{EB3C945B-FE01-FA47-AE59-A0DC3CDF521B}"/>
   </bookViews>
   <sheets>
     <sheet name="Application Structure (2)" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2282" uniqueCount="701">
   <si>
     <t>chart_colours</t>
   </si>
@@ -2490,9 +2490,6 @@
     <t>auto login</t>
   </si>
   <si>
-    <t>rename to app current work list of something</t>
-  </si>
-  <si>
     <t>chart_confg</t>
   </si>
   <si>
@@ -2508,21 +2505,6 @@
     <t>selected_tickers</t>
   </si>
   <si>
-    <t>the function that caches the df for the page should update this list as well</t>
-  </si>
-  <si>
-    <t>loaded_tickers</t>
-  </si>
-  <si>
-    <t>tap</t>
-  </si>
-  <si>
-    <t>exploit</t>
-  </si>
-  <si>
-    <t>wip_tickers</t>
-  </si>
-  <si>
     <t>mined_tickers</t>
   </si>
   <si>
@@ -2533,6 +2515,27 @@
   </si>
   <si>
     <t>place to cache the search results</t>
+  </si>
+  <si>
+    <t>complete list of all available trials - will not mutate</t>
+  </si>
+  <si>
+    <t>trials that are currently active</t>
+  </si>
+  <si>
+    <t>active list</t>
+  </si>
+  <si>
+    <t>trials that add columns</t>
+  </si>
+  <si>
+    <t>complete list of all available charts - will not mutate</t>
+  </si>
+  <si>
+    <t>charts that add columns</t>
+  </si>
+  <si>
+    <t>charts that are currently active</t>
   </si>
 </sst>
 </file>
@@ -2546,7 +2549,7 @@
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="66">
+  <fonts count="67">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3015,6 +3018,13 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFA6A6A6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="20">
     <fill>
@@ -3326,7 +3336,7 @@
     <xf numFmtId="43" fontId="43" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="43" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="490">
+  <cellXfs count="493">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4675,11 +4685,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4997,13 +5016,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4BE9BCD-FFB7-0845-95F9-377ADF3DB526}">
-  <dimension ref="A1:AB108"/>
+  <dimension ref="A1:X110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G82" sqref="G82:L82"/>
+      <selection pane="bottomRight" activeCell="G47" sqref="G47:L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -5070,7 +5089,7 @@
     </row>
     <row r="3" spans="1:24" s="6" customFormat="1" ht="44">
       <c r="B3" s="486" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D3" s="174" t="s">
         <v>343</v>
@@ -5766,7 +5785,7 @@
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="465" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E31" s="466" t="s">
         <v>431</v>
@@ -5797,12 +5816,14 @@
         <v>614</v>
       </c>
       <c r="F32" s="466"/>
-      <c r="G32" s="256"/>
-      <c r="H32" s="256"/>
-      <c r="I32" s="256"/>
-      <c r="J32" s="256"/>
-      <c r="K32" s="256"/>
-      <c r="L32" s="256"/>
+      <c r="G32" s="489" t="s">
+        <v>694</v>
+      </c>
+      <c r="H32" s="489"/>
+      <c r="I32" s="489"/>
+      <c r="J32" s="489"/>
+      <c r="K32" s="489"/>
+      <c r="L32" s="489"/>
       <c r="M32" s="225"/>
       <c r="N32" s="225"/>
       <c r="O32" s="6"/>
@@ -5822,12 +5843,14 @@
         <v>675</v>
       </c>
       <c r="F33" s="466"/>
-      <c r="G33" s="256"/>
-      <c r="H33" s="256"/>
-      <c r="I33" s="256"/>
-      <c r="J33" s="256"/>
-      <c r="K33" s="256"/>
-      <c r="L33" s="256"/>
+      <c r="G33" s="489" t="s">
+        <v>697</v>
+      </c>
+      <c r="H33" s="489"/>
+      <c r="I33" s="489"/>
+      <c r="J33" s="489"/>
+      <c r="K33" s="489"/>
+      <c r="L33" s="489"/>
       <c r="M33" s="225"/>
       <c r="N33" s="225"/>
       <c r="O33" s="6"/>
@@ -5842,42 +5865,44 @@
     <row r="34" spans="2:18" ht="31" customHeight="1">
       <c r="B34" s="485"/>
       <c r="C34" s="6"/>
-      <c r="D34" s="465" t="s">
-        <v>613</v>
-      </c>
-      <c r="E34" s="257" t="s">
-        <v>688</v>
-      </c>
-      <c r="F34" s="258" t="s">
-        <v>445</v>
-      </c>
-      <c r="G34" s="247" t="s">
-        <v>136</v>
-      </c>
-      <c r="H34" s="248"/>
-      <c r="I34" s="233"/>
-      <c r="J34" s="233"/>
-      <c r="K34" s="233"/>
-      <c r="L34" s="233"/>
+      <c r="D34" s="465"/>
+      <c r="E34" s="466" t="s">
+        <v>696</v>
+      </c>
+      <c r="F34" s="466"/>
+      <c r="G34" s="490" t="s">
+        <v>695</v>
+      </c>
+      <c r="H34" s="491"/>
+      <c r="I34" s="491"/>
+      <c r="J34" s="491"/>
+      <c r="K34" s="491"/>
+      <c r="L34" s="492"/>
       <c r="M34" s="225"/>
       <c r="N34" s="225"/>
       <c r="O34" s="6"/>
       <c r="P34" s="133" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q34" s="116" t="s">
-        <v>411</v>
+        <v>91</v>
+      </c>
+      <c r="Q34" s="138" t="s">
+        <v>592</v>
       </c>
       <c r="R34" s="11"/>
     </row>
     <row r="35" spans="2:18" ht="31" customHeight="1">
       <c r="B35" s="485"/>
       <c r="C35" s="6"/>
-      <c r="D35" s="465"/>
-      <c r="E35" s="257"/>
-      <c r="F35" s="258"/>
+      <c r="D35" s="465" t="s">
+        <v>613</v>
+      </c>
+      <c r="E35" s="257" t="s">
+        <v>687</v>
+      </c>
+      <c r="F35" s="258" t="s">
+        <v>445</v>
+      </c>
       <c r="G35" s="247" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H35" s="248"/>
       <c r="I35" s="233"/>
@@ -5888,12 +5913,12 @@
       <c r="N35" s="225"/>
       <c r="O35" s="6"/>
       <c r="P35" s="133" t="s">
-        <v>434</v>
-      </c>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="173" t="s">
-        <v>436</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="Q35" s="116" t="s">
+        <v>411</v>
+      </c>
+      <c r="R35" s="11"/>
     </row>
     <row r="36" spans="2:18" ht="31" customHeight="1">
       <c r="B36" s="485"/>
@@ -5901,25 +5926,23 @@
       <c r="D36" s="465"/>
       <c r="E36" s="257"/>
       <c r="F36" s="258"/>
-      <c r="G36" s="237" t="s">
-        <v>426</v>
-      </c>
-      <c r="H36" s="238"/>
-      <c r="I36" s="247" t="s">
-        <v>141</v>
-      </c>
-      <c r="J36" s="248"/>
-      <c r="K36" s="483"/>
-      <c r="L36" s="484"/>
+      <c r="G36" s="247" t="s">
+        <v>137</v>
+      </c>
+      <c r="H36" s="248"/>
+      <c r="I36" s="233"/>
+      <c r="J36" s="233"/>
+      <c r="K36" s="233"/>
+      <c r="L36" s="233"/>
       <c r="M36" s="225"/>
       <c r="N36" s="225"/>
       <c r="O36" s="6"/>
       <c r="P36" s="133" t="s">
-        <v>141</v>
+        <v>434</v>
       </c>
       <c r="Q36" s="11"/>
-      <c r="R36" s="141" t="s">
-        <v>244</v>
+      <c r="R36" s="173" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="37" spans="2:18" ht="31" customHeight="1">
@@ -5928,23 +5951,25 @@
       <c r="D37" s="465"/>
       <c r="E37" s="257"/>
       <c r="F37" s="258"/>
-      <c r="G37" s="239"/>
-      <c r="H37" s="240"/>
-      <c r="I37" s="250" t="s">
-        <v>146</v>
-      </c>
-      <c r="J37" s="251"/>
+      <c r="G37" s="237" t="s">
+        <v>426</v>
+      </c>
+      <c r="H37" s="238"/>
+      <c r="I37" s="247" t="s">
+        <v>141</v>
+      </c>
+      <c r="J37" s="248"/>
       <c r="K37" s="483"/>
       <c r="L37" s="484"/>
       <c r="M37" s="225"/>
       <c r="N37" s="225"/>
       <c r="O37" s="6"/>
       <c r="P37" s="133" t="s">
-        <v>434</v>
+        <v>141</v>
       </c>
       <c r="Q37" s="11"/>
-      <c r="R37" s="173" t="s">
-        <v>245</v>
+      <c r="R37" s="141" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="38" spans="2:18" ht="31" customHeight="1">
@@ -5956,7 +5981,7 @@
       <c r="G38" s="239"/>
       <c r="H38" s="240"/>
       <c r="I38" s="250" t="s">
-        <v>408</v>
+        <v>146</v>
       </c>
       <c r="J38" s="251"/>
       <c r="K38" s="483"/>
@@ -5969,7 +5994,7 @@
       </c>
       <c r="Q38" s="11"/>
       <c r="R38" s="173" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="2:18" ht="31" customHeight="1">
@@ -5981,7 +6006,7 @@
       <c r="G39" s="239"/>
       <c r="H39" s="240"/>
       <c r="I39" s="250" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J39" s="251"/>
       <c r="K39" s="483"/>
@@ -5990,11 +6015,11 @@
       <c r="N39" s="225"/>
       <c r="O39" s="6"/>
       <c r="P39" s="133" t="s">
-        <v>90</v>
+        <v>434</v>
       </c>
       <c r="Q39" s="11"/>
-      <c r="R39" s="68">
-        <v>4</v>
+      <c r="R39" s="173" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="2:18" ht="31" customHeight="1">
@@ -6003,10 +6028,10 @@
       <c r="D40" s="465"/>
       <c r="E40" s="257"/>
       <c r="F40" s="258"/>
-      <c r="G40" s="241"/>
-      <c r="H40" s="242"/>
+      <c r="G40" s="239"/>
+      <c r="H40" s="240"/>
       <c r="I40" s="250" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J40" s="251"/>
       <c r="K40" s="483"/>
@@ -6019,44 +6044,44 @@
       </c>
       <c r="Q40" s="11"/>
       <c r="R40" s="68">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="2:18" ht="31" customHeight="1">
-      <c r="B41" s="485" t="s">
-        <v>607</v>
-      </c>
+      <c r="B41" s="485"/>
       <c r="C41" s="6"/>
-      <c r="D41" s="465" t="s">
-        <v>686</v>
-      </c>
-      <c r="E41" s="246" t="s">
-        <v>507</v>
-      </c>
-      <c r="F41" s="246"/>
-      <c r="G41" s="256"/>
-      <c r="H41" s="256"/>
-      <c r="I41" s="256"/>
-      <c r="J41" s="256"/>
-      <c r="K41" s="256"/>
-      <c r="L41" s="256"/>
+      <c r="D41" s="465"/>
+      <c r="E41" s="257"/>
+      <c r="F41" s="258"/>
+      <c r="G41" s="241"/>
+      <c r="H41" s="242"/>
+      <c r="I41" s="250" t="s">
+        <v>410</v>
+      </c>
+      <c r="J41" s="251"/>
+      <c r="K41" s="483"/>
+      <c r="L41" s="484"/>
       <c r="M41" s="225"/>
       <c r="N41" s="225"/>
       <c r="O41" s="6"/>
       <c r="P41" s="133" t="s">
         <v>90</v>
       </c>
-      <c r="Q41" s="116">
-        <v>500</v>
-      </c>
-      <c r="R41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="68">
+        <v>10</v>
+      </c>
     </row>
     <row r="42" spans="2:18" ht="31" customHeight="1">
-      <c r="B42" s="485"/>
+      <c r="B42" s="485" t="s">
+        <v>607</v>
+      </c>
       <c r="C42" s="6"/>
-      <c r="D42" s="465"/>
+      <c r="D42" s="465" t="s">
+        <v>685</v>
+      </c>
       <c r="E42" s="246" t="s">
-        <v>279</v>
+        <v>507</v>
       </c>
       <c r="F42" s="246"/>
       <c r="G42" s="256"/>
@@ -6081,7 +6106,7 @@
       <c r="C43" s="6"/>
       <c r="D43" s="465"/>
       <c r="E43" s="246" t="s">
-        <v>379</v>
+        <v>279</v>
       </c>
       <c r="F43" s="246"/>
       <c r="G43" s="256"/>
@@ -6094,19 +6119,19 @@
       <c r="N43" s="225"/>
       <c r="O43" s="6"/>
       <c r="P43" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q43" s="175"/>
-      <c r="R43" s="138" t="s">
-        <v>440</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="Q43" s="116">
+        <v>500</v>
+      </c>
+      <c r="R43" s="11"/>
     </row>
     <row r="44" spans="2:18" ht="31" customHeight="1">
       <c r="B44" s="485"/>
       <c r="C44" s="6"/>
       <c r="D44" s="465"/>
       <c r="E44" s="246" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="F44" s="246"/>
       <c r="G44" s="256"/>
@@ -6121,25 +6146,27 @@
       <c r="P44" s="133" t="s">
         <v>91</v>
       </c>
-      <c r="Q44" s="138" t="s">
-        <v>593</v>
-      </c>
-      <c r="R44" s="11"/>
+      <c r="Q44" s="175"/>
+      <c r="R44" s="138" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="45" spans="2:18" ht="31" customHeight="1">
       <c r="B45" s="485"/>
       <c r="C45" s="6"/>
       <c r="D45" s="465"/>
       <c r="E45" s="246" t="s">
-        <v>675</v>
+        <v>399</v>
       </c>
       <c r="F45" s="246"/>
-      <c r="G45" s="256"/>
-      <c r="H45" s="256"/>
-      <c r="I45" s="256"/>
-      <c r="J45" s="256"/>
-      <c r="K45" s="256"/>
-      <c r="L45" s="256"/>
+      <c r="G45" s="489" t="s">
+        <v>698</v>
+      </c>
+      <c r="H45" s="489"/>
+      <c r="I45" s="489"/>
+      <c r="J45" s="489"/>
+      <c r="K45" s="489"/>
+      <c r="L45" s="489"/>
       <c r="M45" s="225"/>
       <c r="N45" s="225"/>
       <c r="O45" s="6"/>
@@ -6154,31 +6181,27 @@
     <row r="46" spans="2:18" ht="31" customHeight="1">
       <c r="B46" s="485"/>
       <c r="C46" s="6"/>
-      <c r="D46" s="465" t="s">
-        <v>430</v>
-      </c>
-      <c r="E46" s="257" t="s">
-        <v>220</v>
-      </c>
-      <c r="F46" s="258" t="s">
-        <v>444</v>
-      </c>
-      <c r="G46" s="475" t="s">
-        <v>136</v>
-      </c>
-      <c r="H46" s="476"/>
-      <c r="I46" s="399"/>
-      <c r="J46" s="400"/>
-      <c r="K46" s="400"/>
-      <c r="L46" s="401"/>
+      <c r="D46" s="465"/>
+      <c r="E46" s="246" t="s">
+        <v>675</v>
+      </c>
+      <c r="F46" s="246"/>
+      <c r="G46" s="489" t="s">
+        <v>699</v>
+      </c>
+      <c r="H46" s="489"/>
+      <c r="I46" s="489"/>
+      <c r="J46" s="489"/>
+      <c r="K46" s="489"/>
+      <c r="L46" s="489"/>
       <c r="M46" s="225"/>
       <c r="N46" s="225"/>
       <c r="O46" s="6"/>
       <c r="P46" s="133" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q46" s="116" t="s">
-        <v>411</v>
+        <v>92</v>
+      </c>
+      <c r="Q46" s="141" t="s">
+        <v>473</v>
       </c>
       <c r="R46" s="11"/>
     </row>
@@ -6186,35 +6209,43 @@
       <c r="B47" s="485"/>
       <c r="C47" s="6"/>
       <c r="D47" s="465"/>
-      <c r="E47" s="257"/>
-      <c r="F47" s="258"/>
-      <c r="G47" s="475" t="s">
-        <v>137</v>
-      </c>
-      <c r="H47" s="476"/>
-      <c r="I47" s="399"/>
-      <c r="J47" s="400"/>
-      <c r="K47" s="400"/>
-      <c r="L47" s="401"/>
+      <c r="E47" s="466" t="s">
+        <v>696</v>
+      </c>
+      <c r="F47" s="466"/>
+      <c r="G47" s="490" t="s">
+        <v>700</v>
+      </c>
+      <c r="H47" s="491"/>
+      <c r="I47" s="491"/>
+      <c r="J47" s="491"/>
+      <c r="K47" s="491"/>
+      <c r="L47" s="492"/>
       <c r="M47" s="225"/>
       <c r="N47" s="225"/>
       <c r="O47" s="6"/>
       <c r="P47" s="133" t="s">
-        <v>434</v>
-      </c>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="173" t="s">
-        <v>150</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="Q47" s="138" t="s">
+        <v>593</v>
+      </c>
+      <c r="R47" s="11"/>
     </row>
     <row r="48" spans="2:18" ht="31" customHeight="1">
       <c r="B48" s="485"/>
       <c r="C48" s="6"/>
-      <c r="D48" s="465"/>
-      <c r="E48" s="257"/>
-      <c r="F48" s="258"/>
+      <c r="D48" s="465" t="s">
+        <v>430</v>
+      </c>
+      <c r="E48" s="257" t="s">
+        <v>220</v>
+      </c>
+      <c r="F48" s="258" t="s">
+        <v>444</v>
+      </c>
       <c r="G48" s="475" t="s">
-        <v>282</v>
+        <v>136</v>
       </c>
       <c r="H48" s="476"/>
       <c r="I48" s="399"/>
@@ -6227,10 +6258,10 @@
       <c r="P48" s="133" t="s">
         <v>122</v>
       </c>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="116" t="b">
-        <v>0</v>
-      </c>
+      <c r="Q48" s="116" t="s">
+        <v>411</v>
+      </c>
+      <c r="R48" s="11"/>
     </row>
     <row r="49" spans="2:19" ht="31" customHeight="1">
       <c r="B49" s="485"/>
@@ -6239,7 +6270,7 @@
       <c r="E49" s="257"/>
       <c r="F49" s="258"/>
       <c r="G49" s="475" t="s">
-        <v>281</v>
+        <v>137</v>
       </c>
       <c r="H49" s="476"/>
       <c r="I49" s="399"/>
@@ -6250,11 +6281,11 @@
       <c r="N49" s="225"/>
       <c r="O49" s="6"/>
       <c r="P49" s="133" t="s">
-        <v>122</v>
+        <v>434</v>
       </c>
       <c r="Q49" s="11"/>
-      <c r="R49" s="116" t="b">
-        <v>0</v>
+      <c r="R49" s="173" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="2:19" ht="31" customHeight="1">
@@ -6263,25 +6294,23 @@
       <c r="D50" s="465"/>
       <c r="E50" s="257"/>
       <c r="F50" s="258"/>
-      <c r="G50" s="477" t="s">
-        <v>426</v>
-      </c>
-      <c r="H50" s="478"/>
-      <c r="I50" s="249" t="s">
-        <v>141</v>
-      </c>
-      <c r="J50" s="249"/>
-      <c r="K50" s="483"/>
-      <c r="L50" s="484"/>
+      <c r="G50" s="475" t="s">
+        <v>282</v>
+      </c>
+      <c r="H50" s="476"/>
+      <c r="I50" s="399"/>
+      <c r="J50" s="400"/>
+      <c r="K50" s="400"/>
+      <c r="L50" s="401"/>
       <c r="M50" s="225"/>
       <c r="N50" s="225"/>
       <c r="O50" s="6"/>
       <c r="P50" s="133" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="Q50" s="11"/>
-      <c r="R50" s="141" t="s">
-        <v>159</v>
+      <c r="R50" s="116" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:19" ht="31" customHeight="1">
@@ -6290,23 +6319,23 @@
       <c r="D51" s="465"/>
       <c r="E51" s="257"/>
       <c r="F51" s="258"/>
-      <c r="G51" s="479"/>
-      <c r="H51" s="480"/>
-      <c r="I51" s="249" t="s">
-        <v>146</v>
-      </c>
-      <c r="J51" s="249"/>
-      <c r="K51" s="483"/>
-      <c r="L51" s="484"/>
+      <c r="G51" s="475" t="s">
+        <v>281</v>
+      </c>
+      <c r="H51" s="476"/>
+      <c r="I51" s="399"/>
+      <c r="J51" s="400"/>
+      <c r="K51" s="400"/>
+      <c r="L51" s="401"/>
       <c r="M51" s="225"/>
       <c r="N51" s="225"/>
       <c r="O51" s="6"/>
       <c r="P51" s="133" t="s">
-        <v>434</v>
+        <v>122</v>
       </c>
       <c r="Q51" s="11"/>
-      <c r="R51" s="173" t="s">
-        <v>160</v>
+      <c r="R51" s="116" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:19" ht="31" customHeight="1">
@@ -6315,10 +6344,12 @@
       <c r="D52" s="465"/>
       <c r="E52" s="257"/>
       <c r="F52" s="258"/>
-      <c r="G52" s="479"/>
-      <c r="H52" s="480"/>
+      <c r="G52" s="477" t="s">
+        <v>426</v>
+      </c>
+      <c r="H52" s="478"/>
       <c r="I52" s="249" t="s">
-        <v>400</v>
+        <v>141</v>
       </c>
       <c r="J52" s="249"/>
       <c r="K52" s="483"/>
@@ -6327,11 +6358,11 @@
       <c r="N52" s="225"/>
       <c r="O52" s="6"/>
       <c r="P52" s="133" t="s">
-        <v>90</v>
+        <v>141</v>
       </c>
       <c r="Q52" s="11"/>
-      <c r="R52" s="116">
-        <v>26</v>
+      <c r="R52" s="141" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="2:19" ht="31" customHeight="1">
@@ -6340,10 +6371,10 @@
       <c r="D53" s="465"/>
       <c r="E53" s="257"/>
       <c r="F53" s="258"/>
-      <c r="G53" s="481"/>
-      <c r="H53" s="482"/>
+      <c r="G53" s="479"/>
+      <c r="H53" s="480"/>
       <c r="I53" s="249" t="s">
-        <v>401</v>
+        <v>146</v>
       </c>
       <c r="J53" s="249"/>
       <c r="K53" s="483"/>
@@ -6352,11 +6383,11 @@
       <c r="N53" s="225"/>
       <c r="O53" s="6"/>
       <c r="P53" s="133" t="s">
-        <v>90</v>
+        <v>434</v>
       </c>
       <c r="Q53" s="11"/>
-      <c r="R53" s="116">
-        <v>12</v>
+      <c r="R53" s="173" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="2:19" ht="31" customHeight="1">
@@ -6365,12 +6396,10 @@
       <c r="D54" s="465"/>
       <c r="E54" s="257"/>
       <c r="F54" s="258"/>
-      <c r="G54" s="477" t="s">
-        <v>140</v>
-      </c>
-      <c r="H54" s="478"/>
+      <c r="G54" s="479"/>
+      <c r="H54" s="480"/>
       <c r="I54" s="249" t="s">
-        <v>141</v>
+        <v>400</v>
       </c>
       <c r="J54" s="249"/>
       <c r="K54" s="483"/>
@@ -6379,11 +6408,11 @@
       <c r="N54" s="225"/>
       <c r="O54" s="6"/>
       <c r="P54" s="133" t="s">
-        <v>141</v>
+        <v>90</v>
       </c>
       <c r="Q54" s="11"/>
-      <c r="R54" s="141" t="s">
-        <v>158</v>
+      <c r="R54" s="116">
+        <v>26</v>
       </c>
     </row>
     <row r="55" spans="2:19" ht="31" customHeight="1">
@@ -6392,10 +6421,10 @@
       <c r="D55" s="465"/>
       <c r="E55" s="257"/>
       <c r="F55" s="258"/>
-      <c r="G55" s="479"/>
-      <c r="H55" s="480"/>
+      <c r="G55" s="481"/>
+      <c r="H55" s="482"/>
       <c r="I55" s="249" t="s">
-        <v>142</v>
+        <v>401</v>
       </c>
       <c r="J55" s="249"/>
       <c r="K55" s="483"/>
@@ -6404,11 +6433,11 @@
       <c r="N55" s="225"/>
       <c r="O55" s="6"/>
       <c r="P55" s="133" t="s">
-        <v>434</v>
+        <v>90</v>
       </c>
       <c r="Q55" s="11"/>
-      <c r="R55" s="173" t="s">
-        <v>150</v>
+      <c r="R55" s="116">
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="2:19" ht="31" customHeight="1">
@@ -6417,10 +6446,12 @@
       <c r="D56" s="465"/>
       <c r="E56" s="257"/>
       <c r="F56" s="258"/>
-      <c r="G56" s="479"/>
-      <c r="H56" s="480"/>
+      <c r="G56" s="477" t="s">
+        <v>140</v>
+      </c>
+      <c r="H56" s="478"/>
       <c r="I56" s="249" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J56" s="249"/>
       <c r="K56" s="483"/>
@@ -6429,11 +6460,11 @@
       <c r="N56" s="225"/>
       <c r="O56" s="6"/>
       <c r="P56" s="133" t="s">
-        <v>442</v>
+        <v>141</v>
       </c>
       <c r="Q56" s="11"/>
-      <c r="R56" s="140" t="s">
-        <v>441</v>
+      <c r="R56" s="141" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="2:19" ht="31" customHeight="1">
@@ -6442,10 +6473,10 @@
       <c r="D57" s="465"/>
       <c r="E57" s="257"/>
       <c r="F57" s="258"/>
-      <c r="G57" s="481"/>
-      <c r="H57" s="482"/>
+      <c r="G57" s="479"/>
+      <c r="H57" s="480"/>
       <c r="I57" s="249" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J57" s="249"/>
       <c r="K57" s="483"/>
@@ -6458,64 +6489,68 @@
       </c>
       <c r="Q57" s="11"/>
       <c r="R57" s="173" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="2:19" ht="31" customHeight="1">
-      <c r="B58" s="485" t="s">
-        <v>608</v>
-      </c>
-      <c r="D58" s="458" t="s">
-        <v>508</v>
-      </c>
-      <c r="E58" s="459" t="s">
-        <v>513</v>
-      </c>
-      <c r="F58" s="459"/>
-      <c r="G58" s="232"/>
-      <c r="H58" s="232"/>
-      <c r="I58" s="232"/>
-      <c r="J58" s="232"/>
-      <c r="K58" s="232"/>
-      <c r="L58" s="232"/>
+      <c r="B58" s="485"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="465"/>
+      <c r="E58" s="257"/>
+      <c r="F58" s="258"/>
+      <c r="G58" s="479"/>
+      <c r="H58" s="480"/>
+      <c r="I58" s="249" t="s">
+        <v>143</v>
+      </c>
+      <c r="J58" s="249"/>
+      <c r="K58" s="483"/>
+      <c r="L58" s="484"/>
       <c r="M58" s="225"/>
       <c r="N58" s="225"/>
+      <c r="O58" s="6"/>
       <c r="P58" s="133" t="s">
-        <v>453</v>
-      </c>
-      <c r="Q58" s="175"/>
-      <c r="R58" s="116" t="s">
-        <v>454</v>
+        <v>442</v>
+      </c>
+      <c r="Q58" s="11"/>
+      <c r="R58" s="140" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="59" spans="2:19" ht="31" customHeight="1">
       <c r="B59" s="485"/>
-      <c r="D59" s="458"/>
-      <c r="E59" s="459" t="s">
-        <v>510</v>
-      </c>
-      <c r="F59" s="459"/>
-      <c r="G59" s="232"/>
-      <c r="H59" s="232"/>
-      <c r="I59" s="232"/>
-      <c r="J59" s="232"/>
-      <c r="K59" s="232"/>
-      <c r="L59" s="232"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="465"/>
+      <c r="E59" s="257"/>
+      <c r="F59" s="258"/>
+      <c r="G59" s="481"/>
+      <c r="H59" s="482"/>
+      <c r="I59" s="249" t="s">
+        <v>144</v>
+      </c>
+      <c r="J59" s="249"/>
+      <c r="K59" s="483"/>
+      <c r="L59" s="484"/>
       <c r="M59" s="225"/>
       <c r="N59" s="225"/>
+      <c r="O59" s="6"/>
       <c r="P59" s="133" t="s">
-        <v>91</v>
+        <v>434</v>
       </c>
       <c r="Q59" s="11"/>
-      <c r="R59" s="138" t="s">
-        <v>594</v>
+      <c r="R59" s="173" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="2:19" ht="31" customHeight="1">
-      <c r="B60" s="485"/>
-      <c r="D60" s="458"/>
+      <c r="B60" s="485" t="s">
+        <v>608</v>
+      </c>
+      <c r="D60" s="458" t="s">
+        <v>508</v>
+      </c>
       <c r="E60" s="459" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="F60" s="459"/>
       <c r="G60" s="232"/>
@@ -6527,26 +6562,20 @@
       <c r="M60" s="225"/>
       <c r="N60" s="225"/>
       <c r="P60" s="133" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q60" s="163" t="s">
-        <v>509</v>
-      </c>
-      <c r="R60" s="11"/>
+        <v>453</v>
+      </c>
+      <c r="Q60" s="175"/>
+      <c r="R60" s="116" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="61" spans="2:19" ht="31" customHeight="1">
-      <c r="B61" s="485" t="s">
-        <v>609</v>
-      </c>
-      <c r="D61" s="461" t="s">
-        <v>290</v>
-      </c>
-      <c r="E61" s="228" t="s">
-        <v>269</v>
-      </c>
-      <c r="F61" s="229" t="s">
-        <v>455</v>
-      </c>
+      <c r="B61" s="485"/>
+      <c r="D61" s="458"/>
+      <c r="E61" s="459" t="s">
+        <v>510</v>
+      </c>
+      <c r="F61" s="459"/>
       <c r="G61" s="232"/>
       <c r="H61" s="232"/>
       <c r="I61" s="232"/>
@@ -6556,60 +6585,55 @@
       <c r="M61" s="225"/>
       <c r="N61" s="225"/>
       <c r="P61" s="133" t="s">
-        <v>453</v>
-      </c>
-      <c r="Q61" s="141" t="s">
-        <v>473</v>
-      </c>
-      <c r="R61" s="116" t="s">
-        <v>454</v>
+        <v>91</v>
+      </c>
+      <c r="Q61" s="11"/>
+      <c r="R61" s="138" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="62" spans="2:19" ht="31" customHeight="1">
       <c r="B62" s="485"/>
-      <c r="D62" s="462" t="s">
-        <v>515</v>
-      </c>
-      <c r="E62" s="445"/>
-      <c r="F62" s="446"/>
-      <c r="G62" s="446"/>
-      <c r="H62" s="446"/>
-      <c r="I62" s="446"/>
-      <c r="J62" s="446"/>
-      <c r="K62" s="446"/>
-      <c r="L62" s="447"/>
+      <c r="D62" s="458"/>
+      <c r="E62" s="459" t="s">
+        <v>512</v>
+      </c>
+      <c r="F62" s="459"/>
+      <c r="G62" s="232"/>
+      <c r="H62" s="232"/>
+      <c r="I62" s="232"/>
+      <c r="J62" s="232"/>
+      <c r="K62" s="232"/>
+      <c r="L62" s="232"/>
       <c r="M62" s="225"/>
       <c r="N62" s="225"/>
       <c r="P62" s="133" t="s">
-        <v>597</v>
-      </c>
-      <c r="Q62" s="141" t="s">
-        <v>473</v>
+        <v>97</v>
+      </c>
+      <c r="Q62" s="163" t="s">
+        <v>509</v>
       </c>
       <c r="R62" s="11"/>
-      <c r="S62" s="9"/>
     </row>
     <row r="63" spans="2:19" ht="31" customHeight="1">
       <c r="B63" s="485" t="s">
-        <v>611</v>
-      </c>
-      <c r="D63" s="463" t="s">
-        <v>261</v>
-      </c>
-      <c r="E63" s="443" t="s">
+        <v>609</v>
+      </c>
+      <c r="D63" s="461" t="s">
+        <v>290</v>
+      </c>
+      <c r="E63" s="228" t="s">
         <v>269</v>
       </c>
-      <c r="F63" s="444" t="s">
-        <v>683</v>
-      </c>
-      <c r="G63" s="246" t="s">
-        <v>403</v>
-      </c>
-      <c r="H63" s="246"/>
-      <c r="I63" s="399"/>
-      <c r="J63" s="400"/>
-      <c r="K63" s="400"/>
-      <c r="L63" s="401"/>
+      <c r="F63" s="229" t="s">
+        <v>455</v>
+      </c>
+      <c r="G63" s="232"/>
+      <c r="H63" s="232"/>
+      <c r="I63" s="232"/>
+      <c r="J63" s="232"/>
+      <c r="K63" s="232"/>
+      <c r="L63" s="232"/>
       <c r="M63" s="225"/>
       <c r="N63" s="225"/>
       <c r="P63" s="133" t="s">
@@ -6618,86 +6642,95 @@
       <c r="Q63" s="141" t="s">
         <v>473</v>
       </c>
-      <c r="R63" s="11"/>
+      <c r="R63" s="116" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="64" spans="2:19" ht="31" customHeight="1">
       <c r="B64" s="485"/>
-      <c r="D64" s="464"/>
-      <c r="E64" s="443"/>
-      <c r="F64" s="444"/>
-      <c r="G64" s="237" t="s">
-        <v>601</v>
-      </c>
-      <c r="H64" s="238"/>
-      <c r="I64" s="443" t="s">
-        <v>677</v>
-      </c>
-      <c r="J64" s="255" t="s">
-        <v>265</v>
-      </c>
-      <c r="K64" s="246" t="s">
-        <v>403</v>
-      </c>
-      <c r="L64" s="246"/>
+      <c r="D64" s="462" t="s">
+        <v>515</v>
+      </c>
+      <c r="E64" s="445"/>
+      <c r="F64" s="446"/>
+      <c r="G64" s="446"/>
+      <c r="H64" s="446"/>
+      <c r="I64" s="446"/>
+      <c r="J64" s="446"/>
+      <c r="K64" s="446"/>
+      <c r="L64" s="447"/>
       <c r="M64" s="225"/>
       <c r="N64" s="225"/>
       <c r="P64" s="133" t="s">
-        <v>453</v>
+        <v>597</v>
       </c>
       <c r="Q64" s="141" t="s">
         <v>473</v>
       </c>
       <c r="R64" s="11"/>
-    </row>
-    <row r="65" spans="2:19" ht="31" customHeight="1">
-      <c r="B65" s="485"/>
-      <c r="D65" s="464"/>
-      <c r="E65" s="443"/>
-      <c r="F65" s="444"/>
-      <c r="G65" s="239"/>
-      <c r="H65" s="240"/>
-      <c r="I65" s="443"/>
-      <c r="J65" s="255"/>
-      <c r="K65" s="246" t="s">
-        <v>678</v>
-      </c>
-      <c r="L65" s="246"/>
+      <c r="S64" s="9"/>
+    </row>
+    <row r="65" spans="2:18" ht="31" customHeight="1">
+      <c r="B65" s="485" t="s">
+        <v>611</v>
+      </c>
+      <c r="D65" s="463" t="s">
+        <v>261</v>
+      </c>
+      <c r="E65" s="443" t="s">
+        <v>269</v>
+      </c>
+      <c r="F65" s="444" t="s">
+        <v>683</v>
+      </c>
+      <c r="G65" s="246" t="s">
+        <v>403</v>
+      </c>
+      <c r="H65" s="246"/>
+      <c r="I65" s="399"/>
+      <c r="J65" s="400"/>
+      <c r="K65" s="400"/>
+      <c r="L65" s="401"/>
       <c r="M65" s="225"/>
       <c r="N65" s="225"/>
       <c r="P65" s="133" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q65" s="116" t="s">
-        <v>411</v>
+        <v>453</v>
+      </c>
+      <c r="Q65" s="141" t="s">
+        <v>473</v>
       </c>
       <c r="R65" s="11"/>
     </row>
-    <row r="66" spans="2:19" ht="31" customHeight="1">
+    <row r="66" spans="2:18" ht="31" customHeight="1">
       <c r="B66" s="485"/>
       <c r="D66" s="464"/>
       <c r="E66" s="443"/>
       <c r="F66" s="444"/>
-      <c r="G66" s="239"/>
-      <c r="H66" s="240"/>
-      <c r="I66" s="443"/>
-      <c r="J66" s="255"/>
+      <c r="G66" s="237" t="s">
+        <v>601</v>
+      </c>
+      <c r="H66" s="238"/>
+      <c r="I66" s="443" t="s">
+        <v>677</v>
+      </c>
+      <c r="J66" s="255" t="s">
+        <v>265</v>
+      </c>
       <c r="K66" s="246" t="s">
-        <v>680</v>
+        <v>403</v>
       </c>
       <c r="L66" s="246"/>
       <c r="M66" s="225"/>
       <c r="N66" s="225"/>
       <c r="P66" s="133" t="s">
-        <v>681</v>
-      </c>
-      <c r="Q66" s="116" t="s">
-        <v>99</v>
-      </c>
-      <c r="R66" s="116" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="67" spans="2:19" ht="31" customHeight="1">
+        <v>453</v>
+      </c>
+      <c r="Q66" s="141" t="s">
+        <v>473</v>
+      </c>
+      <c r="R66" s="11"/>
+    </row>
+    <row r="67" spans="2:18" ht="31" customHeight="1">
       <c r="B67" s="485"/>
       <c r="D67" s="464"/>
       <c r="E67" s="443"/>
@@ -6706,16 +6739,12 @@
       <c r="H67" s="240"/>
       <c r="I67" s="443"/>
       <c r="J67" s="255"/>
-      <c r="K67" s="255" t="s">
-        <v>679</v>
-      </c>
-      <c r="L67" s="255"/>
-      <c r="M67" s="235" t="s">
-        <v>484</v>
-      </c>
-      <c r="N67" s="226" t="s">
-        <v>477</v>
-      </c>
+      <c r="K67" s="246" t="s">
+        <v>678</v>
+      </c>
+      <c r="L67" s="246"/>
+      <c r="M67" s="225"/>
+      <c r="N67" s="225"/>
       <c r="P67" s="133" t="s">
         <v>122</v>
       </c>
@@ -6724,7 +6753,7 @@
       </c>
       <c r="R67" s="11"/>
     </row>
-    <row r="68" spans="2:19" ht="31" customHeight="1">
+    <row r="68" spans="2:18" ht="31" customHeight="1">
       <c r="B68" s="485"/>
       <c r="D68" s="464"/>
       <c r="E68" s="443"/>
@@ -6733,125 +6762,129 @@
       <c r="H68" s="240"/>
       <c r="I68" s="443"/>
       <c r="J68" s="255"/>
-      <c r="K68" s="255"/>
-      <c r="L68" s="255"/>
-      <c r="M68" s="236"/>
-      <c r="N68" s="226" t="s">
-        <v>482</v>
-      </c>
+      <c r="K68" s="246" t="s">
+        <v>680</v>
+      </c>
+      <c r="L68" s="246"/>
+      <c r="M68" s="225"/>
+      <c r="N68" s="225"/>
       <c r="P68" s="133" t="s">
-        <v>122</v>
+        <v>681</v>
       </c>
       <c r="Q68" s="116" t="s">
-        <v>411</v>
-      </c>
-      <c r="R68" s="11"/>
-    </row>
-    <row r="69" spans="2:19" ht="31" customHeight="1">
+        <v>99</v>
+      </c>
+      <c r="R68" s="116" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="69" spans="2:18" ht="31" customHeight="1">
       <c r="B69" s="485"/>
       <c r="D69" s="464"/>
-      <c r="E69" s="443" t="s">
-        <v>269</v>
-      </c>
-      <c r="F69" s="444" t="s">
-        <v>598</v>
-      </c>
-      <c r="G69" s="246" t="s">
-        <v>403</v>
-      </c>
-      <c r="H69" s="246"/>
-      <c r="I69" s="399"/>
-      <c r="J69" s="400"/>
-      <c r="K69" s="400"/>
-      <c r="L69" s="401"/>
-      <c r="M69" s="225"/>
-      <c r="N69" s="225"/>
+      <c r="E69" s="443"/>
+      <c r="F69" s="444"/>
+      <c r="G69" s="239"/>
+      <c r="H69" s="240"/>
+      <c r="I69" s="443"/>
+      <c r="J69" s="255"/>
+      <c r="K69" s="255" t="s">
+        <v>679</v>
+      </c>
+      <c r="L69" s="255"/>
+      <c r="M69" s="235" t="s">
+        <v>484</v>
+      </c>
+      <c r="N69" s="226" t="s">
+        <v>477</v>
+      </c>
       <c r="P69" s="133" t="s">
-        <v>453</v>
-      </c>
-      <c r="Q69" s="141" t="s">
-        <v>473</v>
+        <v>122</v>
+      </c>
+      <c r="Q69" s="116" t="s">
+        <v>411</v>
       </c>
       <c r="R69" s="11"/>
     </row>
-    <row r="70" spans="2:19" ht="31" customHeight="1">
+    <row r="70" spans="2:18" ht="31" customHeight="1">
       <c r="B70" s="485"/>
       <c r="D70" s="464"/>
       <c r="E70" s="443"/>
       <c r="F70" s="444"/>
-      <c r="G70" s="237" t="s">
-        <v>601</v>
-      </c>
-      <c r="H70" s="238"/>
-      <c r="I70" s="443" t="s">
-        <v>677</v>
-      </c>
-      <c r="J70" s="255" t="s">
-        <v>599</v>
-      </c>
-      <c r="K70" s="246" t="s">
-        <v>403</v>
-      </c>
-      <c r="L70" s="246"/>
-      <c r="M70" s="225"/>
-      <c r="N70" s="225"/>
+      <c r="G70" s="239"/>
+      <c r="H70" s="240"/>
+      <c r="I70" s="443"/>
+      <c r="J70" s="255"/>
+      <c r="K70" s="255"/>
+      <c r="L70" s="255"/>
+      <c r="M70" s="236"/>
+      <c r="N70" s="226" t="s">
+        <v>482</v>
+      </c>
       <c r="P70" s="133" t="s">
-        <v>453</v>
-      </c>
-      <c r="Q70" s="141" t="s">
-        <v>473</v>
+        <v>122</v>
+      </c>
+      <c r="Q70" s="116" t="s">
+        <v>411</v>
       </c>
       <c r="R70" s="11"/>
     </row>
-    <row r="71" spans="2:19" ht="31" customHeight="1">
+    <row r="71" spans="2:18" ht="31" customHeight="1">
       <c r="B71" s="485"/>
       <c r="D71" s="464"/>
-      <c r="E71" s="443"/>
-      <c r="F71" s="444"/>
-      <c r="G71" s="239"/>
-      <c r="H71" s="240"/>
-      <c r="I71" s="443"/>
-      <c r="J71" s="255"/>
-      <c r="K71" s="246" t="s">
-        <v>678</v>
-      </c>
-      <c r="L71" s="246"/>
+      <c r="E71" s="443" t="s">
+        <v>269</v>
+      </c>
+      <c r="F71" s="444" t="s">
+        <v>598</v>
+      </c>
+      <c r="G71" s="246" t="s">
+        <v>403</v>
+      </c>
+      <c r="H71" s="246"/>
+      <c r="I71" s="399"/>
+      <c r="J71" s="400"/>
+      <c r="K71" s="400"/>
+      <c r="L71" s="401"/>
       <c r="M71" s="225"/>
       <c r="N71" s="225"/>
       <c r="P71" s="133" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q71" s="116" t="s">
-        <v>411</v>
+        <v>453</v>
+      </c>
+      <c r="Q71" s="141" t="s">
+        <v>473</v>
       </c>
       <c r="R71" s="11"/>
     </row>
-    <row r="72" spans="2:19" ht="31" customHeight="1">
+    <row r="72" spans="2:18" ht="31" customHeight="1">
       <c r="B72" s="485"/>
       <c r="D72" s="464"/>
       <c r="E72" s="443"/>
       <c r="F72" s="444"/>
-      <c r="G72" s="239"/>
-      <c r="H72" s="240"/>
-      <c r="I72" s="443"/>
-      <c r="J72" s="255"/>
+      <c r="G72" s="237" t="s">
+        <v>601</v>
+      </c>
+      <c r="H72" s="238"/>
+      <c r="I72" s="443" t="s">
+        <v>677</v>
+      </c>
+      <c r="J72" s="255" t="s">
+        <v>599</v>
+      </c>
       <c r="K72" s="246" t="s">
-        <v>680</v>
+        <v>403</v>
       </c>
       <c r="L72" s="246"/>
       <c r="M72" s="225"/>
       <c r="N72" s="225"/>
       <c r="P72" s="133" t="s">
-        <v>681</v>
-      </c>
-      <c r="Q72" s="116" t="s">
-        <v>99</v>
-      </c>
-      <c r="R72" s="116" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="73" spans="2:19" ht="31" customHeight="1">
+        <v>453</v>
+      </c>
+      <c r="Q72" s="141" t="s">
+        <v>473</v>
+      </c>
+      <c r="R72" s="11"/>
+    </row>
+    <row r="73" spans="2:18" ht="31" customHeight="1">
       <c r="B73" s="485"/>
       <c r="D73" s="464"/>
       <c r="E73" s="443"/>
@@ -6860,16 +6893,12 @@
       <c r="H73" s="240"/>
       <c r="I73" s="443"/>
       <c r="J73" s="255"/>
-      <c r="K73" s="255" t="s">
-        <v>679</v>
-      </c>
-      <c r="L73" s="255"/>
-      <c r="M73" s="235" t="s">
-        <v>484</v>
-      </c>
-      <c r="N73" s="226" t="s">
-        <v>477</v>
-      </c>
+      <c r="K73" s="246" t="s">
+        <v>678</v>
+      </c>
+      <c r="L73" s="246"/>
+      <c r="M73" s="225"/>
+      <c r="N73" s="225"/>
       <c r="P73" s="133" t="s">
         <v>122</v>
       </c>
@@ -6878,7 +6907,7 @@
       </c>
       <c r="R73" s="11"/>
     </row>
-    <row r="74" spans="2:19" ht="31" customHeight="1">
+    <row r="74" spans="2:18" ht="31" customHeight="1">
       <c r="B74" s="485"/>
       <c r="D74" s="464"/>
       <c r="E74" s="443"/>
@@ -6887,102 +6916,102 @@
       <c r="H74" s="240"/>
       <c r="I74" s="443"/>
       <c r="J74" s="255"/>
-      <c r="K74" s="255"/>
-      <c r="L74" s="255"/>
-      <c r="M74" s="236"/>
-      <c r="N74" s="226" t="s">
+      <c r="K74" s="246" t="s">
+        <v>680</v>
+      </c>
+      <c r="L74" s="246"/>
+      <c r="M74" s="225"/>
+      <c r="N74" s="225"/>
+      <c r="P74" s="133" t="s">
+        <v>681</v>
+      </c>
+      <c r="Q74" s="116" t="s">
+        <v>99</v>
+      </c>
+      <c r="R74" s="116" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="75" spans="2:18" ht="31" customHeight="1">
+      <c r="B75" s="485"/>
+      <c r="D75" s="464"/>
+      <c r="E75" s="443"/>
+      <c r="F75" s="444"/>
+      <c r="G75" s="239"/>
+      <c r="H75" s="240"/>
+      <c r="I75" s="443"/>
+      <c r="J75" s="255"/>
+      <c r="K75" s="255" t="s">
+        <v>679</v>
+      </c>
+      <c r="L75" s="255"/>
+      <c r="M75" s="235" t="s">
+        <v>484</v>
+      </c>
+      <c r="N75" s="226" t="s">
+        <v>477</v>
+      </c>
+      <c r="P75" s="133" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q75" s="116" t="s">
+        <v>411</v>
+      </c>
+      <c r="R75" s="11"/>
+    </row>
+    <row r="76" spans="2:18" ht="31" customHeight="1">
+      <c r="B76" s="485"/>
+      <c r="D76" s="464"/>
+      <c r="E76" s="443"/>
+      <c r="F76" s="444"/>
+      <c r="G76" s="239"/>
+      <c r="H76" s="240"/>
+      <c r="I76" s="443"/>
+      <c r="J76" s="255"/>
+      <c r="K76" s="255"/>
+      <c r="L76" s="255"/>
+      <c r="M76" s="236"/>
+      <c r="N76" s="226" t="s">
         <v>482</v>
       </c>
-      <c r="P74" s="133" t="s">
+      <c r="P76" s="133" t="s">
         <v>122</v>
       </c>
-      <c r="Q74" s="116" t="s">
+      <c r="Q76" s="116" t="s">
         <v>411</v>
       </c>
-      <c r="R74" s="11"/>
-    </row>
-    <row r="75" spans="2:19" ht="31" customHeight="1">
-      <c r="B75" s="485"/>
-      <c r="D75" s="455" t="s">
+      <c r="R76" s="11"/>
+    </row>
+    <row r="77" spans="2:18" ht="31" customHeight="1">
+      <c r="B77" s="485"/>
+      <c r="D77" s="455" t="s">
         <v>259</v>
       </c>
-      <c r="E75" s="466" t="s">
+      <c r="E77" s="466" t="s">
         <v>270</v>
       </c>
-      <c r="F75" s="466"/>
-      <c r="G75" s="232"/>
-      <c r="H75" s="232"/>
-      <c r="I75" s="232"/>
-      <c r="J75" s="232"/>
-      <c r="K75" s="232"/>
-      <c r="L75" s="232"/>
-      <c r="M75" s="225"/>
-      <c r="N75" s="225"/>
-      <c r="P75" s="133" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q75" s="116">
-        <v>7</v>
-      </c>
-      <c r="R75" s="11"/>
-    </row>
-    <row r="76" spans="2:19" ht="31" customHeight="1">
-      <c r="B76" s="485"/>
-      <c r="D76" s="456"/>
-      <c r="E76" s="466" t="s">
-        <v>268</v>
-      </c>
-      <c r="F76" s="466"/>
-      <c r="G76" s="232"/>
-      <c r="H76" s="232"/>
-      <c r="I76" s="232"/>
-      <c r="J76" s="232"/>
-      <c r="K76" s="232"/>
-      <c r="L76" s="232"/>
-      <c r="M76" s="225"/>
-      <c r="N76" s="225"/>
-      <c r="P76" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q76" s="141" t="s">
-        <v>481</v>
-      </c>
-      <c r="R76" s="11"/>
-    </row>
-    <row r="77" spans="2:19" ht="31" customHeight="1">
-      <c r="B77" s="485"/>
-      <c r="D77" s="456"/>
-      <c r="E77" s="466" t="s">
-        <v>314</v>
-      </c>
       <c r="F77" s="466"/>
-      <c r="G77" s="217" t="s">
-        <v>269</v>
-      </c>
-      <c r="H77" s="226" t="s">
-        <v>458</v>
-      </c>
-      <c r="I77" s="399"/>
-      <c r="J77" s="400"/>
-      <c r="K77" s="400"/>
-      <c r="L77" s="401"/>
+      <c r="G77" s="232"/>
+      <c r="H77" s="232"/>
+      <c r="I77" s="232"/>
+      <c r="J77" s="232"/>
+      <c r="K77" s="232"/>
+      <c r="L77" s="232"/>
       <c r="M77" s="225"/>
       <c r="N77" s="225"/>
       <c r="P77" s="133" t="s">
-        <v>453</v>
-      </c>
-      <c r="Q77" s="141" t="s">
-        <v>473</v>
-      </c>
-      <c r="R77" s="116" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="78" spans="2:19" ht="31" customHeight="1">
+        <v>90</v>
+      </c>
+      <c r="Q77" s="116">
+        <v>7</v>
+      </c>
+      <c r="R77" s="11"/>
+    </row>
+    <row r="78" spans="2:18" ht="31" customHeight="1">
       <c r="B78" s="485"/>
       <c r="D78" s="456"/>
       <c r="E78" s="466" t="s">
-        <v>313</v>
+        <v>268</v>
       </c>
       <c r="F78" s="466"/>
       <c r="G78" s="232"/>
@@ -6997,47 +7026,46 @@
         <v>91</v>
       </c>
       <c r="Q78" s="141" t="s">
-        <v>472</v>
+        <v>481</v>
       </c>
       <c r="R78" s="11"/>
     </row>
-    <row r="79" spans="2:19" ht="31" customHeight="1">
+    <row r="79" spans="2:18" ht="31" customHeight="1">
       <c r="B79" s="485"/>
-      <c r="D79" s="457"/>
+      <c r="D79" s="456"/>
       <c r="E79" s="466" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="F79" s="466"/>
-      <c r="G79" s="232"/>
-      <c r="H79" s="232"/>
-      <c r="I79" s="232"/>
-      <c r="J79" s="232"/>
-      <c r="K79" s="232"/>
-      <c r="L79" s="232"/>
+      <c r="G79" s="217" t="s">
+        <v>269</v>
+      </c>
+      <c r="H79" s="226" t="s">
+        <v>458</v>
+      </c>
+      <c r="I79" s="399"/>
+      <c r="J79" s="400"/>
+      <c r="K79" s="400"/>
+      <c r="L79" s="401"/>
       <c r="M79" s="225"/>
       <c r="N79" s="225"/>
-      <c r="P79" s="144" t="s">
-        <v>457</v>
+      <c r="P79" s="133" t="s">
+        <v>453</v>
       </c>
       <c r="Q79" s="141" t="s">
         <v>473</v>
       </c>
-      <c r="R79" s="11"/>
-      <c r="S79" s="221" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="80" spans="2:19" ht="31" customHeight="1">
-      <c r="B80" s="485" t="s">
-        <v>610</v>
-      </c>
-      <c r="D80" s="449" t="s">
-        <v>601</v>
-      </c>
-      <c r="E80" s="451" t="s">
-        <v>353</v>
-      </c>
-      <c r="F80" s="451"/>
+      <c r="R79" s="116" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="80" spans="2:18" ht="31" customHeight="1">
+      <c r="B80" s="485"/>
+      <c r="D80" s="456"/>
+      <c r="E80" s="466" t="s">
+        <v>313</v>
+      </c>
+      <c r="F80" s="466"/>
       <c r="G80" s="232"/>
       <c r="H80" s="232"/>
       <c r="I80" s="232"/>
@@ -7047,20 +7075,20 @@
       <c r="M80" s="225"/>
       <c r="N80" s="225"/>
       <c r="P80" s="133" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q80" s="116">
-        <v>100</v>
+        <v>91</v>
+      </c>
+      <c r="Q80" s="141" t="s">
+        <v>472</v>
       </c>
       <c r="R80" s="11"/>
     </row>
-    <row r="81" spans="2:28" ht="31" customHeight="1">
+    <row r="81" spans="2:19" ht="31" customHeight="1">
       <c r="B81" s="485"/>
-      <c r="D81" s="450"/>
-      <c r="E81" s="451" t="s">
-        <v>297</v>
-      </c>
-      <c r="F81" s="451"/>
+      <c r="D81" s="457"/>
+      <c r="E81" s="466" t="s">
+        <v>312</v>
+      </c>
+      <c r="F81" s="466"/>
       <c r="G81" s="232"/>
       <c r="H81" s="232"/>
       <c r="I81" s="232"/>
@@ -7069,19 +7097,26 @@
       <c r="L81" s="232"/>
       <c r="M81" s="225"/>
       <c r="N81" s="225"/>
-      <c r="P81" s="133" t="s">
-        <v>596</v>
-      </c>
-      <c r="Q81" s="116" t="s">
-        <v>99</v>
+      <c r="P81" s="144" t="s">
+        <v>457</v>
+      </c>
+      <c r="Q81" s="141" t="s">
+        <v>473</v>
       </c>
       <c r="R81" s="11"/>
-    </row>
-    <row r="82" spans="2:28" ht="31" customHeight="1">
-      <c r="B82" s="485"/>
-      <c r="D82" s="450"/>
+      <c r="S81" s="221" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="82" spans="2:19" ht="31" customHeight="1">
+      <c r="B82" s="485" t="s">
+        <v>610</v>
+      </c>
+      <c r="D82" s="449" t="s">
+        <v>601</v>
+      </c>
       <c r="E82" s="451" t="s">
-        <v>602</v>
+        <v>353</v>
       </c>
       <c r="F82" s="451"/>
       <c r="G82" s="232"/>
@@ -7093,18 +7128,18 @@
       <c r="M82" s="225"/>
       <c r="N82" s="225"/>
       <c r="P82" s="133" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q82" s="172" t="s">
-        <v>107</v>
+        <v>90</v>
+      </c>
+      <c r="Q82" s="116">
+        <v>100</v>
       </c>
       <c r="R82" s="11"/>
     </row>
-    <row r="83" spans="2:28" ht="31" customHeight="1">
+    <row r="83" spans="2:19" ht="31" customHeight="1">
       <c r="B83" s="485"/>
       <c r="D83" s="450"/>
       <c r="E83" s="451" t="s">
-        <v>603</v>
+        <v>297</v>
       </c>
       <c r="F83" s="451"/>
       <c r="G83" s="232"/>
@@ -7116,163 +7151,146 @@
       <c r="M83" s="225"/>
       <c r="N83" s="225"/>
       <c r="P83" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q83" s="138" t="s">
-        <v>595</v>
+        <v>596</v>
+      </c>
+      <c r="Q83" s="116" t="s">
+        <v>99</v>
       </c>
       <c r="R83" s="11"/>
     </row>
-    <row r="84" spans="2:28" ht="31" customHeight="1">
+    <row r="84" spans="2:19" ht="31" customHeight="1">
       <c r="B84" s="485"/>
       <c r="D84" s="450"/>
-      <c r="E84" s="465" t="s">
-        <v>479</v>
-      </c>
-      <c r="F84" s="465"/>
-      <c r="G84" s="466" t="s">
-        <v>516</v>
-      </c>
-      <c r="H84" s="466"/>
-      <c r="I84" s="489" t="s">
-        <v>699</v>
-      </c>
-      <c r="J84" s="489"/>
-      <c r="K84" s="489"/>
-      <c r="L84" s="489"/>
+      <c r="E84" s="451" t="s">
+        <v>602</v>
+      </c>
+      <c r="F84" s="451"/>
+      <c r="G84" s="232"/>
+      <c r="H84" s="232"/>
+      <c r="I84" s="232"/>
+      <c r="J84" s="232"/>
+      <c r="K84" s="232"/>
+      <c r="L84" s="232"/>
       <c r="M84" s="225"/>
       <c r="N84" s="225"/>
       <c r="P84" s="133" t="s">
-        <v>474</v>
-      </c>
-      <c r="Q84" s="141" t="s">
-        <v>472</v>
+        <v>97</v>
+      </c>
+      <c r="Q84" s="172" t="s">
+        <v>107</v>
       </c>
       <c r="R84" s="11"/>
     </row>
-    <row r="85" spans="2:28" ht="31" customHeight="1">
+    <row r="85" spans="2:19" ht="31" customHeight="1">
       <c r="B85" s="485"/>
       <c r="D85" s="450"/>
-      <c r="E85" s="465"/>
-      <c r="F85" s="465"/>
-      <c r="G85" s="466" t="s">
-        <v>690</v>
-      </c>
-      <c r="H85" s="466"/>
-      <c r="I85" s="489" t="s">
-        <v>697</v>
-      </c>
-      <c r="J85" s="489"/>
-      <c r="K85" s="489"/>
-      <c r="L85" s="489"/>
+      <c r="E85" s="451" t="s">
+        <v>603</v>
+      </c>
+      <c r="F85" s="451"/>
+      <c r="G85" s="232"/>
+      <c r="H85" s="232"/>
+      <c r="I85" s="232"/>
+      <c r="J85" s="232"/>
+      <c r="K85" s="232"/>
+      <c r="L85" s="232"/>
       <c r="M85" s="225"/>
       <c r="N85" s="225"/>
       <c r="P85" s="133" t="s">
-        <v>468</v>
-      </c>
-      <c r="Q85" s="141" t="s">
-        <v>472</v>
-      </c>
-      <c r="R85" s="116" t="s">
-        <v>421</v>
-      </c>
-      <c r="S85" s="9" t="s">
-        <v>685</v>
-      </c>
-      <c r="X85" s="4" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="86" spans="2:28" ht="31" customHeight="1">
+        <v>91</v>
+      </c>
+      <c r="Q85" s="138" t="s">
+        <v>595</v>
+      </c>
+      <c r="R85" s="11"/>
+    </row>
+    <row r="86" spans="2:19" ht="31" customHeight="1">
       <c r="B86" s="485"/>
       <c r="D86" s="450"/>
-      <c r="E86" s="465"/>
+      <c r="E86" s="465" t="s">
+        <v>479</v>
+      </c>
       <c r="F86" s="465"/>
       <c r="G86" s="466" t="s">
-        <v>696</v>
+        <v>516</v>
       </c>
       <c r="H86" s="466"/>
-      <c r="I86" s="489" t="s">
-        <v>698</v>
-      </c>
-      <c r="J86" s="489"/>
-      <c r="K86" s="489"/>
-      <c r="L86" s="489"/>
+      <c r="I86" s="488" t="s">
+        <v>693</v>
+      </c>
+      <c r="J86" s="488"/>
+      <c r="K86" s="488"/>
+      <c r="L86" s="488"/>
       <c r="M86" s="225"/>
       <c r="N86" s="225"/>
-      <c r="P86" s="133"/>
-      <c r="Q86" s="141"/>
-      <c r="R86" s="116"/>
-      <c r="X86" s="4" t="s">
-        <v>692</v>
-      </c>
-      <c r="AB86" s="4" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="87" spans="2:28" ht="31" customHeight="1">
+      <c r="P86" s="133" t="s">
+        <v>474</v>
+      </c>
+      <c r="Q86" s="141" t="s">
+        <v>472</v>
+      </c>
+      <c r="R86" s="11"/>
+    </row>
+    <row r="87" spans="2:19" ht="31" customHeight="1">
       <c r="B87" s="485"/>
       <c r="D87" s="450"/>
       <c r="E87" s="465"/>
       <c r="F87" s="465"/>
       <c r="G87" s="466" t="s">
-        <v>388</v>
+        <v>689</v>
       </c>
       <c r="H87" s="466"/>
-      <c r="I87" s="243" t="s">
-        <v>301</v>
-      </c>
-      <c r="J87" s="244"/>
-      <c r="K87" s="233"/>
-      <c r="L87" s="233"/>
+      <c r="I87" s="488" t="s">
+        <v>691</v>
+      </c>
+      <c r="J87" s="488"/>
+      <c r="K87" s="488"/>
+      <c r="L87" s="488"/>
       <c r="M87" s="225"/>
       <c r="N87" s="225"/>
       <c r="P87" s="133" t="s">
-        <v>478</v>
-      </c>
-      <c r="Q87" s="147" t="s">
-        <v>108</v>
-      </c>
-      <c r="R87" s="11"/>
-      <c r="X87" s="4" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="88" spans="2:28" ht="31" customHeight="1">
+        <v>468</v>
+      </c>
+      <c r="Q87" s="141" t="s">
+        <v>472</v>
+      </c>
+      <c r="R87" s="116" t="s">
+        <v>421</v>
+      </c>
+      <c r="S87" s="9"/>
+    </row>
+    <row r="88" spans="2:19" ht="31" customHeight="1">
       <c r="B88" s="485"/>
       <c r="D88" s="450"/>
       <c r="E88" s="465"/>
       <c r="F88" s="465"/>
-      <c r="G88" s="466"/>
+      <c r="G88" s="466" t="s">
+        <v>690</v>
+      </c>
       <c r="H88" s="466"/>
-      <c r="I88" s="243" t="s">
-        <v>268</v>
-      </c>
-      <c r="J88" s="244"/>
-      <c r="K88" s="233"/>
-      <c r="L88" s="233"/>
+      <c r="I88" s="488" t="s">
+        <v>692</v>
+      </c>
+      <c r="J88" s="488"/>
+      <c r="K88" s="488"/>
+      <c r="L88" s="488"/>
       <c r="M88" s="225"/>
       <c r="N88" s="225"/>
-      <c r="P88" s="133" t="s">
-        <v>468</v>
-      </c>
-      <c r="Q88" s="141" t="s">
-        <v>472</v>
-      </c>
-      <c r="R88" s="11"/>
-      <c r="X88" s="4" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="89" spans="2:28" ht="31" customHeight="1">
+      <c r="P88" s="133"/>
+      <c r="Q88" s="141"/>
+      <c r="R88" s="116"/>
+    </row>
+    <row r="89" spans="2:19" ht="31" customHeight="1">
       <c r="B89" s="485"/>
       <c r="D89" s="450"/>
       <c r="E89" s="465"/>
       <c r="F89" s="465"/>
-      <c r="G89" s="466"/>
+      <c r="G89" s="466" t="s">
+        <v>388</v>
+      </c>
       <c r="H89" s="466"/>
       <c r="I89" s="243" t="s">
-        <v>261</v>
+        <v>301</v>
       </c>
       <c r="J89" s="244"/>
       <c r="K89" s="233"/>
@@ -7280,17 +7298,14 @@
       <c r="M89" s="225"/>
       <c r="N89" s="225"/>
       <c r="P89" s="133" t="s">
-        <v>468</v>
-      </c>
-      <c r="Q89" s="141" t="s">
-        <v>472</v>
+        <v>478</v>
+      </c>
+      <c r="Q89" s="147" t="s">
+        <v>108</v>
       </c>
       <c r="R89" s="11"/>
-      <c r="X89" s="4" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="90" spans="2:28" ht="31" customHeight="1">
+    </row>
+    <row r="90" spans="2:19" ht="31" customHeight="1">
       <c r="B90" s="485"/>
       <c r="D90" s="450"/>
       <c r="E90" s="465"/>
@@ -7298,7 +7313,7 @@
       <c r="G90" s="466"/>
       <c r="H90" s="466"/>
       <c r="I90" s="243" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J90" s="244"/>
       <c r="K90" s="233"/>
@@ -7306,77 +7321,72 @@
       <c r="M90" s="225"/>
       <c r="N90" s="225"/>
       <c r="P90" s="133" t="s">
-        <v>478</v>
-      </c>
-      <c r="Q90" s="147" t="s">
-        <v>109</v>
+        <v>468</v>
+      </c>
+      <c r="Q90" s="141" t="s">
+        <v>472</v>
       </c>
       <c r="R90" s="11"/>
-      <c r="X90" s="488" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="91" spans="2:28" ht="31" customHeight="1">
-      <c r="B91" s="485" t="s">
-        <v>612</v>
-      </c>
-      <c r="D91" s="460" t="s">
-        <v>467</v>
-      </c>
-      <c r="E91" s="451" t="s">
-        <v>137</v>
-      </c>
-      <c r="F91" s="451"/>
-      <c r="G91" s="232"/>
-      <c r="H91" s="232"/>
-      <c r="I91" s="232"/>
-      <c r="J91" s="232"/>
-      <c r="K91" s="232"/>
-      <c r="L91" s="232"/>
+    </row>
+    <row r="91" spans="2:19" ht="31" customHeight="1">
+      <c r="B91" s="485"/>
+      <c r="D91" s="450"/>
+      <c r="E91" s="465"/>
+      <c r="F91" s="465"/>
+      <c r="G91" s="466"/>
+      <c r="H91" s="466"/>
+      <c r="I91" s="243" t="s">
+        <v>261</v>
+      </c>
+      <c r="J91" s="244"/>
+      <c r="K91" s="233"/>
+      <c r="L91" s="233"/>
       <c r="M91" s="225"/>
       <c r="N91" s="225"/>
       <c r="P91" s="133" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q91" s="147" t="s">
-        <v>129</v>
+        <v>468</v>
+      </c>
+      <c r="Q91" s="141" t="s">
+        <v>472</v>
       </c>
       <c r="R91" s="11"/>
     </row>
-    <row r="92" spans="2:28" ht="31" customHeight="1">
+    <row r="92" spans="2:19" ht="31" customHeight="1">
       <c r="B92" s="485"/>
-      <c r="D92" s="460"/>
-      <c r="E92" s="451" t="s">
-        <v>283</v>
-      </c>
-      <c r="F92" s="451"/>
-      <c r="G92" s="232"/>
-      <c r="H92" s="232"/>
-      <c r="I92" s="232"/>
-      <c r="J92" s="232"/>
-      <c r="K92" s="232"/>
-      <c r="L92" s="232"/>
+      <c r="D92" s="450"/>
+      <c r="E92" s="465"/>
+      <c r="F92" s="465"/>
+      <c r="G92" s="466"/>
+      <c r="H92" s="466"/>
+      <c r="I92" s="243" t="s">
+        <v>269</v>
+      </c>
+      <c r="J92" s="244"/>
+      <c r="K92" s="233"/>
+      <c r="L92" s="233"/>
       <c r="M92" s="225"/>
       <c r="N92" s="225"/>
       <c r="P92" s="133" t="s">
-        <v>468</v>
-      </c>
-      <c r="Q92" s="138" t="s">
-        <v>469</v>
+        <v>478</v>
+      </c>
+      <c r="Q92" s="147" t="s">
+        <v>109</v>
       </c>
       <c r="R92" s="11"/>
     </row>
-    <row r="93" spans="2:28" ht="31" customHeight="1">
-      <c r="B93" s="485"/>
-      <c r="D93" s="460"/>
+    <row r="93" spans="2:19" ht="31" customHeight="1">
+      <c r="B93" s="485" t="s">
+        <v>612</v>
+      </c>
+      <c r="D93" s="460" t="s">
+        <v>467</v>
+      </c>
       <c r="E93" s="451" t="s">
-        <v>306</v>
+        <v>137</v>
       </c>
       <c r="F93" s="451"/>
-      <c r="G93" s="246" t="s">
-        <v>470</v>
-      </c>
-      <c r="H93" s="246"/>
+      <c r="G93" s="232"/>
+      <c r="H93" s="232"/>
       <c r="I93" s="232"/>
       <c r="J93" s="232"/>
       <c r="K93" s="232"/>
@@ -7384,22 +7394,22 @@
       <c r="M93" s="225"/>
       <c r="N93" s="225"/>
       <c r="P93" s="133" t="s">
-        <v>474</v>
-      </c>
-      <c r="Q93" s="141" t="s">
-        <v>473</v>
+        <v>97</v>
+      </c>
+      <c r="Q93" s="147" t="s">
+        <v>129</v>
       </c>
       <c r="R93" s="11"/>
     </row>
-    <row r="94" spans="2:28" ht="31" customHeight="1">
+    <row r="94" spans="2:19" ht="31" customHeight="1">
       <c r="B94" s="485"/>
       <c r="D94" s="460"/>
-      <c r="E94" s="451"/>
+      <c r="E94" s="451" t="s">
+        <v>283</v>
+      </c>
       <c r="F94" s="451"/>
-      <c r="G94" s="246" t="s">
-        <v>471</v>
-      </c>
-      <c r="H94" s="246"/>
+      <c r="G94" s="232"/>
+      <c r="H94" s="232"/>
       <c r="I94" s="232"/>
       <c r="J94" s="232"/>
       <c r="K94" s="232"/>
@@ -7409,20 +7419,22 @@
       <c r="P94" s="133" t="s">
         <v>468</v>
       </c>
-      <c r="Q94" s="141" t="s">
-        <v>472</v>
+      <c r="Q94" s="138" t="s">
+        <v>469</v>
       </c>
       <c r="R94" s="11"/>
     </row>
-    <row r="95" spans="2:28" ht="31" customHeight="1">
+    <row r="95" spans="2:19" ht="31" customHeight="1">
       <c r="B95" s="485"/>
       <c r="D95" s="460"/>
       <c r="E95" s="451" t="s">
-        <v>28</v>
+        <v>306</v>
       </c>
       <c r="F95" s="451"/>
-      <c r="G95" s="232"/>
-      <c r="H95" s="232"/>
+      <c r="G95" s="246" t="s">
+        <v>470</v>
+      </c>
+      <c r="H95" s="246"/>
       <c r="I95" s="232"/>
       <c r="J95" s="232"/>
       <c r="K95" s="232"/>
@@ -7437,15 +7449,15 @@
       </c>
       <c r="R95" s="11"/>
     </row>
-    <row r="96" spans="2:28" ht="31" customHeight="1">
+    <row r="96" spans="2:19" ht="31" customHeight="1">
       <c r="B96" s="485"/>
       <c r="D96" s="460"/>
-      <c r="E96" s="451" t="s">
-        <v>386</v>
-      </c>
+      <c r="E96" s="451"/>
       <c r="F96" s="451"/>
-      <c r="G96" s="232"/>
-      <c r="H96" s="232"/>
+      <c r="G96" s="246" t="s">
+        <v>471</v>
+      </c>
+      <c r="H96" s="246"/>
       <c r="I96" s="232"/>
       <c r="J96" s="232"/>
       <c r="K96" s="232"/>
@@ -7453,10 +7465,10 @@
       <c r="M96" s="225"/>
       <c r="N96" s="225"/>
       <c r="P96" s="133" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q96" s="116" t="b">
-        <v>1</v>
+        <v>468</v>
+      </c>
+      <c r="Q96" s="141" t="s">
+        <v>472</v>
       </c>
       <c r="R96" s="11"/>
     </row>
@@ -7464,13 +7476,11 @@
       <c r="B97" s="485"/>
       <c r="D97" s="460"/>
       <c r="E97" s="451" t="s">
-        <v>305</v>
+        <v>28</v>
       </c>
       <c r="F97" s="451"/>
-      <c r="G97" s="246" t="s">
-        <v>384</v>
-      </c>
-      <c r="H97" s="246"/>
+      <c r="G97" s="232"/>
+      <c r="H97" s="232"/>
       <c r="I97" s="232"/>
       <c r="J97" s="232"/>
       <c r="K97" s="232"/>
@@ -7478,58 +7488,58 @@
       <c r="M97" s="225"/>
       <c r="N97" s="225"/>
       <c r="P97" s="133" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q97" s="116" t="b">
-        <v>1</v>
+        <v>474</v>
+      </c>
+      <c r="Q97" s="141" t="s">
+        <v>473</v>
       </c>
       <c r="R97" s="11"/>
     </row>
     <row r="98" spans="2:18" ht="31" customHeight="1">
       <c r="B98" s="485"/>
       <c r="D98" s="460"/>
-      <c r="E98" s="451"/>
+      <c r="E98" s="451" t="s">
+        <v>386</v>
+      </c>
       <c r="F98" s="451"/>
-      <c r="G98" s="246" t="s">
-        <v>385</v>
-      </c>
-      <c r="H98" s="246"/>
-      <c r="I98" s="255">
-        <v>1</v>
-      </c>
-      <c r="J98" s="255"/>
-      <c r="K98" s="233"/>
-      <c r="L98" s="233"/>
+      <c r="G98" s="232"/>
+      <c r="H98" s="232"/>
+      <c r="I98" s="232"/>
+      <c r="J98" s="232"/>
+      <c r="K98" s="232"/>
+      <c r="L98" s="232"/>
       <c r="M98" s="225"/>
       <c r="N98" s="225"/>
       <c r="P98" s="133" t="s">
-        <v>475</v>
-      </c>
-      <c r="Q98" s="141" t="s">
-        <v>460</v>
+        <v>122</v>
+      </c>
+      <c r="Q98" s="116" t="b">
+        <v>1</v>
       </c>
       <c r="R98" s="11"/>
     </row>
     <row r="99" spans="2:18" ht="31" customHeight="1">
       <c r="B99" s="485"/>
       <c r="D99" s="460"/>
-      <c r="E99" s="451"/>
+      <c r="E99" s="451" t="s">
+        <v>305</v>
+      </c>
       <c r="F99" s="451"/>
-      <c r="G99" s="246"/>
+      <c r="G99" s="246" t="s">
+        <v>384</v>
+      </c>
       <c r="H99" s="246"/>
-      <c r="I99" s="255">
-        <v>2</v>
-      </c>
-      <c r="J99" s="255"/>
-      <c r="K99" s="233"/>
-      <c r="L99" s="233"/>
+      <c r="I99" s="232"/>
+      <c r="J99" s="232"/>
+      <c r="K99" s="232"/>
+      <c r="L99" s="232"/>
       <c r="M99" s="225"/>
       <c r="N99" s="225"/>
       <c r="P99" s="133" t="s">
-        <v>475</v>
-      </c>
-      <c r="Q99" s="141" t="s">
-        <v>460</v>
+        <v>122</v>
+      </c>
+      <c r="Q99" s="116" t="b">
+        <v>1</v>
       </c>
       <c r="R99" s="11"/>
     </row>
@@ -7538,10 +7548,12 @@
       <c r="D100" s="460"/>
       <c r="E100" s="451"/>
       <c r="F100" s="451"/>
-      <c r="G100" s="246"/>
+      <c r="G100" s="246" t="s">
+        <v>385</v>
+      </c>
       <c r="H100" s="246"/>
       <c r="I100" s="255">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J100" s="255"/>
       <c r="K100" s="233"/>
@@ -7564,7 +7576,7 @@
       <c r="G101" s="246"/>
       <c r="H101" s="246"/>
       <c r="I101" s="255">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J101" s="255"/>
       <c r="K101" s="233"/>
@@ -7582,25 +7594,23 @@
     <row r="102" spans="2:18" ht="31" customHeight="1">
       <c r="B102" s="485"/>
       <c r="D102" s="460"/>
-      <c r="E102" s="451" t="s">
-        <v>307</v>
-      </c>
+      <c r="E102" s="451"/>
       <c r="F102" s="451"/>
-      <c r="G102" s="246" t="s">
-        <v>308</v>
-      </c>
+      <c r="G102" s="246"/>
       <c r="H102" s="246"/>
-      <c r="I102" s="232"/>
-      <c r="J102" s="232"/>
-      <c r="K102" s="232"/>
-      <c r="L102" s="232"/>
+      <c r="I102" s="255">
+        <v>3</v>
+      </c>
+      <c r="J102" s="255"/>
+      <c r="K102" s="233"/>
+      <c r="L102" s="233"/>
       <c r="M102" s="225"/>
       <c r="N102" s="225"/>
       <c r="P102" s="133" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q102" s="116">
-        <v>0</v>
+        <v>475</v>
+      </c>
+      <c r="Q102" s="141" t="s">
+        <v>460</v>
       </c>
       <c r="R102" s="11"/>
     </row>
@@ -7609,14 +7619,14 @@
       <c r="D103" s="460"/>
       <c r="E103" s="451"/>
       <c r="F103" s="451"/>
-      <c r="G103" s="246" t="s">
-        <v>309</v>
-      </c>
+      <c r="G103" s="246"/>
       <c r="H103" s="246"/>
-      <c r="I103" s="232"/>
-      <c r="J103" s="232"/>
-      <c r="K103" s="232"/>
-      <c r="L103" s="232"/>
+      <c r="I103" s="255">
+        <v>4</v>
+      </c>
+      <c r="J103" s="255"/>
+      <c r="K103" s="233"/>
+      <c r="L103" s="233"/>
       <c r="M103" s="225"/>
       <c r="N103" s="225"/>
       <c r="P103" s="133" t="s">
@@ -7627,116 +7637,168 @@
       </c>
       <c r="R103" s="11"/>
     </row>
-    <row r="104" spans="2:18" ht="26">
-      <c r="D104" s="224"/>
-      <c r="E104" s="227"/>
+    <row r="104" spans="2:18" ht="31" customHeight="1">
+      <c r="B104" s="485"/>
+      <c r="D104" s="460"/>
+      <c r="E104" s="451" t="s">
+        <v>307</v>
+      </c>
+      <c r="F104" s="451"/>
+      <c r="G104" s="246" t="s">
+        <v>308</v>
+      </c>
+      <c r="H104" s="246"/>
+      <c r="I104" s="232"/>
+      <c r="J104" s="232"/>
+      <c r="K104" s="232"/>
+      <c r="L104" s="232"/>
       <c r="M104" s="225"/>
       <c r="N104" s="225"/>
-    </row>
-    <row r="105" spans="2:18" ht="26">
-      <c r="D105" s="224"/>
-      <c r="E105" s="227"/>
+      <c r="P104" s="133" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q104" s="116">
+        <v>0</v>
+      </c>
+      <c r="R104" s="11"/>
+    </row>
+    <row r="105" spans="2:18" ht="31" customHeight="1">
+      <c r="B105" s="485"/>
+      <c r="D105" s="460"/>
+      <c r="E105" s="451"/>
+      <c r="F105" s="451"/>
+      <c r="G105" s="246" t="s">
+        <v>309</v>
+      </c>
+      <c r="H105" s="246"/>
+      <c r="I105" s="232"/>
+      <c r="J105" s="232"/>
+      <c r="K105" s="232"/>
+      <c r="L105" s="232"/>
       <c r="M105" s="225"/>
       <c r="N105" s="225"/>
-    </row>
-    <row r="108" spans="2:18">
-      <c r="D108" s="223" t="s">
+      <c r="P105" s="133" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q105" s="141" t="s">
+        <v>460</v>
+      </c>
+      <c r="R105" s="11"/>
+    </row>
+    <row r="106" spans="2:18" ht="26">
+      <c r="D106" s="224"/>
+      <c r="E106" s="227"/>
+      <c r="M106" s="225"/>
+      <c r="N106" s="225"/>
+    </row>
+    <row r="107" spans="2:18" ht="26">
+      <c r="D107" s="224"/>
+      <c r="E107" s="227"/>
+      <c r="M107" s="225"/>
+      <c r="N107" s="225"/>
+    </row>
+    <row r="110" spans="2:18">
+      <c r="D110" s="223" t="s">
         <v>310</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="237">
-    <mergeCell ref="B41:B57"/>
+  <mergeCells count="241">
+    <mergeCell ref="B42:B59"/>
     <mergeCell ref="A1:J1"/>
-    <mergeCell ref="I86:L86"/>
-    <mergeCell ref="D41:D45"/>
-    <mergeCell ref="D46:D57"/>
-    <mergeCell ref="D34:D40"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="E46:E57"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="I88:L88"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:L46"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:L33"/>
+    <mergeCell ref="D42:D47"/>
+    <mergeCell ref="D48:D59"/>
+    <mergeCell ref="D35:D41"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="E48:E59"/>
     <mergeCell ref="G48:H48"/>
     <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G50:H53"/>
-    <mergeCell ref="G54:H57"/>
-    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G52:H55"/>
+    <mergeCell ref="G56:H59"/>
     <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="G41:L41"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H41"/>
     <mergeCell ref="E42:F42"/>
     <mergeCell ref="G42:L42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:L43"/>
     <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M67:M68"/>
-    <mergeCell ref="K67:L68"/>
-    <mergeCell ref="G64:H68"/>
-    <mergeCell ref="E69:E74"/>
-    <mergeCell ref="F69:F74"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="I69:L69"/>
-    <mergeCell ref="G70:H74"/>
-    <mergeCell ref="I70:I74"/>
-    <mergeCell ref="J70:J74"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="M69:M70"/>
+    <mergeCell ref="K69:L70"/>
+    <mergeCell ref="G66:H70"/>
+    <mergeCell ref="E71:E76"/>
+    <mergeCell ref="F71:F76"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="I71:L71"/>
+    <mergeCell ref="G72:H76"/>
+    <mergeCell ref="I72:I76"/>
+    <mergeCell ref="J72:J76"/>
     <mergeCell ref="K72:L72"/>
-    <mergeCell ref="K73:L74"/>
-    <mergeCell ref="M73:M74"/>
-    <mergeCell ref="E62:L62"/>
-    <mergeCell ref="B80:B90"/>
-    <mergeCell ref="B91:B103"/>
-    <mergeCell ref="D75:D79"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="K74:L74"/>
+    <mergeCell ref="K75:L76"/>
+    <mergeCell ref="M75:M76"/>
+    <mergeCell ref="E64:L64"/>
+    <mergeCell ref="B82:B92"/>
+    <mergeCell ref="B93:B105"/>
+    <mergeCell ref="D77:D81"/>
     <mergeCell ref="E77:F77"/>
     <mergeCell ref="E78:F78"/>
     <mergeCell ref="E79:F79"/>
+    <mergeCell ref="E80:F80"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="G80:L80"/>
+    <mergeCell ref="G81:L81"/>
     <mergeCell ref="G78:L78"/>
-    <mergeCell ref="G79:L79"/>
-    <mergeCell ref="G76:L76"/>
-    <mergeCell ref="G75:L75"/>
-    <mergeCell ref="I77:L77"/>
-    <mergeCell ref="G61:L61"/>
-    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G77:L77"/>
+    <mergeCell ref="I79:L79"/>
+    <mergeCell ref="G63:L63"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:L45"/>
+    <mergeCell ref="G88:H88"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="I51:L51"/>
     <mergeCell ref="G44:L44"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="I49:L49"/>
-    <mergeCell ref="G43:L43"/>
-    <mergeCell ref="G45:L45"/>
-    <mergeCell ref="D63:D74"/>
+    <mergeCell ref="G47:L47"/>
+    <mergeCell ref="D65:D76"/>
     <mergeCell ref="B6:B15"/>
     <mergeCell ref="B16:B24"/>
     <mergeCell ref="B25:B30"/>
-    <mergeCell ref="B31:B40"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B63:B79"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:L33"/>
-    <mergeCell ref="E63:E68"/>
-    <mergeCell ref="F63:F68"/>
-    <mergeCell ref="I63:L63"/>
-    <mergeCell ref="I64:I68"/>
-    <mergeCell ref="J64:J68"/>
-    <mergeCell ref="D91:D103"/>
-    <mergeCell ref="D58:D60"/>
+    <mergeCell ref="B31:B41"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B65:B81"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:L34"/>
+    <mergeCell ref="E65:E70"/>
+    <mergeCell ref="F65:F70"/>
+    <mergeCell ref="I65:L65"/>
+    <mergeCell ref="I66:I70"/>
+    <mergeCell ref="J66:J70"/>
+    <mergeCell ref="D93:D105"/>
+    <mergeCell ref="D60:D62"/>
     <mergeCell ref="D16:D24"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E34:E40"/>
-    <mergeCell ref="F34:F40"/>
-    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="E35:E41"/>
+    <mergeCell ref="F35:F41"/>
     <mergeCell ref="I37:J37"/>
     <mergeCell ref="I38:J38"/>
     <mergeCell ref="I39:J39"/>
     <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I34:L34"/>
+    <mergeCell ref="I41:J41"/>
     <mergeCell ref="I35:L35"/>
+    <mergeCell ref="I36:L36"/>
     <mergeCell ref="G31:L31"/>
     <mergeCell ref="G32:L32"/>
-    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="G10:H10"/>
@@ -7744,8 +7806,8 @@
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="F46:F57"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="F48:F59"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I3:J3"/>
@@ -7760,17 +7822,17 @@
     <mergeCell ref="I13:L13"/>
     <mergeCell ref="I14:L14"/>
     <mergeCell ref="I15:L15"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="I51:J51"/>
     <mergeCell ref="I52:J52"/>
     <mergeCell ref="I53:J53"/>
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="I56:J56"/>
     <mergeCell ref="I57:J57"/>
-    <mergeCell ref="I46:L46"/>
-    <mergeCell ref="I47:L47"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="I59:J59"/>
     <mergeCell ref="I48:L48"/>
+    <mergeCell ref="I49:L49"/>
+    <mergeCell ref="I50:L50"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="I16:L16"/>
     <mergeCell ref="I17:L17"/>
@@ -7787,12 +7849,12 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G26:L26"/>
     <mergeCell ref="G25:L25"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E61:F61"/>
     <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="G58:L58"/>
-    <mergeCell ref="G59:L59"/>
     <mergeCell ref="G60:L60"/>
+    <mergeCell ref="G61:L61"/>
+    <mergeCell ref="G62:L62"/>
     <mergeCell ref="I22:L22"/>
     <mergeCell ref="I23:L23"/>
     <mergeCell ref="I24:L24"/>
@@ -7803,65 +7865,65 @@
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G87:H90"/>
-    <mergeCell ref="E80:F80"/>
+    <mergeCell ref="G89:H92"/>
     <mergeCell ref="E82:F82"/>
-    <mergeCell ref="E83:F83"/>
-    <mergeCell ref="E102:F103"/>
-    <mergeCell ref="G102:H102"/>
-    <mergeCell ref="G103:H103"/>
-    <mergeCell ref="G98:H101"/>
-    <mergeCell ref="G97:H97"/>
-    <mergeCell ref="G94:H94"/>
-    <mergeCell ref="E93:F94"/>
-    <mergeCell ref="E97:F101"/>
-    <mergeCell ref="E91:F91"/>
-    <mergeCell ref="E92:F92"/>
-    <mergeCell ref="E96:F96"/>
-    <mergeCell ref="E95:F95"/>
-    <mergeCell ref="I102:L102"/>
-    <mergeCell ref="I103:L103"/>
-    <mergeCell ref="I94:L94"/>
-    <mergeCell ref="K101:L101"/>
-    <mergeCell ref="G93:H93"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="E104:F105"/>
+    <mergeCell ref="G104:H104"/>
+    <mergeCell ref="G105:H105"/>
+    <mergeCell ref="G100:H103"/>
+    <mergeCell ref="G99:H99"/>
+    <mergeCell ref="G96:H96"/>
+    <mergeCell ref="E95:F96"/>
+    <mergeCell ref="E99:F103"/>
+    <mergeCell ref="E93:F93"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="E97:F97"/>
+    <mergeCell ref="I104:L104"/>
+    <mergeCell ref="I105:L105"/>
+    <mergeCell ref="I96:L96"/>
+    <mergeCell ref="K103:L103"/>
+    <mergeCell ref="G95:H95"/>
+    <mergeCell ref="I103:J103"/>
+    <mergeCell ref="I102:J102"/>
     <mergeCell ref="I101:J101"/>
     <mergeCell ref="I100:J100"/>
-    <mergeCell ref="I99:J99"/>
-    <mergeCell ref="I98:J98"/>
-    <mergeCell ref="G95:L95"/>
-    <mergeCell ref="G96:L96"/>
-    <mergeCell ref="I93:L93"/>
+    <mergeCell ref="G97:L97"/>
+    <mergeCell ref="G98:L98"/>
+    <mergeCell ref="I95:L95"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K100:L100"/>
+    <mergeCell ref="K101:L101"/>
+    <mergeCell ref="K102:L102"/>
+    <mergeCell ref="E6:L6"/>
+    <mergeCell ref="I99:L99"/>
+    <mergeCell ref="G93:L93"/>
+    <mergeCell ref="G94:L94"/>
+    <mergeCell ref="K92:L92"/>
+    <mergeCell ref="G85:L85"/>
+    <mergeCell ref="G82:L82"/>
+    <mergeCell ref="G84:L84"/>
+    <mergeCell ref="I92:J92"/>
+    <mergeCell ref="G87:H87"/>
+    <mergeCell ref="I90:J90"/>
+    <mergeCell ref="I91:J91"/>
     <mergeCell ref="K55:L55"/>
     <mergeCell ref="K54:L54"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K98:L98"/>
-    <mergeCell ref="K99:L99"/>
-    <mergeCell ref="K100:L100"/>
-    <mergeCell ref="E6:L6"/>
-    <mergeCell ref="I97:L97"/>
-    <mergeCell ref="G91:L91"/>
-    <mergeCell ref="G92:L92"/>
-    <mergeCell ref="K90:L90"/>
-    <mergeCell ref="G83:L83"/>
-    <mergeCell ref="G80:L80"/>
-    <mergeCell ref="G82:L82"/>
-    <mergeCell ref="I90:J90"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="I88:J88"/>
-    <mergeCell ref="I89:J89"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="K52:L52"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="K36:L36"/>
     <mergeCell ref="K37:L37"/>
     <mergeCell ref="K38:L38"/>
     <mergeCell ref="K39:L39"/>
     <mergeCell ref="K40:L40"/>
-    <mergeCell ref="E81:F81"/>
-    <mergeCell ref="G81:L81"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="I84:L84"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="G83:L83"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="I86:L86"/>
     <mergeCell ref="D7:D15"/>
     <mergeCell ref="E10:F15"/>
     <mergeCell ref="D25:D30"/>
@@ -7871,18 +7933,18 @@
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="E25:F25"/>
-    <mergeCell ref="K64:L64"/>
-    <mergeCell ref="K65:L65"/>
     <mergeCell ref="K66:L66"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="D80:D90"/>
-    <mergeCell ref="E84:F90"/>
-    <mergeCell ref="K87:L87"/>
-    <mergeCell ref="K88:L88"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D82:D92"/>
+    <mergeCell ref="E86:F92"/>
     <mergeCell ref="K89:L89"/>
-    <mergeCell ref="I85:L85"/>
-    <mergeCell ref="I87:J87"/>
+    <mergeCell ref="K90:L90"/>
+    <mergeCell ref="K91:L91"/>
+    <mergeCell ref="I87:L87"/>
+    <mergeCell ref="I89:J89"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor load code into a seperate module withing tickers
</commit_message>
<xml_diff>
--- a/docs/session_variables.xlsx
+++ b/docs/session_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robhay/git_repo/share_screener/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C9D3D2-BB8E-EA4B-A274-A7E8B54747D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A76A6E-775B-554A-8A30-2B0771134F9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-65300" yWindow="-14020" windowWidth="49880" windowHeight="24720" xr2:uid="{EB3C945B-FE01-FA47-AE59-A0DC3CDF521B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{EB3C945B-FE01-FA47-AE59-A0DC3CDF521B}"/>
   </bookViews>
   <sheets>
     <sheet name="Application Structure" sheetId="10" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="669">
   <si>
     <t>chart_colours</t>
   </si>
@@ -2295,6 +2295,18 @@
   </si>
   <si>
     <t>caches the current download type - ie single  or multiple tickers have different schemas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '</t>
+  </si>
+  <si>
+    <t>cba.ax nab.ax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>single_ticker</t>
   </si>
 </sst>
 </file>
@@ -2988,7 +3000,7 @@
     <xf numFmtId="43" fontId="29" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="29" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="303">
+  <cellXfs count="304">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3785,6 +3797,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4108,7 +4123,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G83" sqref="G83:L83"/>
+      <selection pane="bottomRight" activeCell="S75" sqref="S75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -6127,9 +6142,15 @@
       <c r="K82" s="166"/>
       <c r="L82" s="166"/>
       <c r="M82" s="119"/>
-      <c r="O82" s="60"/>
-      <c r="P82" s="64"/>
-      <c r="Q82" s="11"/>
+      <c r="O82" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="P82" s="303" t="s">
+        <v>665</v>
+      </c>
+      <c r="Q82" s="56" t="s">
+        <v>666</v>
+      </c>
       <c r="R82" s="9"/>
     </row>
     <row r="83" spans="2:18" ht="31" customHeight="1">
@@ -6148,9 +6169,15 @@
       <c r="K83" s="166"/>
       <c r="L83" s="166"/>
       <c r="M83" s="119"/>
-      <c r="O83" s="60"/>
-      <c r="P83" s="64"/>
-      <c r="Q83" s="11"/>
+      <c r="O83" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="P83" s="303" t="s">
+        <v>667</v>
+      </c>
+      <c r="Q83" s="56" t="s">
+        <v>668</v>
+      </c>
       <c r="R83" s="9"/>
     </row>
     <row r="84" spans="2:18" ht="31" customHeight="1">
@@ -6175,7 +6202,9 @@
       <c r="P84" s="64" t="s">
         <v>661</v>
       </c>
-      <c r="Q84" s="11"/>
+      <c r="Q84" s="56" t="s">
+        <v>312</v>
+      </c>
       <c r="R84" s="9"/>
     </row>
     <row r="85" spans="2:18" ht="31" customHeight="1">

</xml_diff>